<commit_message>
Update 7-Jan-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="73">
   <si>
     <t>Tgl</t>
   </si>
@@ -195,6 +195,48 @@
   </si>
   <si>
     <t>GUSTAVI</t>
+  </si>
+  <si>
+    <t>TRANSFER BCA</t>
+  </si>
+  <si>
+    <t>A/R</t>
+  </si>
+  <si>
+    <t>BELI sanitizer</t>
+  </si>
+  <si>
+    <t>SALES - cash/retail</t>
+  </si>
+  <si>
+    <t>SELISIH - lebih</t>
+  </si>
+  <si>
+    <t>SETOR KE BANK</t>
+  </si>
+  <si>
+    <t>FREIGHT-IN</t>
+  </si>
+  <si>
+    <t>BELI kresek</t>
+  </si>
+  <si>
+    <t>CHEQUE RECEIVED</t>
+  </si>
+  <si>
+    <t>IURAN DAERAH</t>
+  </si>
+  <si>
+    <t>A/P</t>
+  </si>
+  <si>
+    <t>BENSIN - RUSH</t>
+  </si>
+  <si>
+    <t>TRANSFER DANAMON</t>
+  </si>
+  <si>
+    <t>PARKIR - bulanan</t>
   </si>
 </sst>
 </file>
@@ -562,8 +604,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <pane ySplit="2" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -609,673 +651,886 @@
       <c r="B3" t="s">
         <v>25</v>
       </c>
+      <c r="D3" s="1">
+        <f>45000+240000</f>
+        <v>285000</v>
+      </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>434025</v>
+        <v>149025</v>
       </c>
     </row>
     <row r="4" spans="1:6">
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="1">
+        <f>5170000+1040000+450000+7374000+1338000+586000+3467000+3219000+5170000+40000000+920000</f>
+        <v>68734000</v>
+      </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>434025</v>
+        <v>-68584975</v>
       </c>
     </row>
     <row r="5" spans="1:6">
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="1">
+        <f>7374000+2211000+1500000+100000000+94174000</f>
+        <v>205259000</v>
+      </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>434025</v>
+        <v>136674025</v>
       </c>
     </row>
     <row r="6" spans="1:6">
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="1">
+        <f>50000</f>
+        <v>50000</v>
+      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>434025</v>
+        <v>136624025</v>
       </c>
     </row>
     <row r="7" spans="1:6">
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="1">
+        <f>166645025-43610025-94174000</f>
+        <v>28861000</v>
+      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>434025</v>
+        <v>165485025</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="1">
+        <v>70000</v>
+      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>434025</v>
+        <v>165555025</v>
       </c>
     </row>
     <row r="9" spans="1:6">
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="1">
+        <v>165000000</v>
+      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>434025</v>
+        <v>555025</v>
       </c>
     </row>
     <row r="10" spans="1:6">
+      <c r="A10" s="2">
+        <v>44201</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="1">
+        <f>45000+150000+195000</f>
+        <v>390000</v>
+      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>434025</v>
+        <v>165025</v>
       </c>
     </row>
     <row r="11" spans="1:6">
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="1">
+        <f>5540000+1658000+1012500+440000</f>
+        <v>8650500</v>
+      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>434025</v>
+        <v>-8485475</v>
       </c>
     </row>
     <row r="12" spans="1:6">
+      <c r="B12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1600000</v>
+      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>434025</v>
+        <v>-10085475</v>
       </c>
     </row>
     <row r="13" spans="1:6">
+      <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="1">
+        <f>18006025+9890475-20113000</f>
+        <v>7783500</v>
+      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>434025</v>
+        <v>-2301975</v>
       </c>
     </row>
     <row r="14" spans="1:6">
+      <c r="B14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="1">
+        <f>20113000</f>
+        <v>20113000</v>
+      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>434025</v>
+        <v>17811025</v>
       </c>
     </row>
     <row r="15" spans="1:6">
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="1">
+        <v>20000</v>
+      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>434025</v>
+        <v>17831025</v>
       </c>
     </row>
     <row r="16" spans="1:6">
+      <c r="B16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="1">
+        <v>17000000</v>
+      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>434025</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5">
+        <v>831025</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2">
+        <v>44202</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="1">
+        <f>45000+255000</f>
+        <v>300000</v>
+      </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>434025</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5">
+        <v>531025</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="B18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="1">
+        <f>680000+22000000+6382000+1227000</f>
+        <v>30289000</v>
+      </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>434025</v>
-      </c>
-    </row>
-    <row r="19" spans="5:5">
+        <v>-29757975</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="B19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="1">
+        <f>2000000+5000000+100000000+82801000</f>
+        <v>189801000</v>
+      </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>434025</v>
-      </c>
-    </row>
-    <row r="20" spans="5:5">
+        <v>160043025</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="B20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="1">
+        <f>95000</f>
+        <v>95000</v>
+      </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>434025</v>
-      </c>
-    </row>
-    <row r="21" spans="5:5">
+        <v>159948025</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="1">
+        <f>2169000</f>
+        <v>2169000</v>
+      </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>434025</v>
-      </c>
-    </row>
-    <row r="22" spans="5:5">
+        <v>157779025</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="B22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="1">
+        <f>25000</f>
+        <v>25000</v>
+      </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>434025</v>
-      </c>
-    </row>
-    <row r="23" spans="5:5">
+        <v>157754025</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="B23" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="1">
+        <f>1266000</f>
+        <v>1266000</v>
+      </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>434025</v>
-      </c>
-    </row>
-    <row r="24" spans="5:5">
+        <v>156488025</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="B24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="1">
+        <v>250000</v>
+      </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>434025</v>
-      </c>
-    </row>
-    <row r="25" spans="5:5">
+        <v>156238025</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="B25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="1">
+        <f>166021025-73732025-82801000</f>
+        <v>9488000</v>
+      </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>434025</v>
-      </c>
-    </row>
-    <row r="26" spans="5:5">
+        <v>165726025</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="B26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="1">
+        <v>68000</v>
+      </c>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>434025</v>
-      </c>
-    </row>
-    <row r="27" spans="5:5">
+        <v>165794025</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="B27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="1">
+        <v>165000000</v>
+      </c>
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>434025</v>
-      </c>
-    </row>
-    <row r="28" spans="5:5">
+        <v>794025</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="2">
+        <v>44203</v>
+      </c>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="1">
+        <f>45000</f>
+        <v>45000</v>
+      </c>
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>434025</v>
-      </c>
-    </row>
-    <row r="29" spans="5:5">
+        <v>749025</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="B29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="1">
+        <f>19800000+851000+9149000</f>
+        <v>29800000</v>
+      </c>
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>434025</v>
-      </c>
-    </row>
-    <row r="30" spans="5:5">
+        <v>30549025</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="B30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" s="1">
+        <f>19800000</f>
+        <v>19800000</v>
+      </c>
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>434025</v>
-      </c>
-    </row>
-    <row r="31" spans="5:5">
+        <v>10749025</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="B31" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" s="1">
+        <v>10000</v>
+      </c>
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>434025</v>
-      </c>
-    </row>
-    <row r="32" spans="5:5">
+        <v>10739025</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="B32" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" s="1">
+        <f>215000+308000+1240000</f>
+        <v>1763000</v>
+      </c>
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>434025</v>
-      </c>
-    </row>
-    <row r="33" spans="5:6">
+        <v>8976025</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6">
+      <c r="B33" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" s="1">
+        <v>6400000</v>
+      </c>
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>434025</v>
-      </c>
-    </row>
-    <row r="34" spans="5:6">
+        <v>2576025</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>434025</v>
-      </c>
-    </row>
-    <row r="35" spans="5:6">
+        <v>2576025</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>434025</v>
-      </c>
-    </row>
-    <row r="36" spans="5:6">
+        <v>2576025</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>434025</v>
-      </c>
-    </row>
-    <row r="37" spans="5:6">
+        <v>2576025</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>434025</v>
-      </c>
-    </row>
-    <row r="38" spans="5:6">
+        <v>2576025</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>434025</v>
-      </c>
-    </row>
-    <row r="39" spans="5:6">
+        <v>2576025</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>434025</v>
-      </c>
-    </row>
-    <row r="40" spans="5:6">
+        <v>2576025</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="5:6">
+    <row r="41" spans="2:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>434025</v>
-      </c>
-    </row>
-    <row r="42" spans="5:6">
+        <v>2576025</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>434025</v>
-      </c>
-    </row>
-    <row r="43" spans="5:6">
+        <v>2576025</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>434025</v>
-      </c>
-    </row>
-    <row r="44" spans="5:6">
+        <v>2576025</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>434025</v>
-      </c>
-    </row>
-    <row r="45" spans="5:6">
+        <v>2576025</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>434025</v>
-      </c>
-    </row>
-    <row r="46" spans="5:6">
+        <v>2576025</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>434025</v>
-      </c>
-    </row>
-    <row r="47" spans="5:6">
+        <v>2576025</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>434025</v>
-      </c>
-    </row>
-    <row r="48" spans="5:6">
+        <v>2576025</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>434025</v>
+        <v>2576025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 8-Jan-2021, end of day.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="74">
   <si>
     <t>Tgl</t>
   </si>
@@ -237,6 +237,9 @@
   </si>
   <si>
     <t>PARKIR - bulanan</t>
+  </si>
+  <si>
+    <t>SELISIH - kurang</t>
   </si>
 </sst>
 </file>
@@ -604,8 +607,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -979,12 +982,12 @@
         <v>25</v>
       </c>
       <c r="D28" s="1">
-        <f>45000</f>
-        <v>45000</v>
+        <f>45000+210000</f>
+        <v>255000</v>
       </c>
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>749025</v>
+        <v>539025</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -992,12 +995,12 @@
         <v>60</v>
       </c>
       <c r="C29" s="1">
-        <f>19800000+851000+9149000</f>
-        <v>29800000</v>
+        <f>19800000+851000+9149000+7640000+19960000+10000000+39715000</f>
+        <v>107115000</v>
       </c>
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>30549025</v>
+        <v>107654025</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1010,7 +1013,7 @@
       </c>
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>10749025</v>
+        <v>87854025</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1022,7 +1025,7 @@
       </c>
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>10739025</v>
+        <v>87844025</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1030,15 +1033,15 @@
         <v>59</v>
       </c>
       <c r="D32" s="1">
-        <f>215000+308000+1240000</f>
-        <v>1763000</v>
+        <f>215000+308000+1240000+10000000+19960000+7640000+300000</f>
+        <v>39663000</v>
       </c>
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>8976025</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6">
+        <v>48181025</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="B33" t="s">
         <v>69</v>
       </c>
@@ -1047,490 +1050,533 @@
       </c>
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>2576025</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6">
+        <v>41781025</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="B34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="1">
+        <f>49834025-2276025-39715000</f>
+        <v>7843000</v>
+      </c>
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>2576025</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6">
+        <v>49624025</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="B35" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" s="1">
+        <v>10000</v>
+      </c>
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>2576025</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6">
+        <v>49614025</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="B36" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" s="1">
+        <v>49000000</v>
+      </c>
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>2576025</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6">
+        <v>614025</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B37" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="1">
+        <f>45000</f>
+        <v>45000</v>
+      </c>
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>2576025</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6">
+        <v>569025</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="B38" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38" s="1">
+        <f>500000</f>
+        <v>500000</v>
+      </c>
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>2576025</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6">
+        <v>1069025</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="B39" t="s">
+        <v>59</v>
+      </c>
+      <c r="D39" s="1">
+        <f>75000+4750000</f>
+        <v>4825000</v>
+      </c>
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>2576025</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6">
+        <v>-3755975</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="2:6">
+    <row r="41" spans="1:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>2576025</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6">
+        <v>-3755975</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>2576025</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6">
+        <v>-3755975</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>2576025</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6">
+        <v>-3755975</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>2576025</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6">
+        <v>-3755975</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>2576025</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6">
+        <v>-3755975</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>2576025</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6">
+        <v>-3755975</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>2576025</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6">
+        <v>-3755975</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>2576025</v>
+        <v>-3755975</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 9-Jan-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="75">
   <si>
     <t>Tgl</t>
   </si>
@@ -240,6 +240,9 @@
   </si>
   <si>
     <t>SELISIH - kurang</t>
+  </si>
+  <si>
+    <t>andreas - prive</t>
   </si>
 </sst>
 </file>
@@ -607,8 +610,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
+      <pane ySplit="2" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1098,12 +1101,12 @@
         <v>25</v>
       </c>
       <c r="D37" s="1">
-        <f>45000</f>
-        <v>45000</v>
+        <f>45000+255000</f>
+        <v>300000</v>
       </c>
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>569025</v>
+        <v>314025</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1111,12 +1114,12 @@
         <v>60</v>
       </c>
       <c r="C38" s="1">
-        <f>500000</f>
-        <v>500000</v>
+        <f>500000+51746000</f>
+        <v>52246000</v>
       </c>
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>1069025</v>
+        <v>52560025</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1124,459 +1127,501 @@
         <v>59</v>
       </c>
       <c r="D39" s="1">
-        <f>75000+4750000</f>
-        <v>4825000</v>
+        <f>75000+4750000+120000+500000+844500+6200000+2130000</f>
+        <v>14619500</v>
       </c>
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>-3755975</v>
+        <v>37940525</v>
       </c>
     </row>
     <row r="40" spans="1:6">
+      <c r="B40" t="s">
+        <v>74</v>
+      </c>
+      <c r="D40" s="1">
+        <v>3000000</v>
+      </c>
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>-3755975</v>
+        <v>34940525</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:6">
+      <c r="B41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="1">
+        <f>16550475+46748525-51746000</f>
+        <v>11553000</v>
+      </c>
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>-3755975</v>
+        <v>46493525</v>
       </c>
     </row>
     <row r="42" spans="1:6">
+      <c r="B42" t="s">
+        <v>63</v>
+      </c>
+      <c r="C42" s="1">
+        <v>105000</v>
+      </c>
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>-3755975</v>
+        <v>46598525</v>
       </c>
     </row>
     <row r="43" spans="1:6">
+      <c r="B43" t="s">
+        <v>64</v>
+      </c>
+      <c r="D43" s="1">
+        <v>46000000</v>
+      </c>
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>-3755975</v>
+        <v>598525</v>
       </c>
     </row>
     <row r="44" spans="1:6">
+      <c r="A44" s="2">
+        <v>44205</v>
+      </c>
+      <c r="B44" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" s="1">
+        <f>45000</f>
+        <v>45000</v>
+      </c>
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>-3755975</v>
+        <v>553525</v>
       </c>
     </row>
     <row r="45" spans="1:6">
+      <c r="B45" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" s="1">
+        <f>155000+420000+35000</f>
+        <v>610000</v>
+      </c>
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>-3755975</v>
+        <v>-56475</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 10-Jan-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>Tgl</t>
   </si>
@@ -195,54 +195,6 @@
   </si>
   <si>
     <t>GUSTAVI</t>
-  </si>
-  <si>
-    <t>TRANSFER BCA</t>
-  </si>
-  <si>
-    <t>A/R</t>
-  </si>
-  <si>
-    <t>BELI sanitizer</t>
-  </si>
-  <si>
-    <t>SALES - cash/retail</t>
-  </si>
-  <si>
-    <t>SELISIH - lebih</t>
-  </si>
-  <si>
-    <t>SETOR KE BANK</t>
-  </si>
-  <si>
-    <t>FREIGHT-IN</t>
-  </si>
-  <si>
-    <t>BELI kresek</t>
-  </si>
-  <si>
-    <t>CHEQUE RECEIVED</t>
-  </si>
-  <si>
-    <t>IURAN DAERAH</t>
-  </si>
-  <si>
-    <t>A/P</t>
-  </si>
-  <si>
-    <t>BENSIN - RUSH</t>
-  </si>
-  <si>
-    <t>TRANSFER DANAMON</t>
-  </si>
-  <si>
-    <t>PARKIR - bulanan</t>
-  </si>
-  <si>
-    <t>SELISIH - kurang</t>
-  </si>
-  <si>
-    <t>andreas - prive</t>
   </si>
 </sst>
 </file>
@@ -610,8 +562,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B64" sqref="B64"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -647,981 +599,683 @@
         <v>5</v>
       </c>
       <c r="E2" s="1">
-        <v>434025</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>44200</v>
+        <v>44207</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="1">
-        <f>45000+240000</f>
-        <v>285000</v>
-      </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>149025</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="B4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="1">
-        <f>5170000+1040000+450000+7374000+1338000+586000+3467000+3219000+5170000+40000000+920000</f>
-        <v>68734000</v>
-      </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>-68584975</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="B5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="1">
-        <f>7374000+2211000+1500000+100000000+94174000</f>
-        <v>205259000</v>
-      </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>136674025</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="1">
-        <f>50000</f>
-        <v>50000</v>
-      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>136624025</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="B7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="1">
-        <f>166645025-43610025-94174000</f>
-        <v>28861000</v>
-      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>165485025</v>
+        <v>604525</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="B8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="1">
-        <v>70000</v>
-      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>165555025</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="B9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="1">
-        <v>165000000</v>
-      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>555025</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="2">
-        <v>44201</v>
-      </c>
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="1">
-        <f>45000+150000+195000</f>
-        <v>390000</v>
-      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>165025</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="B11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="1">
-        <f>5540000+1658000+1012500+440000</f>
-        <v>8650500</v>
-      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>-8485475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="B12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D12" s="1">
-        <v>1600000</v>
-      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>-10085475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" s="1">
-        <f>18006025+9890475-20113000</f>
-        <v>7783500</v>
-      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>-2301975</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="B14" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" s="1">
-        <f>20113000</f>
-        <v>20113000</v>
-      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>17811025</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="B15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" s="1">
-        <v>20000</v>
-      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>17831025</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="B16" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" s="1">
-        <v>17000000</v>
-      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>831025</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="2">
-        <v>44202</v>
-      </c>
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="1">
-        <f>45000+255000</f>
-        <v>300000</v>
-      </c>
+        <v>604525</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5">
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>531025</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="B18" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" s="1">
-        <f>680000+22000000+6382000+1227000</f>
-        <v>30289000</v>
-      </c>
+        <v>604525</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5">
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>-29757975</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="B19" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="1">
-        <f>2000000+5000000+100000000+82801000</f>
-        <v>189801000</v>
-      </c>
+        <v>604525</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5">
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>160043025</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="B20" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" s="1">
-        <f>95000</f>
-        <v>95000</v>
-      </c>
+        <v>604525</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5">
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>159948025</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="B21" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" s="1">
-        <f>2169000</f>
-        <v>2169000</v>
-      </c>
+        <v>604525</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5">
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>157779025</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="B22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" s="1">
-        <f>25000</f>
-        <v>25000</v>
-      </c>
+        <v>604525</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>157754025</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="B23" t="s">
-        <v>69</v>
-      </c>
-      <c r="D23" s="1">
-        <f>1266000</f>
-        <v>1266000</v>
-      </c>
+        <v>604525</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>156488025</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="B24" t="s">
-        <v>70</v>
-      </c>
-      <c r="D24" s="1">
-        <v>250000</v>
-      </c>
+        <v>604525</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>156238025</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="B25" t="s">
-        <v>62</v>
-      </c>
-      <c r="C25" s="1">
-        <f>166021025-73732025-82801000</f>
-        <v>9488000</v>
-      </c>
+        <v>604525</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>165726025</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="B26" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" s="1">
-        <v>68000</v>
-      </c>
+        <v>604525</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>165794025</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="B27" t="s">
-        <v>64</v>
-      </c>
-      <c r="D27" s="1">
-        <v>165000000</v>
-      </c>
+        <v>604525</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>794025</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="2">
-        <v>44203</v>
-      </c>
-      <c r="B28" t="s">
-        <v>25</v>
-      </c>
-      <c r="D28" s="1">
-        <f>45000+210000</f>
-        <v>255000</v>
-      </c>
+        <v>604525</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>539025</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="B29" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" s="1">
-        <f>19800000+851000+9149000+7640000+19960000+10000000+39715000</f>
-        <v>107115000</v>
-      </c>
+        <v>604525</v>
+      </c>
+    </row>
+    <row r="29" spans="5:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>107654025</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="B30" t="s">
-        <v>71</v>
-      </c>
-      <c r="D30" s="1">
-        <f>19800000</f>
-        <v>19800000</v>
-      </c>
+        <v>604525</v>
+      </c>
+    </row>
+    <row r="30" spans="5:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>87854025</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="B31" t="s">
-        <v>72</v>
-      </c>
-      <c r="D31" s="1">
-        <v>10000</v>
-      </c>
+        <v>604525</v>
+      </c>
+    </row>
+    <row r="31" spans="5:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>87844025</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="B32" t="s">
-        <v>59</v>
-      </c>
-      <c r="D32" s="1">
-        <f>215000+308000+1240000+10000000+19960000+7640000+300000</f>
-        <v>39663000</v>
-      </c>
+        <v>604525</v>
+      </c>
+    </row>
+    <row r="32" spans="5:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>48181025</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="B33" t="s">
-        <v>69</v>
-      </c>
-      <c r="D33" s="1">
-        <v>6400000</v>
-      </c>
+        <v>604525</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>41781025</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="B34" t="s">
-        <v>62</v>
-      </c>
-      <c r="C34" s="1">
-        <f>49834025-2276025-39715000</f>
-        <v>7843000</v>
-      </c>
+        <v>604525</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>49624025</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="B35" t="s">
-        <v>73</v>
-      </c>
-      <c r="D35" s="1">
-        <v>10000</v>
-      </c>
+        <v>604525</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>49614025</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="B36" t="s">
-        <v>64</v>
-      </c>
-      <c r="D36" s="1">
-        <v>49000000</v>
-      </c>
+        <v>604525</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>614025</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="2">
-        <v>44204</v>
-      </c>
-      <c r="B37" t="s">
-        <v>25</v>
-      </c>
-      <c r="D37" s="1">
-        <f>45000+255000</f>
-        <v>300000</v>
-      </c>
+        <v>604525</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>314025</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="B38" t="s">
-        <v>60</v>
-      </c>
-      <c r="C38" s="1">
-        <f>500000+51746000</f>
-        <v>52246000</v>
-      </c>
+        <v>604525</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>52560025</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="B39" t="s">
-        <v>59</v>
-      </c>
-      <c r="D39" s="1">
-        <f>75000+4750000+120000+500000+844500+6200000+2130000</f>
-        <v>14619500</v>
-      </c>
+        <v>604525</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>37940525</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="B40" t="s">
-        <v>74</v>
-      </c>
-      <c r="D40" s="1">
-        <v>3000000</v>
-      </c>
+        <v>604525</v>
+      </c>
+    </row>
+    <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>34940525</v>
+        <v>604525</v>
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="1:6">
-      <c r="B41" t="s">
-        <v>62</v>
-      </c>
-      <c r="C41" s="1">
-        <f>16550475+46748525-51746000</f>
-        <v>11553000</v>
-      </c>
+    <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>46493525</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="B42" t="s">
-        <v>63</v>
-      </c>
-      <c r="C42" s="1">
-        <v>105000</v>
-      </c>
+        <v>604525</v>
+      </c>
+    </row>
+    <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>46598525</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="B43" t="s">
-        <v>64</v>
-      </c>
-      <c r="D43" s="1">
-        <v>46000000</v>
-      </c>
+        <v>604525</v>
+      </c>
+    </row>
+    <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>598525</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="2">
-        <v>44205</v>
-      </c>
-      <c r="B44" t="s">
-        <v>25</v>
-      </c>
-      <c r="D44" s="1">
-        <f>45000</f>
-        <v>45000</v>
-      </c>
+        <v>604525</v>
+      </c>
+    </row>
+    <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>553525</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="B45" t="s">
-        <v>59</v>
-      </c>
-      <c r="D45" s="1">
-        <f>155000+420000+35000</f>
-        <v>610000</v>
-      </c>
+        <v>604525</v>
+      </c>
+    </row>
+    <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>-56475</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>604525</v>
+      </c>
+    </row>
+    <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>-56475</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>604525</v>
+      </c>
+    </row>
+    <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>-56475</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>604525</v>
+      </c>
+    </row>
+    <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>-56475</v>
+        <v>604525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 12-Jan-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="69">
   <si>
     <t>Tgl</t>
   </si>
@@ -195,6 +195,36 @@
   </si>
   <si>
     <t>GUSTAVI</t>
+  </si>
+  <si>
+    <t>TRANSFER BCA</t>
+  </si>
+  <si>
+    <t>TAX - P.Tata</t>
+  </si>
+  <si>
+    <t>TAX - Iuran ARIESTA</t>
+  </si>
+  <si>
+    <t>prive</t>
+  </si>
+  <si>
+    <t>SALES - cash/retail</t>
+  </si>
+  <si>
+    <t>A/R</t>
+  </si>
+  <si>
+    <t>TRANSFER BCA AA</t>
+  </si>
+  <si>
+    <t>SELISIH - lebih</t>
+  </si>
+  <si>
+    <t>SETOR KE BANK</t>
+  </si>
+  <si>
+    <t>SOLAR - kijang</t>
   </si>
 </sst>
 </file>
@@ -562,8 +592,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <pane ySplit="2" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -609,673 +639,746 @@
       <c r="B3" t="s">
         <v>25</v>
       </c>
+      <c r="D3" s="1">
+        <f>45000+405000</f>
+        <v>450000</v>
+      </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>604525</v>
+        <v>154525</v>
       </c>
     </row>
     <row r="4" spans="1:6">
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="1">
+        <f>8510000+12950000+540000+1385000+975000+800000+140000+6118000</f>
+        <v>31418000</v>
+      </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>604525</v>
+        <v>-31263475</v>
       </c>
     </row>
     <row r="5" spans="1:6">
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="1">
+        <f>200000</f>
+        <v>200000</v>
+      </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>604525</v>
+        <v>-31463475</v>
       </c>
     </row>
     <row r="6" spans="1:6">
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="1">
+        <f>660000</f>
+        <v>660000</v>
+      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>604525</v>
+        <v>-32123475</v>
       </c>
     </row>
     <row r="7" spans="1:6">
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2000000</v>
+      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>604525</v>
+        <v>-34123475</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="1">
+        <f>27600475+23611525+8510000-50104000</f>
+        <v>9618000</v>
+      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>604525</v>
+        <v>-24505475</v>
       </c>
     </row>
     <row r="9" spans="1:6">
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="1">
+        <f>3280000+2838000+27571000+37195000+50104000</f>
+        <v>120988000</v>
+      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>604525</v>
+        <v>96482525</v>
       </c>
     </row>
     <row r="10" spans="1:6">
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="1">
+        <f>64855000</f>
+        <v>64855000</v>
+      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>604525</v>
+        <v>31627525</v>
       </c>
     </row>
     <row r="11" spans="1:6">
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="1">
+        <v>80000</v>
+      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>604525</v>
+        <v>31707525</v>
       </c>
     </row>
     <row r="12" spans="1:6">
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="1">
+        <v>31000000</v>
+      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>604525</v>
+        <v>707525</v>
       </c>
     </row>
     <row r="13" spans="1:6">
+      <c r="B13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="1">
+        <v>300000</v>
+      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="14" spans="1:6">
+      <c r="A14" s="2">
+        <v>44208</v>
+      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="17" spans="5:5">
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="18" spans="5:5">
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="19" spans="5:5">
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="20" spans="5:5">
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="21" spans="5:5">
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="22" spans="5:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="23" spans="5:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="24" spans="5:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="25" spans="5:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="26" spans="5:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="27" spans="5:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="28" spans="5:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="29" spans="5:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="30" spans="5:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="31" spans="5:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="32" spans="5:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>604525</v>
+        <v>407525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 15-Jan-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="77">
   <si>
     <t>Tgl</t>
   </si>
@@ -225,6 +225,30 @@
   </si>
   <si>
     <t>SOLAR - kijang</t>
+  </si>
+  <si>
+    <t>FREIGHT OUT</t>
+  </si>
+  <si>
+    <t>SELISIH - kurang</t>
+  </si>
+  <si>
+    <t>Undangan - RITA</t>
+  </si>
+  <si>
+    <t>BELI kresek</t>
+  </si>
+  <si>
+    <t>PLN - Astar 214</t>
+  </si>
+  <si>
+    <t>PLN - Astar 165</t>
+  </si>
+  <si>
+    <t>Telpon - 5224823</t>
+  </si>
+  <si>
+    <t>prive - andreas</t>
   </si>
 </sst>
 </file>
@@ -592,8 +616,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
+      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -779,606 +803,812 @@
       <c r="A14" s="2">
         <v>44208</v>
       </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="1">
+        <f>45000+210000</f>
+        <v>255000</v>
+      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>407525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="15" spans="1:6">
+      <c r="B15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="1">
+        <f>855000+3210000+445000+120000+2223000+45705000+100000+2200000+155000+3207000+336000</f>
+        <v>58556000</v>
+      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>407525</v>
+        <v>-58403475</v>
       </c>
     </row>
     <row r="16" spans="1:6">
+      <c r="B16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="1">
+        <f>45705000+25212000</f>
+        <v>70917000</v>
+      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>407525</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5">
+        <v>12513525</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="B17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="1">
+        <f>204000</f>
+        <v>204000</v>
+      </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>407525</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5">
+        <v>12309525</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="B18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="1">
+        <f>12692475+22178525-25212000</f>
+        <v>9659000</v>
+      </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>407525</v>
-      </c>
-    </row>
-    <row r="19" spans="5:5">
+        <v>21968525</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="B19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="1">
+        <v>81000</v>
+      </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>407525</v>
-      </c>
-    </row>
-    <row r="20" spans="5:5">
+        <v>21887525</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="B20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="1">
+        <v>21000000</v>
+      </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>407525</v>
-      </c>
-    </row>
-    <row r="21" spans="5:5">
+        <v>887525</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2">
+        <v>44209</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="1">
+        <f>45000+255000</f>
+        <v>300000</v>
+      </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>407525</v>
-      </c>
-    </row>
-    <row r="22" spans="5:5">
+        <v>587525</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="B22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="1">
+        <f>36000000+12000000+285000+320000+757000+9775000+3850000+3247000+34200000+937500+715000</f>
+        <v>102086500</v>
+      </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>407525</v>
-      </c>
-    </row>
-    <row r="23" spans="5:5">
+        <v>-101498975</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="B23" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="1">
+        <f>56000+56000+28000</f>
+        <v>140000</v>
+      </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>407525</v>
-      </c>
-    </row>
-    <row r="24" spans="5:5">
+        <v>-101638975</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="B24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="1">
+        <f>12000000+52700000+34200000+78056500</f>
+        <v>176956500</v>
+      </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>407525</v>
-      </c>
-    </row>
-    <row r="25" spans="5:5">
+        <v>75317525</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="B25" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" s="1">
+        <f>5000000</f>
+        <v>5000000</v>
+      </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>407525</v>
-      </c>
-    </row>
-    <row r="26" spans="5:5">
+        <v>70317525</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="B26" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="1">
+        <f>50000</f>
+        <v>50000</v>
+      </c>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>407525</v>
-      </c>
-    </row>
-    <row r="27" spans="5:5">
+        <v>70267525</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="B27" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" s="1">
+        <f>103000</f>
+        <v>103000</v>
+      </c>
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>407525</v>
-      </c>
-    </row>
-    <row r="28" spans="5:5">
+        <v>70164525</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="B28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="1">
+        <f>7636975+76158025-78056500</f>
+        <v>5738500</v>
+      </c>
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>407525</v>
-      </c>
-    </row>
-    <row r="29" spans="5:5">
+        <v>75903025</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="B29" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="1">
+        <v>48000</v>
+      </c>
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>407525</v>
-      </c>
-    </row>
-    <row r="30" spans="5:5">
+        <v>75951025</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="B30" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="1">
+        <f>75000000</f>
+        <v>75000000</v>
+      </c>
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>407525</v>
-      </c>
-    </row>
-    <row r="31" spans="5:5">
+        <v>951025</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B31" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="1">
+        <f>45000+270000</f>
+        <v>315000</v>
+      </c>
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>407525</v>
-      </c>
-    </row>
-    <row r="32" spans="5:5">
+        <v>636025</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="B32" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="1">
+        <f>20000000+8197500+2000000+39483000</f>
+        <v>69680500</v>
+      </c>
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>407525</v>
-      </c>
-    </row>
-    <row r="33" spans="5:6">
+        <v>70316525</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="B33" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" s="1">
+        <f>1225000+7721000+839000+100000</f>
+        <v>9885000</v>
+      </c>
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>407525</v>
-      </c>
-    </row>
-    <row r="34" spans="5:6">
+        <v>60431525</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="B34" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" s="1">
+        <f>815000</f>
+        <v>815000</v>
+      </c>
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>407525</v>
-      </c>
-    </row>
-    <row r="35" spans="5:6">
+        <v>59616525</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="B35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D35" s="1">
+        <v>252000</v>
+      </c>
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>407525</v>
-      </c>
-    </row>
-    <row r="36" spans="5:6">
+        <v>59364525</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="B36" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" s="1">
+        <f>5000000</f>
+        <v>5000000</v>
+      </c>
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>407525</v>
-      </c>
-    </row>
-    <row r="37" spans="5:6">
+        <v>54364525</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="B37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" s="1">
+        <f>63341525-15251525-39483000</f>
+        <v>8607000</v>
+      </c>
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>407525</v>
-      </c>
-    </row>
-    <row r="38" spans="5:6">
+        <v>62971525</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="B38" t="s">
+        <v>70</v>
+      </c>
+      <c r="D38" s="1">
+        <v>60000</v>
+      </c>
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>407525</v>
-      </c>
-    </row>
-    <row r="39" spans="5:6">
+        <v>62911525</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="B39" t="s">
+        <v>67</v>
+      </c>
+      <c r="D39" s="1">
+        <v>62000000</v>
+      </c>
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>407525</v>
-      </c>
-    </row>
-    <row r="40" spans="5:6">
+        <v>911525</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="2">
+        <v>44211</v>
+      </c>
+      <c r="B40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40" s="1">
+        <f>45000</f>
+        <v>45000</v>
+      </c>
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>407525</v>
+        <v>866525</v>
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="5:6">
+    <row r="41" spans="1:6">
+      <c r="B41" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" s="1">
+        <f>37292000+2308000</f>
+        <v>39600000</v>
+      </c>
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>407525</v>
-      </c>
-    </row>
-    <row r="42" spans="5:6">
+        <v>40466525</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="B42" t="s">
+        <v>59</v>
+      </c>
+      <c r="D42" s="1">
+        <f>39600000+4800000</f>
+        <v>44400000</v>
+      </c>
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>407525</v>
-      </c>
-    </row>
-    <row r="43" spans="5:6">
+        <v>-3933475</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>407525</v>
-      </c>
-    </row>
-    <row r="44" spans="5:6">
+        <v>-3933475</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>407525</v>
-      </c>
-    </row>
-    <row r="45" spans="5:6">
+        <v>-3933475</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>407525</v>
-      </c>
-    </row>
-    <row r="46" spans="5:6">
+        <v>-3933475</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>407525</v>
-      </c>
-    </row>
-    <row r="47" spans="5:6">
+        <v>-3933475</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>407525</v>
-      </c>
-    </row>
-    <row r="48" spans="5:6">
+        <v>-3933475</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>407525</v>
+        <v>-3933475</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 16-Jan-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="77">
   <si>
     <t>Tgl</t>
   </si>
@@ -616,8 +616,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E60" sqref="E60"/>
+      <pane ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1148,12 +1148,12 @@
         <v>25</v>
       </c>
       <c r="D40" s="1">
-        <f>45000</f>
-        <v>45000</v>
+        <f>45000+225000</f>
+        <v>270000</v>
       </c>
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>866525</v>
+        <v>641525</v>
       </c>
       <c r="F40" s="1"/>
     </row>
@@ -1162,12 +1162,12 @@
         <v>64</v>
       </c>
       <c r="C41" s="1">
-        <f>37292000+2308000</f>
-        <v>39600000</v>
+        <f>37292000+2308000+15000000+59269000</f>
+        <v>113869000</v>
       </c>
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>40466525</v>
+        <v>114510525</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1175,440 +1175,465 @@
         <v>59</v>
       </c>
       <c r="D42" s="1">
-        <f>39600000+4800000</f>
-        <v>44400000</v>
+        <f>39600000+4800000+1266000+3915000+1935000+1014000+15000000+2100000</f>
+        <v>69630000</v>
       </c>
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>-3933475</v>
+        <v>44880525</v>
       </c>
     </row>
     <row r="43" spans="1:6">
+      <c r="B43" t="s">
+        <v>63</v>
+      </c>
+      <c r="C43" s="1">
+        <f>55531525+14163475-59269000</f>
+        <v>10426000</v>
+      </c>
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>-3933475</v>
+        <v>55306525</v>
       </c>
     </row>
     <row r="44" spans="1:6">
+      <c r="B44" t="s">
+        <v>66</v>
+      </c>
+      <c r="C44" s="1">
+        <v>23000</v>
+      </c>
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>-3933475</v>
+        <v>55329525</v>
       </c>
     </row>
     <row r="45" spans="1:6">
+      <c r="B45" t="s">
+        <v>67</v>
+      </c>
+      <c r="D45" s="1">
+        <v>55000000</v>
+      </c>
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="46" spans="1:6">
+      <c r="A46" s="2">
+        <v>44212</v>
+      </c>
+      <c r="B46" t="s">
+        <v>25</v>
+      </c>
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>-3933475</v>
+        <v>329525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 18-Jan-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
   <si>
     <t>Tgl</t>
   </si>
@@ -200,55 +200,7 @@
     <t>TRANSFER BCA</t>
   </si>
   <si>
-    <t>TAX - P.Tata</t>
-  </si>
-  <si>
-    <t>TAX - Iuran ARIESTA</t>
-  </si>
-  <si>
-    <t>prive</t>
-  </si>
-  <si>
-    <t>SALES - cash/retail</t>
-  </si>
-  <si>
     <t>A/R</t>
-  </si>
-  <si>
-    <t>TRANSFER BCA AA</t>
-  </si>
-  <si>
-    <t>SELISIH - lebih</t>
-  </si>
-  <si>
-    <t>SETOR KE BANK</t>
-  </si>
-  <si>
-    <t>SOLAR - kijang</t>
-  </si>
-  <si>
-    <t>FREIGHT OUT</t>
-  </si>
-  <si>
-    <t>SELISIH - kurang</t>
-  </si>
-  <si>
-    <t>Undangan - RITA</t>
-  </si>
-  <si>
-    <t>BELI kresek</t>
-  </si>
-  <si>
-    <t>PLN - Astar 214</t>
-  </si>
-  <si>
-    <t>PLN - Astar 165</t>
-  </si>
-  <si>
-    <t>Telpon - 5224823</t>
-  </si>
-  <si>
-    <t>prive - andreas</t>
   </si>
 </sst>
 </file>
@@ -616,8 +568,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -653,987 +605,701 @@
         <v>5</v>
       </c>
       <c r="E2" s="1">
-        <v>604525</v>
+        <v>453525</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>44207</v>
+        <v>44214</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="1">
-        <f>45000+405000</f>
-        <v>450000</v>
+        <f>45000</f>
+        <v>45000</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>154525</v>
+        <v>408525</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="B4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="1">
-        <f>8510000+12950000+540000+1385000+975000+800000+140000+6118000</f>
-        <v>31418000</v>
+        <v>60</v>
+      </c>
+      <c r="C4" s="1">
+        <f>7300000+2800000</f>
+        <v>10100000</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>-31263475</v>
+        <v>10508525</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="B5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D5" s="1">
-        <f>200000</f>
-        <v>200000</v>
+        <f>1787000+1149000</f>
+        <v>2936000</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>-31463475</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="1">
-        <f>660000</f>
-        <v>660000</v>
-      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>-32123475</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="B7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="1">
-        <v>2000000</v>
-      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>-34123475</v>
+        <v>7572525</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="B8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="1">
-        <f>27600475+23611525+8510000-50104000</f>
-        <v>9618000</v>
-      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>-24505475</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="B9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="1">
-        <f>3280000+2838000+27571000+37195000+50104000</f>
-        <v>120988000</v>
-      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>96482525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="B10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="1">
-        <f>64855000</f>
-        <v>64855000</v>
-      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>31627525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="B11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="1">
-        <v>80000</v>
-      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>31707525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="B12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="1">
-        <v>31000000</v>
-      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>707525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" s="1">
-        <v>300000</v>
-      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>407525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="2">
-        <v>44208</v>
-      </c>
-      <c r="B14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="1">
-        <f>45000+210000</f>
-        <v>255000</v>
-      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>152525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="B15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" s="1">
-        <f>855000+3210000+445000+120000+2223000+45705000+100000+2200000+155000+3207000+336000</f>
-        <v>58556000</v>
-      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>-58403475</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="B16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" s="1">
-        <f>45705000+25212000</f>
-        <v>70917000</v>
-      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>12513525</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="B17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" s="1">
-        <f>204000</f>
-        <v>204000</v>
-      </c>
+        <v>7572525</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5">
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>12309525</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="B18" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="1">
-        <f>12692475+22178525-25212000</f>
-        <v>9659000</v>
-      </c>
+        <v>7572525</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5">
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>21968525</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="B19" t="s">
-        <v>70</v>
-      </c>
-      <c r="D19" s="1">
-        <v>81000</v>
-      </c>
+        <v>7572525</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5">
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>21887525</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="B20" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="1">
-        <v>21000000</v>
-      </c>
+        <v>7572525</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5">
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>887525</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="2">
-        <v>44209</v>
-      </c>
-      <c r="B21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="1">
-        <f>45000+255000</f>
-        <v>300000</v>
-      </c>
+        <v>7572525</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5">
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>587525</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="B22" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" s="1">
-        <f>36000000+12000000+285000+320000+757000+9775000+3850000+3247000+34200000+937500+715000</f>
-        <v>102086500</v>
-      </c>
+        <v>7572525</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>-101498975</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="B23" t="s">
-        <v>69</v>
-      </c>
-      <c r="D23" s="1">
-        <f>56000+56000+28000</f>
-        <v>140000</v>
-      </c>
+        <v>7572525</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>-101638975</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="B24" t="s">
-        <v>64</v>
-      </c>
-      <c r="C24" s="1">
-        <f>12000000+52700000+34200000+78056500</f>
-        <v>176956500</v>
-      </c>
+        <v>7572525</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>75317525</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="B25" t="s">
-        <v>71</v>
-      </c>
-      <c r="D25" s="1">
-        <f>5000000</f>
-        <v>5000000</v>
-      </c>
+        <v>7572525</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>70317525</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="B26" t="s">
-        <v>72</v>
-      </c>
-      <c r="D26" s="1">
-        <f>50000</f>
-        <v>50000</v>
-      </c>
+        <v>7572525</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>70267525</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="B27" t="s">
-        <v>73</v>
-      </c>
-      <c r="D27" s="1">
-        <f>103000</f>
-        <v>103000</v>
-      </c>
+        <v>7572525</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>70164525</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="B28" t="s">
-        <v>63</v>
-      </c>
-      <c r="C28" s="1">
-        <f>7636975+76158025-78056500</f>
-        <v>5738500</v>
-      </c>
+        <v>7572525</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>75903025</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="B29" t="s">
-        <v>66</v>
-      </c>
-      <c r="C29" s="1">
-        <v>48000</v>
-      </c>
+        <v>7572525</v>
+      </c>
+    </row>
+    <row r="29" spans="5:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>75951025</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="B30" t="s">
-        <v>67</v>
-      </c>
-      <c r="D30" s="1">
-        <f>75000000</f>
-        <v>75000000</v>
-      </c>
+        <v>7572525</v>
+      </c>
+    </row>
+    <row r="30" spans="5:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>951025</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="2">
-        <v>44210</v>
-      </c>
-      <c r="B31" t="s">
-        <v>25</v>
-      </c>
-      <c r="D31" s="1">
-        <f>45000+270000</f>
-        <v>315000</v>
-      </c>
+        <v>7572525</v>
+      </c>
+    </row>
+    <row r="31" spans="5:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>636025</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="B32" t="s">
-        <v>64</v>
-      </c>
-      <c r="C32" s="1">
-        <f>20000000+8197500+2000000+39483000</f>
-        <v>69680500</v>
-      </c>
+        <v>7572525</v>
+      </c>
+    </row>
+    <row r="32" spans="5:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>70316525</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="B33" t="s">
-        <v>59</v>
-      </c>
-      <c r="D33" s="1">
-        <f>1225000+7721000+839000+100000</f>
-        <v>9885000</v>
-      </c>
+        <v>7572525</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>60431525</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="B34" t="s">
-        <v>74</v>
-      </c>
-      <c r="D34" s="1">
-        <f>815000</f>
-        <v>815000</v>
-      </c>
+        <v>7572525</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>59616525</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="B35" t="s">
-        <v>75</v>
-      </c>
-      <c r="D35" s="1">
-        <v>252000</v>
-      </c>
+        <v>7572525</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>59364525</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="B36" t="s">
-        <v>76</v>
-      </c>
-      <c r="D36" s="1">
-        <f>5000000</f>
-        <v>5000000</v>
-      </c>
+        <v>7572525</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>54364525</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="B37" t="s">
-        <v>63</v>
-      </c>
-      <c r="C37" s="1">
-        <f>63341525-15251525-39483000</f>
-        <v>8607000</v>
-      </c>
+        <v>7572525</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>62971525</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="B38" t="s">
-        <v>70</v>
-      </c>
-      <c r="D38" s="1">
-        <v>60000</v>
-      </c>
+        <v>7572525</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>62911525</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="B39" t="s">
-        <v>67</v>
-      </c>
-      <c r="D39" s="1">
-        <v>62000000</v>
-      </c>
+        <v>7572525</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>911525</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="2">
-        <v>44211</v>
-      </c>
-      <c r="B40" t="s">
-        <v>25</v>
-      </c>
-      <c r="D40" s="1">
-        <f>45000+225000</f>
-        <v>270000</v>
-      </c>
+        <v>7572525</v>
+      </c>
+    </row>
+    <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>641525</v>
+        <v>7572525</v>
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="1:6">
-      <c r="B41" t="s">
-        <v>64</v>
-      </c>
-      <c r="C41" s="1">
-        <f>37292000+2308000+15000000+59269000</f>
-        <v>113869000</v>
-      </c>
+    <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>114510525</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="B42" t="s">
-        <v>59</v>
-      </c>
-      <c r="D42" s="1">
-        <f>39600000+4800000+1266000+3915000+1935000+1014000+15000000+2100000</f>
-        <v>69630000</v>
-      </c>
+        <v>7572525</v>
+      </c>
+    </row>
+    <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>44880525</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="B43" t="s">
-        <v>63</v>
-      </c>
-      <c r="C43" s="1">
-        <f>55531525+14163475-59269000</f>
-        <v>10426000</v>
-      </c>
+        <v>7572525</v>
+      </c>
+    </row>
+    <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>55306525</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="B44" t="s">
-        <v>66</v>
-      </c>
-      <c r="C44" s="1">
-        <v>23000</v>
-      </c>
+        <v>7572525</v>
+      </c>
+    </row>
+    <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>55329525</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="B45" t="s">
-        <v>67</v>
-      </c>
-      <c r="D45" s="1">
-        <v>55000000</v>
-      </c>
+        <v>7572525</v>
+      </c>
+    </row>
+    <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>329525</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" s="2">
-        <v>44212</v>
-      </c>
-      <c r="B46" t="s">
-        <v>25</v>
-      </c>
+        <v>7572525</v>
+      </c>
+    </row>
+    <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>329525</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>7572525</v>
+      </c>
+    </row>
+    <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>329525</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>7572525</v>
+      </c>
+    </row>
+    <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>329525</v>
+        <v>7572525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 20-Jan-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="68">
   <si>
     <t>Tgl</t>
   </si>
@@ -201,6 +201,27 @@
   </si>
   <si>
     <t>A/R</t>
+  </si>
+  <si>
+    <t>TRANSFER DANAMON</t>
+  </si>
+  <si>
+    <t>Dana Kebersihan</t>
+  </si>
+  <si>
+    <t>SALES - cash/retail</t>
+  </si>
+  <si>
+    <t>SELISIH - kurang</t>
+  </si>
+  <si>
+    <t>SETOR KE BANK</t>
+  </si>
+  <si>
+    <t>BELI buku bon</t>
+  </si>
+  <si>
+    <t>BELI lakban</t>
   </si>
 </sst>
 </file>
@@ -568,8 +589,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <pane ySplit="2" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -616,12 +637,12 @@
         <v>25</v>
       </c>
       <c r="D3" s="1">
-        <f>45000</f>
-        <v>45000</v>
+        <f>45000+210000</f>
+        <v>255000</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>408525</v>
+        <v>198525</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -629,12 +650,12 @@
         <v>60</v>
       </c>
       <c r="C4" s="1">
-        <f>7300000+2800000</f>
-        <v>10100000</v>
+        <f>7300000+2800000+51345000+12978000</f>
+        <v>74423000</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>10508525</v>
+        <v>74621525</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -642,664 +663,776 @@
         <v>59</v>
       </c>
       <c r="D5" s="1">
-        <f>1787000+1149000</f>
-        <v>2936000</v>
+        <f>1787000+1149000+360000+25000+225000</f>
+        <v>3546000</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>7572525</v>
+        <v>71075525</v>
       </c>
     </row>
     <row r="6" spans="1:6">
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="1">
+        <f>51345000</f>
+        <v>51345000</v>
+      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>7572525</v>
+        <v>19730525</v>
       </c>
     </row>
     <row r="7" spans="1:6">
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="1">
+        <f>120000</f>
+        <v>120000</v>
+      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>7572525</v>
+        <v>19610525</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="1">
+        <f>42155525-6842525-12978000</f>
+        <v>22335000</v>
+      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>7572525</v>
+        <v>41945525</v>
       </c>
     </row>
     <row r="9" spans="1:6">
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="1">
+        <v>25000</v>
+      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>7572525</v>
+        <v>41920525</v>
       </c>
     </row>
     <row r="10" spans="1:6">
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="1">
+        <v>41000000</v>
+      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>7572525</v>
+        <v>920525</v>
       </c>
     </row>
     <row r="11" spans="1:6">
+      <c r="A11" s="2">
+        <v>44215</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="1">
+        <f>45000+195000</f>
+        <v>240000</v>
+      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>7572525</v>
+        <v>680525</v>
       </c>
     </row>
     <row r="12" spans="1:6">
+      <c r="B12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="1">
+        <f>3167000+3510000+102060000+1280000+19228000+420000</f>
+        <v>129665000</v>
+      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>7572525</v>
+        <v>-128984475</v>
       </c>
     </row>
     <row r="13" spans="1:6">
+      <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="1">
+        <f>3510000+102060000+19228000+12637000</f>
+        <v>137435000</v>
+      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>7572525</v>
+        <v>8450525</v>
       </c>
     </row>
     <row r="14" spans="1:6">
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="1">
+        <f>3991475+14876025-12637000</f>
+        <v>6230500</v>
+      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>7572525</v>
+        <v>14681025</v>
       </c>
     </row>
     <row r="15" spans="1:6">
+      <c r="B15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="1">
+        <v>60000</v>
+      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>7572525</v>
+        <v>14621025</v>
       </c>
     </row>
     <row r="16" spans="1:6">
+      <c r="B16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="1">
+        <v>14000000</v>
+      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>7572525</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5">
+        <v>621025</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2">
+        <v>44216</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="1">
+        <f>45000</f>
+        <v>45000</v>
+      </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>7572525</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5">
+        <v>576025</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="B18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="1">
+        <f>14805000+2565000</f>
+        <v>17370000</v>
+      </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>7572525</v>
-      </c>
-    </row>
-    <row r="19" spans="5:5">
+        <v>-16793975</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="B19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="1">
+        <f>2580000+1410000</f>
+        <v>3990000</v>
+      </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>7572525</v>
-      </c>
-    </row>
-    <row r="20" spans="5:5">
+        <v>-12803975</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="B20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="1">
+        <v>134000</v>
+      </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>7572525</v>
-      </c>
-    </row>
-    <row r="21" spans="5:5">
+        <v>-12937975</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="1">
+        <v>51000</v>
+      </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>7572525</v>
-      </c>
-    </row>
-    <row r="22" spans="5:5">
+        <v>-12988975</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>7572525</v>
-      </c>
-    </row>
-    <row r="23" spans="5:5">
+        <v>-12988975</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>7572525</v>
-      </c>
-    </row>
-    <row r="24" spans="5:5">
+        <v>-12988975</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>7572525</v>
-      </c>
-    </row>
-    <row r="25" spans="5:5">
+        <v>-12988975</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>7572525</v>
-      </c>
-    </row>
-    <row r="26" spans="5:5">
+        <v>-12988975</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>7572525</v>
-      </c>
-    </row>
-    <row r="27" spans="5:5">
+        <v>-12988975</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>7572525</v>
-      </c>
-    </row>
-    <row r="28" spans="5:5">
+        <v>-12988975</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>7572525</v>
-      </c>
-    </row>
-    <row r="29" spans="5:5">
+        <v>-12988975</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>7572525</v>
-      </c>
-    </row>
-    <row r="30" spans="5:5">
+        <v>-12988975</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>7572525</v>
-      </c>
-    </row>
-    <row r="31" spans="5:5">
+        <v>-12988975</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>7572525</v>
-      </c>
-    </row>
-    <row r="32" spans="5:5">
+        <v>-12988975</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>7572525</v>
+        <v>-12988975</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 22-Jan-2021, end of day update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="72">
   <si>
     <t>Tgl</t>
   </si>
@@ -222,6 +222,18 @@
   </si>
   <si>
     <t>BELI lakban</t>
+  </si>
+  <si>
+    <t>SELISIH - lebih</t>
+  </si>
+  <si>
+    <t>CHEQUE RECEIVED</t>
+  </si>
+  <si>
+    <t>A/P</t>
+  </si>
+  <si>
+    <t>prive</t>
   </si>
 </sst>
 </file>
@@ -589,8 +601,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
+      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -822,12 +834,12 @@
         <v>25</v>
       </c>
       <c r="D17" s="1">
-        <f>45000</f>
-        <v>45000</v>
+        <f>45000+195000</f>
+        <v>240000</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>576025</v>
+        <v>381025</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -835,12 +847,12 @@
         <v>59</v>
       </c>
       <c r="D18" s="1">
-        <f>14805000+2565000</f>
-        <v>17370000</v>
+        <f>14805000+2565000+336000+337000</f>
+        <v>18043000</v>
       </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>-16793975</v>
+        <v>-17661975</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -848,12 +860,12 @@
         <v>60</v>
       </c>
       <c r="C19" s="1">
-        <f>2580000+1410000</f>
-        <v>3990000</v>
+        <f>2580000+1410000+28052000</f>
+        <v>32042000</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>-12803975</v>
+        <v>14380025</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -865,7 +877,7 @@
       </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>-12937975</v>
+        <v>14246025</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -877,562 +889,647 @@
       </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>-12988975</v>
+        <v>14195025</v>
       </c>
     </row>
     <row r="22" spans="1:5">
+      <c r="B22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="1">
+        <f>13661975+30077025-28052000</f>
+        <v>15687000</v>
+      </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>-12988975</v>
+        <v>29882025</v>
       </c>
     </row>
     <row r="23" spans="1:5">
+      <c r="B23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="1">
+        <v>140000</v>
+      </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>-12988975</v>
+        <v>30022025</v>
       </c>
     </row>
     <row r="24" spans="1:5">
+      <c r="B24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="1">
+        <v>29000000</v>
+      </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>-12988975</v>
+        <v>1022025</v>
       </c>
     </row>
     <row r="25" spans="1:5">
+      <c r="A25" s="2">
+        <v>44217</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="1">
+        <f>45000+225000</f>
+        <v>270000</v>
+      </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>-12988975</v>
+        <v>752025</v>
       </c>
     </row>
     <row r="26" spans="1:5">
+      <c r="B26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="1">
+        <f>1630000+2050000+280000+371500</f>
+        <v>4331500</v>
+      </c>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>-12988975</v>
+        <v>-3579475</v>
       </c>
     </row>
     <row r="27" spans="1:5">
+      <c r="B27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" s="1">
+        <f>1619000</f>
+        <v>1619000</v>
+      </c>
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>-12988975</v>
+        <v>-5198475</v>
       </c>
     </row>
     <row r="28" spans="1:5">
+      <c r="B28" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" s="1">
+        <f>3925000</f>
+        <v>3925000</v>
+      </c>
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>-12988975</v>
+        <v>-9123475</v>
       </c>
     </row>
     <row r="29" spans="1:5">
+      <c r="B29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="1">
+        <f>18910500</f>
+        <v>18910500</v>
+      </c>
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>-12988975</v>
+        <v>9787025</v>
       </c>
     </row>
     <row r="30" spans="1:5">
+      <c r="B30" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="1">
+        <f>8526975+21744025-18910500</f>
+        <v>11360500</v>
+      </c>
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>-12988975</v>
+        <v>21147525</v>
       </c>
     </row>
     <row r="31" spans="1:5">
+      <c r="B31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1000000</v>
+      </c>
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>-12988975</v>
+        <v>20147525</v>
       </c>
     </row>
     <row r="32" spans="1:5">
+      <c r="B32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" s="1">
+        <v>420000</v>
+      </c>
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>-12988975</v>
-      </c>
-    </row>
-    <row r="33" spans="5:6">
+        <v>20567525</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="B33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="1">
+        <v>20000000</v>
+      </c>
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>-12988975</v>
-      </c>
-    </row>
-    <row r="34" spans="5:6">
+        <v>567525</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="2">
+        <v>44218</v>
+      </c>
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>-12988975</v>
-      </c>
-    </row>
-    <row r="35" spans="5:6">
+        <v>567525</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>-12988975</v>
-      </c>
-    </row>
-    <row r="36" spans="5:6">
+        <v>567525</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>-12988975</v>
-      </c>
-    </row>
-    <row r="37" spans="5:6">
+        <v>567525</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>-12988975</v>
-      </c>
-    </row>
-    <row r="38" spans="5:6">
+        <v>567525</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>-12988975</v>
-      </c>
-    </row>
-    <row r="39" spans="5:6">
+        <v>567525</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>-12988975</v>
-      </c>
-    </row>
-    <row r="40" spans="5:6">
+        <v>567525</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="5:6">
+    <row r="41" spans="1:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>-12988975</v>
-      </c>
-    </row>
-    <row r="42" spans="5:6">
+        <v>567525</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>-12988975</v>
-      </c>
-    </row>
-    <row r="43" spans="5:6">
+        <v>567525</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>-12988975</v>
-      </c>
-    </row>
-    <row r="44" spans="5:6">
+        <v>567525</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>-12988975</v>
-      </c>
-    </row>
-    <row r="45" spans="5:6">
+        <v>567525</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>-12988975</v>
-      </c>
-    </row>
-    <row r="46" spans="5:6">
+        <v>567525</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>-12988975</v>
-      </c>
-    </row>
-    <row r="47" spans="5:6">
+        <v>567525</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>-12988975</v>
-      </c>
-    </row>
-    <row r="48" spans="5:6">
+        <v>567525</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>-12988975</v>
+        <v>567525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 25-Jan-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
   <si>
     <t>Tgl</t>
   </si>
@@ -201,39 +201,6 @@
   </si>
   <si>
     <t>A/R</t>
-  </si>
-  <si>
-    <t>TRANSFER DANAMON</t>
-  </si>
-  <si>
-    <t>Dana Kebersihan</t>
-  </si>
-  <si>
-    <t>SALES - cash/retail</t>
-  </si>
-  <si>
-    <t>SELISIH - kurang</t>
-  </si>
-  <si>
-    <t>SETOR KE BANK</t>
-  </si>
-  <si>
-    <t>BELI buku bon</t>
-  </si>
-  <si>
-    <t>BELI lakban</t>
-  </si>
-  <si>
-    <t>SELISIH - lebih</t>
-  </si>
-  <si>
-    <t>CHEQUE RECEIVED</t>
-  </si>
-  <si>
-    <t>A/P</t>
-  </si>
-  <si>
-    <t>prive</t>
   </si>
 </sst>
 </file>
@@ -601,8 +568,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C54" sqref="C54"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -638,898 +605,701 @@
         <v>5</v>
       </c>
       <c r="E2" s="1">
-        <v>453525</v>
+        <v>715525</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>44214</v>
+        <v>44221</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="1">
-        <f>45000+210000</f>
-        <v>255000</v>
+        <f>45000</f>
+        <v>45000</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>198525</v>
+        <v>670525</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="B4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="1">
-        <f>7300000+2800000+51345000+12978000</f>
-        <v>74423000</v>
+        <v>59</v>
+      </c>
+      <c r="D4" s="1">
+        <f>49000+37256000+3465000+6240000</f>
+        <v>47010000</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>74621525</v>
+        <v>-46339475</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="B5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="1">
-        <f>1787000+1149000+360000+25000+225000</f>
-        <v>3546000</v>
+        <v>60</v>
+      </c>
+      <c r="C5" s="1">
+        <f>37256000</f>
+        <v>37256000</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>71075525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="1">
-        <f>51345000</f>
-        <v>51345000</v>
-      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>19730525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="B7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="1">
-        <f>120000</f>
-        <v>120000</v>
-      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>19610525</v>
+        <v>-9083475</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="B8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="1">
-        <f>42155525-6842525-12978000</f>
-        <v>22335000</v>
-      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>41945525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="B9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="1">
-        <v>25000</v>
-      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>41920525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="B10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="1">
-        <v>41000000</v>
-      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>920525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="2">
-        <v>44215</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="1">
-        <f>45000+195000</f>
-        <v>240000</v>
-      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>680525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="B12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" s="1">
-        <f>3167000+3510000+102060000+1280000+19228000+420000</f>
-        <v>129665000</v>
-      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>-128984475</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="1">
-        <f>3510000+102060000+19228000+12637000</f>
-        <v>137435000</v>
-      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>8450525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="B14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="1">
-        <f>3991475+14876025-12637000</f>
-        <v>6230500</v>
-      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>14681025</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="B15" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" s="1">
-        <v>60000</v>
-      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>14621025</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="B16" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="1">
-        <v>14000000</v>
-      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>621025</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="2">
-        <v>44216</v>
-      </c>
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="1">
-        <f>45000+195000</f>
-        <v>240000</v>
-      </c>
+        <v>-9083475</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5">
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>381025</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="B18" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" s="1">
-        <f>14805000+2565000+336000+337000</f>
-        <v>18043000</v>
-      </c>
+        <v>-9083475</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5">
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>-17661975</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="B19" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="1">
-        <f>2580000+1410000+28052000</f>
-        <v>32042000</v>
-      </c>
+        <v>-9083475</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5">
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>14380025</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="B20" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" s="1">
-        <v>134000</v>
-      </c>
+        <v>-9083475</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5">
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>14246025</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="B21" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" s="1">
-        <v>51000</v>
-      </c>
+        <v>-9083475</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5">
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>14195025</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="B22" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="1">
-        <f>13661975+30077025-28052000</f>
-        <v>15687000</v>
-      </c>
+        <v>-9083475</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>29882025</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="B23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" s="1">
-        <v>140000</v>
-      </c>
+        <v>-9083475</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>30022025</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="B24" t="s">
-        <v>65</v>
-      </c>
-      <c r="D24" s="1">
-        <v>29000000</v>
-      </c>
+        <v>-9083475</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>1022025</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="2">
-        <v>44217</v>
-      </c>
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="1">
-        <f>45000+225000</f>
-        <v>270000</v>
-      </c>
+        <v>-9083475</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>752025</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="B26" t="s">
-        <v>59</v>
-      </c>
-      <c r="D26" s="1">
-        <f>1630000+2050000+280000+371500</f>
-        <v>4331500</v>
-      </c>
+        <v>-9083475</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>-3579475</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="B27" t="s">
-        <v>69</v>
-      </c>
-      <c r="D27" s="1">
-        <f>1619000</f>
-        <v>1619000</v>
-      </c>
+        <v>-9083475</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>-5198475</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="B28" t="s">
-        <v>70</v>
-      </c>
-      <c r="D28" s="1">
-        <f>3925000</f>
-        <v>3925000</v>
-      </c>
+        <v>-9083475</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>-9123475</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="B29" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" s="1">
-        <f>18910500</f>
-        <v>18910500</v>
-      </c>
+        <v>-9083475</v>
+      </c>
+    </row>
+    <row r="29" spans="5:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>9787025</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="B30" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" s="1">
-        <f>8526975+21744025-18910500</f>
-        <v>11360500</v>
-      </c>
+        <v>-9083475</v>
+      </c>
+    </row>
+    <row r="30" spans="5:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>21147525</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="B31" t="s">
-        <v>71</v>
-      </c>
-      <c r="D31" s="1">
-        <v>1000000</v>
-      </c>
+        <v>-9083475</v>
+      </c>
+    </row>
+    <row r="31" spans="5:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>20147525</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="B32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C32" s="1">
-        <v>420000</v>
-      </c>
+        <v>-9083475</v>
+      </c>
+    </row>
+    <row r="32" spans="5:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>20567525</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="B33" t="s">
-        <v>65</v>
-      </c>
-      <c r="D33" s="1">
-        <v>20000000</v>
-      </c>
+        <v>-9083475</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>567525</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="2">
-        <v>44218</v>
-      </c>
+        <v>-9083475</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>567525</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+        <v>-9083475</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>567525</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>-9083475</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>567525</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+        <v>-9083475</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>567525</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+        <v>-9083475</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>567525</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+        <v>-9083475</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>567525</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>-9083475</v>
+      </c>
+    </row>
+    <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>567525</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+        <v>-9083475</v>
+      </c>
+    </row>
+    <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>567525</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>-9083475</v>
+      </c>
+    </row>
+    <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>567525</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>-9083475</v>
+      </c>
+    </row>
+    <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>567525</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>-9083475</v>
+      </c>
+    </row>
+    <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>567525</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>-9083475</v>
+      </c>
+    </row>
+    <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>567525</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>-9083475</v>
+      </c>
+    </row>
+    <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>567525</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>-9083475</v>
+      </c>
+    </row>
+    <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>567525</v>
+        <v>-9083475</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 26-Jan-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="66">
   <si>
     <t>Tgl</t>
   </si>
@@ -201,6 +201,21 @@
   </si>
   <si>
     <t>A/R</t>
+  </si>
+  <si>
+    <t>A/P</t>
+  </si>
+  <si>
+    <t>PRIVE - andreas</t>
+  </si>
+  <si>
+    <t>SALES - cash/retail</t>
+  </si>
+  <si>
+    <t>SELISIH - lebih</t>
+  </si>
+  <si>
+    <t>SETOR KE BANK</t>
   </si>
 </sst>
 </file>
@@ -568,8 +583,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <pane ySplit="2" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -616,12 +631,12 @@
         <v>25</v>
       </c>
       <c r="D3" s="1">
-        <f>45000</f>
-        <v>45000</v>
+        <f>45000+195000</f>
+        <v>240000</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>670525</v>
+        <v>475525</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -629,12 +644,12 @@
         <v>59</v>
       </c>
       <c r="D4" s="1">
-        <f>49000+37256000+3465000+6240000</f>
-        <v>47010000</v>
+        <f>49000+37256000+3465000+6240000+1375000+2424000-1215000</f>
+        <v>49594000</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>-46339475</v>
+        <v>-49118475</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -642,664 +657,701 @@
         <v>60</v>
       </c>
       <c r="C5" s="1">
-        <f>37256000</f>
-        <v>37256000</v>
+        <f>37256000+28367500</f>
+        <v>65623500</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>-9083475</v>
+        <v>16505025</v>
       </c>
     </row>
     <row r="6" spans="1:6">
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="1">
+        <f>1266000</f>
+        <v>1266000</v>
+      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>-9083475</v>
+        <v>15239025</v>
       </c>
     </row>
     <row r="7" spans="1:6">
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5000000</v>
+      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>-9083475</v>
+        <v>10239025</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="1">
+        <f>15349475+25076525-28367500</f>
+        <v>12058500</v>
+      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>-9083475</v>
+        <v>22297525</v>
       </c>
     </row>
     <row r="9" spans="1:6">
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="1">
+        <f>100000-65500</f>
+        <v>34500</v>
+      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>-9083475</v>
+        <v>22332025</v>
       </c>
     </row>
     <row r="10" spans="1:6">
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="1">
+        <f>22000000</f>
+        <v>22000000</v>
+      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="11" spans="1:6">
+      <c r="A11" s="2">
+        <v>44222</v>
+      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="17" spans="5:5">
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="18" spans="5:5">
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="19" spans="5:5">
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="20" spans="5:5">
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="21" spans="5:5">
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="22" spans="5:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="23" spans="5:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="24" spans="5:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="25" spans="5:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="26" spans="5:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="27" spans="5:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="28" spans="5:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="29" spans="5:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="30" spans="5:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="31" spans="5:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="32" spans="5:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>-9083475</v>
+        <v>332025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 27-Jan-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="70">
   <si>
     <t>Tgl</t>
   </si>
@@ -216,6 +216,18 @@
   </si>
   <si>
     <t>SETOR KE BANK</t>
+  </si>
+  <si>
+    <t>BIAYA materai</t>
+  </si>
+  <si>
+    <t>TRANSFER BCA AA</t>
+  </si>
+  <si>
+    <t>FREIGHT OUT</t>
+  </si>
+  <si>
+    <t>andreas - prive</t>
   </si>
 </sst>
 </file>
@@ -583,8 +595,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
+      <pane ySplit="2" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -734,624 +746,693 @@
       <c r="A11" s="2">
         <v>44222</v>
       </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="1">
+        <f>45000+180000</f>
+        <v>225000</v>
+      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>332025</v>
+        <v>107025</v>
       </c>
     </row>
     <row r="12" spans="1:6">
+      <c r="B12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="1">
+        <f>70000000+3203000+56774000</f>
+        <v>129977000</v>
+      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>332025</v>
+        <v>130084025</v>
       </c>
     </row>
     <row r="13" spans="1:6">
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="1">
+        <f>70000000+1280000+81000+4360000+900000+7000000+1634000+155000</f>
+        <v>85410000</v>
+      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>332025</v>
+        <v>44674025</v>
       </c>
     </row>
     <row r="14" spans="1:6">
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="1">
+        <v>12000</v>
+      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>332025</v>
+        <v>44662025</v>
       </c>
     </row>
     <row r="15" spans="1:6">
+      <c r="B15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="1">
+        <f>3203000</f>
+        <v>3203000</v>
+      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>332025</v>
+        <v>41459025</v>
       </c>
     </row>
     <row r="16" spans="1:6">
+      <c r="B16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="1">
+        <f>36000</f>
+        <v>36000</v>
+      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>332025</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5">
+        <v>41423025</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="B17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="1">
+        <v>5000000</v>
+      </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>332025</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5">
+        <v>36423025</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="B18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="1">
+        <f>20170975+45761025-56774000</f>
+        <v>9158000</v>
+      </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>332025</v>
-      </c>
-    </row>
-    <row r="19" spans="5:5">
+        <v>45581025</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="B19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="1">
+        <v>336000</v>
+      </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>332025</v>
-      </c>
-    </row>
-    <row r="20" spans="5:5">
+        <v>45917025</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="B20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="1">
+        <v>45000000</v>
+      </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>332025</v>
-      </c>
-    </row>
-    <row r="21" spans="5:5">
+        <v>917025</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2">
+        <v>44223</v>
+      </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>332025</v>
-      </c>
-    </row>
-    <row r="22" spans="5:5">
+        <v>917025</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>332025</v>
-      </c>
-    </row>
-    <row r="23" spans="5:5">
+        <v>917025</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>332025</v>
-      </c>
-    </row>
-    <row r="24" spans="5:5">
+        <v>917025</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>332025</v>
-      </c>
-    </row>
-    <row r="25" spans="5:5">
+        <v>917025</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>332025</v>
-      </c>
-    </row>
-    <row r="26" spans="5:5">
+        <v>917025</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>332025</v>
-      </c>
-    </row>
-    <row r="27" spans="5:5">
+        <v>917025</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>332025</v>
-      </c>
-    </row>
-    <row r="28" spans="5:5">
+        <v>917025</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>332025</v>
-      </c>
-    </row>
-    <row r="29" spans="5:5">
+        <v>917025</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>332025</v>
-      </c>
-    </row>
-    <row r="30" spans="5:5">
+        <v>917025</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>332025</v>
-      </c>
-    </row>
-    <row r="31" spans="5:5">
+        <v>917025</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>332025</v>
-      </c>
-    </row>
-    <row r="32" spans="5:5">
+        <v>917025</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>332025</v>
+        <v>917025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 28-Jan-2021, end of day update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="72">
   <si>
     <t>Tgl</t>
   </si>
@@ -228,6 +228,12 @@
   </si>
   <si>
     <t>andreas - prive</t>
+  </si>
+  <si>
+    <t>SELISIH - kurang</t>
+  </si>
+  <si>
+    <t>BELI kresek</t>
   </si>
 </sst>
 </file>
@@ -596,7 +602,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -875,564 +881,648 @@
       <c r="A21" s="2">
         <v>44223</v>
       </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="1">
+        <f>60000+260000</f>
+        <v>320000</v>
+      </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>917025</v>
+        <v>597025</v>
       </c>
     </row>
     <row r="22" spans="1:5">
+      <c r="B22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="1">
+        <f>1831000+10000000+57476000</f>
+        <v>69307000</v>
+      </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>917025</v>
+        <v>69904025</v>
       </c>
     </row>
     <row r="23" spans="1:5">
+      <c r="B23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="1">
+        <f>1831000</f>
+        <v>1831000</v>
+      </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>917025</v>
+        <v>68073025</v>
       </c>
     </row>
     <row r="24" spans="1:5">
+      <c r="B24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="1">
+        <f>27770000+1096000</f>
+        <v>28866000</v>
+      </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>917025</v>
+        <v>39207025</v>
       </c>
     </row>
     <row r="25" spans="1:5">
+      <c r="B25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="1">
+        <v>5100000</v>
+      </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>917025</v>
+        <v>34107025</v>
       </c>
     </row>
     <row r="26" spans="1:5">
+      <c r="B26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="1">
+        <f>23008975+43182025-57476000</f>
+        <v>8715000</v>
+      </c>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>917025</v>
+        <v>42822025</v>
       </c>
     </row>
     <row r="27" spans="1:5">
+      <c r="B27" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="1">
+        <v>28000</v>
+      </c>
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>917025</v>
+        <v>42794025</v>
       </c>
     </row>
     <row r="28" spans="1:5">
+      <c r="B28" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="1">
+        <v>42000000</v>
+      </c>
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>917025</v>
+        <v>794025</v>
       </c>
     </row>
     <row r="29" spans="1:5">
+      <c r="A29" s="2">
+        <v>44224</v>
+      </c>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="1">
+        <f>60000</f>
+        <v>60000</v>
+      </c>
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>917025</v>
+        <v>734025</v>
       </c>
     </row>
     <row r="30" spans="1:5">
+      <c r="B30" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="1">
+        <f>13320000+18450000+40274000+29120000+16368000+14266000</f>
+        <v>131798000</v>
+      </c>
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>917025</v>
+        <v>132532025</v>
       </c>
     </row>
     <row r="31" spans="1:5">
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" s="1">
+        <f>29370000+14266000</f>
+        <v>43636000</v>
+      </c>
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>917025</v>
+        <v>88896025</v>
       </c>
     </row>
     <row r="32" spans="1:5">
+      <c r="B32" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="1">
+        <f>99000</f>
+        <v>99000</v>
+      </c>
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>917025</v>
+        <v>88797025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 30-Jan-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="76">
   <si>
     <t>Tgl</t>
   </si>
@@ -234,6 +234,18 @@
   </si>
   <si>
     <t>BELI kresek</t>
+  </si>
+  <si>
+    <t>CHEQUE RECEIVED</t>
+  </si>
+  <si>
+    <t>SERVICE - pintu</t>
+  </si>
+  <si>
+    <t>FREIGHT IN</t>
+  </si>
+  <si>
+    <t>BELI ban</t>
   </si>
 </sst>
 </file>
@@ -601,8 +613,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
+      <pane ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -989,12 +1001,12 @@
         <v>25</v>
       </c>
       <c r="D29" s="1">
-        <f>60000</f>
-        <v>60000</v>
+        <f>60000+280000</f>
+        <v>340000</v>
       </c>
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>734025</v>
+        <v>454025</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1002,12 +1014,12 @@
         <v>60</v>
       </c>
       <c r="C30" s="1">
-        <f>13320000+18450000+40274000+29120000+16368000+14266000</f>
-        <v>131798000</v>
+        <f>13320000+18450000+40274000+29120000+16368000+14266000+500000+20616000</f>
+        <v>152914000</v>
       </c>
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>132532025</v>
+        <v>153368025</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1015,12 +1027,12 @@
         <v>59</v>
       </c>
       <c r="D31" s="1">
-        <f>29370000+14266000</f>
-        <v>43636000</v>
+        <f>29370000+14266000+2000000+301000</f>
+        <v>45937000</v>
       </c>
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>88896025</v>
+        <v>107431025</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1033,496 +1045,601 @@
       </c>
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>88797025</v>
-      </c>
-    </row>
-    <row r="33" spans="5:6">
+        <v>107332025</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="B33" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" s="1">
+        <f>2162000</f>
+        <v>2162000</v>
+      </c>
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>88797025</v>
-      </c>
-    </row>
-    <row r="34" spans="5:6">
+        <v>105170025</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="B34" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" s="1">
+        <v>5000000</v>
+      </c>
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>88797025</v>
-      </c>
-    </row>
-    <row r="35" spans="5:6">
+        <v>100170025</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="B35" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="1">
+        <f>111913025-79834025-20616000</f>
+        <v>11463000</v>
+      </c>
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>88797025</v>
-      </c>
-    </row>
-    <row r="36" spans="5:6">
+        <v>111633025</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="B36" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" s="1">
+        <v>350000</v>
+      </c>
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>88797025</v>
-      </c>
-    </row>
-    <row r="37" spans="5:6">
+        <v>111283025</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="B37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" s="1">
+        <v>35000</v>
+      </c>
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>88797025</v>
-      </c>
-    </row>
-    <row r="38" spans="5:6">
+        <v>111318025</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="B38" t="s">
+        <v>65</v>
+      </c>
+      <c r="D38" s="1">
+        <v>111000000</v>
+      </c>
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>88797025</v>
-      </c>
-    </row>
-    <row r="39" spans="5:6">
+        <v>318025</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B39" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" s="1">
+        <f>60000+300000+300000</f>
+        <v>660000</v>
+      </c>
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>88797025</v>
-      </c>
-    </row>
-    <row r="40" spans="5:6">
+        <v>-341975</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="B40" t="s">
+        <v>60</v>
+      </c>
+      <c r="C40" s="1">
+        <f>5000000+17850000+6490000+26626500</f>
+        <v>55966500</v>
+      </c>
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>88797025</v>
+        <v>55624525</v>
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="5:6">
+    <row r="41" spans="1:6">
+      <c r="B41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D41" s="1">
+        <f>17850000+180000+430000+6490000+425000+2249500</f>
+        <v>27624500</v>
+      </c>
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>88797025</v>
-      </c>
-    </row>
-    <row r="42" spans="5:6">
+        <v>28000025</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="B42" t="s">
+        <v>74</v>
+      </c>
+      <c r="D42" s="1">
+        <f>2715500</f>
+        <v>2715500</v>
+      </c>
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>88797025</v>
-      </c>
-    </row>
-    <row r="43" spans="5:6">
+        <v>25284525</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="B43" t="s">
+        <v>63</v>
+      </c>
+      <c r="C43" s="1">
+        <f>31726525+1041975-26626500</f>
+        <v>6142000</v>
+      </c>
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>88797025</v>
-      </c>
-    </row>
-    <row r="44" spans="5:6">
+        <v>31426525</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="B44" t="s">
+        <v>64</v>
+      </c>
+      <c r="C44" s="1">
+        <v>83500</v>
+      </c>
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>88797025</v>
-      </c>
-    </row>
-    <row r="45" spans="5:6">
+        <v>31510025</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="B45" t="s">
+        <v>65</v>
+      </c>
+      <c r="D45" s="1">
+        <v>20000000</v>
+      </c>
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>88797025</v>
-      </c>
-    </row>
-    <row r="46" spans="5:6">
+        <v>11510025</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="2">
+        <v>44226</v>
+      </c>
+      <c r="B46" t="s">
+        <v>25</v>
+      </c>
+      <c r="D46" s="1">
+        <f>60000</f>
+        <v>60000</v>
+      </c>
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>88797025</v>
-      </c>
-    </row>
-    <row r="47" spans="5:6">
+        <v>11450025</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="B47" t="s">
+        <v>75</v>
+      </c>
+      <c r="D47" s="1">
+        <f>698500</f>
+        <v>698500</v>
+      </c>
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>88797025</v>
-      </c>
-    </row>
-    <row r="48" spans="5:6">
+        <v>10751525</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>88797025</v>
+        <v>10751525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 1-Feb-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>Tgl</t>
   </si>
@@ -195,57 +195,6 @@
   </si>
   <si>
     <t>GUSTAVI</t>
-  </si>
-  <si>
-    <t>TRANSFER BCA</t>
-  </si>
-  <si>
-    <t>A/R</t>
-  </si>
-  <si>
-    <t>A/P</t>
-  </si>
-  <si>
-    <t>PRIVE - andreas</t>
-  </si>
-  <si>
-    <t>SALES - cash/retail</t>
-  </si>
-  <si>
-    <t>SELISIH - lebih</t>
-  </si>
-  <si>
-    <t>SETOR KE BANK</t>
-  </si>
-  <si>
-    <t>BIAYA materai</t>
-  </si>
-  <si>
-    <t>TRANSFER BCA AA</t>
-  </si>
-  <si>
-    <t>FREIGHT OUT</t>
-  </si>
-  <si>
-    <t>andreas - prive</t>
-  </si>
-  <si>
-    <t>SELISIH - kurang</t>
-  </si>
-  <si>
-    <t>BELI kresek</t>
-  </si>
-  <si>
-    <t>CHEQUE RECEIVED</t>
-  </si>
-  <si>
-    <t>SERVICE - pintu</t>
-  </si>
-  <si>
-    <t>FREIGHT IN</t>
-  </si>
-  <si>
-    <t>BELI ban</t>
   </si>
 </sst>
 </file>
@@ -613,8 +562,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A66" sqref="A66"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -650,996 +599,683 @@
         <v>5</v>
       </c>
       <c r="E2" s="1">
-        <v>715525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>44221</v>
+        <v>44228</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="1">
-        <f>45000+195000</f>
-        <v>240000</v>
-      </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>475525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="B4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="1">
-        <f>49000+37256000+3465000+6240000+1375000+2424000-1215000</f>
-        <v>49594000</v>
-      </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>-49118475</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="B5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="1">
-        <f>37256000+28367500</f>
-        <v>65623500</v>
-      </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>16505025</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="1">
-        <f>1266000</f>
-        <v>1266000</v>
-      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>15239025</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="B7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="1">
-        <v>5000000</v>
-      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>10239025</v>
+        <v>433525</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="B8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="1">
-        <f>15349475+25076525-28367500</f>
-        <v>12058500</v>
-      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>22297525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="B9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="1">
-        <f>100000-65500</f>
-        <v>34500</v>
-      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>22332025</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="B10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="1">
-        <f>22000000</f>
-        <v>22000000</v>
-      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>332025</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="2">
-        <v>44222</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="1">
-        <f>45000+180000</f>
-        <v>225000</v>
-      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>107025</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="B12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="1">
-        <f>70000000+3203000+56774000</f>
-        <v>129977000</v>
-      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>130084025</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="1">
-        <f>70000000+1280000+81000+4360000+900000+7000000+1634000+155000</f>
-        <v>85410000</v>
-      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>44674025</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="B14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" s="1">
-        <v>12000</v>
-      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>44662025</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="B15" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" s="1">
-        <f>3203000</f>
-        <v>3203000</v>
-      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>41459025</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="B16" t="s">
-        <v>68</v>
-      </c>
-      <c r="D16" s="1">
-        <f>36000</f>
-        <v>36000</v>
-      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>41423025</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="B17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" s="1">
-        <v>5000000</v>
-      </c>
+        <v>433525</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5">
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>36423025</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="B18" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="1">
-        <f>20170975+45761025-56774000</f>
-        <v>9158000</v>
-      </c>
+        <v>433525</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5">
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>45581025</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="B19" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="1">
-        <v>336000</v>
-      </c>
+        <v>433525</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5">
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>45917025</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="B20" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" s="1">
-        <v>45000000</v>
-      </c>
+        <v>433525</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5">
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>917025</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="2">
-        <v>44223</v>
-      </c>
-      <c r="B21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="1">
-        <f>60000+260000</f>
-        <v>320000</v>
-      </c>
+        <v>433525</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5">
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>597025</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="B22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" s="1">
-        <f>1831000+10000000+57476000</f>
-        <v>69307000</v>
-      </c>
+        <v>433525</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>69904025</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="B23" t="s">
-        <v>67</v>
-      </c>
-      <c r="D23" s="1">
-        <f>1831000</f>
-        <v>1831000</v>
-      </c>
+        <v>433525</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>68073025</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="B24" t="s">
-        <v>59</v>
-      </c>
-      <c r="D24" s="1">
-        <f>27770000+1096000</f>
-        <v>28866000</v>
-      </c>
+        <v>433525</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>39207025</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="B25" t="s">
-        <v>69</v>
-      </c>
-      <c r="D25" s="1">
-        <v>5100000</v>
-      </c>
+        <v>433525</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>34107025</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="B26" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" s="1">
-        <f>23008975+43182025-57476000</f>
-        <v>8715000</v>
-      </c>
+        <v>433525</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>42822025</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="B27" t="s">
-        <v>70</v>
-      </c>
-      <c r="D27" s="1">
-        <v>28000</v>
-      </c>
+        <v>433525</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>42794025</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="B28" t="s">
-        <v>65</v>
-      </c>
-      <c r="D28" s="1">
-        <v>42000000</v>
-      </c>
+        <v>433525</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>794025</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="2">
-        <v>44224</v>
-      </c>
-      <c r="B29" t="s">
-        <v>25</v>
-      </c>
-      <c r="D29" s="1">
-        <f>60000+280000</f>
-        <v>340000</v>
-      </c>
+        <v>433525</v>
+      </c>
+    </row>
+    <row r="29" spans="5:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>454025</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="B30" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="1">
-        <f>13320000+18450000+40274000+29120000+16368000+14266000+500000+20616000</f>
-        <v>152914000</v>
-      </c>
+        <v>433525</v>
+      </c>
+    </row>
+    <row r="30" spans="5:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>153368025</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="B31" t="s">
-        <v>59</v>
-      </c>
-      <c r="D31" s="1">
-        <f>29370000+14266000+2000000+301000</f>
-        <v>45937000</v>
-      </c>
+        <v>433525</v>
+      </c>
+    </row>
+    <row r="31" spans="5:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>107431025</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="B32" t="s">
-        <v>71</v>
-      </c>
-      <c r="D32" s="1">
-        <f>99000</f>
-        <v>99000</v>
-      </c>
+        <v>433525</v>
+      </c>
+    </row>
+    <row r="32" spans="5:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>107332025</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="B33" t="s">
-        <v>72</v>
-      </c>
-      <c r="D33" s="1">
-        <f>2162000</f>
-        <v>2162000</v>
-      </c>
+        <v>433525</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>105170025</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="B34" t="s">
-        <v>62</v>
-      </c>
-      <c r="D34" s="1">
-        <v>5000000</v>
-      </c>
+        <v>433525</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>100170025</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="B35" t="s">
-        <v>63</v>
-      </c>
-      <c r="C35" s="1">
-        <f>111913025-79834025-20616000</f>
-        <v>11463000</v>
-      </c>
+        <v>433525</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>111633025</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="B36" t="s">
-        <v>73</v>
-      </c>
-      <c r="D36" s="1">
-        <v>350000</v>
-      </c>
+        <v>433525</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>111283025</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="B37" t="s">
-        <v>64</v>
-      </c>
-      <c r="C37" s="1">
-        <v>35000</v>
-      </c>
+        <v>433525</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>111318025</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="B38" t="s">
-        <v>65</v>
-      </c>
-      <c r="D38" s="1">
-        <v>111000000</v>
-      </c>
+        <v>433525</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>318025</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="2">
-        <v>44225</v>
-      </c>
-      <c r="B39" t="s">
-        <v>25</v>
-      </c>
-      <c r="D39" s="1">
-        <f>60000+300000+300000</f>
-        <v>660000</v>
-      </c>
+        <v>433525</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>-341975</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="B40" t="s">
-        <v>60</v>
-      </c>
-      <c r="C40" s="1">
-        <f>5000000+17850000+6490000+26626500</f>
-        <v>55966500</v>
-      </c>
+        <v>433525</v>
+      </c>
+    </row>
+    <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>55624525</v>
+        <v>433525</v>
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="1:6">
-      <c r="B41" t="s">
-        <v>59</v>
-      </c>
-      <c r="D41" s="1">
-        <f>17850000+180000+430000+6490000+425000+2249500</f>
-        <v>27624500</v>
-      </c>
+    <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>28000025</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="B42" t="s">
-        <v>74</v>
-      </c>
-      <c r="D42" s="1">
-        <f>2715500</f>
-        <v>2715500</v>
-      </c>
+        <v>433525</v>
+      </c>
+    </row>
+    <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>25284525</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="B43" t="s">
-        <v>63</v>
-      </c>
-      <c r="C43" s="1">
-        <f>31726525+1041975-26626500</f>
-        <v>6142000</v>
-      </c>
+        <v>433525</v>
+      </c>
+    </row>
+    <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>31426525</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="B44" t="s">
-        <v>64</v>
-      </c>
-      <c r="C44" s="1">
-        <v>83500</v>
-      </c>
+        <v>433525</v>
+      </c>
+    </row>
+    <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>31510025</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="B45" t="s">
-        <v>65</v>
-      </c>
-      <c r="D45" s="1">
-        <v>20000000</v>
-      </c>
+        <v>433525</v>
+      </c>
+    </row>
+    <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>11510025</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" s="2">
-        <v>44226</v>
-      </c>
-      <c r="B46" t="s">
-        <v>25</v>
-      </c>
-      <c r="D46" s="1">
-        <f>60000</f>
-        <v>60000</v>
-      </c>
+        <v>433525</v>
+      </c>
+    </row>
+    <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>11450025</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="B47" t="s">
-        <v>75</v>
-      </c>
-      <c r="D47" s="1">
-        <f>698500</f>
-        <v>698500</v>
-      </c>
+        <v>433525</v>
+      </c>
+    </row>
+    <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>10751525</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>433525</v>
+      </c>
+    </row>
+    <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>10751525</v>
+        <v>433525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 3-Feb-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="67">
   <si>
     <t>Tgl</t>
   </si>
@@ -195,6 +195,30 @@
   </si>
   <si>
     <t>GUSTAVI</t>
+  </si>
+  <si>
+    <t>TRANSFER BCA</t>
+  </si>
+  <si>
+    <t>A/R</t>
+  </si>
+  <si>
+    <t>SALES - cash/retail</t>
+  </si>
+  <si>
+    <t>SELISIH - kurang</t>
+  </si>
+  <si>
+    <t>SETOR KE BANK</t>
+  </si>
+  <si>
+    <t>SOLAR - kijang D-1682-QU</t>
+  </si>
+  <si>
+    <t>andreas - prive</t>
+  </si>
+  <si>
+    <t>SELISIH - lebih</t>
   </si>
 </sst>
 </file>
@@ -562,8 +586,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <pane ySplit="2" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -609,673 +633,771 @@
       <c r="B3" t="s">
         <v>25</v>
       </c>
+      <c r="D3" s="1">
+        <f>60000+260000</f>
+        <v>320000</v>
+      </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>433525</v>
+        <v>113525</v>
       </c>
     </row>
     <row r="4" spans="1:6">
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="1">
+        <f>980000+3200000+741500+438000+2000000+630000+50000</f>
+        <v>8039500</v>
+      </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>433525</v>
+        <v>-7925975</v>
       </c>
     </row>
     <row r="5" spans="1:6">
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="1">
+        <f>1000000+2800000+31305500</f>
+        <v>35105500</v>
+      </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>433525</v>
+        <v>27179525</v>
       </c>
     </row>
     <row r="6" spans="1:6">
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="1">
+        <f>43189525+4125975-31305500</f>
+        <v>16010000</v>
+      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>433525</v>
+        <v>43189525</v>
       </c>
     </row>
     <row r="7" spans="1:6">
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="1">
+        <v>80000</v>
+      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>433525</v>
+        <v>43109525</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="1">
+        <v>42000000</v>
+      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>433525</v>
+        <v>1109525</v>
       </c>
     </row>
     <row r="9" spans="1:6">
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="1">
+        <v>350000</v>
+      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>433525</v>
+        <v>759525</v>
       </c>
     </row>
     <row r="10" spans="1:6">
+      <c r="A10" s="2">
+        <v>44229</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="1">
+        <f>60000+260000</f>
+        <v>320000</v>
+      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>433525</v>
+        <v>439525</v>
       </c>
     </row>
     <row r="11" spans="1:6">
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="1">
+        <f>60000000+795000+2282000+2769000+1945000</f>
+        <v>67791000</v>
+      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>433525</v>
+        <v>-67351475</v>
       </c>
     </row>
     <row r="12" spans="1:6">
+      <c r="B12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="1">
+        <f>200000000+1945000+25527000</f>
+        <v>227472000</v>
+      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>433525</v>
+        <v>160120525</v>
       </c>
     </row>
     <row r="13" spans="1:6">
+      <c r="B13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="1">
+        <v>5000000</v>
+      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>433525</v>
+        <v>155120525</v>
       </c>
     </row>
     <row r="14" spans="1:6">
+      <c r="B14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="1">
+        <f>162853525-129853525-25527000</f>
+        <v>7473000</v>
+      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>433525</v>
+        <v>162593525</v>
       </c>
     </row>
     <row r="15" spans="1:6">
+      <c r="B15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="1">
+        <v>110000</v>
+      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>433525</v>
+        <v>162703525</v>
       </c>
     </row>
     <row r="16" spans="1:6">
+      <c r="B16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="1">
+        <v>162000000</v>
+      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>433525</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5">
+        <v>703525</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2">
+        <v>44230</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>433525</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5">
+        <v>703525</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>433525</v>
-      </c>
-    </row>
-    <row r="19" spans="5:5">
+        <v>703525</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>433525</v>
-      </c>
-    </row>
-    <row r="20" spans="5:5">
+        <v>703525</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>433525</v>
-      </c>
-    </row>
-    <row r="21" spans="5:5">
+        <v>703525</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>433525</v>
-      </c>
-    </row>
-    <row r="22" spans="5:5">
+        <v>703525</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>433525</v>
-      </c>
-    </row>
-    <row r="23" spans="5:5">
+        <v>703525</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>433525</v>
-      </c>
-    </row>
-    <row r="24" spans="5:5">
+        <v>703525</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>433525</v>
-      </c>
-    </row>
-    <row r="25" spans="5:5">
+        <v>703525</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>433525</v>
-      </c>
-    </row>
-    <row r="26" spans="5:5">
+        <v>703525</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>433525</v>
-      </c>
-    </row>
-    <row r="27" spans="5:5">
+        <v>703525</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>433525</v>
-      </c>
-    </row>
-    <row r="28" spans="5:5">
+        <v>703525</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>433525</v>
-      </c>
-    </row>
-    <row r="29" spans="5:5">
+        <v>703525</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>433525</v>
-      </c>
-    </row>
-    <row r="30" spans="5:5">
+        <v>703525</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>433525</v>
-      </c>
-    </row>
-    <row r="31" spans="5:5">
+        <v>703525</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>433525</v>
-      </c>
-    </row>
-    <row r="32" spans="5:5">
+        <v>703525</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>433525</v>
+        <v>703525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 4-Feb-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="69">
   <si>
     <t>Tgl</t>
   </si>
@@ -219,6 +219,12 @@
   </si>
   <si>
     <t>SELISIH - lebih</t>
+  </si>
+  <si>
+    <t>LPG</t>
+  </si>
+  <si>
+    <t>IURAN DAERAH</t>
   </si>
 </sst>
 </file>
@@ -586,8 +592,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
+      <pane ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -816,588 +822,657 @@
       <c r="B17" t="s">
         <v>25</v>
       </c>
+      <c r="D17" s="1">
+        <f>60000+300000</f>
+        <v>360000</v>
+      </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>703525</v>
+        <v>343525</v>
       </c>
     </row>
     <row r="18" spans="1:5">
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="1">
+        <f>20400000+5820000+38426000</f>
+        <v>64646000</v>
+      </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>703525</v>
+        <v>64989525</v>
       </c>
     </row>
     <row r="19" spans="1:5">
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="1">
+        <f>20400000+2574000+5000000+2262000+850000</f>
+        <v>31086000</v>
+      </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>703525</v>
+        <v>33903525</v>
       </c>
     </row>
     <row r="20" spans="1:5">
+      <c r="B20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="1">
+        <v>145000</v>
+      </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>703525</v>
+        <v>33758525</v>
       </c>
     </row>
     <row r="21" spans="1:5">
+      <c r="B21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="1">
+        <f>25000</f>
+        <v>25000</v>
+      </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>703525</v>
+        <v>33733525</v>
       </c>
     </row>
     <row r="22" spans="1:5">
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="1">
+        <f>4392475+42166525-38426000</f>
+        <v>8133000</v>
+      </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>703525</v>
+        <v>41866525</v>
       </c>
     </row>
     <row r="23" spans="1:5">
+      <c r="B23" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="1">
+        <f>41000000</f>
+        <v>41000000</v>
+      </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>703525</v>
+        <v>866525</v>
       </c>
     </row>
     <row r="24" spans="1:5">
+      <c r="A24" s="2">
+        <v>44231</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="1">
+        <f>60000</f>
+        <v>60000</v>
+      </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>703525</v>
+        <v>806525</v>
       </c>
     </row>
     <row r="25" spans="1:5">
+      <c r="B25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="1">
+        <f>1550000+41600000</f>
+        <v>43150000</v>
+      </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>703525</v>
+        <v>-42343475</v>
       </c>
     </row>
     <row r="26" spans="1:5">
+      <c r="B26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="1">
+        <f>17240000+24360000</f>
+        <v>41600000</v>
+      </c>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>703525</v>
+        <v>-743475</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 5-Feb-2021, end of day update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="72">
   <si>
     <t>Tgl</t>
   </si>
@@ -225,6 +225,15 @@
   </si>
   <si>
     <t>IURAN DAERAH</t>
+  </si>
+  <si>
+    <t>A/P</t>
+  </si>
+  <si>
+    <t>FREIGHT OUT</t>
+  </si>
+  <si>
+    <t>DOKTER - qiu</t>
   </si>
 </sst>
 </file>
@@ -592,8 +601,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
+      <pane ySplit="2" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -916,12 +925,12 @@
         <v>25</v>
       </c>
       <c r="D24" s="1">
-        <f>60000</f>
-        <v>60000</v>
+        <f>60000+260000</f>
+        <v>320000</v>
       </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>806525</v>
+        <v>546525</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -929,12 +938,12 @@
         <v>59</v>
       </c>
       <c r="D25" s="1">
-        <f>1550000+41600000</f>
-        <v>43150000</v>
+        <f>1550000+41600000+900000+600000</f>
+        <v>44650000</v>
       </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>-42343475</v>
+        <v>-44103475</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -942,537 +951,600 @@
         <v>60</v>
       </c>
       <c r="C26" s="1">
-        <f>17240000+24360000</f>
-        <v>41600000</v>
+        <f>17240000+24360000+26415000</f>
+        <v>68015000</v>
       </c>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>-743475</v>
+        <v>23911525</v>
       </c>
     </row>
     <row r="27" spans="1:5">
+      <c r="B27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" s="1">
+        <f>1877000</f>
+        <v>1877000</v>
+      </c>
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>-743475</v>
+        <v>22034525</v>
       </c>
     </row>
     <row r="28" spans="1:5">
+      <c r="B28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="1">
+        <f>4120475+30658525-26415000</f>
+        <v>8364000</v>
+      </c>
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>-743475</v>
+        <v>30398525</v>
       </c>
     </row>
     <row r="29" spans="1:5">
+      <c r="B29" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" s="1">
+        <v>54000</v>
+      </c>
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>-743475</v>
+        <v>30344525</v>
       </c>
     </row>
     <row r="30" spans="1:5">
+      <c r="B30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="1">
+        <v>425000</v>
+      </c>
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>-743475</v>
+        <v>29919525</v>
       </c>
     </row>
     <row r="31" spans="1:5">
+      <c r="B31" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" s="1">
+        <f>29000000</f>
+        <v>29000000</v>
+      </c>
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>-743475</v>
+        <v>919525</v>
       </c>
     </row>
     <row r="32" spans="1:5">
+      <c r="B32" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="1">
+        <v>800000</v>
+      </c>
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>-743475</v>
-      </c>
-    </row>
-    <row r="33" spans="5:6">
+        <v>119525</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B33" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" s="1">
+        <f>60000</f>
+        <v>60000</v>
+      </c>
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>-743475</v>
-      </c>
-    </row>
-    <row r="34" spans="5:6">
+        <v>59525</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="B34" t="s">
+        <v>59</v>
+      </c>
+      <c r="D34" s="1">
+        <f>2216000+154800000+1130000+55000</f>
+        <v>158201000</v>
+      </c>
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>-743475</v>
-      </c>
-    </row>
-    <row r="35" spans="5:6">
+        <v>-158141475</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="B35" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="1">
+        <f>154800000</f>
+        <v>154800000</v>
+      </c>
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>-743475</v>
-      </c>
-    </row>
-    <row r="36" spans="5:6">
+        <v>-3341475</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>-743475</v>
-      </c>
-    </row>
-    <row r="37" spans="5:6">
+        <v>-3341475</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>-743475</v>
-      </c>
-    </row>
-    <row r="38" spans="5:6">
+        <v>-3341475</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>-743475</v>
-      </c>
-    </row>
-    <row r="39" spans="5:6">
+        <v>-3341475</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>-743475</v>
-      </c>
-    </row>
-    <row r="40" spans="5:6">
+        <v>-3341475</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="5:6">
+    <row r="41" spans="1:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>-743475</v>
-      </c>
-    </row>
-    <row r="42" spans="5:6">
+        <v>-3341475</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>-743475</v>
-      </c>
-    </row>
-    <row r="43" spans="5:6">
+        <v>-3341475</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>-743475</v>
-      </c>
-    </row>
-    <row r="44" spans="5:6">
+        <v>-3341475</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>-743475</v>
-      </c>
-    </row>
-    <row r="45" spans="5:6">
+        <v>-3341475</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>-743475</v>
-      </c>
-    </row>
-    <row r="46" spans="5:6">
+        <v>-3341475</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>-743475</v>
-      </c>
-    </row>
-    <row r="47" spans="5:6">
+        <v>-3341475</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>-743475</v>
-      </c>
-    </row>
-    <row r="48" spans="5:6">
+        <v>-3341475</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>-743475</v>
+        <v>-3341475</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 6-Feb-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="74">
   <si>
     <t>Tgl</t>
   </si>
@@ -234,6 +234,12 @@
   </si>
   <si>
     <t>DOKTER - qiu</t>
+  </si>
+  <si>
+    <t>BELI kresek</t>
+  </si>
+  <si>
+    <t>BENSIN - rush</t>
   </si>
 </sst>
 </file>
@@ -601,8 +607,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
+      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1042,12 +1048,12 @@
         <v>25</v>
       </c>
       <c r="D33" s="1">
-        <f>60000</f>
-        <v>60000</v>
+        <f>60000+260000</f>
+        <v>320000</v>
       </c>
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>59525</v>
+        <v>-200475</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1055,12 +1061,12 @@
         <v>59</v>
       </c>
       <c r="D34" s="1">
-        <f>2216000+154800000+1130000+55000</f>
-        <v>158201000</v>
+        <f>2216000+154800000+1130000+55000+5070000</f>
+        <v>163271000</v>
       </c>
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>-158141475</v>
+        <v>-163471475</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1068,483 +1074,538 @@
         <v>60</v>
       </c>
       <c r="C35" s="1">
-        <f>154800000</f>
-        <v>154800000</v>
+        <f>154800000+14262000</f>
+        <v>169062000</v>
       </c>
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>-3341475</v>
+        <v>5590525</v>
       </c>
     </row>
     <row r="36" spans="1:6">
+      <c r="B36" t="s">
+        <v>72</v>
+      </c>
+      <c r="D36" s="1">
+        <v>82000</v>
+      </c>
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>-3341475</v>
+        <v>5508525</v>
       </c>
     </row>
     <row r="37" spans="1:6">
+      <c r="B37" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="1">
+        <f>8493475+11686525-14262000</f>
+        <v>5918000</v>
+      </c>
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>-3341475</v>
+        <v>11426525</v>
       </c>
     </row>
     <row r="38" spans="1:6">
+      <c r="B38" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" s="1">
+        <v>60000</v>
+      </c>
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>-3341475</v>
+        <v>11486525</v>
       </c>
     </row>
     <row r="39" spans="1:6">
+      <c r="B39" t="s">
+        <v>63</v>
+      </c>
+      <c r="D39" s="1">
+        <v>11000000</v>
+      </c>
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>-3341475</v>
+        <v>486525</v>
       </c>
     </row>
     <row r="40" spans="1:6">
+      <c r="A40" s="2">
+        <v>44233</v>
+      </c>
+      <c r="B40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40" s="1">
+        <f>60000</f>
+        <v>60000</v>
+      </c>
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>-3341475</v>
+        <v>426525</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:6">
+      <c r="B41" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" s="1">
+        <f>500000+16610000+12250000</f>
+        <v>29360000</v>
+      </c>
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>-3341475</v>
+        <v>29786525</v>
       </c>
     </row>
     <row r="42" spans="1:6">
+      <c r="B42" t="s">
+        <v>59</v>
+      </c>
+      <c r="D42" s="1">
+        <f>28860000+2100000</f>
+        <v>30960000</v>
+      </c>
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>-3341475</v>
+        <v>-1173475</v>
       </c>
     </row>
     <row r="43" spans="1:6">
+      <c r="B43" t="s">
+        <v>73</v>
+      </c>
+      <c r="D43" s="1">
+        <v>250000</v>
+      </c>
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>-3341475</v>
+        <v>-1423475</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 7-Feb-2021, end of day update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>Tgl</t>
   </si>
@@ -195,51 +195,6 @@
   </si>
   <si>
     <t>GUSTAVI</t>
-  </si>
-  <si>
-    <t>TRANSFER BCA</t>
-  </si>
-  <si>
-    <t>A/R</t>
-  </si>
-  <si>
-    <t>SALES - cash/retail</t>
-  </si>
-  <si>
-    <t>SELISIH - kurang</t>
-  </si>
-  <si>
-    <t>SETOR KE BANK</t>
-  </si>
-  <si>
-    <t>SOLAR - kijang D-1682-QU</t>
-  </si>
-  <si>
-    <t>andreas - prive</t>
-  </si>
-  <si>
-    <t>SELISIH - lebih</t>
-  </si>
-  <si>
-    <t>LPG</t>
-  </si>
-  <si>
-    <t>IURAN DAERAH</t>
-  </si>
-  <si>
-    <t>A/P</t>
-  </si>
-  <si>
-    <t>FREIGHT OUT</t>
-  </si>
-  <si>
-    <t>DOKTER - qiu</t>
-  </si>
-  <si>
-    <t>BELI kresek</t>
-  </si>
-  <si>
-    <t>BENSIN - rush</t>
   </si>
 </sst>
 </file>
@@ -607,8 +562,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C60" sqref="C60"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -644,968 +599,683 @@
         <v>5</v>
       </c>
       <c r="E2" s="1">
-        <v>433525</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>44228</v>
+        <v>44235</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="1">
-        <f>60000+260000</f>
-        <v>320000</v>
-      </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>113525</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="B4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="1">
-        <f>980000+3200000+741500+438000+2000000+630000+50000</f>
-        <v>8039500</v>
-      </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>-7925975</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="B5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="1">
-        <f>1000000+2800000+31305500</f>
-        <v>35105500</v>
-      </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>27179525</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="1">
-        <f>43189525+4125975-31305500</f>
-        <v>16010000</v>
-      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>43189525</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="B7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="1">
-        <v>80000</v>
-      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>43109525</v>
+        <v>934525</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="B8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" s="1">
-        <v>42000000</v>
-      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>1109525</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="B9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="1">
-        <v>350000</v>
-      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>759525</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="2">
-        <v>44229</v>
-      </c>
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="1">
-        <f>60000+260000</f>
-        <v>320000</v>
-      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>439525</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="B11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="1">
-        <f>60000000+795000+2282000+2769000+1945000</f>
-        <v>67791000</v>
-      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>-67351475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="B12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="1">
-        <f>200000000+1945000+25527000</f>
-        <v>227472000</v>
-      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>160120525</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13" s="1">
-        <v>5000000</v>
-      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>155120525</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="B14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" s="1">
-        <f>162853525-129853525-25527000</f>
-        <v>7473000</v>
-      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>162593525</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="B15" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" s="1">
-        <v>110000</v>
-      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>162703525</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="B16" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="1">
-        <v>162000000</v>
-      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>703525</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="2">
-        <v>44230</v>
-      </c>
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="1">
-        <f>60000+300000</f>
-        <v>360000</v>
-      </c>
+        <v>934525</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5">
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>343525</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="B18" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="1">
-        <f>20400000+5820000+38426000</f>
-        <v>64646000</v>
-      </c>
+        <v>934525</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5">
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>64989525</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="B19" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" s="1">
-        <f>20400000+2574000+5000000+2262000+850000</f>
-        <v>31086000</v>
-      </c>
+        <v>934525</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5">
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>33903525</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="B20" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="1">
-        <v>145000</v>
-      </c>
+        <v>934525</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5">
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>33758525</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="B21" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="1">
-        <f>25000</f>
-        <v>25000</v>
-      </c>
+        <v>934525</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5">
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>33733525</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="B22" t="s">
-        <v>61</v>
-      </c>
-      <c r="C22" s="1">
-        <f>4392475+42166525-38426000</f>
-        <v>8133000</v>
-      </c>
+        <v>934525</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>41866525</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="B23" t="s">
-        <v>63</v>
-      </c>
-      <c r="D23" s="1">
-        <f>41000000</f>
-        <v>41000000</v>
-      </c>
+        <v>934525</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>866525</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="2">
-        <v>44231</v>
-      </c>
-      <c r="B24" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="1">
-        <f>60000+260000</f>
-        <v>320000</v>
-      </c>
+        <v>934525</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>546525</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="B25" t="s">
-        <v>59</v>
-      </c>
-      <c r="D25" s="1">
-        <f>1550000+41600000+900000+600000</f>
-        <v>44650000</v>
-      </c>
+        <v>934525</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>-44103475</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="B26" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" s="1">
-        <f>17240000+24360000+26415000</f>
-        <v>68015000</v>
-      </c>
+        <v>934525</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>23911525</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="B27" t="s">
-        <v>69</v>
-      </c>
-      <c r="D27" s="1">
-        <f>1877000</f>
-        <v>1877000</v>
-      </c>
+        <v>934525</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>22034525</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="B28" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" s="1">
-        <f>4120475+30658525-26415000</f>
-        <v>8364000</v>
-      </c>
+        <v>934525</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>30398525</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="B29" t="s">
-        <v>70</v>
-      </c>
-      <c r="D29" s="1">
-        <v>54000</v>
-      </c>
+        <v>934525</v>
+      </c>
+    </row>
+    <row r="29" spans="5:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>30344525</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="B30" t="s">
-        <v>62</v>
-      </c>
-      <c r="D30" s="1">
-        <v>425000</v>
-      </c>
+        <v>934525</v>
+      </c>
+    </row>
+    <row r="30" spans="5:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>29919525</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="B31" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" s="1">
-        <f>29000000</f>
-        <v>29000000</v>
-      </c>
+        <v>934525</v>
+      </c>
+    </row>
+    <row r="31" spans="5:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>919525</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="B32" t="s">
-        <v>71</v>
-      </c>
-      <c r="D32" s="1">
-        <v>800000</v>
-      </c>
+        <v>934525</v>
+      </c>
+    </row>
+    <row r="32" spans="5:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>119525</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="2">
-        <v>44232</v>
-      </c>
-      <c r="B33" t="s">
-        <v>25</v>
-      </c>
-      <c r="D33" s="1">
-        <f>60000+260000</f>
-        <v>320000</v>
-      </c>
+        <v>934525</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>-200475</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="B34" t="s">
-        <v>59</v>
-      </c>
-      <c r="D34" s="1">
-        <f>2216000+154800000+1130000+55000+5070000</f>
-        <v>163271000</v>
-      </c>
+        <v>934525</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>-163471475</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="B35" t="s">
-        <v>60</v>
-      </c>
-      <c r="C35" s="1">
-        <f>154800000+14262000</f>
-        <v>169062000</v>
-      </c>
+        <v>934525</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>5590525</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="B36" t="s">
-        <v>72</v>
-      </c>
-      <c r="D36" s="1">
-        <v>82000</v>
-      </c>
+        <v>934525</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>5508525</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="B37" t="s">
-        <v>61</v>
-      </c>
-      <c r="C37" s="1">
-        <f>8493475+11686525-14262000</f>
-        <v>5918000</v>
-      </c>
+        <v>934525</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>11426525</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="B38" t="s">
-        <v>66</v>
-      </c>
-      <c r="C38" s="1">
-        <v>60000</v>
-      </c>
+        <v>934525</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>11486525</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="B39" t="s">
-        <v>63</v>
-      </c>
-      <c r="D39" s="1">
-        <v>11000000</v>
-      </c>
+        <v>934525</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>486525</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="2">
-        <v>44233</v>
-      </c>
-      <c r="B40" t="s">
-        <v>25</v>
-      </c>
-      <c r="D40" s="1">
-        <f>60000</f>
-        <v>60000</v>
-      </c>
+        <v>934525</v>
+      </c>
+    </row>
+    <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>426525</v>
+        <v>934525</v>
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="1:6">
-      <c r="B41" t="s">
-        <v>60</v>
-      </c>
-      <c r="C41" s="1">
-        <f>500000+16610000+12250000</f>
-        <v>29360000</v>
-      </c>
+    <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>29786525</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="B42" t="s">
-        <v>59</v>
-      </c>
-      <c r="D42" s="1">
-        <f>28860000+2100000</f>
-        <v>30960000</v>
-      </c>
+        <v>934525</v>
+      </c>
+    </row>
+    <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>-1173475</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="B43" t="s">
-        <v>73</v>
-      </c>
-      <c r="D43" s="1">
-        <v>250000</v>
-      </c>
+        <v>934525</v>
+      </c>
+    </row>
+    <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>-1423475</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>934525</v>
+      </c>
+    </row>
+    <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>-1423475</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>934525</v>
+      </c>
+    </row>
+    <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>-1423475</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>934525</v>
+      </c>
+    </row>
+    <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>-1423475</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>934525</v>
+      </c>
+    </row>
+    <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>-1423475</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>934525</v>
+      </c>
+    </row>
+    <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>-1423475</v>
+        <v>934525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 9-Feb-2021, end of day update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="66">
   <si>
     <t>Tgl</t>
   </si>
@@ -195,6 +195,27 @@
   </si>
   <si>
     <t>GUSTAVI</t>
+  </si>
+  <si>
+    <t>TAX - IURAN ARIESTA</t>
+  </si>
+  <si>
+    <t>TAX - P.Tata</t>
+  </si>
+  <si>
+    <t>A/R</t>
+  </si>
+  <si>
+    <t>TRANSFER BCA</t>
+  </si>
+  <si>
+    <t>SALES - cash/retail</t>
+  </si>
+  <si>
+    <t>SELISIH - lebih</t>
+  </si>
+  <si>
+    <t>SETOR KE BANK</t>
   </si>
 </sst>
 </file>
@@ -563,7 +584,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -609,673 +630,746 @@
       <c r="B3" t="s">
         <v>25</v>
       </c>
+      <c r="D3" s="1">
+        <f>60000+260000</f>
+        <v>320000</v>
+      </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>934525</v>
+        <v>614525</v>
       </c>
     </row>
     <row r="4" spans="1:6">
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="1">
+        <v>660000</v>
+      </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>934525</v>
+        <v>-45475</v>
       </c>
     </row>
     <row r="5" spans="1:6">
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="1">
+        <v>200000</v>
+      </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>934525</v>
+        <v>-245475</v>
       </c>
     </row>
     <row r="6" spans="1:6">
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="1">
+        <f>6420000+5580000+5000000+1794000+1900000+70000000+29598000</f>
+        <v>120292000</v>
+      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>934525</v>
+        <v>120046525</v>
       </c>
     </row>
     <row r="7" spans="1:6">
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="1">
+        <f>1787000+1794000</f>
+        <v>3581000</v>
+      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>934525</v>
+        <v>116465525</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="1">
+        <f>124499525-87127525-29598000</f>
+        <v>7774000</v>
+      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>934525</v>
+        <v>124239525</v>
       </c>
     </row>
     <row r="9" spans="1:6">
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="1">
+        <v>446500</v>
+      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>934525</v>
+        <v>124686025</v>
       </c>
     </row>
     <row r="10" spans="1:6">
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="1">
+        <v>124000000</v>
+      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>934525</v>
+        <v>686025</v>
       </c>
     </row>
     <row r="11" spans="1:6">
+      <c r="A11" s="2">
+        <v>44236</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="1">
+        <f>60000</f>
+        <v>60000</v>
+      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>934525</v>
+        <v>626025</v>
       </c>
     </row>
     <row r="12" spans="1:6">
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="1">
+        <f>8839000+6709000+3720000+842000+25000000</f>
+        <v>45110000</v>
+      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>934525</v>
+        <v>-44483975</v>
       </c>
     </row>
     <row r="13" spans="1:6">
+      <c r="B13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="1">
+        <f>6000000</f>
+        <v>6000000</v>
+      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="17" spans="5:5">
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="18" spans="5:5">
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="19" spans="5:5">
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="20" spans="5:5">
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="21" spans="5:5">
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="22" spans="5:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="23" spans="5:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="24" spans="5:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="25" spans="5:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="26" spans="5:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="27" spans="5:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="28" spans="5:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="29" spans="5:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="30" spans="5:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="31" spans="5:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="32" spans="5:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>934525</v>
+        <v>-38483975</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 11-Feb-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="69">
   <si>
     <t>Tgl</t>
   </si>
@@ -216,6 +216,15 @@
   </si>
   <si>
     <t>SETOR KE BANK</t>
+  </si>
+  <si>
+    <t>SELISIH - kurang</t>
+  </si>
+  <si>
+    <t>FREIGHT OUT</t>
+  </si>
+  <si>
+    <t>CHEQUE RECEIVED</t>
   </si>
 </sst>
 </file>
@@ -583,8 +592,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <pane ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -735,12 +744,12 @@
         <v>25</v>
       </c>
       <c r="D11" s="1">
-        <f>60000</f>
-        <v>60000</v>
+        <f>60000+300000</f>
+        <v>360000</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>626025</v>
+        <v>326025</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -748,12 +757,12 @@
         <v>62</v>
       </c>
       <c r="D12" s="1">
-        <f>8839000+6709000+3720000+842000+25000000</f>
-        <v>45110000</v>
+        <f>8839000+6709000+3720000+842500+25000000+900000+1488000</f>
+        <v>47498500</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>-44483975</v>
+        <v>-47172475</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -761,615 +770,714 @@
         <v>61</v>
       </c>
       <c r="C13" s="1">
-        <f>6000000</f>
-        <v>6000000</v>
+        <f>6000000+4332500+56547500</f>
+        <v>66880000</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>-38483975</v>
+        <v>19707525</v>
       </c>
     </row>
     <row r="14" spans="1:6">
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="1">
+        <f>36539975+27017525-56547500</f>
+        <v>7010000</v>
+      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>-38483975</v>
+        <v>26717525</v>
       </c>
     </row>
     <row r="15" spans="1:6">
+      <c r="B15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="1">
+        <v>70500</v>
+      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>-38483975</v>
+        <v>26647025</v>
       </c>
     </row>
     <row r="16" spans="1:6">
+      <c r="B16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="1">
+        <v>26000000</v>
+      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>-38483975</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5">
+        <v>647025</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2">
+        <v>44237</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="1">
+        <f>60000+260000</f>
+        <v>320000</v>
+      </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>-38483975</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5">
+        <v>327025</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="B18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="1">
+        <f>6550000+10079000</f>
+        <v>16629000</v>
+      </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>-38483975</v>
-      </c>
-    </row>
-    <row r="19" spans="5:5">
+        <v>16956025</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="B19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="1">
+        <v>135000</v>
+      </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>-38483975</v>
-      </c>
-    </row>
-    <row r="20" spans="5:5">
+        <v>16821025</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="1">
+        <f>5175000+3900000+1004000+70000</f>
+        <v>10149000</v>
+      </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>-38483975</v>
-      </c>
-    </row>
-    <row r="21" spans="5:5">
+        <v>6672025</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="1">
+        <f>3146975+11687025-10079000</f>
+        <v>4755000</v>
+      </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>-38483975</v>
-      </c>
-    </row>
-    <row r="22" spans="5:5">
+        <v>11427025</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="B22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="1">
+        <v>114500</v>
+      </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>-38483975</v>
-      </c>
-    </row>
-    <row r="23" spans="5:5">
+        <v>11541525</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="B23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="1">
+        <v>11000000</v>
+      </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>-38483975</v>
-      </c>
-    </row>
-    <row r="24" spans="5:5">
+        <v>541525</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="2">
+        <v>44238</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="1">
+        <f>60000</f>
+        <v>60000</v>
+      </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>-38483975</v>
-      </c>
-    </row>
-    <row r="25" spans="5:5">
+        <v>481525</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="B25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="1">
+        <f>2000000+762500+5840000</f>
+        <v>8602500</v>
+      </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>-38483975</v>
-      </c>
-    </row>
-    <row r="26" spans="5:5">
+        <v>9084025</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="B26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="1">
+        <f>762500</f>
+        <v>762500</v>
+      </c>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>-38483975</v>
-      </c>
-    </row>
-    <row r="27" spans="5:5">
+        <v>8321525</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="B27" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="1">
+        <f>3155000</f>
+        <v>3155000</v>
+      </c>
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>-38483975</v>
-      </c>
-    </row>
-    <row r="28" spans="5:5">
+        <v>5166525</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>-38483975</v>
-      </c>
-    </row>
-    <row r="29" spans="5:5">
+        <v>5166525</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>-38483975</v>
-      </c>
-    </row>
-    <row r="30" spans="5:5">
+        <v>5166525</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>-38483975</v>
-      </c>
-    </row>
-    <row r="31" spans="5:5">
+        <v>5166525</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>-38483975</v>
-      </c>
-    </row>
-    <row r="32" spans="5:5">
+        <v>5166525</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>-38483975</v>
+        <v>5166525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 13-Feb-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="69">
   <si>
     <t>Tgl</t>
   </si>
@@ -592,8 +592,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E44" sqref="E44"/>
+      <pane ySplit="2" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -914,12 +914,12 @@
         <v>25</v>
       </c>
       <c r="D24" s="1">
-        <f>60000</f>
-        <v>60000</v>
+        <f>60000+260000</f>
+        <v>320000</v>
       </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>481525</v>
+        <v>221525</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -927,12 +927,12 @@
         <v>61</v>
       </c>
       <c r="C25" s="1">
-        <f>2000000+762500+5840000</f>
-        <v>8602500</v>
+        <f>2000000+762500+5840000+15740000+3850000+21101000</f>
+        <v>49293500</v>
       </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>9084025</v>
+        <v>49515025</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -940,12 +940,12 @@
         <v>62</v>
       </c>
       <c r="D26" s="1">
-        <f>762500</f>
-        <v>762500</v>
+        <f>762500+15740000+2072000</f>
+        <v>18574500</v>
       </c>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>8321525</v>
+        <v>30940525</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -958,526 +958,569 @@
       </c>
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>5166525</v>
+        <v>27785525</v>
       </c>
     </row>
     <row r="28" spans="1:5">
+      <c r="B28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="1">
+        <f>40460525-9016525-21101000</f>
+        <v>10343000</v>
+      </c>
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>5166525</v>
+        <v>38128525</v>
       </c>
     </row>
     <row r="29" spans="1:5">
+      <c r="B29" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="1">
+        <v>10000</v>
+      </c>
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>5166525</v>
+        <v>38138525</v>
       </c>
     </row>
     <row r="30" spans="1:5">
+      <c r="B30" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30" s="1">
+        <v>38000000</v>
+      </c>
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>5166525</v>
+        <v>138525</v>
       </c>
     </row>
     <row r="31" spans="1:5">
+      <c r="A31" s="2">
+        <v>44513</v>
+      </c>
+      <c r="B31" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="1">
+        <f>60000</f>
+        <v>60000</v>
+      </c>
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>5166525</v>
+        <v>78525</v>
       </c>
     </row>
     <row r="32" spans="1:5">
+      <c r="B32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="1">
+        <f>5250000+90000000</f>
+        <v>95250000</v>
+      </c>
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>5166525</v>
-      </c>
-    </row>
-    <row r="33" spans="5:6">
+        <v>95328525</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6">
+      <c r="B33" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" s="1">
+        <f>5250000+50000000+2500000</f>
+        <v>57750000</v>
+      </c>
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>5166525</v>
-      </c>
-    </row>
-    <row r="34" spans="5:6">
+        <v>37578525</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>5166525</v>
-      </c>
-    </row>
-    <row r="35" spans="5:6">
+        <v>37578525</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>5166525</v>
-      </c>
-    </row>
-    <row r="36" spans="5:6">
+        <v>37578525</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>5166525</v>
-      </c>
-    </row>
-    <row r="37" spans="5:6">
+        <v>37578525</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>5166525</v>
-      </c>
-    </row>
-    <row r="38" spans="5:6">
+        <v>37578525</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>5166525</v>
-      </c>
-    </row>
-    <row r="39" spans="5:6">
+        <v>37578525</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>5166525</v>
-      </c>
-    </row>
-    <row r="40" spans="5:6">
+        <v>37578525</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="5:6">
+    <row r="41" spans="2:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>5166525</v>
-      </c>
-    </row>
-    <row r="42" spans="5:6">
+        <v>37578525</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>5166525</v>
-      </c>
-    </row>
-    <row r="43" spans="5:6">
+        <v>37578525</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>5166525</v>
-      </c>
-    </row>
-    <row r="44" spans="5:6">
+        <v>37578525</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>5166525</v>
-      </c>
-    </row>
-    <row r="45" spans="5:6">
+        <v>37578525</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>5166525</v>
-      </c>
-    </row>
-    <row r="46" spans="5:6">
+        <v>37578525</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>5166525</v>
-      </c>
-    </row>
-    <row r="47" spans="5:6">
+        <v>37578525</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>5166525</v>
-      </c>
-    </row>
-    <row r="48" spans="5:6">
+        <v>37578525</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>5166525</v>
+        <v>37578525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 15 Feb 2021, end of day update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>Tgl</t>
   </si>
@@ -195,36 +195,6 @@
   </si>
   <si>
     <t>GUSTAVI</t>
-  </si>
-  <si>
-    <t>TAX - IURAN ARIESTA</t>
-  </si>
-  <si>
-    <t>TAX - P.Tata</t>
-  </si>
-  <si>
-    <t>A/R</t>
-  </si>
-  <si>
-    <t>TRANSFER BCA</t>
-  </si>
-  <si>
-    <t>SALES - cash/retail</t>
-  </si>
-  <si>
-    <t>SELISIH - lebih</t>
-  </si>
-  <si>
-    <t>SETOR KE BANK</t>
-  </si>
-  <si>
-    <t>SELISIH - kurang</t>
-  </si>
-  <si>
-    <t>FREIGHT OUT</t>
-  </si>
-  <si>
-    <t>CHEQUE RECEIVED</t>
   </si>
 </sst>
 </file>
@@ -592,8 +562,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -629,898 +599,683 @@
         <v>5</v>
       </c>
       <c r="E2" s="1">
-        <v>934525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>44235</v>
+        <v>44242</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="1">
-        <f>60000+260000</f>
-        <v>320000</v>
-      </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>614525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="B4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="1">
-        <v>660000</v>
-      </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>-45475</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="B5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="1">
-        <v>200000</v>
-      </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>-245475</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="1">
-        <f>6420000+5580000+5000000+1794000+1900000+70000000+29598000</f>
-        <v>120292000</v>
-      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>120046525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="B7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="1">
-        <f>1787000+1794000</f>
-        <v>3581000</v>
-      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>116465525</v>
+        <v>854500</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="B8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="1">
-        <f>124499525-87127525-29598000</f>
-        <v>7774000</v>
-      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>124239525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="B9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="1">
-        <v>446500</v>
-      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>124686025</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="B10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="1">
-        <v>124000000</v>
-      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>686025</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="2">
-        <v>44236</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="1">
-        <f>60000+300000</f>
-        <v>360000</v>
-      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>326025</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="B12" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" s="1">
-        <f>8839000+6709000+3720000+842500+25000000+900000+1488000</f>
-        <v>47498500</v>
-      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>-47172475</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="1">
-        <f>6000000+4332500+56547500</f>
-        <v>66880000</v>
-      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>19707525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="B14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="1">
-        <f>36539975+27017525-56547500</f>
-        <v>7010000</v>
-      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>26717525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="B15" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" s="1">
-        <v>70500</v>
-      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>26647025</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="B16" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="1">
-        <v>26000000</v>
-      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>647025</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="2">
-        <v>44237</v>
-      </c>
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="1">
-        <f>60000+260000</f>
-        <v>320000</v>
-      </c>
+        <v>854500</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5">
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>327025</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="B18" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="1">
-        <f>6550000+10079000</f>
-        <v>16629000</v>
-      </c>
+        <v>854500</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5">
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>16956025</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="B19" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" s="1">
-        <v>135000</v>
-      </c>
+        <v>854500</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5">
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>16821025</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="B20" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="1">
-        <f>5175000+3900000+1004000+70000</f>
-        <v>10149000</v>
-      </c>
+        <v>854500</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5">
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>6672025</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="B21" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" s="1">
-        <f>3146975+11687025-10079000</f>
-        <v>4755000</v>
-      </c>
+        <v>854500</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5">
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>11427025</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="B22" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" s="1">
-        <v>114500</v>
-      </c>
+        <v>854500</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>11541525</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="B23" t="s">
-        <v>65</v>
-      </c>
-      <c r="D23" s="1">
-        <v>11000000</v>
-      </c>
+        <v>854500</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>541525</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="2">
-        <v>44238</v>
-      </c>
-      <c r="B24" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="1">
-        <f>60000+260000</f>
-        <v>320000</v>
-      </c>
+        <v>854500</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>221525</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="B25" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" s="1">
-        <f>2000000+762500+5840000+15740000+3850000+21101000</f>
-        <v>49293500</v>
-      </c>
+        <v>854500</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>49515025</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="B26" t="s">
-        <v>62</v>
-      </c>
-      <c r="D26" s="1">
-        <f>762500+15740000+2072000</f>
-        <v>18574500</v>
-      </c>
+        <v>854500</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>30940525</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="B27" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27" s="1">
-        <f>3155000</f>
-        <v>3155000</v>
-      </c>
+        <v>854500</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>27785525</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="B28" t="s">
-        <v>63</v>
-      </c>
-      <c r="C28" s="1">
-        <f>40460525-9016525-21101000</f>
-        <v>10343000</v>
-      </c>
+        <v>854500</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>38128525</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="B29" t="s">
-        <v>64</v>
-      </c>
-      <c r="C29" s="1">
-        <v>10000</v>
-      </c>
+        <v>854500</v>
+      </c>
+    </row>
+    <row r="29" spans="5:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>38138525</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="B30" t="s">
-        <v>65</v>
-      </c>
-      <c r="D30" s="1">
-        <v>38000000</v>
-      </c>
+        <v>854500</v>
+      </c>
+    </row>
+    <row r="30" spans="5:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>138525</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="2">
-        <v>44513</v>
-      </c>
-      <c r="B31" t="s">
-        <v>25</v>
-      </c>
-      <c r="D31" s="1">
-        <f>60000</f>
-        <v>60000</v>
-      </c>
+        <v>854500</v>
+      </c>
+    </row>
+    <row r="31" spans="5:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>78525</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="B32" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="1">
-        <f>5250000+90000000</f>
-        <v>95250000</v>
-      </c>
+        <v>854500</v>
+      </c>
+    </row>
+    <row r="32" spans="5:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>95328525</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6">
-      <c r="B33" t="s">
-        <v>62</v>
-      </c>
-      <c r="D33" s="1">
-        <f>5250000+50000000+2500000</f>
-        <v>57750000</v>
-      </c>
+        <v>854500</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>37578525</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6">
+        <v>854500</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>37578525</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6">
+        <v>854500</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>37578525</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6">
+        <v>854500</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>37578525</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6">
+        <v>854500</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>37578525</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6">
+        <v>854500</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>37578525</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6">
+        <v>854500</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>37578525</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6">
+        <v>854500</v>
+      </c>
+    </row>
+    <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="2:6">
+    <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>37578525</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6">
+        <v>854500</v>
+      </c>
+    </row>
+    <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>37578525</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6">
+        <v>854500</v>
+      </c>
+    </row>
+    <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>37578525</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6">
+        <v>854500</v>
+      </c>
+    </row>
+    <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>37578525</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6">
+        <v>854500</v>
+      </c>
+    </row>
+    <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>37578525</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6">
+        <v>854500</v>
+      </c>
+    </row>
+    <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>37578525</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6">
+        <v>854500</v>
+      </c>
+    </row>
+    <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>37578525</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6">
+        <v>854500</v>
+      </c>
+    </row>
+    <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>37578525</v>
+        <v>854500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 18-Feb-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="73">
   <si>
     <t>Tgl</t>
   </si>
@@ -195,6 +195,48 @@
   </si>
   <si>
     <t>GUSTAVI</t>
+  </si>
+  <si>
+    <t>TRANSFER BCA</t>
+  </si>
+  <si>
+    <t>PLN - Astar 165</t>
+  </si>
+  <si>
+    <t>TELPON - 5224823</t>
+  </si>
+  <si>
+    <t>FREIGHT OUT</t>
+  </si>
+  <si>
+    <t>A/R</t>
+  </si>
+  <si>
+    <t>SALES - cash/retail</t>
+  </si>
+  <si>
+    <t>SETOR KE BANK</t>
+  </si>
+  <si>
+    <t>SELISIH - lebih</t>
+  </si>
+  <si>
+    <t>DANA KEBERSIHAN</t>
+  </si>
+  <si>
+    <t>A/P</t>
+  </si>
+  <si>
+    <t>TRANSFER BCA AA</t>
+  </si>
+  <si>
+    <t>BELI tali rafia</t>
+  </si>
+  <si>
+    <t>QIU - dokter gigi</t>
+  </si>
+  <si>
+    <t>SERVICE sepatu</t>
   </si>
 </sst>
 </file>
@@ -562,8 +604,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <pane ySplit="2" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -599,7 +641,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="1">
-        <v>854500</v>
+        <v>854525</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -609,673 +651,866 @@
       <c r="B3" t="s">
         <v>25</v>
       </c>
+      <c r="D3" s="1">
+        <f>60000+240000</f>
+        <v>300000</v>
+      </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>854500</v>
+        <v>554525</v>
       </c>
     </row>
     <row r="4" spans="1:6">
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="1">
+        <f>225000+300000+60000+3878000+90000+601000</f>
+        <v>5154000</v>
+      </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>854500</v>
+        <v>-4599475</v>
       </c>
     </row>
     <row r="5" spans="1:6">
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="1">
+        <f>848000</f>
+        <v>848000</v>
+      </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>854500</v>
+        <v>-5447475</v>
       </c>
     </row>
     <row r="6" spans="1:6">
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="1">
+        <f>465000</f>
+        <v>465000</v>
+      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>854500</v>
+        <v>-5912475</v>
       </c>
     </row>
     <row r="7" spans="1:6">
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="1">
+        <f>36000</f>
+        <v>36000</v>
+      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>854500</v>
+        <v>-5948475</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="1">
+        <f>16079000</f>
+        <v>16079000</v>
+      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>854500</v>
+        <v>10130525</v>
       </c>
     </row>
     <row r="9" spans="1:6">
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="1">
+        <f>5708475+21263525+1096000+1661000-16079000</f>
+        <v>13650000</v>
+      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>854500</v>
+        <v>23780525</v>
       </c>
     </row>
     <row r="10" spans="1:6">
+      <c r="B10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="1">
+        <v>20000</v>
+      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>854500</v>
+        <v>23800525</v>
       </c>
     </row>
     <row r="11" spans="1:6">
+      <c r="B11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="1">
+        <v>23000000</v>
+      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>854500</v>
+        <v>800525</v>
       </c>
     </row>
     <row r="12" spans="1:6">
+      <c r="A12" s="2">
+        <v>44243</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="1">
+        <f>60000+280000</f>
+        <v>340000</v>
+      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>854500</v>
+        <v>460525</v>
       </c>
     </row>
     <row r="13" spans="1:6">
+      <c r="B13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="1">
+        <f>22548000+12454000+1825000+1815500+600000+7762500+36687000</f>
+        <v>83692000</v>
+      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>854500</v>
+        <v>84152525</v>
       </c>
     </row>
     <row r="14" spans="1:6">
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="1">
+        <f>22548000+1617000+12454000+8094000+3640500+600000+1100000+40000+1750000</f>
+        <v>51843500</v>
+      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>854500</v>
+        <v>32309025</v>
       </c>
     </row>
     <row r="15" spans="1:6">
+      <c r="B15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="1">
+        <f>38000</f>
+        <v>38000</v>
+      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>854500</v>
+        <v>32271025</v>
       </c>
     </row>
     <row r="16" spans="1:6">
+      <c r="B16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="1">
+        <f>120000</f>
+        <v>120000</v>
+      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>854500</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5">
+        <v>32151025</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="B17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="1">
+        <f>6374500</f>
+        <v>6374500</v>
+      </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>854500</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5">
+        <v>25776525</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="B18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="1">
+        <f>10630475+34491525-36687000</f>
+        <v>8435000</v>
+      </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>854500</v>
-      </c>
-    </row>
-    <row r="19" spans="5:5">
+        <v>34211525</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="B19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="1">
+        <v>13000</v>
+      </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>854500</v>
-      </c>
-    </row>
-    <row r="20" spans="5:5">
+        <v>34224525</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="B20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="1">
+        <v>34000000</v>
+      </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>854500</v>
-      </c>
-    </row>
-    <row r="21" spans="5:5">
+        <v>224525</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2">
+        <v>44244</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="1">
+        <f>60000+260000</f>
+        <v>320000</v>
+      </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>854500</v>
-      </c>
-    </row>
-    <row r="22" spans="5:5">
+        <v>-95475</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="B22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="1">
+        <f>4350000+850000+6564000+1560000+2143000+1361000+17715130+130000+2400000+1412000</f>
+        <v>38485130</v>
+      </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>854500</v>
-      </c>
-    </row>
-    <row r="23" spans="5:5">
+        <v>-38580605</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="B23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="1">
+        <f>12089000+13786000+62976000</f>
+        <v>88851000</v>
+      </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>854500</v>
-      </c>
-    </row>
-    <row r="24" spans="5:5">
+        <v>50270395</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="B24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="1">
+        <f>12000000</f>
+        <v>12000000</v>
+      </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>854500</v>
-      </c>
-    </row>
-    <row r="25" spans="5:5">
+        <v>38270395</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="B25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="1">
+        <v>87500</v>
+      </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>854500</v>
-      </c>
-    </row>
-    <row r="26" spans="5:5">
+        <v>38182895</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="B26" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1550000</v>
+      </c>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>854500</v>
-      </c>
-    </row>
-    <row r="27" spans="5:5">
+        <v>36632895</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="B27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="1">
+        <f>47624895+24671105-62976000</f>
+        <v>9320000</v>
+      </c>
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>854500</v>
-      </c>
-    </row>
-    <row r="28" spans="5:5">
+        <v>45952895</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="B28" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" s="1">
+        <v>15000</v>
+      </c>
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>854500</v>
-      </c>
-    </row>
-    <row r="29" spans="5:5">
+        <v>45937895</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="B29" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="1">
+        <v>24630</v>
+      </c>
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>854500</v>
-      </c>
-    </row>
-    <row r="30" spans="5:5">
+        <v>45962525</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="B30" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30" s="1">
+        <v>45000000</v>
+      </c>
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>854500</v>
-      </c>
-    </row>
-    <row r="31" spans="5:5">
+        <v>962525</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="2">
+        <v>44245</v>
+      </c>
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>854500</v>
-      </c>
-    </row>
-    <row r="32" spans="5:5">
+        <v>962525</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>854500</v>
+        <v>962525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 19-Feb-2021, end of day update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="74">
   <si>
     <t>Tgl</t>
   </si>
@@ -237,6 +237,9 @@
   </si>
   <si>
     <t>SERVICE sepatu</t>
+  </si>
+  <si>
+    <t>SELISIH - kurang</t>
   </si>
 </sst>
 </file>
@@ -605,7 +608,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E51" sqref="E51"/>
+      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1013,504 +1016,563 @@
       <c r="A31" s="2">
         <v>44245</v>
       </c>
+      <c r="B31" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="1">
+        <f>60000+240000</f>
+        <v>300000</v>
+      </c>
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>962525</v>
+        <v>662525</v>
       </c>
     </row>
     <row r="32" spans="1:5">
+      <c r="B32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="1">
+        <f>1750000+4202500</f>
+        <v>5952500</v>
+      </c>
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>962525</v>
-      </c>
-    </row>
-    <row r="33" spans="5:6">
+        <v>6615025</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="B33" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" s="1">
+        <f>1040000+980000+1330000+240000</f>
+        <v>3590000</v>
+      </c>
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>962525</v>
-      </c>
-    </row>
-    <row r="34" spans="5:6">
+        <v>3025025</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="B34" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="1">
+        <f>167500</f>
+        <v>167500</v>
+      </c>
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>962525</v>
-      </c>
-    </row>
-    <row r="35" spans="5:6">
+        <v>2857525</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="B35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" s="1">
+        <f>1104975+9430025-4202500</f>
+        <v>6332500</v>
+      </c>
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>962525</v>
-      </c>
-    </row>
-    <row r="36" spans="5:6">
+        <v>9190025</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="B36" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" s="1">
+        <v>5000</v>
+      </c>
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>962525</v>
-      </c>
-    </row>
-    <row r="37" spans="5:6">
+        <v>9185025</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="B37" t="s">
+        <v>65</v>
+      </c>
+      <c r="D37" s="1">
+        <v>8000000</v>
+      </c>
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>962525</v>
-      </c>
-    </row>
-    <row r="38" spans="5:6">
+        <v>1185025</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="2">
+        <v>44246</v>
+      </c>
+      <c r="B38" t="s">
+        <v>25</v>
+      </c>
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>962525</v>
-      </c>
-    </row>
-    <row r="39" spans="5:6">
+        <v>1185025</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="B39" t="s">
+        <v>63</v>
+      </c>
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>962525</v>
-      </c>
-    </row>
-    <row r="40" spans="5:6">
+        <v>1185025</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="B40" t="s">
+        <v>59</v>
+      </c>
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="5:6">
+    <row r="41" spans="1:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>962525</v>
-      </c>
-    </row>
-    <row r="42" spans="5:6">
+        <v>1185025</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>962525</v>
-      </c>
-    </row>
-    <row r="43" spans="5:6">
+        <v>1185025</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>962525</v>
-      </c>
-    </row>
-    <row r="44" spans="5:6">
+        <v>1185025</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>962525</v>
-      </c>
-    </row>
-    <row r="45" spans="5:6">
+        <v>1185025</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>962525</v>
-      </c>
-    </row>
-    <row r="46" spans="5:6">
+        <v>1185025</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>962525</v>
-      </c>
-    </row>
-    <row r="47" spans="5:6">
+        <v>1185025</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>962525</v>
-      </c>
-    </row>
-    <row r="48" spans="5:6">
+        <v>1185025</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>962525</v>
+        <v>1185025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 20-Feb-2021, end of day update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="74">
   <si>
     <t>Tgl</t>
   </si>
@@ -607,8 +607,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
+      <pane ySplit="2" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1111,468 +1111,505 @@
       <c r="B38" t="s">
         <v>25</v>
       </c>
+      <c r="D38" s="1">
+        <f>60000+300000</f>
+        <v>360000</v>
+      </c>
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>1185025</v>
+        <v>825025</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="B39" t="s">
         <v>63</v>
       </c>
+      <c r="C39" s="1">
+        <f>145000+19813000</f>
+        <v>19958000</v>
+      </c>
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>1185025</v>
+        <v>20783025</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="B40" t="s">
         <v>59</v>
       </c>
+      <c r="D40" s="1">
+        <f>145000+1940000+120000</f>
+        <v>2205000</v>
+      </c>
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>1185025</v>
+        <v>18578025</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:6">
+      <c r="B41" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" s="1">
+        <f>934975+28543525-19813000</f>
+        <v>9665500</v>
+      </c>
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>1185025</v>
+        <v>28243525</v>
       </c>
     </row>
     <row r="42" spans="1:6">
+      <c r="B42" t="s">
+        <v>73</v>
+      </c>
+      <c r="D42" s="1">
+        <v>20000</v>
+      </c>
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>1185025</v>
+        <v>28223525</v>
       </c>
     </row>
     <row r="43" spans="1:6">
+      <c r="B43" t="s">
+        <v>65</v>
+      </c>
+      <c r="D43" s="1">
+        <v>28000000</v>
+      </c>
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="44" spans="1:6">
+      <c r="A44" s="2">
+        <v>44247</v>
+      </c>
+      <c r="B44" t="s">
+        <v>25</v>
+      </c>
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>1185025</v>
+        <v>223525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 22 Feb 2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
   <si>
     <t>Tgl</t>
   </si>
@@ -200,46 +200,7 @@
     <t>TRANSFER BCA</t>
   </si>
   <si>
-    <t>PLN - Astar 165</t>
-  </si>
-  <si>
-    <t>TELPON - 5224823</t>
-  </si>
-  <si>
-    <t>FREIGHT OUT</t>
-  </si>
-  <si>
     <t>A/R</t>
-  </si>
-  <si>
-    <t>SALES - cash/retail</t>
-  </si>
-  <si>
-    <t>SETOR KE BANK</t>
-  </si>
-  <si>
-    <t>SELISIH - lebih</t>
-  </si>
-  <si>
-    <t>DANA KEBERSIHAN</t>
-  </si>
-  <si>
-    <t>A/P</t>
-  </si>
-  <si>
-    <t>TRANSFER BCA AA</t>
-  </si>
-  <si>
-    <t>BELI tali rafia</t>
-  </si>
-  <si>
-    <t>QIU - dokter gigi</t>
-  </si>
-  <si>
-    <t>SERVICE sepatu</t>
-  </si>
-  <si>
-    <t>SELISIH - kurang</t>
   </si>
 </sst>
 </file>
@@ -607,8 +568,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -644,23 +605,23 @@
         <v>5</v>
       </c>
       <c r="E2" s="1">
-        <v>854525</v>
+        <v>755525</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>44242</v>
+        <v>44249</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="1">
-        <f>60000+240000</f>
-        <v>300000</v>
+        <f>60000+150000</f>
+        <v>210000</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>554525</v>
+        <v>545525</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -668,948 +629,677 @@
         <v>59</v>
       </c>
       <c r="D4" s="1">
-        <f>225000+300000+60000+3878000+90000+601000</f>
-        <v>5154000</v>
+        <f>1275000+425000+9270000+10890000</f>
+        <v>21860000</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>-4599475</v>
+        <v>-21314475</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="B5" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="1">
-        <f>848000</f>
-        <v>848000</v>
+      <c r="C5" s="1">
+        <f>9270000+10890000</f>
+        <v>20160000</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>-5447475</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="1">
-        <f>465000</f>
-        <v>465000</v>
-      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>-5912475</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="B7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="1">
-        <f>36000</f>
-        <v>36000</v>
-      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>-5948475</v>
+        <v>-1154475</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="B8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="1">
-        <f>16079000</f>
-        <v>16079000</v>
-      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>10130525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="B9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="1">
-        <f>5708475+21263525+1096000+1661000-16079000</f>
-        <v>13650000</v>
-      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>23780525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="B10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C10" s="1">
-        <v>20000</v>
-      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>23800525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="B11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" s="1">
-        <v>23000000</v>
-      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>800525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="2">
-        <v>44243</v>
-      </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="1">
-        <f>60000+280000</f>
-        <v>340000</v>
-      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>460525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="1">
-        <f>22548000+12454000+1825000+1815500+600000+7762500+36687000</f>
-        <v>83692000</v>
-      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>84152525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="B14" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="1">
-        <f>22548000+1617000+12454000+8094000+3640500+600000+1100000+40000+1750000</f>
-        <v>51843500</v>
-      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>32309025</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="B15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="1">
-        <f>38000</f>
-        <v>38000</v>
-      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>32271025</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="B16" t="s">
-        <v>67</v>
-      </c>
-      <c r="D16" s="1">
-        <f>120000</f>
-        <v>120000</v>
-      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>32151025</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="B17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" s="1">
-        <f>6374500</f>
-        <v>6374500</v>
-      </c>
+        <v>-1154475</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5">
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>25776525</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="B18" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" s="1">
-        <f>10630475+34491525-36687000</f>
-        <v>8435000</v>
-      </c>
+        <v>-1154475</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5">
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>34211525</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="B19" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="1">
-        <v>13000</v>
-      </c>
+        <v>-1154475</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5">
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>34224525</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="B20" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" s="1">
-        <v>34000000</v>
-      </c>
+        <v>-1154475</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5">
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>224525</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="2">
-        <v>44244</v>
-      </c>
-      <c r="B21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="1">
-        <f>60000+260000</f>
-        <v>320000</v>
-      </c>
+        <v>-1154475</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5">
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>-95475</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="B22" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" s="1">
-        <f>4350000+850000+6564000+1560000+2143000+1361000+17715130+130000+2400000+1412000</f>
-        <v>38485130</v>
-      </c>
+        <v>-1154475</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>-38580605</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="B23" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" s="1">
-        <f>12089000+13786000+62976000</f>
-        <v>88851000</v>
-      </c>
+        <v>-1154475</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>50270395</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="B24" t="s">
-        <v>69</v>
-      </c>
-      <c r="D24" s="1">
-        <f>12000000</f>
-        <v>12000000</v>
-      </c>
+        <v>-1154475</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>38270395</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="B25" t="s">
-        <v>70</v>
-      </c>
-      <c r="D25" s="1">
-        <v>87500</v>
-      </c>
+        <v>-1154475</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>38182895</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="B26" t="s">
-        <v>71</v>
-      </c>
-      <c r="D26" s="1">
-        <v>1550000</v>
-      </c>
+        <v>-1154475</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>36632895</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="B27" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27" s="1">
-        <f>47624895+24671105-62976000</f>
-        <v>9320000</v>
-      </c>
+        <v>-1154475</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>45952895</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="B28" t="s">
-        <v>72</v>
-      </c>
-      <c r="D28" s="1">
-        <v>15000</v>
-      </c>
+        <v>-1154475</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>45937895</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="B29" t="s">
-        <v>66</v>
-      </c>
-      <c r="C29" s="1">
-        <v>24630</v>
-      </c>
+        <v>-1154475</v>
+      </c>
+    </row>
+    <row r="29" spans="5:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>45962525</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="B30" t="s">
-        <v>65</v>
-      </c>
-      <c r="D30" s="1">
-        <v>45000000</v>
-      </c>
+        <v>-1154475</v>
+      </c>
+    </row>
+    <row r="30" spans="5:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>962525</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="2">
-        <v>44245</v>
-      </c>
-      <c r="B31" t="s">
-        <v>25</v>
-      </c>
-      <c r="D31" s="1">
-        <f>60000+240000</f>
-        <v>300000</v>
-      </c>
+        <v>-1154475</v>
+      </c>
+    </row>
+    <row r="31" spans="5:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>662525</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="B32" t="s">
-        <v>63</v>
-      </c>
-      <c r="C32" s="1">
-        <f>1750000+4202500</f>
-        <v>5952500</v>
-      </c>
+        <v>-1154475</v>
+      </c>
+    </row>
+    <row r="32" spans="5:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>6615025</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="B33" t="s">
-        <v>59</v>
-      </c>
-      <c r="D33" s="1">
-        <f>1040000+980000+1330000+240000</f>
-        <v>3590000</v>
-      </c>
+        <v>-1154475</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>3025025</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="B34" t="s">
-        <v>68</v>
-      </c>
-      <c r="D34" s="1">
-        <f>167500</f>
-        <v>167500</v>
-      </c>
+        <v>-1154475</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>2857525</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="B35" t="s">
-        <v>64</v>
-      </c>
-      <c r="C35" s="1">
-        <f>1104975+9430025-4202500</f>
-        <v>6332500</v>
-      </c>
+        <v>-1154475</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>9190025</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="B36" t="s">
-        <v>73</v>
-      </c>
-      <c r="D36" s="1">
-        <v>5000</v>
-      </c>
+        <v>-1154475</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>9185025</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="B37" t="s">
-        <v>65</v>
-      </c>
-      <c r="D37" s="1">
-        <v>8000000</v>
-      </c>
+        <v>-1154475</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>1185025</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="2">
-        <v>44246</v>
-      </c>
-      <c r="B38" t="s">
-        <v>25</v>
-      </c>
-      <c r="D38" s="1">
-        <f>60000+300000</f>
-        <v>360000</v>
-      </c>
+        <v>-1154475</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>825025</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="B39" t="s">
-        <v>63</v>
-      </c>
-      <c r="C39" s="1">
-        <f>145000+19813000</f>
-        <v>19958000</v>
-      </c>
+        <v>-1154475</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>20783025</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="B40" t="s">
-        <v>59</v>
-      </c>
-      <c r="D40" s="1">
-        <f>145000+1940000+120000</f>
-        <v>2205000</v>
-      </c>
+        <v>-1154475</v>
+      </c>
+    </row>
+    <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>18578025</v>
+        <v>-1154475</v>
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="1:6">
-      <c r="B41" t="s">
-        <v>64</v>
-      </c>
-      <c r="C41" s="1">
-        <f>934975+28543525-19813000</f>
-        <v>9665500</v>
-      </c>
+    <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>28243525</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="B42" t="s">
-        <v>73</v>
-      </c>
-      <c r="D42" s="1">
-        <v>20000</v>
-      </c>
+        <v>-1154475</v>
+      </c>
+    </row>
+    <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>28223525</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="B43" t="s">
-        <v>65</v>
-      </c>
-      <c r="D43" s="1">
-        <v>28000000</v>
-      </c>
+        <v>-1154475</v>
+      </c>
+    </row>
+    <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>223525</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="2">
-        <v>44247</v>
-      </c>
-      <c r="B44" t="s">
-        <v>25</v>
-      </c>
+        <v>-1154475</v>
+      </c>
+    </row>
+    <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>223525</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>-1154475</v>
+      </c>
+    </row>
+    <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>223525</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>-1154475</v>
+      </c>
+    </row>
+    <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>223525</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>-1154475</v>
+      </c>
+    </row>
+    <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>223525</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>-1154475</v>
+      </c>
+    </row>
+    <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>223525</v>
+        <v>-1154475</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 24-Feb-2021, end of day update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="69">
   <si>
     <t>Tgl</t>
   </si>
@@ -201,6 +201,30 @@
   </si>
   <si>
     <t>A/R</t>
+  </si>
+  <si>
+    <t>BELI kresek</t>
+  </si>
+  <si>
+    <t>SALES - cash/retail</t>
+  </si>
+  <si>
+    <t>BENSIN - RUSH</t>
+  </si>
+  <si>
+    <t>SELISIH - lebih</t>
+  </si>
+  <si>
+    <t>SETOR KE BANK</t>
+  </si>
+  <si>
+    <t>A/P</t>
+  </si>
+  <si>
+    <t>SERVICE - pintu</t>
+  </si>
+  <si>
+    <t>DOKTER - qiu</t>
   </si>
 </sst>
 </file>
@@ -568,8 +592,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -616,12 +640,12 @@
         <v>25</v>
       </c>
       <c r="D3" s="1">
-        <f>60000+150000</f>
-        <v>210000</v>
+        <f>60000+150000+260000</f>
+        <v>470000</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>545525</v>
+        <v>285525</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -629,12 +653,12 @@
         <v>59</v>
       </c>
       <c r="D4" s="1">
-        <f>1275000+425000+9270000+10890000</f>
-        <v>21860000</v>
+        <f>1275000+425000+9270000+10890000+2280000+1631500+2177000+550000</f>
+        <v>28498500</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>-21314475</v>
+        <v>-28212975</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -642,664 +666,802 @@
         <v>60</v>
       </c>
       <c r="C5" s="1">
-        <f>9270000+10890000</f>
-        <v>20160000</v>
+        <f>9270000+10890000+24154500</f>
+        <v>44314500</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>-1154475</v>
+        <v>16101525</v>
       </c>
     </row>
     <row r="6" spans="1:6">
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="1">
+        <v>85000</v>
+      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>-1154475</v>
+        <v>16016525</v>
       </c>
     </row>
     <row r="7" spans="1:6">
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="1">
+        <f>8137975+31027525-24154500</f>
+        <v>15011000</v>
+      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>-1154475</v>
+        <v>31027525</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="1">
+        <v>200000</v>
+      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>-1154475</v>
+        <v>30827525</v>
       </c>
     </row>
     <row r="9" spans="1:6">
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="1">
+        <v>20000</v>
+      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>-1154475</v>
+        <v>30847525</v>
       </c>
     </row>
     <row r="10" spans="1:6">
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="1">
+        <v>30000000</v>
+      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>-1154475</v>
+        <v>847525</v>
       </c>
     </row>
     <row r="11" spans="1:6">
+      <c r="A11" s="2">
+        <v>44250</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="1">
+        <f>45000+195000</f>
+        <v>240000</v>
+      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>-1154475</v>
+        <v>607525</v>
       </c>
     </row>
     <row r="12" spans="1:6">
+      <c r="B12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="1">
+        <f>18638000+6750500</f>
+        <v>25388500</v>
+      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>-1154475</v>
+        <v>25996025</v>
       </c>
     </row>
     <row r="13" spans="1:6">
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="1">
+        <f>18638000+496000</f>
+        <v>19134000</v>
+      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>-1154475</v>
+        <v>6862025</v>
       </c>
     </row>
     <row r="14" spans="1:6">
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1266000</v>
+      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>-1154475</v>
+        <v>5596025</v>
       </c>
     </row>
     <row r="15" spans="1:6">
+      <c r="B15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="1">
+        <f>959475+16415025-6750500</f>
+        <v>10624000</v>
+      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>-1154475</v>
+        <v>16220025</v>
       </c>
     </row>
     <row r="16" spans="1:6">
+      <c r="B16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="1">
+        <v>10000</v>
+      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>-1154475</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5">
+        <v>16230025</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="B17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="1">
+        <f>16000000</f>
+        <v>16000000</v>
+      </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>-1154475</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5">
+        <v>230025</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="2">
+        <v>44251</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="1">
+        <f>45000+285000</f>
+        <v>330000</v>
+      </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>-1154475</v>
-      </c>
-    </row>
-    <row r="19" spans="5:5">
+        <v>-99975</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="1">
+        <f>91000+1458000+95000+1541000+1527000+900000</f>
+        <v>5612000</v>
+      </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>-1154475</v>
-      </c>
-    </row>
-    <row r="20" spans="5:5">
+        <v>-5711975</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="B20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="1">
+        <f>1458000+28067000</f>
+        <v>29525000</v>
+      </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>-1154475</v>
-      </c>
-    </row>
-    <row r="21" spans="5:5">
+        <v>23813025</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="1">
+        <f>300000</f>
+        <v>300000</v>
+      </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>-1154475</v>
-      </c>
-    </row>
-    <row r="22" spans="5:5">
+        <v>23513025</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="B22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="1">
+        <f>5900000</f>
+        <v>5900000</v>
+      </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>-1154475</v>
-      </c>
-    </row>
-    <row r="23" spans="5:5">
+        <v>17613025</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="B23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="1">
+        <f>10168975+28924025-28067000</f>
+        <v>11026000</v>
+      </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>-1154475</v>
-      </c>
-    </row>
-    <row r="24" spans="5:5">
+        <v>28639025</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="B24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="1">
+        <v>28000000</v>
+      </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>-1154475</v>
-      </c>
-    </row>
-    <row r="25" spans="5:5">
+        <v>639025</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="2">
+        <v>44252</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>-1154475</v>
-      </c>
-    </row>
-    <row r="26" spans="5:5">
+        <v>639025</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>-1154475</v>
-      </c>
-    </row>
-    <row r="27" spans="5:5">
+        <v>639025</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>-1154475</v>
-      </c>
-    </row>
-    <row r="28" spans="5:5">
+        <v>639025</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>-1154475</v>
-      </c>
-    </row>
-    <row r="29" spans="5:5">
+        <v>639025</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>-1154475</v>
-      </c>
-    </row>
-    <row r="30" spans="5:5">
+        <v>639025</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>-1154475</v>
-      </c>
-    </row>
-    <row r="31" spans="5:5">
+        <v>639025</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>-1154475</v>
-      </c>
-    </row>
-    <row r="32" spans="5:5">
+        <v>639025</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>-1154475</v>
+        <v>639025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 26-Feb-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="69">
   <si>
     <t>Tgl</t>
   </si>
@@ -592,8 +592,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
+      <pane ySplit="2" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -928,540 +928,609 @@
       <c r="B25" t="s">
         <v>25</v>
       </c>
+      <c r="D25" s="1">
+        <f>45000+195000</f>
+        <v>240000</v>
+      </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>639025</v>
+        <v>399025</v>
       </c>
     </row>
     <row r="26" spans="1:5">
+      <c r="B26" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" s="1">
+        <f>630000</f>
+        <v>630000</v>
+      </c>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>639025</v>
+        <v>-230975</v>
       </c>
     </row>
     <row r="27" spans="1:5">
+      <c r="B27" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="1">
+        <f>500000</f>
+        <v>500000</v>
+      </c>
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>639025</v>
+        <v>-730975</v>
       </c>
     </row>
     <row r="28" spans="1:5">
+      <c r="B28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="1">
+        <f>16271000</f>
+        <v>16271000</v>
+      </c>
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>639025</v>
+        <v>15540025</v>
       </c>
     </row>
     <row r="29" spans="1:5">
+      <c r="B29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="1">
+        <f>535975+21185025-16271000</f>
+        <v>5450000</v>
+      </c>
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>639025</v>
+        <v>20990025</v>
       </c>
     </row>
     <row r="30" spans="1:5">
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="1">
+        <f>4250000</f>
+        <v>4250000</v>
+      </c>
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>639025</v>
+        <v>16740025</v>
       </c>
     </row>
     <row r="31" spans="1:5">
+      <c r="B31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" s="1">
+        <v>16000000</v>
+      </c>
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>639025</v>
+        <v>740025</v>
       </c>
     </row>
     <row r="32" spans="1:5">
+      <c r="A32" s="2">
+        <v>44253</v>
+      </c>
+      <c r="B32" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="1">
+        <f>45000</f>
+        <v>45000</v>
+      </c>
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>639025</v>
-      </c>
-    </row>
-    <row r="33" spans="5:6">
+        <v>695025</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6">
+      <c r="B33" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" s="1">
+        <f>1275000+1556500+9360000</f>
+        <v>12191500</v>
+      </c>
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>639025</v>
-      </c>
-    </row>
-    <row r="34" spans="5:6">
+        <v>-11496475</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6">
+      <c r="B34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="1">
+        <f>9360000</f>
+        <v>9360000</v>
+      </c>
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>639025</v>
-      </c>
-    </row>
-    <row r="35" spans="5:6">
+        <v>-2136475</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>639025</v>
-      </c>
-    </row>
-    <row r="36" spans="5:6">
+        <v>-2136475</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>639025</v>
-      </c>
-    </row>
-    <row r="37" spans="5:6">
+        <v>-2136475</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>639025</v>
-      </c>
-    </row>
-    <row r="38" spans="5:6">
+        <v>-2136475</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>639025</v>
-      </c>
-    </row>
-    <row r="39" spans="5:6">
+        <v>-2136475</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>639025</v>
-      </c>
-    </row>
-    <row r="40" spans="5:6">
+        <v>-2136475</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="5:6">
+    <row r="41" spans="2:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>639025</v>
-      </c>
-    </row>
-    <row r="42" spans="5:6">
+        <v>-2136475</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>639025</v>
-      </c>
-    </row>
-    <row r="43" spans="5:6">
+        <v>-2136475</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>639025</v>
-      </c>
-    </row>
-    <row r="44" spans="5:6">
+        <v>-2136475</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>639025</v>
-      </c>
-    </row>
-    <row r="45" spans="5:6">
+        <v>-2136475</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>639025</v>
-      </c>
-    </row>
-    <row r="46" spans="5:6">
+        <v>-2136475</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>639025</v>
-      </c>
-    </row>
-    <row r="47" spans="5:6">
+        <v>-2136475</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>639025</v>
-      </c>
-    </row>
-    <row r="48" spans="5:6">
+        <v>-2136475</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>639025</v>
+        <v>-2136475</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 28-Feb-2021, end of day.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>Tgl</t>
   </si>
@@ -195,36 +195,6 @@
   </si>
   <si>
     <t>GUSTAVI</t>
-  </si>
-  <si>
-    <t>TRANSFER BCA</t>
-  </si>
-  <si>
-    <t>A/R</t>
-  </si>
-  <si>
-    <t>BELI kresek</t>
-  </si>
-  <si>
-    <t>SALES - cash/retail</t>
-  </si>
-  <si>
-    <t>BENSIN - RUSH</t>
-  </si>
-  <si>
-    <t>SELISIH - lebih</t>
-  </si>
-  <si>
-    <t>SETOR KE BANK</t>
-  </si>
-  <si>
-    <t>A/P</t>
-  </si>
-  <si>
-    <t>SERVICE - pintu</t>
-  </si>
-  <si>
-    <t>DOKTER - qiu</t>
   </si>
 </sst>
 </file>
@@ -592,8 +562,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -629,908 +599,683 @@
         <v>5</v>
       </c>
       <c r="E2" s="1">
-        <v>755525</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>44249</v>
+        <v>44256</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="1">
-        <f>60000+150000+260000</f>
-        <v>470000</v>
-      </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>285525</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="B4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="1">
-        <f>1275000+425000+9270000+10890000+2280000+1631500+2177000+550000</f>
-        <v>28498500</v>
-      </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>-28212975</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="B5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="1">
-        <f>9270000+10890000+24154500</f>
-        <v>44314500</v>
-      </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>16101525</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="1">
-        <v>85000</v>
-      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>16016525</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="B7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="1">
-        <f>8137975+31027525-24154500</f>
-        <v>15011000</v>
-      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>31027525</v>
+        <v>687025</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="B8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" s="1">
-        <v>200000</v>
-      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>30827525</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="B9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="1">
-        <v>20000</v>
-      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>30847525</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="B10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="1">
-        <v>30000000</v>
-      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>847525</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="2">
-        <v>44250</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="1">
-        <f>45000+195000</f>
-        <v>240000</v>
-      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>607525</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="B12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="1">
-        <f>18638000+6750500</f>
-        <v>25388500</v>
-      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>25996025</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="1">
-        <f>18638000+496000</f>
-        <v>19134000</v>
-      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>6862025</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="B14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" s="1">
-        <v>1266000</v>
-      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>5596025</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="B15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" s="1">
-        <f>959475+16415025-6750500</f>
-        <v>10624000</v>
-      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>16220025</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="B16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" s="1">
-        <v>10000</v>
-      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>16230025</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="B17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" s="1">
-        <f>16000000</f>
-        <v>16000000</v>
-      </c>
+        <v>687025</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5">
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>230025</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="2">
-        <v>44251</v>
-      </c>
-      <c r="B18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="1">
-        <f>45000+285000</f>
-        <v>330000</v>
-      </c>
+        <v>687025</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5">
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>-99975</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="B19" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" s="1">
-        <f>91000+1458000+95000+1541000+1527000+900000</f>
-        <v>5612000</v>
-      </c>
+        <v>687025</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5">
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>-5711975</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="B20" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" s="1">
-        <f>1458000+28067000</f>
-        <v>29525000</v>
-      </c>
+        <v>687025</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5">
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>23813025</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="B21" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" s="1">
-        <f>300000</f>
-        <v>300000</v>
-      </c>
+        <v>687025</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5">
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>23513025</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="B22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" s="1">
-        <f>5900000</f>
-        <v>5900000</v>
-      </c>
+        <v>687025</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>17613025</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="B23" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="1">
-        <f>10168975+28924025-28067000</f>
-        <v>11026000</v>
-      </c>
+        <v>687025</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>28639025</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="B24" t="s">
-        <v>65</v>
-      </c>
-      <c r="D24" s="1">
-        <v>28000000</v>
-      </c>
+        <v>687025</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>639025</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="2">
-        <v>44252</v>
-      </c>
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="1">
-        <f>45000+195000</f>
-        <v>240000</v>
-      </c>
+        <v>687025</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>399025</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="B26" t="s">
-        <v>66</v>
-      </c>
-      <c r="D26" s="1">
-        <f>630000</f>
-        <v>630000</v>
-      </c>
+        <v>687025</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>-230975</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="B27" t="s">
-        <v>67</v>
-      </c>
-      <c r="D27" s="1">
-        <f>500000</f>
-        <v>500000</v>
-      </c>
+        <v>687025</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>-730975</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="B28" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="1">
-        <f>16271000</f>
-        <v>16271000</v>
-      </c>
+        <v>687025</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>15540025</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="B29" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="1">
-        <f>535975+21185025-16271000</f>
-        <v>5450000</v>
-      </c>
+        <v>687025</v>
+      </c>
+    </row>
+    <row r="29" spans="5:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>20990025</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="B30" t="s">
-        <v>59</v>
-      </c>
-      <c r="D30" s="1">
-        <f>4250000</f>
-        <v>4250000</v>
-      </c>
+        <v>687025</v>
+      </c>
+    </row>
+    <row r="30" spans="5:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>16740025</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="B31" t="s">
-        <v>65</v>
-      </c>
-      <c r="D31" s="1">
-        <v>16000000</v>
-      </c>
+        <v>687025</v>
+      </c>
+    </row>
+    <row r="31" spans="5:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>740025</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="2">
-        <v>44253</v>
-      </c>
-      <c r="B32" t="s">
-        <v>25</v>
-      </c>
-      <c r="D32" s="1">
-        <f>45000</f>
-        <v>45000</v>
-      </c>
+        <v>687025</v>
+      </c>
+    </row>
+    <row r="32" spans="5:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>695025</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6">
-      <c r="B33" t="s">
-        <v>59</v>
-      </c>
-      <c r="D33" s="1">
-        <f>1275000+1556500+9360000</f>
-        <v>12191500</v>
-      </c>
+        <v>687025</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>-11496475</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6">
-      <c r="B34" t="s">
-        <v>60</v>
-      </c>
-      <c r="C34" s="1">
-        <f>9360000</f>
-        <v>9360000</v>
-      </c>
+        <v>687025</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>-2136475</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6">
+        <v>687025</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>-2136475</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6">
+        <v>687025</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>-2136475</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6">
+        <v>687025</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>-2136475</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6">
+        <v>687025</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>-2136475</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6">
+        <v>687025</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>-2136475</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6">
+        <v>687025</v>
+      </c>
+    </row>
+    <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="2:6">
+    <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>-2136475</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6">
+        <v>687025</v>
+      </c>
+    </row>
+    <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>-2136475</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6">
+        <v>687025</v>
+      </c>
+    </row>
+    <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>-2136475</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6">
+        <v>687025</v>
+      </c>
+    </row>
+    <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>-2136475</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6">
+        <v>687025</v>
+      </c>
+    </row>
+    <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>-2136475</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6">
+        <v>687025</v>
+      </c>
+    </row>
+    <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>-2136475</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6">
+        <v>687025</v>
+      </c>
+    </row>
+    <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>-2136475</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6">
+        <v>687025</v>
+      </c>
+    </row>
+    <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>-2136475</v>
+        <v>687025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 3-Mar-2021, end of day.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="67">
   <si>
     <t>Tgl</t>
   </si>
@@ -195,6 +195,30 @@
   </si>
   <si>
     <t>GUSTAVI</t>
+  </si>
+  <si>
+    <t>A/R</t>
+  </si>
+  <si>
+    <t>TRANSFER BCA</t>
+  </si>
+  <si>
+    <t>SALES - cash/retail</t>
+  </si>
+  <si>
+    <t>SELISIH - kurang</t>
+  </si>
+  <si>
+    <t>SETOR KE BANK</t>
+  </si>
+  <si>
+    <t>BELI kresek</t>
+  </si>
+  <si>
+    <t>SELISIH - lebih</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -562,8 +586,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -609,673 +633,812 @@
       <c r="B3" t="s">
         <v>25</v>
       </c>
+      <c r="D3" s="1">
+        <f>45000+195000</f>
+        <v>240000</v>
+      </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>687025</v>
+        <v>447025</v>
       </c>
     </row>
     <row r="4" spans="1:6">
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="1">
+        <f>5400000+810000+43500000+45874000</f>
+        <v>95584000</v>
+      </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>687025</v>
+        <v>96031025</v>
       </c>
     </row>
     <row r="5" spans="1:6">
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="1">
+        <f>1800000+2567000+810000+30000000+720000</f>
+        <v>35897000</v>
+      </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>687025</v>
+        <v>60134025</v>
       </c>
     </row>
     <row r="6" spans="1:6">
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="1">
+        <f>69749025-14455025-45874000</f>
+        <v>9420000</v>
+      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>687025</v>
+        <v>69554025</v>
       </c>
     </row>
     <row r="7" spans="1:6">
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="1">
+        <v>50000</v>
+      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>687025</v>
+        <v>69504025</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="1">
+        <v>69000000</v>
+      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>687025</v>
+        <v>504025</v>
       </c>
     </row>
     <row r="9" spans="1:6">
+      <c r="A9" s="2">
+        <v>44257</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="1">
+        <f>45000+180000</f>
+        <v>225000</v>
+      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>687025</v>
+        <v>279025</v>
       </c>
     </row>
     <row r="10" spans="1:6">
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="1">
+        <f>900000+1519000+220000</f>
+        <v>2639000</v>
+      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>687025</v>
+        <v>-2359975</v>
       </c>
     </row>
     <row r="11" spans="1:6">
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="1">
+        <f>52000</f>
+        <v>52000</v>
+      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>687025</v>
+        <v>-2411975</v>
       </c>
     </row>
     <row r="12" spans="1:6">
+      <c r="B12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="1">
+        <f>9000000+9566000</f>
+        <v>18566000</v>
+      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>687025</v>
+        <v>16154025</v>
       </c>
     </row>
     <row r="13" spans="1:6">
+      <c r="B13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="1">
+        <f>2231975+16952025-9566000</f>
+        <v>9618000</v>
+      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>687025</v>
+        <v>25772025</v>
       </c>
     </row>
     <row r="14" spans="1:6">
+      <c r="B14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="1">
+        <v>470000</v>
+      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>687025</v>
+        <v>26242025</v>
       </c>
     </row>
     <row r="15" spans="1:6">
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="1">
+        <v>26000000</v>
+      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>687025</v>
+        <v>242025</v>
       </c>
     </row>
     <row r="16" spans="1:6">
+      <c r="A16" s="2">
+        <v>44258</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="1">
+        <f>45000+210000</f>
+        <v>255000</v>
+      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>687025</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5">
+        <v>-12975</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="B17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="1">
+        <f>1744500+7700000+84925000+18837500</f>
+        <v>113207000</v>
+      </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>687025</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5">
+        <v>113194025</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="1">
+        <f>1744500+7700000+7057500+84925000+1365000</f>
+        <v>102792000</v>
+      </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>687025</v>
-      </c>
-    </row>
-    <row r="19" spans="5:5">
+        <v>10402025</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="B19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="1">
+        <f>8225475+18785525-18837500</f>
+        <v>8173500</v>
+      </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>687025</v>
-      </c>
-    </row>
-    <row r="20" spans="5:5">
-      <c r="E20" s="1">
-        <f t="shared" si="0"/>
-        <v>687025</v>
-      </c>
-    </row>
-    <row r="21" spans="5:5">
-      <c r="E21" s="1">
-        <f t="shared" si="0"/>
-        <v>687025</v>
-      </c>
-    </row>
-    <row r="22" spans="5:5">
-      <c r="E22" s="1">
-        <f t="shared" si="0"/>
-        <v>687025</v>
-      </c>
-    </row>
-    <row r="23" spans="5:5">
-      <c r="E23" s="1">
-        <f t="shared" si="0"/>
-        <v>687025</v>
-      </c>
-    </row>
-    <row r="24" spans="5:5">
-      <c r="E24" s="1">
-        <f t="shared" si="0"/>
-        <v>687025</v>
-      </c>
-    </row>
-    <row r="25" spans="5:5">
-      <c r="E25" s="1">
-        <f t="shared" si="0"/>
-        <v>687025</v>
-      </c>
-    </row>
-    <row r="26" spans="5:5">
-      <c r="E26" s="1">
-        <f t="shared" si="0"/>
-        <v>687025</v>
-      </c>
-    </row>
-    <row r="27" spans="5:5">
-      <c r="E27" s="1">
-        <f t="shared" si="0"/>
-        <v>687025</v>
-      </c>
-    </row>
-    <row r="28" spans="5:5">
-      <c r="E28" s="1">
-        <f t="shared" si="0"/>
-        <v>687025</v>
-      </c>
-    </row>
-    <row r="29" spans="5:5">
-      <c r="E29" s="1">
-        <f t="shared" si="0"/>
-        <v>687025</v>
-      </c>
-    </row>
-    <row r="30" spans="5:5">
-      <c r="E30" s="1">
-        <f t="shared" si="0"/>
-        <v>687025</v>
-      </c>
-    </row>
-    <row r="31" spans="5:5">
-      <c r="E31" s="1">
-        <f t="shared" si="0"/>
-        <v>687025</v>
-      </c>
-    </row>
-    <row r="32" spans="5:5">
-      <c r="E32" s="1">
-        <f t="shared" si="0"/>
-        <v>687025</v>
+        <v>18575525</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="1">
+        <v>100000</v>
+      </c>
+      <c r="E20" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="1">
+        <v>18000000</v>
+      </c>
+      <c r="E21" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="2">
+        <v>44259</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="E23" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="E24" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="E25" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="E26" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="E27" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="E28" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="E29" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="E30" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="E31" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="E32" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="33" spans="5:6">
-      <c r="E33" s="1">
-        <f t="shared" si="0"/>
-        <v>687025</v>
+      <c r="E33" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="34" spans="5:6">
-      <c r="E34" s="1">
-        <f t="shared" si="0"/>
-        <v>687025</v>
+      <c r="E34" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="35" spans="5:6">
-      <c r="E35" s="1">
+      <c r="E35" s="1" t="e">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>687025</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="36" spans="5:6">
-      <c r="E36" s="1">
-        <f t="shared" si="1"/>
-        <v>687025</v>
+      <c r="E36" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="37" spans="5:6">
-      <c r="E37" s="1">
-        <f t="shared" si="1"/>
-        <v>687025</v>
+      <c r="E37" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="38" spans="5:6">
-      <c r="E38" s="1">
-        <f t="shared" si="1"/>
-        <v>687025</v>
+      <c r="E38" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="39" spans="5:6">
-      <c r="E39" s="1">
-        <f t="shared" si="1"/>
-        <v>687025</v>
+      <c r="E39" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="40" spans="5:6">
-      <c r="E40" s="1">
-        <f t="shared" si="1"/>
-        <v>687025</v>
+      <c r="E40" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="5:6">
-      <c r="E41" s="1">
-        <f t="shared" si="1"/>
-        <v>687025</v>
+      <c r="E41" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="42" spans="5:6">
-      <c r="E42" s="1">
-        <f t="shared" si="1"/>
-        <v>687025</v>
+      <c r="E42" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="43" spans="5:6">
-      <c r="E43" s="1">
-        <f t="shared" si="1"/>
-        <v>687025</v>
+      <c r="E43" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="44" spans="5:6">
-      <c r="E44" s="1">
-        <f t="shared" si="1"/>
-        <v>687025</v>
+      <c r="E44" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="45" spans="5:6">
-      <c r="E45" s="1">
-        <f t="shared" si="1"/>
-        <v>687025</v>
+      <c r="E45" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="46" spans="5:6">
-      <c r="E46" s="1">
-        <f t="shared" si="1"/>
-        <v>687025</v>
+      <c r="E46" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="47" spans="5:6">
-      <c r="E47" s="1">
-        <f t="shared" si="1"/>
-        <v>687025</v>
+      <c r="E47" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="48" spans="5:6">
-      <c r="E48" s="1">
-        <f t="shared" si="1"/>
-        <v>687025</v>
+      <c r="E48" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="49" spans="5:6">
-      <c r="E49" s="1">
-        <f t="shared" si="1"/>
-        <v>687025</v>
+      <c r="E49" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="50" spans="5:6">
-      <c r="E50" s="1">
-        <f t="shared" si="1"/>
-        <v>687025</v>
+      <c r="E50" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="51" spans="5:6">
-      <c r="E51" s="1">
-        <f t="shared" si="1"/>
-        <v>687025</v>
+      <c r="E51" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
-      <c r="E52" s="1">
-        <f t="shared" si="1"/>
-        <v>687025</v>
+      <c r="E52" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="53" spans="5:6">
-      <c r="E53" s="1">
-        <f t="shared" si="1"/>
-        <v>687025</v>
+      <c r="E53" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="54" spans="5:6">
-      <c r="E54" s="1">
-        <f t="shared" si="1"/>
-        <v>687025</v>
+      <c r="E54" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="55" spans="5:6">
-      <c r="E55" s="1">
-        <f t="shared" si="1"/>
-        <v>687025</v>
+      <c r="E55" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="56" spans="5:6">
-      <c r="E56" s="1">
-        <f t="shared" si="1"/>
-        <v>687025</v>
+      <c r="E56" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="57" spans="5:6">
-      <c r="E57" s="1">
-        <f t="shared" si="1"/>
-        <v>687025</v>
+      <c r="E57" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="58" spans="5:6">
-      <c r="E58" s="1">
-        <f t="shared" si="1"/>
-        <v>687025</v>
+      <c r="E58" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="59" spans="5:6">
-      <c r="E59" s="1">
-        <f t="shared" si="1"/>
-        <v>687025</v>
+      <c r="E59" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="60" spans="5:6">
-      <c r="E60" s="1">
-        <f t="shared" si="1"/>
-        <v>687025</v>
+      <c r="E60" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="61" spans="5:6">
-      <c r="E61" s="1">
-        <f t="shared" si="1"/>
-        <v>687025</v>
+      <c r="E61" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="62" spans="5:6">
-      <c r="E62" s="1">
-        <f t="shared" si="1"/>
-        <v>687025</v>
+      <c r="E62" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="63" spans="5:6">
-      <c r="E63" s="1">
-        <f t="shared" si="1"/>
-        <v>687025</v>
+      <c r="E63" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="64" spans="5:6">
-      <c r="E64" s="1">
-        <f t="shared" si="1"/>
-        <v>687025</v>
+      <c r="E64" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="65" spans="5:7">
-      <c r="E65" s="1">
-        <f t="shared" si="1"/>
-        <v>687025</v>
+      <c r="E65" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="66" spans="5:7">
-      <c r="E66" s="1">
-        <f t="shared" si="1"/>
-        <v>687025</v>
+      <c r="E66" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="67" spans="5:7">
-      <c r="E67" s="1">
+      <c r="E67" s="1" t="e">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>687025</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="68" spans="5:7">
-      <c r="E68" s="1">
-        <f t="shared" si="2"/>
-        <v>687025</v>
+      <c r="E68" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="69" spans="5:7">
-      <c r="E69" s="1">
-        <f t="shared" si="2"/>
-        <v>687025</v>
+      <c r="E69" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="70" spans="5:7">
-      <c r="E70" s="1">
-        <f t="shared" si="2"/>
-        <v>687025</v>
+      <c r="E70" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="71" spans="5:7">
-      <c r="E71" s="1">
-        <f t="shared" si="2"/>
-        <v>687025</v>
+      <c r="E71" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="72" spans="5:7">
-      <c r="E72" s="1">
-        <f t="shared" si="2"/>
-        <v>687025</v>
+      <c r="E72" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="73" spans="5:7">
-      <c r="E73" s="1">
-        <f t="shared" si="2"/>
-        <v>687025</v>
+      <c r="E73" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="74" spans="5:7">
-      <c r="E74" s="1">
-        <f t="shared" si="2"/>
-        <v>687025</v>
+      <c r="E74" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="75" spans="5:7">
-      <c r="E75" s="1">
-        <f t="shared" si="2"/>
-        <v>687025</v>
+      <c r="E75" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="76" spans="5:7">
-      <c r="E76" s="1">
-        <f t="shared" si="2"/>
-        <v>687025</v>
+      <c r="E76" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="77" spans="5:7">
-      <c r="E77" s="1">
-        <f t="shared" si="2"/>
-        <v>687025</v>
+      <c r="E77" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="78" spans="5:7">
-      <c r="E78" s="1">
-        <f t="shared" si="2"/>
-        <v>687025</v>
+      <c r="E78" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="79" spans="5:7">
-      <c r="E79" s="1">
-        <f t="shared" si="2"/>
-        <v>687025</v>
+      <c r="E79" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
-      <c r="E80" s="1">
-        <f t="shared" si="2"/>
-        <v>687025</v>
+      <c r="E80" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="81" spans="5:5">
-      <c r="E81" s="1">
-        <f t="shared" si="2"/>
-        <v>687025</v>
+      <c r="E81" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="82" spans="5:5">
-      <c r="E82" s="1">
-        <f t="shared" si="2"/>
-        <v>687025</v>
+      <c r="E82" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="83" spans="5:5">
-      <c r="E83" s="1">
-        <f t="shared" si="2"/>
-        <v>687025</v>
+      <c r="E83" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="84" spans="5:5">
-      <c r="E84" s="1">
-        <f t="shared" si="2"/>
-        <v>687025</v>
+      <c r="E84" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="85" spans="5:5">
-      <c r="E85" s="1">
-        <f t="shared" si="2"/>
-        <v>687025</v>
+      <c r="E85" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="86" spans="5:5">
-      <c r="E86" s="1">
-        <f t="shared" si="2"/>
-        <v>687025</v>
+      <c r="E86" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="87" spans="5:5">
-      <c r="E87" s="1">
-        <f t="shared" si="2"/>
-        <v>687025</v>
+      <c r="E87" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="88" spans="5:5">
-      <c r="E88" s="1">
-        <f t="shared" si="2"/>
-        <v>687025</v>
+      <c r="E88" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="89" spans="5:5">
-      <c r="E89" s="1">
-        <f t="shared" si="2"/>
-        <v>687025</v>
+      <c r="E89" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="90" spans="5:5">
-      <c r="E90" s="1">
-        <f t="shared" si="2"/>
-        <v>687025</v>
+      <c r="E90" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="91" spans="5:5">
-      <c r="E91" s="1">
-        <f t="shared" si="2"/>
-        <v>687025</v>
+      <c r="E91" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="92" spans="5:5">
-      <c r="E92" s="1">
-        <f t="shared" si="2"/>
-        <v>687025</v>
+      <c r="E92" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="93" spans="5:5">
-      <c r="E93" s="1">
-        <f t="shared" si="2"/>
-        <v>687025</v>
+      <c r="E93" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="94" spans="5:5">
-      <c r="E94" s="1">
-        <f t="shared" si="2"/>
-        <v>687025</v>
+      <c r="E94" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="95" spans="5:5">
-      <c r="E95" s="1">
-        <f t="shared" si="2"/>
-        <v>687025</v>
+      <c r="E95" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="96" spans="5:5">
-      <c r="E96" s="1">
-        <f t="shared" si="2"/>
-        <v>687025</v>
+      <c r="E96" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="97" spans="5:5">
-      <c r="E97" s="1">
-        <f t="shared" si="2"/>
-        <v>687025</v>
+      <c r="E97" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="98" spans="5:5">
-      <c r="E98" s="1">
-        <f t="shared" si="2"/>
-        <v>687025</v>
+      <c r="E98" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="99" spans="5:5">
-      <c r="E99" s="1">
+      <c r="E99" s="1" t="e">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>687025</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="100" spans="5:5">
-      <c r="E100" s="1">
+      <c r="E100" s="1" t="e">
         <f t="shared" si="3"/>
-        <v>687025</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="101" spans="5:5">
-      <c r="E101" s="1">
+      <c r="E101" s="1" t="e">
         <f t="shared" si="3"/>
-        <v>687025</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="102" spans="5:5">
-      <c r="E102" s="1">
+      <c r="E102" s="1" t="e">
         <f t="shared" si="3"/>
-        <v>687025</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="103" spans="5:5">
-      <c r="E103" s="1">
+      <c r="E103" s="1" t="e">
         <f t="shared" si="3"/>
-        <v>687025</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="104" spans="5:5">
-      <c r="E104" s="1">
+      <c r="E104" s="1" t="e">
         <f t="shared" si="3"/>
-        <v>687025</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="105" spans="5:5">
-      <c r="E105" s="1">
+      <c r="E105" s="1" t="e">
         <f t="shared" si="3"/>
-        <v>687025</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="106" spans="5:5">
-      <c r="E106" s="1">
+      <c r="E106" s="1" t="e">
         <f t="shared" si="3"/>
-        <v>687025</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="107" spans="5:5">
-      <c r="E107" s="1">
+      <c r="E107" s="1" t="e">
         <f t="shared" si="3"/>
-        <v>687025</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="108" spans="5:5">
-      <c r="E108" s="1">
+      <c r="E108" s="1" t="e">
         <f t="shared" si="3"/>
-        <v>687025</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="109" spans="5:5">
-      <c r="E109" s="1">
+      <c r="E109" s="1" t="e">
         <f t="shared" si="3"/>
-        <v>687025</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="110" spans="5:5">
-      <c r="E110" s="1">
+      <c r="E110" s="1" t="e">
         <f t="shared" si="3"/>
-        <v>687025</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="111" spans="5:5">
-      <c r="E111" s="1">
+      <c r="E111" s="1" t="e">
         <f t="shared" si="3"/>
-        <v>687025</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="112" spans="5:5">
-      <c r="E112" s="1">
+      <c r="E112" s="1" t="e">
         <f t="shared" si="3"/>
-        <v>687025</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="113" spans="5:5">
-      <c r="E113" s="1">
+      <c r="E113" s="1" t="e">
         <f t="shared" si="3"/>
-        <v>687025</v>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 4 Mar 2021, end of day.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="67">
   <si>
     <t>Tgl</t>
   </si>
@@ -218,7 +218,7 @@
     <t>SELISIH - lebih</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>FREIGHT OUT</t>
   </si>
 </sst>
 </file>
@@ -587,7 +587,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -857,15 +857,12 @@
       <c r="B20" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="D20" s="1">
-        <v>100000</v>
-      </c>
-      <c r="E20" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>10000</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="0"/>
+        <v>18565525</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -875,9 +872,9 @@
       <c r="D21" s="1">
         <v>18000000</v>
       </c>
-      <c r="E21" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="E21" s="1">
+        <f t="shared" si="0"/>
+        <v>565525</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -887,558 +884,576 @@
       <c r="B22" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="D22" s="1">
+        <f>45000</f>
+        <v>45000</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="0"/>
+        <v>520525</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="E23" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="B23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="1">
+        <f>450000+487500</f>
+        <v>937500</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="0"/>
+        <v>-416975</v>
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="E24" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="B24" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="1">
+        <f>65000</f>
+        <v>65000</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="0"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="E25" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="E25" s="1">
+        <f t="shared" si="0"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="E26" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="E26" s="1">
+        <f t="shared" si="0"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="E27" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="E27" s="1">
+        <f t="shared" si="0"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="E28" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="E28" s="1">
+        <f t="shared" si="0"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="E29" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="E29" s="1">
+        <f t="shared" si="0"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="E30" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="E30" s="1">
+        <f t="shared" si="0"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="E31" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="E31" s="1">
+        <f t="shared" si="0"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="E32" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="E32" s="1">
+        <f t="shared" si="0"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="33" spans="5:6">
-      <c r="E33" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="E33" s="1">
+        <f t="shared" si="0"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="34" spans="5:6">
-      <c r="E34" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="E34" s="1">
+        <f t="shared" si="0"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="35" spans="5:6">
-      <c r="E35" s="1" t="e">
+      <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>#VALUE!</v>
+        <v>-481975</v>
       </c>
     </row>
     <row r="36" spans="5:6">
-      <c r="E36" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="E36" s="1">
+        <f t="shared" si="1"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="37" spans="5:6">
-      <c r="E37" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="E37" s="1">
+        <f t="shared" si="1"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="38" spans="5:6">
-      <c r="E38" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="E38" s="1">
+        <f t="shared" si="1"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="39" spans="5:6">
-      <c r="E39" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="E39" s="1">
+        <f t="shared" si="1"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="40" spans="5:6">
-      <c r="E40" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="E40" s="1">
+        <f t="shared" si="1"/>
+        <v>-481975</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="5:6">
-      <c r="E41" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="E41" s="1">
+        <f t="shared" si="1"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="42" spans="5:6">
-      <c r="E42" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="E42" s="1">
+        <f t="shared" si="1"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="43" spans="5:6">
-      <c r="E43" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="E43" s="1">
+        <f t="shared" si="1"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="44" spans="5:6">
-      <c r="E44" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="E44" s="1">
+        <f t="shared" si="1"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="45" spans="5:6">
-      <c r="E45" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="E45" s="1">
+        <f t="shared" si="1"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="46" spans="5:6">
-      <c r="E46" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="E46" s="1">
+        <f t="shared" si="1"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="47" spans="5:6">
-      <c r="E47" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="E47" s="1">
+        <f t="shared" si="1"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="48" spans="5:6">
-      <c r="E48" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="E48" s="1">
+        <f t="shared" si="1"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="49" spans="5:6">
-      <c r="E49" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="E49" s="1">
+        <f t="shared" si="1"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="50" spans="5:6">
-      <c r="E50" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="E50" s="1">
+        <f t="shared" si="1"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="51" spans="5:6">
-      <c r="E51" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="E51" s="1">
+        <f t="shared" si="1"/>
+        <v>-481975</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
-      <c r="E52" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="E52" s="1">
+        <f t="shared" si="1"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="53" spans="5:6">
-      <c r="E53" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="E53" s="1">
+        <f t="shared" si="1"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="54" spans="5:6">
-      <c r="E54" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="E54" s="1">
+        <f t="shared" si="1"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="55" spans="5:6">
-      <c r="E55" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="E55" s="1">
+        <f t="shared" si="1"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="56" spans="5:6">
-      <c r="E56" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="E56" s="1">
+        <f t="shared" si="1"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="57" spans="5:6">
-      <c r="E57" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="E57" s="1">
+        <f t="shared" si="1"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="58" spans="5:6">
-      <c r="E58" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="E58" s="1">
+        <f t="shared" si="1"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="59" spans="5:6">
-      <c r="E59" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="E59" s="1">
+        <f t="shared" si="1"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="60" spans="5:6">
-      <c r="E60" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="E60" s="1">
+        <f t="shared" si="1"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="61" spans="5:6">
-      <c r="E61" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="E61" s="1">
+        <f t="shared" si="1"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="62" spans="5:6">
-      <c r="E62" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="E62" s="1">
+        <f t="shared" si="1"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="63" spans="5:6">
-      <c r="E63" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="E63" s="1">
+        <f t="shared" si="1"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="64" spans="5:6">
-      <c r="E64" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="E64" s="1">
+        <f t="shared" si="1"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="65" spans="5:7">
-      <c r="E65" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="E65" s="1">
+        <f t="shared" si="1"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="66" spans="5:7">
-      <c r="E66" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="E66" s="1">
+        <f t="shared" si="1"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="67" spans="5:7">
-      <c r="E67" s="1" t="e">
+      <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>#VALUE!</v>
+        <v>-481975</v>
       </c>
     </row>
     <row r="68" spans="5:7">
-      <c r="E68" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="E68" s="1">
+        <f t="shared" si="2"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="69" spans="5:7">
-      <c r="E69" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="E69" s="1">
+        <f t="shared" si="2"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="70" spans="5:7">
-      <c r="E70" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="E70" s="1">
+        <f t="shared" si="2"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="71" spans="5:7">
-      <c r="E71" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="E71" s="1">
+        <f t="shared" si="2"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="72" spans="5:7">
-      <c r="E72" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="E72" s="1">
+        <f t="shared" si="2"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="73" spans="5:7">
-      <c r="E73" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="E73" s="1">
+        <f t="shared" si="2"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="74" spans="5:7">
-      <c r="E74" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="E74" s="1">
+        <f t="shared" si="2"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="75" spans="5:7">
-      <c r="E75" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="E75" s="1">
+        <f t="shared" si="2"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="76" spans="5:7">
-      <c r="E76" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="E76" s="1">
+        <f t="shared" si="2"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="77" spans="5:7">
-      <c r="E77" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="E77" s="1">
+        <f t="shared" si="2"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="78" spans="5:7">
-      <c r="E78" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="E78" s="1">
+        <f t="shared" si="2"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="79" spans="5:7">
-      <c r="E79" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="E79" s="1">
+        <f t="shared" si="2"/>
+        <v>-481975</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
-      <c r="E80" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="E80" s="1">
+        <f t="shared" si="2"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="81" spans="5:5">
-      <c r="E81" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="E81" s="1">
+        <f t="shared" si="2"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="82" spans="5:5">
-      <c r="E82" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="E82" s="1">
+        <f t="shared" si="2"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="83" spans="5:5">
-      <c r="E83" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="E83" s="1">
+        <f t="shared" si="2"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="84" spans="5:5">
-      <c r="E84" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="E84" s="1">
+        <f t="shared" si="2"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="85" spans="5:5">
-      <c r="E85" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="E85" s="1">
+        <f t="shared" si="2"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="86" spans="5:5">
-      <c r="E86" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="E86" s="1">
+        <f t="shared" si="2"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="87" spans="5:5">
-      <c r="E87" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="E87" s="1">
+        <f t="shared" si="2"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="88" spans="5:5">
-      <c r="E88" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="E88" s="1">
+        <f t="shared" si="2"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="89" spans="5:5">
-      <c r="E89" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="E89" s="1">
+        <f t="shared" si="2"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="90" spans="5:5">
-      <c r="E90" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="E90" s="1">
+        <f t="shared" si="2"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="91" spans="5:5">
-      <c r="E91" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="E91" s="1">
+        <f t="shared" si="2"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="92" spans="5:5">
-      <c r="E92" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="E92" s="1">
+        <f t="shared" si="2"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="93" spans="5:5">
-      <c r="E93" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="E93" s="1">
+        <f t="shared" si="2"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="94" spans="5:5">
-      <c r="E94" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="E94" s="1">
+        <f t="shared" si="2"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="95" spans="5:5">
-      <c r="E95" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="E95" s="1">
+        <f t="shared" si="2"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="96" spans="5:5">
-      <c r="E96" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="E96" s="1">
+        <f t="shared" si="2"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="97" spans="5:5">
-      <c r="E97" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="E97" s="1">
+        <f t="shared" si="2"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="98" spans="5:5">
-      <c r="E98" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="E98" s="1">
+        <f t="shared" si="2"/>
+        <v>-481975</v>
       </c>
     </row>
     <row r="99" spans="5:5">
-      <c r="E99" s="1" t="e">
+      <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>#VALUE!</v>
+        <v>-481975</v>
       </c>
     </row>
     <row r="100" spans="5:5">
-      <c r="E100" s="1" t="e">
+      <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>-481975</v>
       </c>
     </row>
     <row r="101" spans="5:5">
-      <c r="E101" s="1" t="e">
+      <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>-481975</v>
       </c>
     </row>
     <row r="102" spans="5:5">
-      <c r="E102" s="1" t="e">
+      <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>-481975</v>
       </c>
     </row>
     <row r="103" spans="5:5">
-      <c r="E103" s="1" t="e">
+      <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>-481975</v>
       </c>
     </row>
     <row r="104" spans="5:5">
-      <c r="E104" s="1" t="e">
+      <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>-481975</v>
       </c>
     </row>
     <row r="105" spans="5:5">
-      <c r="E105" s="1" t="e">
+      <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>-481975</v>
       </c>
     </row>
     <row r="106" spans="5:5">
-      <c r="E106" s="1" t="e">
+      <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>-481975</v>
       </c>
     </row>
     <row r="107" spans="5:5">
-      <c r="E107" s="1" t="e">
+      <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>-481975</v>
       </c>
     </row>
     <row r="108" spans="5:5">
-      <c r="E108" s="1" t="e">
+      <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>-481975</v>
       </c>
     </row>
     <row r="109" spans="5:5">
-      <c r="E109" s="1" t="e">
+      <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>-481975</v>
       </c>
     </row>
     <row r="110" spans="5:5">
-      <c r="E110" s="1" t="e">
+      <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>-481975</v>
       </c>
     </row>
     <row r="111" spans="5:5">
-      <c r="E111" s="1" t="e">
+      <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>-481975</v>
       </c>
     </row>
     <row r="112" spans="5:5">
-      <c r="E112" s="1" t="e">
+      <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>-481975</v>
       </c>
     </row>
     <row r="113" spans="5:5">
-      <c r="E113" s="1" t="e">
+      <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>-481975</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 6 Mar 2021, end of day update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="74">
   <si>
     <t>Tgl</t>
   </si>
@@ -219,6 +219,27 @@
   </si>
   <si>
     <t>FREIGHT OUT</t>
+  </si>
+  <si>
+    <t>GARRETH - lab</t>
+  </si>
+  <si>
+    <t>A/P</t>
+  </si>
+  <si>
+    <t>QIU - dokter</t>
+  </si>
+  <si>
+    <t>BELI stempet</t>
+  </si>
+  <si>
+    <t>IURAN DAERAH</t>
+  </si>
+  <si>
+    <t>PARKIR - bulanan</t>
+  </si>
+  <si>
+    <t>BENSIN - RUSH</t>
   </si>
 </sst>
 </file>
@@ -586,8 +607,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+      <pane ySplit="2" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -819,7 +840,6 @@
         <v>59</v>
       </c>
       <c r="C17" s="1">
-        <f>1744500+7700000+84925000+18837500</f>
         <v>113207000</v>
       </c>
       <c r="E17" s="1">
@@ -845,7 +865,6 @@
         <v>61</v>
       </c>
       <c r="C19" s="1">
-        <f>8225475+18785525-18837500</f>
         <v>8173500</v>
       </c>
       <c r="E19" s="1">
@@ -858,11 +877,11 @@
         <v>62</v>
       </c>
       <c r="D20" s="1">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>18565525</v>
+        <v>18475525</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -874,7 +893,7 @@
       </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>565525</v>
+        <v>475525</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -885,12 +904,12 @@
         <v>25</v>
       </c>
       <c r="D22" s="1">
-        <f>45000</f>
-        <v>45000</v>
+        <f>45000+180000</f>
+        <v>225000</v>
       </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>520525</v>
+        <v>250525</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -898,12 +917,12 @@
         <v>60</v>
       </c>
       <c r="D23" s="1">
-        <f>450000+487500</f>
-        <v>937500</v>
+        <f>450000+487500+485000</f>
+        <v>1422500</v>
       </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>-416975</v>
+        <v>-1171975</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -916,544 +935,702 @@
       </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>-481975</v>
+        <v>-1236975</v>
       </c>
     </row>
     <row r="25" spans="1:5">
+      <c r="B25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="1">
+        <f>1150000</f>
+        <v>1150000</v>
+      </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>-481975</v>
+        <v>-2386975</v>
       </c>
     </row>
     <row r="26" spans="1:5">
+      <c r="B26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="1">
+        <f>9560000+18340500</f>
+        <v>27900500</v>
+      </c>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>-481975</v>
+        <v>25513525</v>
       </c>
     </row>
     <row r="27" spans="1:5">
+      <c r="B27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="1">
+        <f>37514525-7353025-18340500</f>
+        <v>11821000</v>
+      </c>
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>-481975</v>
+        <v>37334525</v>
       </c>
     </row>
     <row r="28" spans="1:5">
+      <c r="B28" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="1">
+        <v>3000</v>
+      </c>
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>-481975</v>
+        <v>37331525</v>
       </c>
     </row>
     <row r="29" spans="1:5">
+      <c r="B29" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="1">
+        <v>37000000</v>
+      </c>
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>-481975</v>
+        <v>331525</v>
       </c>
     </row>
     <row r="30" spans="1:5">
+      <c r="A30" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="1">
+        <f>45000+195000</f>
+        <v>240000</v>
+      </c>
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>-481975</v>
+        <v>91525</v>
       </c>
     </row>
     <row r="31" spans="1:5">
+      <c r="B31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="1">
+        <f>2600000</f>
+        <v>2600000</v>
+      </c>
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>-481975</v>
+        <v>-2508475</v>
       </c>
     </row>
     <row r="32" spans="1:5">
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="1">
+        <f>3700000+4500000+1649500+5020000+2100000</f>
+        <v>16969500</v>
+      </c>
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>-481975</v>
-      </c>
-    </row>
-    <row r="33" spans="5:6">
+        <v>-19477975</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="B33" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="1">
+        <f>29190500</f>
+        <v>29190500</v>
+      </c>
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>-481975</v>
-      </c>
-    </row>
-    <row r="34" spans="5:6">
+        <v>9712525</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="B34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="1">
+        <f>19282975+20997025-29190500</f>
+        <v>11089500</v>
+      </c>
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>-481975</v>
-      </c>
-    </row>
-    <row r="35" spans="5:6">
+        <v>20802025</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="B35" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35" s="1">
+        <f>300000</f>
+        <v>300000</v>
+      </c>
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>-481975</v>
-      </c>
-    </row>
-    <row r="36" spans="5:6">
+        <v>20502025</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="B36" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" s="1">
+        <v>11000</v>
+      </c>
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>-481975</v>
-      </c>
-    </row>
-    <row r="37" spans="5:6">
+        <v>20513025</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="B37" t="s">
+        <v>63</v>
+      </c>
+      <c r="D37" s="1">
+        <v>20000000</v>
+      </c>
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>-481975</v>
-      </c>
-    </row>
-    <row r="38" spans="5:6">
+        <v>513025</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="2">
+        <v>44261</v>
+      </c>
+      <c r="B38" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" s="1">
+        <f>45000+1180000</f>
+        <v>1225000</v>
+      </c>
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>-481975</v>
-      </c>
-    </row>
-    <row r="39" spans="5:6">
+        <v>-711975</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="B39" t="s">
+        <v>70</v>
+      </c>
+      <c r="D39" s="1">
+        <f>18000</f>
+        <v>18000</v>
+      </c>
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>-481975</v>
-      </c>
-    </row>
-    <row r="40" spans="5:6">
+        <v>-729975</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="B40" t="s">
+        <v>60</v>
+      </c>
+      <c r="D40" s="1">
+        <f>85000+200000+840000+1280000+2907000+30000000</f>
+        <v>35312000</v>
+      </c>
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>-481975</v>
+        <v>-36041975</v>
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="5:6">
+    <row r="41" spans="1:6">
+      <c r="B41" t="s">
+        <v>71</v>
+      </c>
+      <c r="D41" s="1">
+        <v>25000</v>
+      </c>
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>-481975</v>
-      </c>
-    </row>
-    <row r="42" spans="5:6">
+        <v>-36066975</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="B42" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42" s="1">
+        <v>10000</v>
+      </c>
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>-481975</v>
-      </c>
-    </row>
-    <row r="43" spans="5:6">
+        <v>-36076975</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="B43" t="s">
+        <v>73</v>
+      </c>
+      <c r="D43" s="1">
+        <v>250000</v>
+      </c>
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>-481975</v>
-      </c>
-    </row>
-    <row r="44" spans="5:6">
+        <v>-36326975</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="B44" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" s="1">
+        <f>47072000+30000000</f>
+        <v>77072000</v>
+      </c>
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>-481975</v>
-      </c>
-    </row>
-    <row r="45" spans="5:6">
+        <v>40745025</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="B45" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45" s="1">
+        <f>5146975+47526025-47072000</f>
+        <v>5601000</v>
+      </c>
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>-481975</v>
-      </c>
-    </row>
-    <row r="46" spans="5:6">
+        <v>46346025</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="B46" t="s">
+        <v>65</v>
+      </c>
+      <c r="C46" s="1">
+        <v>140000</v>
+      </c>
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>-481975</v>
-      </c>
-    </row>
-    <row r="47" spans="5:6">
+        <v>46486025</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="B47" t="s">
+        <v>63</v>
+      </c>
+      <c r="D47" s="1">
+        <v>46000000</v>
+      </c>
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>-481975</v>
-      </c>
-    </row>
-    <row r="48" spans="5:6">
+        <v>486025</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>-481975</v>
+        <v>486025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 11-Mar-2021, end of day.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="68">
   <si>
     <t>Tgl</t>
   </si>
@@ -206,40 +206,22 @@
     <t>SALES - cash/retail</t>
   </si>
   <si>
-    <t>SELISIH - kurang</t>
-  </si>
-  <si>
     <t>SETOR KE BANK</t>
   </si>
   <si>
-    <t>BELI kresek</t>
-  </si>
-  <si>
     <t>SELISIH - lebih</t>
   </si>
   <si>
     <t>FREIGHT OUT</t>
   </si>
   <si>
-    <t>GARRETH - lab</t>
-  </si>
-  <si>
-    <t>A/P</t>
-  </si>
-  <si>
-    <t>QIU - dokter</t>
-  </si>
-  <si>
-    <t>BELI stempet</t>
-  </si>
-  <si>
-    <t>IURAN DAERAH</t>
-  </si>
-  <si>
-    <t>PARKIR - bulanan</t>
-  </si>
-  <si>
-    <t>BENSIN - RUSH</t>
+    <t>BELI karet gelang</t>
+  </si>
+  <si>
+    <t>PRIVE - andreas</t>
+  </si>
+  <si>
+    <t>CHEQUE RECEIVED</t>
   </si>
 </sst>
 </file>
@@ -607,8 +589,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -644,49 +626,49 @@
         <v>5</v>
       </c>
       <c r="E2" s="1">
-        <v>687025</v>
+        <v>486025</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>44256</v>
+        <v>44263</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="1">
-        <f>45000+195000</f>
-        <v>240000</v>
+        <f>45000+235000</f>
+        <v>280000</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>447025</v>
+        <v>206025</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="B4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="1">
-        <f>5400000+810000+43500000+45874000</f>
-        <v>95584000</v>
+        <v>60</v>
+      </c>
+      <c r="D4" s="1">
+        <f>2510000+1795000+1900000+850000+900000+1280000+140000+165000+2095000+840000+850000</f>
+        <v>13325000</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>96031025</v>
+        <v>-13118975</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="B5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="1">
-        <f>1800000+2567000+810000+30000000+720000</f>
-        <v>35897000</v>
+        <v>59</v>
+      </c>
+      <c r="C5" s="1">
+        <f>1795000+7960000+31702000</f>
+        <v>41457000</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>60134025</v>
+        <v>28338025</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -694,943 +676,830 @@
         <v>61</v>
       </c>
       <c r="C6" s="1">
-        <f>69749025-14455025-45874000</f>
-        <v>9420000</v>
+        <f>2278975+39393025-31702000</f>
+        <v>9970000</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>69554025</v>
+        <v>38308025</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="B7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="1">
-        <v>50000</v>
+        <v>63</v>
+      </c>
+      <c r="C7" s="1">
+        <v>10000</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>69504025</v>
+        <v>38318025</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
       <c r="B8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D8" s="1">
-        <v>69000000</v>
+        <f>38000000</f>
+        <v>38000000</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>504025</v>
+        <v>318025</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2">
-        <v>44257</v>
+        <v>44264</v>
       </c>
       <c r="B9" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="1">
-        <f>45000+180000</f>
-        <v>225000</v>
+        <f>45000+225000</f>
+        <v>270000</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>279025</v>
+        <v>48025</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="B10" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D10" s="1">
-        <f>900000+1519000+220000</f>
-        <v>2639000</v>
+        <f>30000</f>
+        <v>30000</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>-2359975</v>
+        <v>18025</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="B11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D11" s="1">
-        <f>52000</f>
-        <v>52000</v>
+        <f>4250000</f>
+        <v>4250000</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>-2411975</v>
+        <v>-4231975</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="B12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" s="1">
-        <f>9000000+9566000</f>
-        <v>18566000</v>
+        <v>64</v>
+      </c>
+      <c r="D12" s="1">
+        <f>15000+42000</f>
+        <v>57000</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>16154025</v>
+        <v>-4288975</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="B13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C13" s="1">
-        <f>2231975+16952025-9566000</f>
-        <v>9618000</v>
+        <f>118450000+36773000</f>
+        <v>155223000</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>25772025</v>
+        <v>150934025</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="B14" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C14" s="1">
-        <v>470000</v>
+        <f>160810025-114386025-36773000</f>
+        <v>9651000</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>26242025</v>
+        <v>160585025</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="B15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="1">
+        <v>15000000</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="0"/>
+        <v>145585025</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="B16" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="1">
-        <v>26000000</v>
-      </c>
-      <c r="E15" s="1">
-        <f t="shared" si="0"/>
-        <v>242025</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="2">
-        <v>44258</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="C16" s="1">
+        <v>135000</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="0"/>
+        <v>145720025</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="B17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="1">
+        <v>145000000</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="0"/>
+        <v>720025</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="2">
+        <v>44265</v>
+      </c>
+      <c r="B18" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D18" s="1">
         <f>45000+210000</f>
         <v>255000</v>
       </c>
-      <c r="E16" s="1">
-        <f t="shared" si="0"/>
-        <v>-12975</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="B17" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" s="1">
-        <v>113207000</v>
-      </c>
-      <c r="E17" s="1">
-        <f t="shared" si="0"/>
-        <v>113194025</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="B18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D18" s="1">
-        <f>1744500+7700000+7057500+84925000+1365000</f>
-        <v>102792000</v>
-      </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>10402025</v>
+        <v>465025</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="B19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="1">
-        <v>8173500</v>
+        <v>67</v>
+      </c>
+      <c r="D19" s="1">
+        <f>3440000</f>
+        <v>3440000</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>18575525</v>
+        <v>-2974975</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="B20" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="1">
-        <v>100000</v>
+        <v>59</v>
+      </c>
+      <c r="C20" s="1">
+        <f>92400000+7020000+30000000+25680000+39822000+60411500</f>
+        <v>255333500</v>
       </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>18475525</v>
+        <v>252358525</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="B21" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D21" s="1">
-        <v>18000000</v>
+        <f>92400000+1202000+19162000+7020000+6000000+1225000+5580000+1838500+25680000</f>
+        <v>160107500</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>475525</v>
+        <v>92251025</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="2">
-        <v>44259</v>
-      </c>
       <c r="B22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" s="1">
-        <f>45000+180000</f>
-        <v>225000</v>
+        <v>61</v>
+      </c>
+      <c r="C22" s="1">
+        <f>106292025-32049525-60411500</f>
+        <v>13831000</v>
       </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>250525</v>
+        <v>106082025</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="B23" t="s">
-        <v>60</v>
-      </c>
-      <c r="D23" s="1">
-        <f>450000+487500+485000</f>
-        <v>1422500</v>
+        <v>63</v>
+      </c>
+      <c r="C23" s="1">
+        <v>75000</v>
       </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>-1171975</v>
+        <v>106157025</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="B24" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D24" s="1">
-        <f>65000</f>
-        <v>65000</v>
+        <v>106000000</v>
       </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>-1236975</v>
+        <v>157025</v>
       </c>
     </row>
     <row r="25" spans="1:5">
+      <c r="A25" s="2">
+        <v>44266</v>
+      </c>
       <c r="B25" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="D25" s="1">
-        <f>1150000</f>
-        <v>1150000</v>
+        <f>45000+195000</f>
+        <v>240000</v>
       </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>-2386975</v>
+        <v>-82975</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="B26" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="1">
-        <f>9560000+18340500</f>
-        <v>27900500</v>
+        <v>60</v>
+      </c>
+      <c r="D26" s="1">
+        <f>25224000+908500+220000+2565000</f>
+        <v>28917500</v>
       </c>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>25513525</v>
+        <v>-29000475</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="B27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C27" s="1">
-        <f>37514525-7353025-18340500</f>
-        <v>11821000</v>
+        <f>25224000+3473500</f>
+        <v>28697500</v>
       </c>
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>37334525</v>
+        <v>-302975</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="B28" t="s">
-        <v>62</v>
-      </c>
-      <c r="D28" s="1">
-        <v>3000</v>
+        <v>61</v>
+      </c>
+      <c r="C28" s="1">
+        <f>3581475+9212025-3473500</f>
+        <v>9320000</v>
       </c>
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>37331525</v>
+        <v>9017025</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="B29" t="s">
         <v>63</v>
       </c>
-      <c r="D29" s="1">
-        <v>37000000</v>
+      <c r="C29" s="1">
+        <v>6000</v>
       </c>
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>331525</v>
+        <v>9023025</v>
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="2">
-        <v>44260</v>
-      </c>
       <c r="B30" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="D30" s="1">
-        <f>45000+195000</f>
-        <v>240000</v>
+        <v>8000000</v>
       </c>
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>91525</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="B31" t="s">
-        <v>68</v>
-      </c>
-      <c r="D31" s="1">
-        <f>2600000</f>
-        <v>2600000</v>
+      <c r="A31" s="2">
+        <v>44267</v>
       </c>
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>-2508475</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="B32" t="s">
-        <v>60</v>
-      </c>
-      <c r="D32" s="1">
-        <f>3700000+4500000+1649500+5020000+2100000</f>
-        <v>16969500</v>
-      </c>
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>-19477975</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="B33" t="s">
-        <v>59</v>
-      </c>
-      <c r="C33" s="1">
-        <f>29190500</f>
-        <v>29190500</v>
-      </c>
+        <v>1023025</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>9712525</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="B34" t="s">
-        <v>61</v>
-      </c>
-      <c r="C34" s="1">
-        <f>19282975+20997025-29190500</f>
-        <v>11089500</v>
-      </c>
+        <v>1023025</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>20802025</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="B35" t="s">
-        <v>69</v>
-      </c>
-      <c r="D35" s="1">
-        <f>300000</f>
-        <v>300000</v>
-      </c>
+        <v>1023025</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>20502025</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="B36" t="s">
-        <v>65</v>
-      </c>
-      <c r="C36" s="1">
-        <v>11000</v>
-      </c>
+        <v>1023025</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>20513025</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="B37" t="s">
-        <v>63</v>
-      </c>
-      <c r="D37" s="1">
-        <v>20000000</v>
-      </c>
+        <v>1023025</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>513025</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="2">
-        <v>44261</v>
-      </c>
-      <c r="B38" t="s">
-        <v>25</v>
-      </c>
-      <c r="D38" s="1">
-        <f>45000+1180000</f>
-        <v>1225000</v>
-      </c>
+        <v>1023025</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>-711975</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="B39" t="s">
-        <v>70</v>
-      </c>
-      <c r="D39" s="1">
-        <f>18000</f>
-        <v>18000</v>
-      </c>
+        <v>1023025</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>-729975</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="B40" t="s">
-        <v>60</v>
-      </c>
-      <c r="D40" s="1">
-        <f>85000+200000+840000+1280000+2907000+30000000</f>
-        <v>35312000</v>
-      </c>
+        <v>1023025</v>
+      </c>
+    </row>
+    <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>-36041975</v>
+        <v>1023025</v>
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="1:6">
-      <c r="B41" t="s">
-        <v>71</v>
-      </c>
-      <c r="D41" s="1">
-        <v>25000</v>
-      </c>
+    <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>-36066975</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="B42" t="s">
-        <v>72</v>
-      </c>
-      <c r="D42" s="1">
-        <v>10000</v>
-      </c>
+        <v>1023025</v>
+      </c>
+    </row>
+    <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>-36076975</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="B43" t="s">
-        <v>73</v>
-      </c>
-      <c r="D43" s="1">
-        <v>250000</v>
-      </c>
+        <v>1023025</v>
+      </c>
+    </row>
+    <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>-36326975</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="B44" t="s">
-        <v>59</v>
-      </c>
-      <c r="C44" s="1">
-        <f>47072000+30000000</f>
-        <v>77072000</v>
-      </c>
+        <v>1023025</v>
+      </c>
+    </row>
+    <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>40745025</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="B45" t="s">
-        <v>61</v>
-      </c>
-      <c r="C45" s="1">
-        <f>5146975+47526025-47072000</f>
-        <v>5601000</v>
-      </c>
+        <v>1023025</v>
+      </c>
+    </row>
+    <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>46346025</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="B46" t="s">
-        <v>65</v>
-      </c>
-      <c r="C46" s="1">
-        <v>140000</v>
-      </c>
+        <v>1023025</v>
+      </c>
+    </row>
+    <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>46486025</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="B47" t="s">
-        <v>63</v>
-      </c>
-      <c r="D47" s="1">
-        <v>46000000</v>
-      </c>
+        <v>1023025</v>
+      </c>
+    </row>
+    <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>486025</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>1023025</v>
+      </c>
+    </row>
+    <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>486025</v>
+        <v>1023025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 12 Mar 2021, end of day update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="69">
   <si>
     <t>Tgl</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>CHEQUE RECEIVED</t>
+  </si>
+  <si>
+    <t>SELISIH - kurang</t>
   </si>
 </sst>
 </file>
@@ -589,8 +592,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
+      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1002,504 +1005,547 @@
       <c r="A31" s="2">
         <v>44267</v>
       </c>
+      <c r="B31" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="1">
+        <f>45000+225000</f>
+        <v>270000</v>
+      </c>
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>1023025</v>
+        <v>753025</v>
       </c>
     </row>
     <row r="32" spans="1:5">
+      <c r="B32" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="1">
+        <f>20400000+500000+9510000+21309500</f>
+        <v>51719500</v>
+      </c>
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>1023025</v>
-      </c>
-    </row>
-    <row r="33" spans="5:6">
+        <v>52472525</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="B33" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" s="1">
+        <f>20400000+450000+725000+180000</f>
+        <v>21755000</v>
+      </c>
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>1023025</v>
-      </c>
-    </row>
-    <row r="34" spans="5:6">
+        <v>30717525</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="B34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="1">
+        <f>41389525-9633025-21309500</f>
+        <v>10447000</v>
+      </c>
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>1023025</v>
-      </c>
-    </row>
-    <row r="35" spans="5:6">
+        <v>41164525</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="B35" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1000</v>
+      </c>
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>1023025</v>
-      </c>
-    </row>
-    <row r="36" spans="5:6">
+        <v>41163525</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="B36" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36" s="1">
+        <v>41000000</v>
+      </c>
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>1023025</v>
-      </c>
-    </row>
-    <row r="37" spans="5:6">
+        <v>163525</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="2">
+        <v>44268</v>
+      </c>
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>1023025</v>
-      </c>
-    </row>
-    <row r="38" spans="5:6">
+        <v>163525</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>1023025</v>
-      </c>
-    </row>
-    <row r="39" spans="5:6">
+        <v>163525</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>1023025</v>
-      </c>
-    </row>
-    <row r="40" spans="5:6">
+        <v>163525</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="5:6">
+    <row r="41" spans="1:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>1023025</v>
-      </c>
-    </row>
-    <row r="42" spans="5:6">
+        <v>163525</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>1023025</v>
-      </c>
-    </row>
-    <row r="43" spans="5:6">
+        <v>163525</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>1023025</v>
-      </c>
-    </row>
-    <row r="44" spans="5:6">
+        <v>163525</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>1023025</v>
-      </c>
-    </row>
-    <row r="45" spans="5:6">
+        <v>163525</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>1023025</v>
-      </c>
-    </row>
-    <row r="46" spans="5:6">
+        <v>163525</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>1023025</v>
-      </c>
-    </row>
-    <row r="47" spans="5:6">
+        <v>163525</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>1023025</v>
-      </c>
-    </row>
-    <row r="48" spans="5:6">
+        <v>163525</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>1023025</v>
+        <v>163525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 17-Mar-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
   <si>
     <t>Tgl</t>
   </si>
@@ -203,28 +203,7 @@
     <t>TRANSFER BCA</t>
   </si>
   <si>
-    <t>SALES - cash/retail</t>
-  </si>
-  <si>
-    <t>SETOR KE BANK</t>
-  </si>
-  <si>
-    <t>SELISIH - lebih</t>
-  </si>
-  <si>
-    <t>FREIGHT OUT</t>
-  </si>
-  <si>
-    <t>BELI karet gelang</t>
-  </si>
-  <si>
-    <t>PRIVE - andreas</t>
-  </si>
-  <si>
-    <t>CHEQUE RECEIVED</t>
-  </si>
-  <si>
-    <t>SELISIH - kurang</t>
+    <t>STNK - motor</t>
   </si>
 </sst>
 </file>
@@ -592,8 +571,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -629,23 +608,23 @@
         <v>5</v>
       </c>
       <c r="E2" s="1">
-        <v>486025</v>
+        <v>660525</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>44263</v>
+        <v>44270</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="1">
-        <f>45000+235000</f>
-        <v>280000</v>
+        <f>45000</f>
+        <v>45000</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>206025</v>
+        <v>615525</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -653,12 +632,12 @@
         <v>60</v>
       </c>
       <c r="D4" s="1">
-        <f>2510000+1795000+1900000+850000+900000+1280000+140000+165000+2095000+840000+850000</f>
-        <v>13325000</v>
+        <f>450000+1061000+80000000+1917500</f>
+        <v>83428500</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>-13118975</v>
+        <v>-82812975</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -666,886 +645,670 @@
         <v>59</v>
       </c>
       <c r="C5" s="1">
-        <f>1795000+7960000+31702000</f>
-        <v>41457000</v>
+        <f>80000000</f>
+        <v>80000000</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>28338025</v>
+        <v>-2812975</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="B6" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="1">
-        <f>2278975+39393025-31702000</f>
-        <v>9970000</v>
+      <c r="D6" s="1">
+        <v>199000</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>38308025</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="B7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="1">
-        <v>10000</v>
-      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>38318025</v>
+        <v>-3011975</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="B8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" s="1">
-        <f>38000000</f>
-        <v>38000000</v>
-      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>318025</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="2">
-        <v>44264</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="1">
-        <f>45000+225000</f>
-        <v>270000</v>
-      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>48025</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="B10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="1">
-        <f>30000</f>
-        <v>30000</v>
-      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>18025</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="B11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="1">
-        <f>4250000</f>
-        <v>4250000</v>
-      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>-4231975</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="B12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12" s="1">
-        <f>15000+42000</f>
-        <v>57000</v>
-      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>-4288975</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="1">
-        <f>118450000+36773000</f>
-        <v>155223000</v>
-      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>150934025</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="B14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" s="1">
-        <f>160810025-114386025-36773000</f>
-        <v>9651000</v>
-      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>160585025</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="B15" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" s="1">
-        <v>15000000</v>
-      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>145585025</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="B16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="1">
-        <v>135000</v>
-      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>145720025</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="B17" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" s="1">
-        <v>145000000</v>
-      </c>
+        <v>-3011975</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5">
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>720025</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="2">
-        <v>44265</v>
-      </c>
-      <c r="B18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="1">
-        <f>45000+210000</f>
-        <v>255000</v>
-      </c>
+        <v>-3011975</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5">
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>465025</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="B19" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" s="1">
-        <f>3440000</f>
-        <v>3440000</v>
-      </c>
+        <v>-3011975</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5">
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>-2974975</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="B20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="1">
-        <f>92400000+7020000+30000000+25680000+39822000+60411500</f>
-        <v>255333500</v>
-      </c>
+        <v>-3011975</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5">
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>252358525</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="B21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D21" s="1">
-        <f>92400000+1202000+19162000+7020000+6000000+1225000+5580000+1838500+25680000</f>
-        <v>160107500</v>
-      </c>
+        <v>-3011975</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5">
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>92251025</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="B22" t="s">
-        <v>61</v>
-      </c>
-      <c r="C22" s="1">
-        <f>106292025-32049525-60411500</f>
-        <v>13831000</v>
-      </c>
+        <v>-3011975</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>106082025</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="B23" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" s="1">
-        <v>75000</v>
-      </c>
+        <v>-3011975</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>106157025</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="B24" t="s">
-        <v>62</v>
-      </c>
-      <c r="D24" s="1">
-        <v>106000000</v>
-      </c>
+        <v>-3011975</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>157025</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="2">
-        <v>44266</v>
-      </c>
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="1">
-        <f>45000+195000</f>
-        <v>240000</v>
-      </c>
+        <v>-3011975</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>-82975</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="B26" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26" s="1">
-        <f>25224000+908500+220000+2565000</f>
-        <v>28917500</v>
-      </c>
+        <v>-3011975</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>-29000475</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="B27" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" s="1">
-        <f>25224000+3473500</f>
-        <v>28697500</v>
-      </c>
+        <v>-3011975</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>-302975</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="B28" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" s="1">
-        <f>3581475+9212025-3473500</f>
-        <v>9320000</v>
-      </c>
+        <v>-3011975</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>9017025</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="B29" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" s="1">
-        <v>6000</v>
-      </c>
+        <v>-3011975</v>
+      </c>
+    </row>
+    <row r="29" spans="5:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>9023025</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="B30" t="s">
-        <v>62</v>
-      </c>
-      <c r="D30" s="1">
-        <v>8000000</v>
-      </c>
+        <v>-3011975</v>
+      </c>
+    </row>
+    <row r="30" spans="5:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>1023025</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="2">
-        <v>44267</v>
-      </c>
-      <c r="B31" t="s">
-        <v>25</v>
-      </c>
-      <c r="D31" s="1">
-        <f>45000+225000</f>
-        <v>270000</v>
-      </c>
+        <v>-3011975</v>
+      </c>
+    </row>
+    <row r="31" spans="5:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>753025</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="B32" t="s">
-        <v>59</v>
-      </c>
-      <c r="C32" s="1">
-        <f>20400000+500000+9510000+21309500</f>
-        <v>51719500</v>
-      </c>
+        <v>-3011975</v>
+      </c>
+    </row>
+    <row r="32" spans="5:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>52472525</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="B33" t="s">
-        <v>60</v>
-      </c>
-      <c r="D33" s="1">
-        <f>20400000+450000+725000+180000</f>
-        <v>21755000</v>
-      </c>
+        <v>-3011975</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>30717525</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="B34" t="s">
-        <v>61</v>
-      </c>
-      <c r="C34" s="1">
-        <f>41389525-9633025-21309500</f>
-        <v>10447000</v>
-      </c>
+        <v>-3011975</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>41164525</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="B35" t="s">
-        <v>68</v>
-      </c>
-      <c r="D35" s="1">
-        <v>1000</v>
-      </c>
+        <v>-3011975</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>41163525</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="B36" t="s">
-        <v>62</v>
-      </c>
-      <c r="D36" s="1">
-        <v>41000000</v>
-      </c>
+        <v>-3011975</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>163525</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="2">
-        <v>44268</v>
-      </c>
+        <v>-3011975</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>163525</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+        <v>-3011975</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>163525</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+        <v>-3011975</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>163525</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>-3011975</v>
+      </c>
+    </row>
+    <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>163525</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+        <v>-3011975</v>
+      </c>
+    </row>
+    <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>163525</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>-3011975</v>
+      </c>
+    </row>
+    <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>163525</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>-3011975</v>
+      </c>
+    </row>
+    <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>163525</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>-3011975</v>
+      </c>
+    </row>
+    <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>163525</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>-3011975</v>
+      </c>
+    </row>
+    <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>163525</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>-3011975</v>
+      </c>
+    </row>
+    <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>163525</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>-3011975</v>
+      </c>
+    </row>
+    <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>163525</v>
+        <v>-3011975</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 17-Mar-2021, end of day.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="15135" windowHeight="8130"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="73">
   <si>
     <t>Tgl</t>
   </si>
@@ -204,6 +204,39 @@
   </si>
   <si>
     <t>STNK - motor</t>
+  </si>
+  <si>
+    <t>TRANSFER BCA AA</t>
+  </si>
+  <si>
+    <t>SERVICE rumah MH27</t>
+  </si>
+  <si>
+    <t>FREIGHT OUT</t>
+  </si>
+  <si>
+    <t>JASON - kacamata</t>
+  </si>
+  <si>
+    <t>SALES - cash/retail</t>
+  </si>
+  <si>
+    <t>SELISIH - lebih</t>
+  </si>
+  <si>
+    <t>SETOR KE BANK</t>
+  </si>
+  <si>
+    <t>BELI amplop + buku bon</t>
+  </si>
+  <si>
+    <t>A/P</t>
+  </si>
+  <si>
+    <t>DANA KEBERSIHAN</t>
+  </si>
+  <si>
+    <t>FREIGHT IN</t>
   </si>
 </sst>
 </file>
@@ -571,8 +604,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -619,12 +652,12 @@
         <v>25</v>
       </c>
       <c r="D3" s="1">
-        <f>45000</f>
-        <v>45000</v>
+        <f>45000+195000</f>
+        <v>240000</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>615525</v>
+        <v>420525</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -632,12 +665,12 @@
         <v>60</v>
       </c>
       <c r="D4" s="1">
-        <f>450000+1061000+80000000+1917500</f>
-        <v>83428500</v>
+        <f>450000+1061000+80000000+1917500+34760000</f>
+        <v>118188500</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>-82812975</v>
+        <v>-117767975</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -645,12 +678,12 @@
         <v>59</v>
       </c>
       <c r="C5" s="1">
-        <f>80000000</f>
-        <v>80000000</v>
+        <f>80000000+59220000+109760000+11058500</f>
+        <v>260038500</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>-2812975</v>
+        <v>142270525</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -662,653 +695,809 @@
       </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>-3011975</v>
+        <v>142071525</v>
       </c>
     </row>
     <row r="7" spans="1:6">
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="1">
+        <f>59220000</f>
+        <v>59220000</v>
+      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>-3011975</v>
+        <v>82851525</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="1">
+        <v>25000</v>
+      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>-3011975</v>
+        <v>82826525</v>
       </c>
     </row>
     <row r="9" spans="1:6">
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="1">
+        <f>15000</f>
+        <v>15000</v>
+      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>-3011975</v>
+        <v>82811525</v>
       </c>
     </row>
     <row r="10" spans="1:6">
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="1">
+        <v>700000</v>
+      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>-3011975</v>
+        <v>82111525</v>
       </c>
     </row>
     <row r="11" spans="1:6">
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="1">
+        <f>92788525-71248025-11058500</f>
+        <v>10482000</v>
+      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>-3011975</v>
+        <v>92593525</v>
       </c>
     </row>
     <row r="12" spans="1:6">
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="1">
+        <v>210000</v>
+      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>-3011975</v>
+        <v>92803525</v>
       </c>
     </row>
     <row r="13" spans="1:6">
+      <c r="B13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="1">
+        <v>92000000</v>
+      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>-3011975</v>
+        <v>803525</v>
       </c>
     </row>
     <row r="14" spans="1:6">
+      <c r="A14" s="2">
+        <v>44271</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="1">
+        <f>45000+195000</f>
+        <v>240000</v>
+      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>-3011975</v>
+        <v>563525</v>
       </c>
     </row>
     <row r="15" spans="1:6">
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="1">
+        <f>390000+21990000+1559000+356000+380000</f>
+        <v>24675000</v>
+      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>-3011975</v>
+        <v>-24111475</v>
       </c>
     </row>
     <row r="16" spans="1:6">
+      <c r="B16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="1">
+        <f>232500</f>
+        <v>232500</v>
+      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>-3011975</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5">
+        <v>-24343975</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="1">
+        <f>1900000</f>
+        <v>1900000</v>
+      </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>-3011975</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5">
+        <v>-26243975</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="B18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="1">
+        <f>1500000+380000+22346000</f>
+        <v>24226000</v>
+      </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>-3011975</v>
-      </c>
-    </row>
-    <row r="19" spans="5:5">
+        <v>-2017975</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="B19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="1">
+        <f>7822025+24168975-22346000</f>
+        <v>9645000</v>
+      </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>-3011975</v>
-      </c>
-    </row>
-    <row r="20" spans="5:5">
+        <v>7627025</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="B20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="1">
+        <v>7000000</v>
+      </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>-3011975</v>
-      </c>
-    </row>
-    <row r="21" spans="5:5">
+        <v>627025</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2">
+        <v>44272</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="1">
+        <f>45000+300000+180000</f>
+        <v>525000</v>
+      </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>-3011975</v>
-      </c>
-    </row>
-    <row r="22" spans="5:5">
+        <v>102025</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="B22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="1">
+        <f>2840000+3214000+537000+450000</f>
+        <v>7041000</v>
+      </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>-3011975</v>
-      </c>
-    </row>
-    <row r="23" spans="5:5">
+        <v>-6938975</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="B23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="1">
+        <f>10420000+13847000</f>
+        <v>24267000</v>
+      </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>-3011975</v>
-      </c>
-    </row>
-    <row r="24" spans="5:5">
+        <v>17328025</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="B24" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="1">
+        <f>120000</f>
+        <v>120000</v>
+      </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>-3011975</v>
-      </c>
-    </row>
-    <row r="25" spans="5:5">
+        <v>17208025</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="B25" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="1">
+        <f>2715000</f>
+        <v>2715000</v>
+      </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>-3011975</v>
-      </c>
-    </row>
-    <row r="26" spans="5:5">
+        <v>14493025</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="B26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="1">
+        <f>22157025-826025+535000+537000-13847000</f>
+        <v>8556000</v>
+      </c>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>-3011975</v>
-      </c>
-    </row>
-    <row r="27" spans="5:5">
+        <v>23049025</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="B27" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="1">
+        <v>45000</v>
+      </c>
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>-3011975</v>
-      </c>
-    </row>
-    <row r="28" spans="5:5">
+        <v>23094025</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="B28" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" s="1">
+        <v>23000000</v>
+      </c>
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>-3011975</v>
-      </c>
-    </row>
-    <row r="29" spans="5:5">
+        <v>94025</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="2">
+        <v>44273</v>
+      </c>
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>-3011975</v>
-      </c>
-    </row>
-    <row r="30" spans="5:5">
+        <v>94025</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>-3011975</v>
-      </c>
-    </row>
-    <row r="31" spans="5:5">
+        <v>94025</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>-3011975</v>
-      </c>
-    </row>
-    <row r="32" spans="5:5">
+        <v>94025</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>-3011975</v>
+        <v>94025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 20-Mei-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="78">
   <si>
     <t>Tgl</t>
   </si>
@@ -237,6 +237,21 @@
   </si>
   <si>
     <t>FREIGHT IN</t>
+  </si>
+  <si>
+    <t>BELI kresek</t>
+  </si>
+  <si>
+    <t>TELPON - 5224823</t>
+  </si>
+  <si>
+    <t>PLN - Astar 165</t>
+  </si>
+  <si>
+    <t>CHEQUE RECEIVED</t>
+  </si>
+  <si>
+    <t>PRIVE - andreas</t>
   </si>
 </sst>
 </file>
@@ -604,8 +619,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
+      <pane ySplit="2" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -988,516 +1003,644 @@
       <c r="A29" s="2">
         <v>44273</v>
       </c>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="1">
+        <f>45000+195000</f>
+        <v>240000</v>
+      </c>
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>94025</v>
+        <v>-145975</v>
       </c>
     </row>
     <row r="30" spans="1:5">
+      <c r="B30" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" s="1">
+        <v>97000</v>
+      </c>
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>94025</v>
+        <v>-242975</v>
       </c>
     </row>
     <row r="31" spans="1:5">
+      <c r="B31" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="1">
+        <f>464000+3680000+170000+230000+1082000</f>
+        <v>5626000</v>
+      </c>
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>94025</v>
+        <v>-5868975</v>
       </c>
     </row>
     <row r="32" spans="1:5">
+      <c r="B32" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32" s="1">
+        <v>681500</v>
+      </c>
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>94025</v>
-      </c>
-    </row>
-    <row r="33" spans="5:6">
+        <v>-6550475</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="B33" t="s">
+        <v>75</v>
+      </c>
+      <c r="D33" s="1">
+        <f>791500</f>
+        <v>791500</v>
+      </c>
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>94025</v>
-      </c>
-    </row>
-    <row r="34" spans="5:6">
+        <v>-7341975</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="B34" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" s="1">
+        <f>1670000</f>
+        <v>1670000</v>
+      </c>
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>94025</v>
-      </c>
-    </row>
-    <row r="35" spans="5:6">
+        <v>-9011975</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="B35" t="s">
+        <v>77</v>
+      </c>
+      <c r="D35" s="1">
+        <v>5000000</v>
+      </c>
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>94025</v>
-      </c>
-    </row>
-    <row r="36" spans="5:6">
+        <v>-14011975</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="B36" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="1">
+        <f>22846000</f>
+        <v>22846000</v>
+      </c>
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>94025</v>
-      </c>
-    </row>
-    <row r="37" spans="5:6">
+        <v>8834025</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="B37" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" s="1">
+        <f>12734975+15933525-22846000</f>
+        <v>5822500</v>
+      </c>
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>94025</v>
-      </c>
-    </row>
-    <row r="38" spans="5:6">
+        <v>14656525</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="B38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" s="1">
+        <v>14000000</v>
+      </c>
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>94025</v>
-      </c>
-    </row>
-    <row r="39" spans="5:6">
+        <v>656525</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B39" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" s="1">
+        <f>45000+195000</f>
+        <v>240000</v>
+      </c>
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>94025</v>
-      </c>
-    </row>
-    <row r="40" spans="5:6">
+        <v>416525</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="B40" t="s">
+        <v>60</v>
+      </c>
+      <c r="D40" s="1">
+        <f>500000+788000+415000+18600000+14500000</f>
+        <v>34803000</v>
+      </c>
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>94025</v>
+        <v>-34386475</v>
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="5:6">
+    <row r="41" spans="1:6">
+      <c r="B41" t="s">
+        <v>70</v>
+      </c>
+      <c r="D41" s="1">
+        <f>2150000</f>
+        <v>2150000</v>
+      </c>
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>94025</v>
-      </c>
-    </row>
-    <row r="42" spans="5:6">
+        <v>-36536475</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="B42" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" s="1">
+        <f>18268000+13000000+7236000+10013000</f>
+        <v>48517000</v>
+      </c>
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>94025</v>
-      </c>
-    </row>
-    <row r="43" spans="5:6">
+        <v>11980525</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="B43" t="s">
+        <v>66</v>
+      </c>
+      <c r="C43" s="1">
+        <f>24668525-2162525-10013000</f>
+        <v>12493000</v>
+      </c>
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>94025</v>
-      </c>
-    </row>
-    <row r="44" spans="5:6">
+        <v>24473525</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="B44" t="s">
+        <v>63</v>
+      </c>
+      <c r="D44" s="1">
+        <v>500000</v>
+      </c>
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>94025</v>
-      </c>
-    </row>
-    <row r="45" spans="5:6">
+        <v>23973525</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="B45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C45" s="1">
+        <v>500</v>
+      </c>
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>94025</v>
-      </c>
-    </row>
-    <row r="46" spans="5:6">
+        <v>23974025</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="B46" t="s">
+        <v>68</v>
+      </c>
+      <c r="D46" s="1">
+        <v>23000000</v>
+      </c>
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>94025</v>
-      </c>
-    </row>
-    <row r="47" spans="5:6">
+        <v>974025</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="2">
+        <v>44275</v>
+      </c>
+      <c r="B47" t="s">
+        <v>25</v>
+      </c>
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>94025</v>
-      </c>
-    </row>
-    <row r="48" spans="5:6">
+        <v>974025</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>94025</v>
+        <v>974025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 24-Mar-2021, end of day.'
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="69">
   <si>
     <t>Tgl</t>
   </si>
@@ -195,6 +195,36 @@
   </si>
   <si>
     <t>GUSTAVI</t>
+  </si>
+  <si>
+    <t>TRANSFER BCA</t>
+  </si>
+  <si>
+    <t>A/R</t>
+  </si>
+  <si>
+    <t>TRANSFER DANAMON</t>
+  </si>
+  <si>
+    <t>A/P</t>
+  </si>
+  <si>
+    <t>SALES - cash/retail</t>
+  </si>
+  <si>
+    <t>BENSIN - RUSH</t>
+  </si>
+  <si>
+    <t>SELISIH - lebih</t>
+  </si>
+  <si>
+    <t>SETOR KE BANK</t>
+  </si>
+  <si>
+    <t>PRIVE - andreas</t>
+  </si>
+  <si>
+    <t>FREIGHT OUT</t>
   </si>
 </sst>
 </file>
@@ -562,8 +592,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -609,673 +639,781 @@
       <c r="B3" t="s">
         <v>25</v>
       </c>
+      <c r="D3" s="1">
+        <f>45000+240000</f>
+        <v>285000</v>
+      </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>947025</v>
+        <v>662025</v>
       </c>
     </row>
     <row r="4" spans="1:6">
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="1">
+        <f>5373000+2500000+1100000+2497500+375000+780000+75000</f>
+        <v>12700500</v>
+      </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>947025</v>
+        <v>-12038475</v>
       </c>
     </row>
     <row r="5" spans="1:6">
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="1">
+        <f>49925000+12500000+36879500</f>
+        <v>99304500</v>
+      </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>947025</v>
+        <v>87266025</v>
       </c>
     </row>
     <row r="6" spans="1:6">
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="1">
+        <f>49925000</f>
+        <v>49925000</v>
+      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>947025</v>
+        <v>37341025</v>
       </c>
     </row>
     <row r="7" spans="1:6">
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="1">
+        <v>450000</v>
+      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>947025</v>
+        <v>36891025</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="1">
+        <f>48964025-251525-36879500</f>
+        <v>11833000</v>
+      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>947025</v>
+        <v>48724025</v>
       </c>
     </row>
     <row r="9" spans="1:6">
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="1">
+        <v>250000</v>
+      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>947025</v>
+        <v>48474025</v>
       </c>
     </row>
     <row r="10" spans="1:6">
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="1">
+        <v>65000</v>
+      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>947025</v>
+        <v>48539025</v>
       </c>
     </row>
     <row r="11" spans="1:6">
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="1">
+        <v>48000000</v>
+      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>947025</v>
+        <v>539025</v>
       </c>
     </row>
     <row r="12" spans="1:6">
+      <c r="A12" s="2">
+        <v>44278</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="1">
+        <f>60000+280000</f>
+        <v>340000</v>
+      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>947025</v>
+        <v>199025</v>
       </c>
     </row>
     <row r="13" spans="1:6">
+      <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="1">
+        <f>10600000+452500+3547500+5579000+849000+263632000</f>
+        <v>284660000</v>
+      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>947025</v>
+        <v>284859025</v>
       </c>
     </row>
     <row r="14" spans="1:6">
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="1">
+        <f>2600000+1500000+184620000+1796000+5579000+849000</f>
+        <v>196944000</v>
+      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>947025</v>
+        <v>87915025</v>
       </c>
     </row>
     <row r="15" spans="1:6">
+      <c r="B15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="1">
+        <v>15000000</v>
+      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>947025</v>
+        <v>72915025</v>
       </c>
     </row>
     <row r="16" spans="1:6">
+      <c r="B16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="1">
+        <v>56000</v>
+      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>947025</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5">
+        <v>72859025</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="1">
+        <f>190492975+100522525-263632000</f>
+        <v>27383500</v>
+      </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>947025</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5">
+        <v>100242525</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="B18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="1">
+        <v>100000000</v>
+      </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>947025</v>
-      </c>
-    </row>
-    <row r="19" spans="5:5">
+        <v>242525</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="2">
+        <v>44279</v>
+      </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>947025</v>
-      </c>
-    </row>
-    <row r="20" spans="5:5">
+        <v>242525</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>947025</v>
-      </c>
-    </row>
-    <row r="21" spans="5:5">
+        <v>242525</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>947025</v>
-      </c>
-    </row>
-    <row r="22" spans="5:5">
+        <v>242525</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>947025</v>
-      </c>
-    </row>
-    <row r="23" spans="5:5">
+        <v>242525</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>947025</v>
-      </c>
-    </row>
-    <row r="24" spans="5:5">
+        <v>242525</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>947025</v>
-      </c>
-    </row>
-    <row r="25" spans="5:5">
+        <v>242525</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>947025</v>
-      </c>
-    </row>
-    <row r="26" spans="5:5">
+        <v>242525</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>947025</v>
-      </c>
-    </row>
-    <row r="27" spans="5:5">
+        <v>242525</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>947025</v>
-      </c>
-    </row>
-    <row r="28" spans="5:5">
+        <v>242525</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>947025</v>
-      </c>
-    </row>
-    <row r="29" spans="5:5">
+        <v>242525</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>947025</v>
-      </c>
-    </row>
-    <row r="30" spans="5:5">
+        <v>242525</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>947025</v>
-      </c>
-    </row>
-    <row r="31" spans="5:5">
+        <v>242525</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>947025</v>
-      </c>
-    </row>
-    <row r="32" spans="5:5">
+        <v>242525</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>947025</v>
+        <v>242525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 26-Mar-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="74">
   <si>
     <t>Tgl</t>
   </si>
@@ -225,6 +225,21 @@
   </si>
   <si>
     <t>FREIGHT OUT</t>
+  </si>
+  <si>
+    <t>PLN - Astar 214</t>
+  </si>
+  <si>
+    <t>SELISIH - kurang</t>
+  </si>
+  <si>
+    <t>Materai</t>
+  </si>
+  <si>
+    <t>BELI lampu</t>
+  </si>
+  <si>
+    <t>LPG</t>
   </si>
 </sst>
 </file>
@@ -592,8 +607,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
+      <pane ySplit="2" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -844,576 +859,704 @@
       <c r="A19" s="2">
         <v>44279</v>
       </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="1">
+        <f>60000+240000</f>
+        <v>300000</v>
+      </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>242525</v>
+        <v>-57475</v>
       </c>
     </row>
     <row r="20" spans="1:5">
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="1">
+        <f>600000+1650000</f>
+        <v>2250000</v>
+      </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>242525</v>
+        <v>-2307475</v>
       </c>
     </row>
     <row r="21" spans="1:5">
+      <c r="B21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="1">
+        <v>103000</v>
+      </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>242525</v>
+        <v>-2410475</v>
       </c>
     </row>
     <row r="22" spans="1:5">
+      <c r="B22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="1">
+        <f>2250000</f>
+        <v>2250000</v>
+      </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>242525</v>
+        <v>-160475</v>
       </c>
     </row>
     <row r="23" spans="1:5">
+      <c r="B23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="1">
+        <f>7112525+520475-2250000</f>
+        <v>5383000</v>
+      </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>242525</v>
+        <v>5222525</v>
       </c>
     </row>
     <row r="24" spans="1:5">
+      <c r="B24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="1">
+        <v>160000</v>
+      </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>242525</v>
+        <v>5062525</v>
       </c>
     </row>
     <row r="25" spans="1:5">
+      <c r="B25" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="1">
+        <v>5000000</v>
+      </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>242525</v>
+        <v>62525</v>
       </c>
     </row>
     <row r="26" spans="1:5">
+      <c r="A26" s="2">
+        <v>44280</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="1">
+        <f>60000+260000</f>
+        <v>320000</v>
+      </c>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>242525</v>
+        <v>-257475</v>
       </c>
     </row>
     <row r="27" spans="1:5">
+      <c r="B27" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="1">
+        <f>12000</f>
+        <v>12000</v>
+      </c>
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>242525</v>
+        <v>-269475</v>
       </c>
     </row>
     <row r="28" spans="1:5">
+      <c r="B28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="1">
+        <f>2396000+43000000</f>
+        <v>45396000</v>
+      </c>
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>242525</v>
+        <v>-45665475</v>
       </c>
     </row>
     <row r="29" spans="1:5">
+      <c r="B29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="1">
+        <f>43000000+26143000</f>
+        <v>69143000</v>
+      </c>
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>242525</v>
+        <v>23477525</v>
       </c>
     </row>
     <row r="30" spans="1:5">
+      <c r="B30" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="1">
+        <f>2405475+33554025-26143000</f>
+        <v>9816500</v>
+      </c>
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>242525</v>
+        <v>33294025</v>
       </c>
     </row>
     <row r="31" spans="1:5">
+      <c r="B31" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="1">
+        <v>33000000</v>
+      </c>
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>242525</v>
+        <v>294025</v>
       </c>
     </row>
     <row r="32" spans="1:5">
+      <c r="A32" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B32" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="1">
+        <f>60000</f>
+        <v>60000</v>
+      </c>
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>242525</v>
-      </c>
-    </row>
-    <row r="33" spans="5:6">
+        <v>234025</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6">
+      <c r="B33" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" s="1">
+        <f>20000</f>
+        <v>20000</v>
+      </c>
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>242525</v>
-      </c>
-    </row>
-    <row r="34" spans="5:6">
+        <v>214025</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6">
+      <c r="B34" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" s="1">
+        <f>35000</f>
+        <v>35000</v>
+      </c>
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>242525</v>
-      </c>
-    </row>
-    <row r="35" spans="5:6">
+        <v>179025</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6">
+      <c r="B35" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" s="1">
+        <f>2690000</f>
+        <v>2690000</v>
+      </c>
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>242525</v>
-      </c>
-    </row>
-    <row r="36" spans="5:6">
+        <v>-2510975</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6">
+      <c r="B36" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" s="1">
+        <f>145000</f>
+        <v>145000</v>
+      </c>
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>242525</v>
-      </c>
-    </row>
-    <row r="37" spans="5:6">
+        <v>-2655975</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>242525</v>
-      </c>
-    </row>
-    <row r="38" spans="5:6">
+        <v>-2655975</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>242525</v>
-      </c>
-    </row>
-    <row r="39" spans="5:6">
+        <v>-2655975</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>242525</v>
-      </c>
-    </row>
-    <row r="40" spans="5:6">
+        <v>-2655975</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="5:6">
+    <row r="41" spans="2:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>242525</v>
-      </c>
-    </row>
-    <row r="42" spans="5:6">
+        <v>-2655975</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>242525</v>
-      </c>
-    </row>
-    <row r="43" spans="5:6">
+        <v>-2655975</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>242525</v>
-      </c>
-    </row>
-    <row r="44" spans="5:6">
+        <v>-2655975</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>242525</v>
-      </c>
-    </row>
-    <row r="45" spans="5:6">
+        <v>-2655975</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>242525</v>
-      </c>
-    </row>
-    <row r="46" spans="5:6">
+        <v>-2655975</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>242525</v>
-      </c>
-    </row>
-    <row r="47" spans="5:6">
+        <v>-2655975</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>242525</v>
-      </c>
-    </row>
-    <row r="48" spans="5:6">
+        <v>-2655975</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>242525</v>
+        <v>-2655975</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 30-Mar-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="66">
   <si>
     <t>Tgl</t>
   </si>
@@ -206,40 +206,16 @@
     <t>TRANSFER DANAMON</t>
   </si>
   <si>
-    <t>A/P</t>
+    <t>BELI kresek</t>
   </si>
   <si>
     <t>SALES - cash/retail</t>
   </si>
   <si>
-    <t>BENSIN - RUSH</t>
-  </si>
-  <si>
-    <t>SELISIH - lebih</t>
+    <t>SELISIH - kurang</t>
   </si>
   <si>
     <t>SETOR KE BANK</t>
-  </si>
-  <si>
-    <t>PRIVE - andreas</t>
-  </si>
-  <si>
-    <t>FREIGHT OUT</t>
-  </si>
-  <si>
-    <t>PLN - Astar 214</t>
-  </si>
-  <si>
-    <t>SELISIH - kurang</t>
-  </si>
-  <si>
-    <t>Materai</t>
-  </si>
-  <si>
-    <t>BELI lampu</t>
-  </si>
-  <si>
-    <t>LPG</t>
   </si>
 </sst>
 </file>
@@ -607,8 +583,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -644,74 +620,75 @@
         <v>5</v>
       </c>
       <c r="E2" s="1">
-        <v>947025</v>
+        <v>838525</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>44277</v>
+        <v>44284</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="1">
-        <f>45000+240000</f>
-        <v>285000</v>
+        <f>60000+260000</f>
+        <v>320000</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>662025</v>
+        <v>518525</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="B4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D4" s="1">
-        <f>5373000+2500000+1100000+2497500+375000+780000+75000</f>
-        <v>12700500</v>
+        <f>54000</f>
+        <v>54000</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>-12038475</v>
+        <v>464525</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="B5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="1">
-        <f>49925000+12500000+36879500</f>
-        <v>99304500</v>
+        <v>59</v>
+      </c>
+      <c r="D5" s="1">
+        <f>1207500+19680000+577500+368500+400000</f>
+        <v>22233500</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>87266025</v>
+        <v>-21768975</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="B6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="1">
-        <f>49925000</f>
-        <v>49925000</v>
+        <v>60</v>
+      </c>
+      <c r="C6" s="1">
+        <f>45000000+6000000+29663500</f>
+        <v>80663500</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>37341025</v>
+        <v>58894525</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="B7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7" s="1">
-        <v>450000</v>
+        <f>45000000</f>
+        <v>45000000</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>36891025</v>
+        <v>13894525</v>
       </c>
       <c r="F7" s="1"/>
     </row>
@@ -720,12 +697,12 @@
         <v>63</v>
       </c>
       <c r="C8" s="1">
-        <f>48964025-251525-36879500</f>
-        <v>11833000</v>
+        <f>21643525+15508975-29663500</f>
+        <v>7489000</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>48724025</v>
+        <v>21383525</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -733,830 +710,669 @@
         <v>64</v>
       </c>
       <c r="D9" s="1">
-        <v>250000</v>
+        <v>135000</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>48474025</v>
+        <v>21248525</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="B10" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="1">
-        <v>65000</v>
+      <c r="D10" s="1">
+        <f>21000000</f>
+        <v>21000000</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>48539025</v>
+        <v>248525</v>
       </c>
     </row>
     <row r="11" spans="1:6">
+      <c r="A11" s="2">
+        <v>44285</v>
+      </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="D11" s="1">
-        <v>48000000</v>
+        <f>60000</f>
+        <v>60000</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>539025</v>
+        <v>188525</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="2">
-        <v>44278</v>
-      </c>
       <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="1">
-        <f>60000+280000</f>
-        <v>340000</v>
+        <v>60</v>
+      </c>
+      <c r="C12" s="1">
+        <f>16250000</f>
+        <v>16250000</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>199025</v>
+        <v>16438525</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="B13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="1">
-        <f>10600000+452500+3547500+5579000+849000+263632000</f>
-        <v>284660000</v>
+        <v>59</v>
+      </c>
+      <c r="D13" s="1">
+        <f>16250000+910000+1458000</f>
+        <v>18618000</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>284859025</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="B14" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="1">
-        <f>2600000+1500000+184620000+1796000+5579000+849000</f>
-        <v>196944000</v>
-      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>87915025</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="B15" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" s="1">
-        <v>15000000</v>
-      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>72915025</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="B16" t="s">
-        <v>68</v>
-      </c>
-      <c r="D16" s="1">
-        <v>56000</v>
-      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>72859025</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="B17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="1">
-        <f>190492975+100522525-263632000</f>
-        <v>27383500</v>
-      </c>
+        <v>-2179475</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5">
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>100242525</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="B18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" s="1">
-        <v>100000000</v>
-      </c>
+        <v>-2179475</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5">
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>242525</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="2">
-        <v>44279</v>
-      </c>
-      <c r="B19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="1">
-        <f>60000+240000</f>
-        <v>300000</v>
-      </c>
+        <v>-2179475</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5">
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>-57475</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="B20" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" s="1">
-        <f>600000+1650000</f>
-        <v>2250000</v>
-      </c>
+        <v>-2179475</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5">
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>-2307475</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="B21" t="s">
-        <v>69</v>
-      </c>
-      <c r="D21" s="1">
-        <v>103000</v>
-      </c>
+        <v>-2179475</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5">
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>-2410475</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="B22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" s="1">
-        <f>2250000</f>
-        <v>2250000</v>
-      </c>
+        <v>-2179475</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>-160475</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="B23" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" s="1">
-        <f>7112525+520475-2250000</f>
-        <v>5383000</v>
-      </c>
+        <v>-2179475</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>5222525</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="B24" t="s">
-        <v>70</v>
-      </c>
-      <c r="D24" s="1">
-        <v>160000</v>
-      </c>
+        <v>-2179475</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>5062525</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="B25" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25" s="1">
-        <v>5000000</v>
-      </c>
+        <v>-2179475</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>62525</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="2">
-        <v>44280</v>
-      </c>
-      <c r="B26" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" s="1">
-        <f>60000+260000</f>
-        <v>320000</v>
-      </c>
+        <v>-2179475</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>-257475</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="B27" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27" s="1">
-        <f>12000</f>
-        <v>12000</v>
-      </c>
+        <v>-2179475</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>-269475</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="B28" t="s">
-        <v>59</v>
-      </c>
-      <c r="D28" s="1">
-        <f>2396000+43000000</f>
-        <v>45396000</v>
-      </c>
+        <v>-2179475</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>-45665475</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="B29" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" s="1">
-        <f>43000000+26143000</f>
-        <v>69143000</v>
-      </c>
+        <v>-2179475</v>
+      </c>
+    </row>
+    <row r="29" spans="5:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>23477525</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="B30" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" s="1">
-        <f>2405475+33554025-26143000</f>
-        <v>9816500</v>
-      </c>
+        <v>-2179475</v>
+      </c>
+    </row>
+    <row r="30" spans="5:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>33294025</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="B31" t="s">
-        <v>66</v>
-      </c>
-      <c r="D31" s="1">
-        <v>33000000</v>
-      </c>
+        <v>-2179475</v>
+      </c>
+    </row>
+    <row r="31" spans="5:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>294025</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="2">
-        <v>44281</v>
-      </c>
-      <c r="B32" t="s">
-        <v>25</v>
-      </c>
-      <c r="D32" s="1">
-        <f>60000</f>
-        <v>60000</v>
-      </c>
+        <v>-2179475</v>
+      </c>
+    </row>
+    <row r="32" spans="5:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>234025</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6">
-      <c r="B33" t="s">
-        <v>71</v>
-      </c>
-      <c r="D33" s="1">
-        <f>20000</f>
-        <v>20000</v>
-      </c>
+        <v>-2179475</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>214025</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6">
-      <c r="B34" t="s">
-        <v>72</v>
-      </c>
-      <c r="D34" s="1">
-        <f>35000</f>
-        <v>35000</v>
-      </c>
+        <v>-2179475</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>179025</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6">
-      <c r="B35" t="s">
-        <v>59</v>
-      </c>
-      <c r="D35" s="1">
-        <f>2690000</f>
-        <v>2690000</v>
-      </c>
+        <v>-2179475</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>-2510975</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6">
-      <c r="B36" t="s">
-        <v>73</v>
-      </c>
-      <c r="D36" s="1">
-        <f>145000</f>
-        <v>145000</v>
-      </c>
+        <v>-2179475</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>-2655975</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6">
+        <v>-2179475</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>-2655975</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6">
+        <v>-2179475</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>-2655975</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6">
+        <v>-2179475</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>-2655975</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6">
+        <v>-2179475</v>
+      </c>
+    </row>
+    <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="2:6">
+    <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>-2655975</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6">
+        <v>-2179475</v>
+      </c>
+    </row>
+    <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>-2655975</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6">
+        <v>-2179475</v>
+      </c>
+    </row>
+    <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>-2655975</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6">
+        <v>-2179475</v>
+      </c>
+    </row>
+    <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>-2655975</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6">
+        <v>-2179475</v>
+      </c>
+    </row>
+    <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>-2655975</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6">
+        <v>-2179475</v>
+      </c>
+    </row>
+    <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>-2655975</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6">
+        <v>-2179475</v>
+      </c>
+    </row>
+    <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>-2655975</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6">
+        <v>-2179475</v>
+      </c>
+    </row>
+    <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>-2655975</v>
+        <v>-2179475</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 31-Mar-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="67">
   <si>
     <t>Tgl</t>
   </si>
@@ -216,6 +216,9 @@
   </si>
   <si>
     <t>SETOR KE BANK</t>
+  </si>
+  <si>
+    <t>SELISIH - lebih</t>
   </si>
 </sst>
 </file>
@@ -583,8 +586,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <pane ySplit="2" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -738,12 +741,12 @@
         <v>25</v>
       </c>
       <c r="D11" s="1">
-        <f>60000</f>
-        <v>60000</v>
+        <f>60000+260000</f>
+        <v>320000</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>188525</v>
+        <v>-71475</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -751,12 +754,12 @@
         <v>60</v>
       </c>
       <c r="C12" s="1">
-        <f>16250000</f>
-        <v>16250000</v>
+        <f>16250000+680000+9516000</f>
+        <v>26446000</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>16438525</v>
+        <v>26374525</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -764,615 +767,658 @@
         <v>59</v>
       </c>
       <c r="D13" s="1">
-        <f>16250000+910000+1458000</f>
-        <v>18618000</v>
+        <f>16250000+910000+1458000+560000+516000+450000</f>
+        <v>20144000</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>-2179475</v>
+        <v>6230525</v>
       </c>
     </row>
     <row r="14" spans="1:6">
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="1">
+        <f>14496525+3025475-9516000</f>
+        <v>8006000</v>
+      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>-2179475</v>
+        <v>14236525</v>
       </c>
     </row>
     <row r="15" spans="1:6">
+      <c r="B15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="1">
+        <v>5000</v>
+      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>-2179475</v>
+        <v>14241525</v>
       </c>
     </row>
     <row r="16" spans="1:6">
+      <c r="B16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="1">
+        <v>14000000</v>
+      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>-2179475</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5">
+        <v>241525</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2">
+        <v>44286</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="1">
+        <f>60000</f>
+        <v>60000</v>
+      </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>-2179475</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5">
+        <v>181525</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="1">
+        <f>100000000</f>
+        <v>100000000</v>
+      </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>-2179475</v>
-      </c>
-    </row>
-    <row r="19" spans="5:5">
+        <v>100181525</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="1">
+        <f>100000000+2150000</f>
+        <v>102150000</v>
+      </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>-2179475</v>
-      </c>
-    </row>
-    <row r="20" spans="5:5">
+        <v>-1968475</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>-2179475</v>
-      </c>
-    </row>
-    <row r="21" spans="5:5">
+        <v>-1968475</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>-2179475</v>
-      </c>
-    </row>
-    <row r="22" spans="5:5">
+        <v>-1968475</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>-2179475</v>
-      </c>
-    </row>
-    <row r="23" spans="5:5">
+        <v>-1968475</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>-2179475</v>
-      </c>
-    </row>
-    <row r="24" spans="5:5">
+        <v>-1968475</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>-2179475</v>
-      </c>
-    </row>
-    <row r="25" spans="5:5">
+        <v>-1968475</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>-2179475</v>
-      </c>
-    </row>
-    <row r="26" spans="5:5">
+        <v>-1968475</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>-2179475</v>
-      </c>
-    </row>
-    <row r="27" spans="5:5">
+        <v>-1968475</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>-2179475</v>
-      </c>
-    </row>
-    <row r="28" spans="5:5">
+        <v>-1968475</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>-2179475</v>
-      </c>
-    </row>
-    <row r="29" spans="5:5">
+        <v>-1968475</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>-2179475</v>
-      </c>
-    </row>
-    <row r="30" spans="5:5">
+        <v>-1968475</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>-2179475</v>
-      </c>
-    </row>
-    <row r="31" spans="5:5">
+        <v>-1968475</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>-2179475</v>
-      </c>
-    </row>
-    <row r="32" spans="5:5">
+        <v>-1968475</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>-2179475</v>
+        <v>-1968475</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 1-Apr-2021, end of day.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="69">
   <si>
     <t>Tgl</t>
   </si>
@@ -219,6 +219,12 @@
   </si>
   <si>
     <t>SELISIH - lebih</t>
+  </si>
+  <si>
+    <t>PRIVE - andreas</t>
+  </si>
+  <si>
+    <t>PRIVE - bulanan</t>
   </si>
 </sst>
 </file>
@@ -586,8 +592,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -820,12 +826,12 @@
         <v>25</v>
       </c>
       <c r="D17" s="1">
-        <f>60000</f>
-        <v>60000</v>
+        <f>60000+7010000</f>
+        <v>7070000</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>181525</v>
+        <v>-6828475</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -833,12 +839,12 @@
         <v>60</v>
       </c>
       <c r="C18" s="1">
-        <f>100000000</f>
-        <v>100000000</v>
+        <f>100000000+18000000+38573000</f>
+        <v>156573000</v>
       </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>100181525</v>
+        <v>149744525</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -846,579 +852,613 @@
         <v>59</v>
       </c>
       <c r="D19" s="1">
-        <f>100000000+2150000</f>
-        <v>102150000</v>
+        <f>100000000+2150000+28384000+609000</f>
+        <v>131143000</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>-1968475</v>
+        <v>18601525</v>
       </c>
     </row>
     <row r="20" spans="1:5">
+      <c r="B20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="1">
+        <f>12961475+31166525-38573000</f>
+        <v>5555000</v>
+      </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>-1968475</v>
+        <v>24156525</v>
       </c>
     </row>
     <row r="21" spans="1:5">
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="1">
+        <v>2000000</v>
+      </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>-1968475</v>
+        <v>22156525</v>
       </c>
     </row>
     <row r="22" spans="1:5">
+      <c r="B22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="1">
+        <v>425000</v>
+      </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>-1968475</v>
+        <v>22581525</v>
       </c>
     </row>
     <row r="23" spans="1:5">
+      <c r="B23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="1">
+        <v>16000000</v>
+      </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>-1968475</v>
+        <v>6581525</v>
       </c>
     </row>
     <row r="24" spans="1:5">
+      <c r="B24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="1">
+        <v>6000000</v>
+      </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="25" spans="1:5">
+      <c r="A25" s="2">
+        <v>44287</v>
+      </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>-1968475</v>
+        <v>581525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 4-Apr-2021, end of day update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>Tgl</t>
   </si>
@@ -195,36 +195,6 @@
   </si>
   <si>
     <t>GUSTAVI</t>
-  </si>
-  <si>
-    <t>TRANSFER BCA</t>
-  </si>
-  <si>
-    <t>A/R</t>
-  </si>
-  <si>
-    <t>TRANSFER DANAMON</t>
-  </si>
-  <si>
-    <t>BELI kresek</t>
-  </si>
-  <si>
-    <t>SALES - cash/retail</t>
-  </si>
-  <si>
-    <t>SELISIH - kurang</t>
-  </si>
-  <si>
-    <t>SETOR KE BANK</t>
-  </si>
-  <si>
-    <t>SELISIH - lebih</t>
-  </si>
-  <si>
-    <t>PRIVE - andreas</t>
-  </si>
-  <si>
-    <t>PRIVE - bulanan</t>
   </si>
 </sst>
 </file>
@@ -592,8 +562,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -629,836 +599,683 @@
         <v>5</v>
       </c>
       <c r="E2" s="1">
-        <v>838525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>44284</v>
+        <v>44291</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="1">
-        <f>60000+260000</f>
-        <v>320000</v>
-      </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>518525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="B4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" s="1">
-        <f>54000</f>
-        <v>54000</v>
-      </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>464525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="B5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="1">
-        <f>1207500+19680000+577500+368500+400000</f>
-        <v>22233500</v>
-      </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>-21768975</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="B6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" s="1">
-        <f>45000000+6000000+29663500</f>
-        <v>80663500</v>
-      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>58894525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="B7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" s="1">
-        <f>45000000</f>
-        <v>45000000</v>
-      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>13894525</v>
+        <v>864025</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="B8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="1">
-        <f>21643525+15508975-29663500</f>
-        <v>7489000</v>
-      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>21383525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="B9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="1">
-        <v>135000</v>
-      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>21248525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="B10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="1">
-        <f>21000000</f>
-        <v>21000000</v>
-      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>248525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="2">
-        <v>44285</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="1">
-        <f>60000+260000</f>
-        <v>320000</v>
-      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>-71475</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="B12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="1">
-        <f>16250000+680000+9516000</f>
-        <v>26446000</v>
-      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>26374525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="1">
-        <f>16250000+910000+1458000+560000+516000+450000</f>
-        <v>20144000</v>
-      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>6230525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="B14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="1">
-        <f>14496525+3025475-9516000</f>
-        <v>8006000</v>
-      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>14236525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="B15" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" s="1">
-        <v>5000</v>
-      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>14241525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="B16" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="1">
-        <v>14000000</v>
-      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>241525</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="2">
-        <v>44286</v>
-      </c>
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="1">
-        <f>60000+7010000</f>
-        <v>7070000</v>
-      </c>
+        <v>864025</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5">
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>-6828475</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="B18" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="1">
-        <f>100000000+18000000+38573000</f>
-        <v>156573000</v>
-      </c>
+        <v>864025</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5">
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>149744525</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="B19" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" s="1">
-        <f>100000000+2150000+28384000+609000</f>
-        <v>131143000</v>
-      </c>
+        <v>864025</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5">
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>18601525</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="B20" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="1">
-        <f>12961475+31166525-38573000</f>
-        <v>5555000</v>
-      </c>
+        <v>864025</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5">
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>24156525</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="B21" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" s="1">
-        <v>2000000</v>
-      </c>
+        <v>864025</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5">
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>22156525</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="B22" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" s="1">
-        <v>425000</v>
-      </c>
+        <v>864025</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>22581525</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="B23" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" s="1">
-        <v>16000000</v>
-      </c>
+        <v>864025</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>6581525</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="B24" t="s">
-        <v>65</v>
-      </c>
-      <c r="D24" s="1">
-        <v>6000000</v>
-      </c>
+        <v>864025</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>581525</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="2">
-        <v>44287</v>
-      </c>
+        <v>864025</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>581525</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+        <v>864025</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>581525</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>864025</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>581525</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>864025</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>581525</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+        <v>864025</v>
+      </c>
+    </row>
+    <row r="29" spans="5:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>581525</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+        <v>864025</v>
+      </c>
+    </row>
+    <row r="30" spans="5:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>581525</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>864025</v>
+      </c>
+    </row>
+    <row r="31" spans="5:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>581525</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+        <v>864025</v>
+      </c>
+    </row>
+    <row r="32" spans="5:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>581525</v>
+        <v>864025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 7-Apr-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="75">
   <si>
     <t>Tgl</t>
   </si>
@@ -195,6 +195,54 @@
   </si>
   <si>
     <t>GUSTAVI</t>
+  </si>
+  <si>
+    <t>A/P</t>
+  </si>
+  <si>
+    <t>A/R</t>
+  </si>
+  <si>
+    <t>TRANSFER BCA</t>
+  </si>
+  <si>
+    <t>TAX - P.Tata</t>
+  </si>
+  <si>
+    <t>CHEQUE RECEIVED</t>
+  </si>
+  <si>
+    <t>TAX - Iuran ARIESTA</t>
+  </si>
+  <si>
+    <t>TAX - SPT 2020 Andreas</t>
+  </si>
+  <si>
+    <t>TAX - SPT 2020 Juntas</t>
+  </si>
+  <si>
+    <t>IURAN DAERAH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FREIGHT OUT </t>
+  </si>
+  <si>
+    <t>PPh 21 - bonus bibit</t>
+  </si>
+  <si>
+    <t>SALES - cash/retail</t>
+  </si>
+  <si>
+    <t>SOLAR - kijang D-1682-QU</t>
+  </si>
+  <si>
+    <t>SELISIH - lebih</t>
+  </si>
+  <si>
+    <t>SETOR KE BANK</t>
+  </si>
+  <si>
+    <t>BELI kresek</t>
   </si>
 </sst>
 </file>
@@ -562,8 +610,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -609,673 +657,800 @@
       <c r="B3" t="s">
         <v>25</v>
       </c>
+      <c r="D3" s="1">
+        <f>60000+200000+260000</f>
+        <v>520000</v>
+      </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>864025</v>
+        <v>344025</v>
       </c>
     </row>
     <row r="4" spans="1:6">
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="1">
+        <f>1877000+1374000</f>
+        <v>3251000</v>
+      </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>864025</v>
+        <v>-2906975</v>
       </c>
     </row>
     <row r="5" spans="1:6">
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="1">
+        <f>18043000+1957000+85500000+20266000+8820000+47760000+13213500</f>
+        <v>195559500</v>
+      </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>864025</v>
+        <v>192652525</v>
       </c>
     </row>
     <row r="6" spans="1:6">
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="1">
+        <f>85500000+20266000+8820000+600000+47760000+2682000+885000+1192500</f>
+        <v>167705500</v>
+      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>864025</v>
+        <v>24947025</v>
       </c>
     </row>
     <row r="7" spans="1:6">
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="1">
+        <f>400000</f>
+        <v>400000</v>
+      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>864025</v>
+        <v>24547025</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="1">
+        <f>5430000</f>
+        <v>5430000</v>
+      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>864025</v>
+        <v>19117025</v>
       </c>
     </row>
     <row r="9" spans="1:6">
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="1">
+        <v>660000</v>
+      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>864025</v>
+        <v>18457025</v>
       </c>
     </row>
     <row r="10" spans="1:6">
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="1">
+        <f>3250000</f>
+        <v>3250000</v>
+      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>864025</v>
+        <v>15207025</v>
       </c>
     </row>
     <row r="11" spans="1:6">
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="1">
+        <f>4750000</f>
+        <v>4750000</v>
+      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>864025</v>
+        <v>10457025</v>
       </c>
     </row>
     <row r="12" spans="1:6">
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="1">
+        <f>25000</f>
+        <v>25000</v>
+      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>864025</v>
+        <v>10432025</v>
       </c>
     </row>
     <row r="13" spans="1:6">
+      <c r="B13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="1">
+        <f>150000</f>
+        <v>150000</v>
+      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>864025</v>
+        <v>10282025</v>
       </c>
     </row>
     <row r="14" spans="1:6">
+      <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="1">
+        <v>35000</v>
+      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>864025</v>
+        <v>10247025</v>
       </c>
     </row>
     <row r="15" spans="1:6">
+      <c r="B15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="1">
+        <f>2706475+20844025-13213500</f>
+        <v>10337000</v>
+      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>864025</v>
+        <v>20584025</v>
       </c>
     </row>
     <row r="16" spans="1:6">
+      <c r="B16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="1">
+        <v>300000</v>
+      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>864025</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5">
+        <v>20284025</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="B17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="1">
+        <v>85000</v>
+      </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>864025</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5">
+        <v>20369025</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="B18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="1">
+        <v>20000000</v>
+      </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>864025</v>
-      </c>
-    </row>
-    <row r="19" spans="5:5">
+        <v>369025</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="2">
+        <v>44292</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="1">
+        <f>60000</f>
+        <v>60000</v>
+      </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>864025</v>
-      </c>
-    </row>
-    <row r="20" spans="5:5">
+        <v>309025</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="B20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="1">
+        <v>146500</v>
+      </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>864025</v>
-      </c>
-    </row>
-    <row r="21" spans="5:5">
+        <v>162525</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="B21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="1">
+        <f>504000</f>
+        <v>504000</v>
+      </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>864025</v>
-      </c>
-    </row>
-    <row r="22" spans="5:5">
+        <v>-341475</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>864025</v>
-      </c>
-    </row>
-    <row r="23" spans="5:5">
+        <v>-341475</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>864025</v>
-      </c>
-    </row>
-    <row r="24" spans="5:5">
+        <v>-341475</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>864025</v>
-      </c>
-    </row>
-    <row r="25" spans="5:5">
+        <v>-341475</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>864025</v>
-      </c>
-    </row>
-    <row r="26" spans="5:5">
+        <v>-341475</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>864025</v>
-      </c>
-    </row>
-    <row r="27" spans="5:5">
+        <v>-341475</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>864025</v>
-      </c>
-    </row>
-    <row r="28" spans="5:5">
+        <v>-341475</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>864025</v>
-      </c>
-    </row>
-    <row r="29" spans="5:5">
+        <v>-341475</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>864025</v>
-      </c>
-    </row>
-    <row r="30" spans="5:5">
+        <v>-341475</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>864025</v>
-      </c>
-    </row>
-    <row r="31" spans="5:5">
+        <v>-341475</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>864025</v>
-      </c>
-    </row>
-    <row r="32" spans="5:5">
+        <v>-341475</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>864025</v>
+        <v>-341475</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 8 Apr 2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="75">
   <si>
     <t>Tgl</t>
   </si>
@@ -611,7 +611,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
+      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -865,12 +865,12 @@
         <v>25</v>
       </c>
       <c r="D19" s="1">
-        <f>60000</f>
-        <v>60000</v>
+        <f>60000+260000</f>
+        <v>320000</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>309025</v>
+        <v>49025</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -882,7 +882,7 @@
       </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>162525</v>
+        <v>-97475</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -890,567 +890,641 @@
         <v>61</v>
       </c>
       <c r="D21" s="1">
-        <f>504000</f>
-        <v>504000</v>
+        <f>504000+1057500+750000+3040000+40000000+35111000+11215000+3324000+2600000</f>
+        <v>97601500</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>-341475</v>
+        <v>-97698975</v>
       </c>
     </row>
     <row r="22" spans="1:5">
+      <c r="B22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="1">
+        <f>40000000+855000+11215000+2600000+46251500</f>
+        <v>100921500</v>
+      </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>-341475</v>
+        <v>3222525</v>
       </c>
     </row>
     <row r="23" spans="1:5">
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="1">
+        <f>11216525+42768975-46251500</f>
+        <v>7734000</v>
+      </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>-341475</v>
+        <v>10956525</v>
       </c>
     </row>
     <row r="24" spans="1:5">
+      <c r="B24" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="1">
+        <v>30000</v>
+      </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>-341475</v>
+        <v>10986525</v>
       </c>
     </row>
     <row r="25" spans="1:5">
+      <c r="B25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="1">
+        <v>10000000</v>
+      </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>-341475</v>
+        <v>986525</v>
       </c>
     </row>
     <row r="26" spans="1:5">
+      <c r="A26" s="2">
+        <v>44293</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="1">
+        <f>60000+240000</f>
+        <v>300000</v>
+      </c>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>-341475</v>
+        <v>686525</v>
       </c>
     </row>
     <row r="27" spans="1:5">
+      <c r="B27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="1">
+        <f>300000+13000000+8311000</f>
+        <v>21611000</v>
+      </c>
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>-341475</v>
+        <v>-20924475</v>
       </c>
     </row>
     <row r="28" spans="1:5">
+      <c r="B28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="1">
+        <f>13000000+8751000</f>
+        <v>21751000</v>
+      </c>
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>-341475</v>
+        <v>826525</v>
       </c>
     </row>
     <row r="29" spans="1:5">
+      <c r="B29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="1">
+        <f>478000</f>
+        <v>478000</v>
+      </c>
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>-341475</v>
+        <v>348525</v>
       </c>
     </row>
     <row r="30" spans="1:5">
+      <c r="B30" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" s="1">
+        <f>8162475+4973525-8751000</f>
+        <v>4385000</v>
+      </c>
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>-341475</v>
+        <v>4733525</v>
       </c>
     </row>
     <row r="31" spans="1:5">
+      <c r="B31" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31" s="1">
+        <f>4000000</f>
+        <v>4000000</v>
+      </c>
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="32" spans="1:5">
+      <c r="A32" s="2">
+        <v>44294</v>
+      </c>
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>-341475</v>
+        <v>733525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 12-Apr-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>Tgl</t>
   </si>
@@ -195,54 +195,6 @@
   </si>
   <si>
     <t>GUSTAVI</t>
-  </si>
-  <si>
-    <t>A/P</t>
-  </si>
-  <si>
-    <t>A/R</t>
-  </si>
-  <si>
-    <t>TRANSFER BCA</t>
-  </si>
-  <si>
-    <t>TAX - P.Tata</t>
-  </si>
-  <si>
-    <t>CHEQUE RECEIVED</t>
-  </si>
-  <si>
-    <t>TAX - Iuran ARIESTA</t>
-  </si>
-  <si>
-    <t>TAX - SPT 2020 Andreas</t>
-  </si>
-  <si>
-    <t>TAX - SPT 2020 Juntas</t>
-  </si>
-  <si>
-    <t>IURAN DAERAH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FREIGHT OUT </t>
-  </si>
-  <si>
-    <t>PPh 21 - bonus bibit</t>
-  </si>
-  <si>
-    <t>SALES - cash/retail</t>
-  </si>
-  <si>
-    <t>SOLAR - kijang D-1682-QU</t>
-  </si>
-  <si>
-    <t>SELISIH - lebih</t>
-  </si>
-  <si>
-    <t>SETOR KE BANK</t>
-  </si>
-  <si>
-    <t>BELI kresek</t>
   </si>
 </sst>
 </file>
@@ -610,8 +562,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -647,884 +599,683 @@
         <v>5</v>
       </c>
       <c r="E2" s="1">
-        <v>864025</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>44291</v>
+        <v>44298</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="1">
-        <f>60000+200000+260000</f>
-        <v>520000</v>
-      </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>344025</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="B4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="1">
-        <f>1877000+1374000</f>
-        <v>3251000</v>
-      </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>-2906975</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="B5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="1">
-        <f>18043000+1957000+85500000+20266000+8820000+47760000+13213500</f>
-        <v>195559500</v>
-      </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>192652525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="1">
-        <f>85500000+20266000+8820000+600000+47760000+2682000+885000+1192500</f>
-        <v>167705500</v>
-      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>24947025</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="B7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="1">
-        <f>400000</f>
-        <v>400000</v>
-      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>24547025</v>
+        <v>152525</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="B8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" s="1">
-        <f>5430000</f>
-        <v>5430000</v>
-      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>19117025</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="B9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="1">
-        <v>660000</v>
-      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>18457025</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="B10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="1">
-        <f>3250000</f>
-        <v>3250000</v>
-      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>15207025</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="B11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="1">
-        <f>4750000</f>
-        <v>4750000</v>
-      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>10457025</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="B12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="1">
-        <f>25000</f>
-        <v>25000</v>
-      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>10432025</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" s="1">
-        <f>150000</f>
-        <v>150000</v>
-      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>10282025</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="B14" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14" s="1">
-        <v>35000</v>
-      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>10247025</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="B15" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15" s="1">
-        <f>2706475+20844025-13213500</f>
-        <v>10337000</v>
-      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>20584025</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="B16" t="s">
-        <v>71</v>
-      </c>
-      <c r="D16" s="1">
-        <v>300000</v>
-      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>20284025</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="B17" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" s="1">
-        <v>85000</v>
-      </c>
+        <v>152525</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5">
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>20369025</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="B18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D18" s="1">
-        <v>20000000</v>
-      </c>
+        <v>152525</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5">
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>369025</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="2">
-        <v>44292</v>
-      </c>
-      <c r="B19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="1">
-        <f>60000+260000</f>
-        <v>320000</v>
-      </c>
+        <v>152525</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5">
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>49025</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="B20" t="s">
-        <v>74</v>
-      </c>
-      <c r="D20" s="1">
-        <v>146500</v>
-      </c>
+        <v>152525</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5">
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>-97475</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="B21" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21" s="1">
-        <f>504000+1057500+750000+3040000+40000000+35111000+11215000+3324000+2600000</f>
-        <v>97601500</v>
-      </c>
+        <v>152525</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5">
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>-97698975</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="B22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" s="1">
-        <f>40000000+855000+11215000+2600000+46251500</f>
-        <v>100921500</v>
-      </c>
+        <v>152525</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>3222525</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="B23" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="1">
-        <f>11216525+42768975-46251500</f>
-        <v>7734000</v>
-      </c>
+        <v>152525</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>10956525</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="B24" t="s">
-        <v>72</v>
-      </c>
-      <c r="C24" s="1">
-        <v>30000</v>
-      </c>
+        <v>152525</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>10986525</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="B25" t="s">
-        <v>73</v>
-      </c>
-      <c r="D25" s="1">
-        <v>10000000</v>
-      </c>
+        <v>152525</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>986525</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="2">
-        <v>44293</v>
-      </c>
-      <c r="B26" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" s="1">
-        <f>60000+240000</f>
-        <v>300000</v>
-      </c>
+        <v>152525</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>686525</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="B27" t="s">
-        <v>61</v>
-      </c>
-      <c r="D27" s="1">
-        <f>300000+13000000+8311000</f>
-        <v>21611000</v>
-      </c>
+        <v>152525</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>-20924475</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="B28" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="1">
-        <f>13000000+8751000</f>
-        <v>21751000</v>
-      </c>
+        <v>152525</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>826525</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="B29" t="s">
-        <v>59</v>
-      </c>
-      <c r="D29" s="1">
-        <f>478000</f>
-        <v>478000</v>
-      </c>
+        <v>152525</v>
+      </c>
+    </row>
+    <row r="29" spans="5:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>348525</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="B30" t="s">
-        <v>70</v>
-      </c>
-      <c r="C30" s="1">
-        <f>8162475+4973525-8751000</f>
-        <v>4385000</v>
-      </c>
+        <v>152525</v>
+      </c>
+    </row>
+    <row r="30" spans="5:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>4733525</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="B31" t="s">
-        <v>73</v>
-      </c>
-      <c r="D31" s="1">
-        <f>4000000</f>
-        <v>4000000</v>
-      </c>
+        <v>152525</v>
+      </c>
+    </row>
+    <row r="31" spans="5:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>733525</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="2">
-        <v>44294</v>
-      </c>
+        <v>152525</v>
+      </c>
+    </row>
+    <row r="32" spans="5:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>733525</v>
+        <v>152525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 15-Apr-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="68">
   <si>
     <t>Tgl</t>
   </si>
@@ -195,6 +195,33 @@
   </si>
   <si>
     <t>GUSTAVI</t>
+  </si>
+  <si>
+    <t>TRANSFER BCA</t>
+  </si>
+  <si>
+    <t>A/R</t>
+  </si>
+  <si>
+    <t>SALES - cash/retail</t>
+  </si>
+  <si>
+    <t>SELISIH - lebih</t>
+  </si>
+  <si>
+    <t>SETOR KE BANK</t>
+  </si>
+  <si>
+    <t>KELEBIHAN setoran ke bank</t>
+  </si>
+  <si>
+    <t>PAPA - beli obat</t>
+  </si>
+  <si>
+    <t>JASON - les</t>
+  </si>
+  <si>
+    <t>SELISIH - kurang</t>
   </si>
 </sst>
 </file>
@@ -562,8 +589,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <pane ySplit="2" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -609,673 +636,778 @@
       <c r="B3" t="s">
         <v>25</v>
       </c>
+      <c r="D3" s="1">
+        <f>60000+240000</f>
+        <v>300000</v>
+      </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>152525</v>
+        <v>-147475</v>
       </c>
     </row>
     <row r="4" spans="1:6">
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="1">
+        <f>2340000+1600000+360000+900000+1900000</f>
+        <v>7100000</v>
+      </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>152525</v>
+        <v>-7247475</v>
       </c>
     </row>
     <row r="5" spans="1:6">
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="1">
+        <f>360000+900000+4372000</f>
+        <v>5632000</v>
+      </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>152525</v>
+        <v>-1615475</v>
       </c>
     </row>
     <row r="6" spans="1:6">
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="1">
+        <f>3150525+5747475-4372000</f>
+        <v>4526000</v>
+      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>152525</v>
+        <v>2910525</v>
       </c>
     </row>
     <row r="7" spans="1:6">
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="1">
+        <f>247000</f>
+        <v>247000</v>
+      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>152525</v>
+        <v>3157525</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3000000</v>
+      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>152525</v>
+        <v>157525</v>
       </c>
     </row>
     <row r="9" spans="1:6">
+      <c r="A9" s="2">
+        <v>44299</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="1">
+        <f>60000+240000</f>
+        <v>300000</v>
+      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>152525</v>
+        <v>-142475</v>
       </c>
     </row>
     <row r="10" spans="1:6">
+      <c r="B10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="1">
+        <f>947500+2595000+3560000</f>
+        <v>7102500</v>
+      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>152525</v>
+        <v>-7244975</v>
       </c>
     </row>
     <row r="11" spans="1:6">
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="1">
+        <v>100000</v>
+      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>152525</v>
+        <v>-7144975</v>
       </c>
     </row>
     <row r="12" spans="1:6">
+      <c r="B12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="1">
+        <f>350000</f>
+        <v>350000</v>
+      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>152525</v>
+        <v>-7494975</v>
       </c>
     </row>
     <row r="13" spans="1:6">
+      <c r="B13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="1">
+        <f>600000</f>
+        <v>600000</v>
+      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>152525</v>
+        <v>-8094975</v>
       </c>
     </row>
     <row r="14" spans="1:6">
+      <c r="B14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="1">
+        <f>7002025+8094975-10339500</f>
+        <v>4757500</v>
+      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>152525</v>
+        <v>-3337475</v>
       </c>
     </row>
     <row r="15" spans="1:6">
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="1">
+        <f>10339500</f>
+        <v>10339500</v>
+      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>152525</v>
+        <v>7002025</v>
       </c>
     </row>
     <row r="16" spans="1:6">
+      <c r="B16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="1">
+        <v>5000</v>
+      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>152525</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5">
+        <v>6997025</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="1">
+        <f>6000000</f>
+        <v>6000000</v>
+      </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>152525</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5">
+        <v>997025</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="2">
+        <v>44300</v>
+      </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>152525</v>
-      </c>
-    </row>
-    <row r="19" spans="5:5">
+        <v>997025</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>152525</v>
-      </c>
-    </row>
-    <row r="20" spans="5:5">
+        <v>997025</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>152525</v>
-      </c>
-    </row>
-    <row r="21" spans="5:5">
+        <v>997025</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>152525</v>
-      </c>
-    </row>
-    <row r="22" spans="5:5">
+        <v>997025</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>152525</v>
-      </c>
-    </row>
-    <row r="23" spans="5:5">
+        <v>997025</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>152525</v>
-      </c>
-    </row>
-    <row r="24" spans="5:5">
+        <v>997025</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>152525</v>
-      </c>
-    </row>
-    <row r="25" spans="5:5">
+        <v>997025</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>152525</v>
-      </c>
-    </row>
-    <row r="26" spans="5:5">
+        <v>997025</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>152525</v>
-      </c>
-    </row>
-    <row r="27" spans="5:5">
+        <v>997025</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>152525</v>
-      </c>
-    </row>
-    <row r="28" spans="5:5">
+        <v>997025</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>152525</v>
-      </c>
-    </row>
-    <row r="29" spans="5:5">
+        <v>997025</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>152525</v>
-      </c>
-    </row>
-    <row r="30" spans="5:5">
+        <v>997025</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>152525</v>
-      </c>
-    </row>
-    <row r="31" spans="5:5">
+        <v>997025</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>152525</v>
-      </c>
-    </row>
-    <row r="32" spans="5:5">
+        <v>997025</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>152525</v>
+        <v>997025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 16-Apr-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="73">
   <si>
     <t>Tgl</t>
   </si>
@@ -222,6 +222,21 @@
   </si>
   <si>
     <t>SELISIH - kurang</t>
+  </si>
+  <si>
+    <t>BELI lampu</t>
+  </si>
+  <si>
+    <t>FREIGHT OUT</t>
+  </si>
+  <si>
+    <t>TELPON - 5224823</t>
+  </si>
+  <si>
+    <t>PLN - Astar 165</t>
+  </si>
+  <si>
+    <t>PLN - Astar 214</t>
   </si>
 </sst>
 </file>
@@ -589,8 +604,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <pane ySplit="2" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -832,582 +847,727 @@
       <c r="A18" s="2">
         <v>44300</v>
       </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="1">
+        <f>60000+260000</f>
+        <v>320000</v>
+      </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>997025</v>
+        <v>677025</v>
       </c>
     </row>
     <row r="19" spans="1:5">
+      <c r="B19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="1">
+        <f>1170000+3615000+6235000+6777500</f>
+        <v>17797500</v>
+      </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>997025</v>
+        <v>18474525</v>
       </c>
     </row>
     <row r="20" spans="1:5">
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="1">
+        <f>1170000+3615000+140000+480500</f>
+        <v>5405500</v>
+      </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>997025</v>
+        <v>13069025</v>
       </c>
     </row>
     <row r="21" spans="1:5">
+      <c r="B21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="1">
+        <v>105000</v>
+      </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>997025</v>
+        <v>12964025</v>
       </c>
     </row>
     <row r="22" spans="1:5">
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="1">
+        <f>21068025-6446525-6777500</f>
+        <v>7844000</v>
+      </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>997025</v>
+        <v>20808025</v>
       </c>
     </row>
     <row r="23" spans="1:5">
+      <c r="B23" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="1">
+        <f>150000</f>
+        <v>150000</v>
+      </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>997025</v>
+        <v>20658025</v>
       </c>
     </row>
     <row r="24" spans="1:5">
+      <c r="B24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="1">
+        <v>10000</v>
+      </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>997025</v>
+        <v>20668025</v>
       </c>
     </row>
     <row r="25" spans="1:5">
+      <c r="B25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="1">
+        <v>20000000</v>
+      </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>997025</v>
+        <v>668025</v>
       </c>
     </row>
     <row r="26" spans="1:5">
+      <c r="A26" s="2">
+        <v>44301</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="1">
+        <f>60000+280000</f>
+        <v>340000</v>
+      </c>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>997025</v>
+        <v>328025</v>
       </c>
     </row>
     <row r="27" spans="1:5">
+      <c r="B27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="1">
+        <f>13015000+448000+300000000+4800000+17000000+31001000+5400000</f>
+        <v>371664000</v>
+      </c>
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>997025</v>
+        <v>-371335975</v>
       </c>
     </row>
     <row r="28" spans="1:5">
+      <c r="B28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="1">
+        <f>300000000+31001000+42923000</f>
+        <v>373924000</v>
+      </c>
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>997025</v>
+        <v>2588025</v>
       </c>
     </row>
     <row r="29" spans="1:5">
+      <c r="B29" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" s="1">
+        <v>330000</v>
+      </c>
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>997025</v>
+        <v>2258025</v>
       </c>
     </row>
     <row r="30" spans="1:5">
+      <c r="B30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" s="1">
+        <v>817500</v>
+      </c>
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>997025</v>
+        <v>1440525</v>
       </c>
     </row>
     <row r="31" spans="1:5">
+      <c r="B31" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" s="1">
+        <v>103000</v>
+      </c>
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>997025</v>
+        <v>1337525</v>
       </c>
     </row>
     <row r="32" spans="1:5">
+      <c r="B32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="1">
+        <f>41305475+6108025-42923000</f>
+        <v>4490500</v>
+      </c>
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>997025</v>
-      </c>
-    </row>
-    <row r="33" spans="5:6">
+        <v>5828025</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="B33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="1">
+        <v>45000</v>
+      </c>
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>997025</v>
-      </c>
-    </row>
-    <row r="34" spans="5:6">
+        <v>5873025</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="B34" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" s="1">
+        <v>5000000</v>
+      </c>
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>997025</v>
-      </c>
-    </row>
-    <row r="35" spans="5:6">
+        <v>873025</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="2">
+        <v>44302</v>
+      </c>
+      <c r="B35" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" s="1">
+        <f>60000</f>
+        <v>60000</v>
+      </c>
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>997025</v>
-      </c>
-    </row>
-    <row r="36" spans="5:6">
+        <v>813025</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="B36" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" s="1">
+        <f>5000000+9750000</f>
+        <v>14750000</v>
+      </c>
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>997025</v>
-      </c>
-    </row>
-    <row r="37" spans="5:6">
+        <v>-13936975</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="B37" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" s="1">
+        <f>9750000</f>
+        <v>9750000</v>
+      </c>
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>997025</v>
-      </c>
-    </row>
-    <row r="38" spans="5:6">
+        <v>-4186975</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="B38" t="s">
+        <v>69</v>
+      </c>
+      <c r="D38" s="1">
+        <f>63000</f>
+        <v>63000</v>
+      </c>
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>997025</v>
-      </c>
-    </row>
-    <row r="39" spans="5:6">
+        <v>-4249975</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>997025</v>
-      </c>
-    </row>
-    <row r="40" spans="5:6">
+        <v>-4249975</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="5:6">
+    <row r="41" spans="1:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>997025</v>
-      </c>
-    </row>
-    <row r="42" spans="5:6">
+        <v>-4249975</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>997025</v>
-      </c>
-    </row>
-    <row r="43" spans="5:6">
+        <v>-4249975</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>997025</v>
-      </c>
-    </row>
-    <row r="44" spans="5:6">
+        <v>-4249975</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>997025</v>
-      </c>
-    </row>
-    <row r="45" spans="5:6">
+        <v>-4249975</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>997025</v>
-      </c>
-    </row>
-    <row r="46" spans="5:6">
+        <v>-4249975</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>997025</v>
-      </c>
-    </row>
-    <row r="47" spans="5:6">
+        <v>-4249975</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>997025</v>
-      </c>
-    </row>
-    <row r="48" spans="5:6">
+        <v>-4249975</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>997025</v>
+        <v>-4249975</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 19-Apr-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
   <si>
     <t>Tgl</t>
   </si>
@@ -604,8 +604,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
+      <pane ySplit="2" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1070,12 +1070,12 @@
         <v>25</v>
       </c>
       <c r="D35" s="1">
-        <f>60000</f>
-        <v>60000</v>
+        <f>60000+300000</f>
+        <v>360000</v>
       </c>
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>813025</v>
+        <v>513025</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1083,12 +1083,12 @@
         <v>59</v>
       </c>
       <c r="D36" s="1">
-        <f>5000000+9750000</f>
-        <v>14750000</v>
+        <f>5000000+9750000+900000+1209000</f>
+        <v>16859000</v>
       </c>
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>-13936975</v>
+        <v>-16345975</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1096,12 +1096,12 @@
         <v>60</v>
       </c>
       <c r="C37" s="1">
-        <f>9750000</f>
-        <v>9750000</v>
+        <f>9750000+51187000</f>
+        <v>60937000</v>
       </c>
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>-4186975</v>
+        <v>44591025</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1114,460 +1114,488 @@
       </c>
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>-4249975</v>
+        <v>44528025</v>
       </c>
     </row>
     <row r="39" spans="1:6">
+      <c r="B39" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39" s="1">
+        <v>350000</v>
+      </c>
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>-4249975</v>
+        <v>44178025</v>
       </c>
     </row>
     <row r="40" spans="1:6">
+      <c r="B40" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="1">
+        <f>59197025+6708975-51187000</f>
+        <v>14719000</v>
+      </c>
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>-4249975</v>
+        <v>58897025</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:6">
+      <c r="B41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="1">
+        <v>95000</v>
+      </c>
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>-4249975</v>
+        <v>58992025</v>
       </c>
     </row>
     <row r="42" spans="1:6">
+      <c r="B42" t="s">
+        <v>63</v>
+      </c>
+      <c r="D42" s="1">
+        <v>58000000</v>
+      </c>
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="43" spans="1:6">
+      <c r="A43" s="2">
+        <v>44303</v>
+      </c>
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>-4249975</v>
+        <v>992025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 19 Apr 2021, end of day update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="63">
   <si>
     <t>Tgl</t>
   </si>
@@ -203,40 +203,10 @@
     <t>A/R</t>
   </si>
   <si>
-    <t>SALES - cash/retail</t>
-  </si>
-  <si>
-    <t>SELISIH - lebih</t>
-  </si>
-  <si>
-    <t>SETOR KE BANK</t>
-  </si>
-  <si>
-    <t>KELEBIHAN setoran ke bank</t>
-  </si>
-  <si>
-    <t>PAPA - beli obat</t>
-  </si>
-  <si>
-    <t>JASON - les</t>
-  </si>
-  <si>
-    <t>SELISIH - kurang</t>
-  </si>
-  <si>
-    <t>BELI lampu</t>
-  </si>
-  <si>
-    <t>FREIGHT OUT</t>
-  </si>
-  <si>
-    <t>TELPON - 5224823</t>
-  </si>
-  <si>
-    <t>PLN - Astar 165</t>
-  </si>
-  <si>
-    <t>PLN - Astar 214</t>
+    <t>DANA KEBERSIHAN</t>
+  </si>
+  <si>
+    <t>CHEQUE RECEIVED</t>
   </si>
 </sst>
 </file>
@@ -604,8 +574,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B43" sqref="B43"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -641,23 +611,23 @@
         <v>5</v>
       </c>
       <c r="E2" s="1">
-        <v>152525</v>
+        <v>391025</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>44298</v>
+        <v>44305</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="1">
-        <f>60000+240000</f>
-        <v>300000</v>
+        <f>60000</f>
+        <v>60000</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>-147475</v>
+        <v>331025</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -665,12 +635,12 @@
         <v>59</v>
       </c>
       <c r="D4" s="1">
-        <f>2340000+1600000+360000+900000+1900000</f>
-        <v>7100000</v>
+        <f>2685000+360000+6385000+11150000+4200000+504000+1509500+503500</f>
+        <v>27297000</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>-7247475</v>
+        <v>-26965975</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -678,924 +648,678 @@
         <v>60</v>
       </c>
       <c r="C5" s="1">
-        <f>360000+900000+4372000</f>
-        <v>5632000</v>
+        <f>11150000+2400000</f>
+        <v>13550000</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>-1615475</v>
+        <v>-13415975</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="B6" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="1">
-        <f>3150525+5747475-4372000</f>
-        <v>4526000</v>
+      <c r="D6" s="1">
+        <f>120000</f>
+        <v>120000</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>2910525</v>
+        <v>-13535975</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="B7" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="1">
-        <f>247000</f>
-        <v>247000</v>
+      <c r="D7" s="1">
+        <f>3360000</f>
+        <v>3360000</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>3157525</v>
+        <v>-16895975</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="B8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" s="1">
-        <v>3000000</v>
-      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>157525</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="2">
-        <v>44299</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="1">
-        <f>60000+240000</f>
-        <v>300000</v>
-      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>-142475</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="B10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="1">
-        <f>947500+2595000+3560000</f>
-        <v>7102500</v>
-      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>-7244975</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="B11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" s="1">
-        <v>100000</v>
-      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>-7144975</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="B12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D12" s="1">
-        <f>350000</f>
-        <v>350000</v>
-      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>-7494975</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13" s="1">
-        <f>600000</f>
-        <v>600000</v>
-      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>-8094975</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="B14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" s="1">
-        <f>7002025+8094975-10339500</f>
-        <v>4757500</v>
-      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>-3337475</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="B15" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="1">
-        <f>10339500</f>
-        <v>10339500</v>
-      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>7002025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="B16" t="s">
-        <v>67</v>
-      </c>
-      <c r="D16" s="1">
-        <v>5000</v>
-      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>6997025</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="B17" t="s">
-        <v>63</v>
-      </c>
-      <c r="D17" s="1">
-        <f>6000000</f>
-        <v>6000000</v>
-      </c>
+        <v>-16895975</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5">
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>997025</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="2">
-        <v>44300</v>
-      </c>
-      <c r="B18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="1">
-        <f>60000+260000</f>
-        <v>320000</v>
-      </c>
+        <v>-16895975</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5">
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>677025</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="B19" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="1">
-        <f>1170000+3615000+6235000+6777500</f>
-        <v>17797500</v>
-      </c>
+        <v>-16895975</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5">
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>18474525</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="B20" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" s="1">
-        <f>1170000+3615000+140000+480500</f>
-        <v>5405500</v>
-      </c>
+        <v>-16895975</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5">
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>13069025</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="B21" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="1">
-        <v>105000</v>
-      </c>
+        <v>-16895975</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5">
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>12964025</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="B22" t="s">
-        <v>61</v>
-      </c>
-      <c r="C22" s="1">
-        <f>21068025-6446525-6777500</f>
-        <v>7844000</v>
-      </c>
+        <v>-16895975</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>20808025</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="B23" t="s">
-        <v>69</v>
-      </c>
-      <c r="D23" s="1">
-        <f>150000</f>
-        <v>150000</v>
-      </c>
+        <v>-16895975</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>20658025</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="B24" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" s="1">
-        <v>10000</v>
-      </c>
+        <v>-16895975</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>20668025</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="B25" t="s">
-        <v>63</v>
-      </c>
-      <c r="D25" s="1">
-        <v>20000000</v>
-      </c>
+        <v>-16895975</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>668025</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="2">
-        <v>44301</v>
-      </c>
-      <c r="B26" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" s="1">
-        <f>60000+280000</f>
-        <v>340000</v>
-      </c>
+        <v>-16895975</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>328025</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="B27" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="1">
-        <f>13015000+448000+300000000+4800000+17000000+31001000+5400000</f>
-        <v>371664000</v>
-      </c>
+        <v>-16895975</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>-371335975</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="B28" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="1">
-        <f>300000000+31001000+42923000</f>
-        <v>373924000</v>
-      </c>
+        <v>-16895975</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>2588025</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="B29" t="s">
-        <v>70</v>
-      </c>
-      <c r="D29" s="1">
-        <v>330000</v>
-      </c>
+        <v>-16895975</v>
+      </c>
+    </row>
+    <row r="29" spans="5:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>2258025</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="B30" t="s">
-        <v>71</v>
-      </c>
-      <c r="D30" s="1">
-        <v>817500</v>
-      </c>
+        <v>-16895975</v>
+      </c>
+    </row>
+    <row r="30" spans="5:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>1440525</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="B31" t="s">
-        <v>72</v>
-      </c>
-      <c r="D31" s="1">
-        <v>103000</v>
-      </c>
+        <v>-16895975</v>
+      </c>
+    </row>
+    <row r="31" spans="5:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>1337525</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="B32" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="1">
-        <f>41305475+6108025-42923000</f>
-        <v>4490500</v>
-      </c>
+        <v>-16895975</v>
+      </c>
+    </row>
+    <row r="32" spans="5:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>5828025</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="B33" t="s">
-        <v>62</v>
-      </c>
-      <c r="C33" s="1">
-        <v>45000</v>
-      </c>
+        <v>-16895975</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>5873025</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="B34" t="s">
-        <v>63</v>
-      </c>
-      <c r="D34" s="1">
-        <v>5000000</v>
-      </c>
+        <v>-16895975</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>873025</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="2">
-        <v>44302</v>
-      </c>
-      <c r="B35" t="s">
-        <v>25</v>
-      </c>
-      <c r="D35" s="1">
-        <f>60000+300000</f>
-        <v>360000</v>
-      </c>
+        <v>-16895975</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>513025</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="B36" t="s">
-        <v>59</v>
-      </c>
-      <c r="D36" s="1">
-        <f>5000000+9750000+900000+1209000</f>
-        <v>16859000</v>
-      </c>
+        <v>-16895975</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>-16345975</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="B37" t="s">
-        <v>60</v>
-      </c>
-      <c r="C37" s="1">
-        <f>9750000+51187000</f>
-        <v>60937000</v>
-      </c>
+        <v>-16895975</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>44591025</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="B38" t="s">
-        <v>69</v>
-      </c>
-      <c r="D38" s="1">
-        <f>63000</f>
-        <v>63000</v>
-      </c>
+        <v>-16895975</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>44528025</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="B39" t="s">
-        <v>65</v>
-      </c>
-      <c r="D39" s="1">
-        <v>350000</v>
-      </c>
+        <v>-16895975</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>44178025</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="B40" t="s">
-        <v>61</v>
-      </c>
-      <c r="C40" s="1">
-        <f>59197025+6708975-51187000</f>
-        <v>14719000</v>
-      </c>
+        <v>-16895975</v>
+      </c>
+    </row>
+    <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>58897025</v>
+        <v>-16895975</v>
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="1:6">
-      <c r="B41" t="s">
-        <v>62</v>
-      </c>
-      <c r="C41" s="1">
-        <v>95000</v>
-      </c>
+    <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>58992025</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="B42" t="s">
-        <v>63</v>
-      </c>
-      <c r="D42" s="1">
-        <v>58000000</v>
-      </c>
+        <v>-16895975</v>
+      </c>
+    </row>
+    <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>992025</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="2">
-        <v>44303</v>
-      </c>
+        <v>-16895975</v>
+      </c>
+    </row>
+    <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>992025</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>-16895975</v>
+      </c>
+    </row>
+    <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>992025</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>-16895975</v>
+      </c>
+    </row>
+    <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>992025</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>-16895975</v>
+      </c>
+    </row>
+    <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>992025</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>-16895975</v>
+      </c>
+    </row>
+    <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>992025</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>-16895975</v>
+      </c>
+    </row>
+    <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>992025</v>
+        <v>-16895975</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 21-Apr-2021, end of day.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="69">
   <si>
     <t>Tgl</t>
   </si>
@@ -207,6 +207,24 @@
   </si>
   <si>
     <t>CHEQUE RECEIVED</t>
+  </si>
+  <si>
+    <t>SALES - cash/retail</t>
+  </si>
+  <si>
+    <t>SELISIH - lebih</t>
+  </si>
+  <si>
+    <t>SETOR KE BANK</t>
+  </si>
+  <si>
+    <t>SHIPPING cost</t>
+  </si>
+  <si>
+    <t>PAPA - obat</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -574,8 +592,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <pane ySplit="2" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -622,12 +640,12 @@
         <v>25</v>
       </c>
       <c r="D3" s="1">
-        <f>60000</f>
-        <v>60000</v>
+        <f>60000+240000</f>
+        <v>300000</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>331025</v>
+        <v>91025</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -640,7 +658,7 @@
       </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>-26965975</v>
+        <v>-27205975</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -648,12 +666,12 @@
         <v>60</v>
       </c>
       <c r="C5" s="1">
-        <f>11150000+2400000</f>
-        <v>13550000</v>
+        <f>11150000+2400000+20842000</f>
+        <v>34392000</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>-13415975</v>
+        <v>7186025</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -666,7 +684,7 @@
       </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>-13535975</v>
+        <v>7066025</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -679,647 +697,705 @@
       </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>-16895975</v>
+        <v>3706025</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="1">
+        <f>12487025+16895975-20842000</f>
+        <v>8541000</v>
+      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>-16895975</v>
+        <v>12247025</v>
       </c>
     </row>
     <row r="9" spans="1:6">
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2000</v>
+      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>-16895975</v>
+        <v>12249025</v>
       </c>
     </row>
     <row r="10" spans="1:6">
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="1">
+        <v>12000000</v>
+      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>-16895975</v>
+        <v>249025</v>
       </c>
     </row>
     <row r="11" spans="1:6">
+      <c r="A11" s="2">
+        <v>44306</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="1">
+        <f>60000</f>
+        <v>60000</v>
+      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>-16895975</v>
+        <v>189025</v>
       </c>
     </row>
     <row r="12" spans="1:6">
+      <c r="B12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="1">
+        <f>45650000+15937500+40500000+6025000+100000000</f>
+        <v>208112500</v>
+      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>-16895975</v>
+        <v>208301525</v>
       </c>
     </row>
     <row r="13" spans="1:6">
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="1">
+        <f>45650000+6100000+284500+6025000+100000000</f>
+        <v>158059500</v>
+      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>-16895975</v>
+        <v>50242025</v>
       </c>
     </row>
     <row r="14" spans="1:6">
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="1">
+        <v>225000</v>
+      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>-16895975</v>
+        <v>50017025</v>
       </c>
     </row>
     <row r="15" spans="1:6">
+      <c r="B15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="1">
+        <v>350000</v>
+      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="16" spans="1:6">
+      <c r="A16" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="17" spans="5:5">
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="18" spans="5:5">
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="19" spans="5:5">
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="20" spans="5:5">
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="21" spans="5:5">
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="22" spans="5:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="23" spans="5:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="24" spans="5:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="25" spans="5:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="26" spans="5:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="27" spans="5:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="28" spans="5:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="29" spans="5:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="30" spans="5:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="31" spans="5:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="32" spans="5:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>-16895975</v>
+        <v>49667025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 26-Apr-2021, end of day update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
   <si>
     <t>Tgl</t>
   </si>
@@ -198,45 +198,6 @@
   </si>
   <si>
     <t>TRANSFER BCA</t>
-  </si>
-  <si>
-    <t>A/R</t>
-  </si>
-  <si>
-    <t>DANA KEBERSIHAN</t>
-  </si>
-  <si>
-    <t>CHEQUE RECEIVED</t>
-  </si>
-  <si>
-    <t>SALES - cash/retail</t>
-  </si>
-  <si>
-    <t>SELISIH - lebih</t>
-  </si>
-  <si>
-    <t>SETOR KE BANK</t>
-  </si>
-  <si>
-    <t>SHIPPING cost</t>
-  </si>
-  <si>
-    <t>PAPA - obat</t>
-  </si>
-  <si>
-    <t>SOLAR - kijang</t>
-  </si>
-  <si>
-    <t>FREIGHT OUT</t>
-  </si>
-  <si>
-    <t>SELISIH - kurang</t>
-  </si>
-  <si>
-    <t>BELI beras</t>
-  </si>
-  <si>
-    <t>BELI sayur</t>
   </si>
 </sst>
 </file>
@@ -604,8 +565,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -641,23 +602,23 @@
         <v>5</v>
       </c>
       <c r="E2" s="1">
-        <v>391025</v>
+        <v>685500</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>44305</v>
+        <v>44312</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="1">
-        <f>60000+240000</f>
-        <v>300000</v>
+        <f>60000</f>
+        <v>60000</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>91025</v>
+        <v>625500</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -665,932 +626,670 @@
         <v>59</v>
       </c>
       <c r="D4" s="1">
-        <f>2685000+360000+6385000+11150000+4200000+504000+1509500+503500</f>
-        <v>27297000</v>
+        <f>2877500+1537000+3649500</f>
+        <v>8064000</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>-27205975</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="B5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="1">
-        <f>11150000+2400000+20842000</f>
-        <v>34392000</v>
-      </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>7186025</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="1">
-        <f>120000</f>
-        <v>120000</v>
-      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>7066025</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="B7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="1">
-        <f>3360000</f>
-        <v>3360000</v>
-      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>3706025</v>
+        <v>-7438500</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="B8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="1">
-        <f>12487025+16895975-20842000</f>
-        <v>8541000</v>
-      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>12247025</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="B9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="1">
-        <v>2000</v>
-      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>12249025</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="B10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="1">
-        <v>12000000</v>
-      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>249025</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="2">
-        <v>44306</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="1">
-        <f>60000+240000</f>
-        <v>300000</v>
-      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>-50975</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="B12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="1">
-        <f>45650000+15937500+40500000+6025000+100000000+619500</f>
-        <v>208732000</v>
-      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>208681025</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="1">
-        <f>45650000+6100000+284500+6025000+100000000+335000</f>
-        <v>158394500</v>
-      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>50286525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="B14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" s="1">
-        <v>225000</v>
-      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>50061525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="B15" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" s="1">
-        <v>350000</v>
-      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>49711525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="B16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="1">
-        <f>60722025-49667025-619500</f>
-        <v>10435500</v>
-      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>60147025</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="B17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" s="1">
-        <f>300000</f>
-        <v>300000</v>
-      </c>
+        <v>-7438500</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5">
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>59847025</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="B18" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" s="1">
-        <v>8500</v>
-      </c>
+        <v>-7438500</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5">
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>59855525</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="B19" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" s="1">
-        <f>59000000</f>
-        <v>59000000</v>
-      </c>
+        <v>-7438500</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5">
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>855525</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="2">
-        <v>44307</v>
-      </c>
-      <c r="B20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="1">
-        <f>60000+260000</f>
-        <v>320000</v>
-      </c>
+        <v>-7438500</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5">
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>535525</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="B21" t="s">
-        <v>69</v>
-      </c>
-      <c r="D21" s="1">
-        <f>48000</f>
-        <v>48000</v>
-      </c>
+        <v>-7438500</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5">
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>487525</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="B22" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" s="1">
-        <f>486000+4800000+1835000+800000+694000</f>
-        <v>8615000</v>
-      </c>
+        <v>-7438500</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>-8127475</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="B23" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="1">
-        <f>16825000</f>
-        <v>16825000</v>
-      </c>
+        <v>-7438500</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>8697525</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="B24" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="1">
-        <f>7867475+20230025-16825000</f>
-        <v>11272500</v>
-      </c>
+        <v>-7438500</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>19970025</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="B25" t="s">
-        <v>70</v>
-      </c>
-      <c r="D25" s="1">
-        <v>10000</v>
-      </c>
+        <v>-7438500</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>19960025</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="B26" t="s">
-        <v>65</v>
-      </c>
-      <c r="D26" s="1">
-        <v>19000000</v>
-      </c>
+        <v>-7438500</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>960025</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="2">
-        <v>44308</v>
-      </c>
-      <c r="B27" t="s">
-        <v>25</v>
-      </c>
-      <c r="D27" s="1">
-        <f>60000+240000</f>
-        <v>300000</v>
-      </c>
+        <v>-7438500</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>660025</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="B28" t="s">
-        <v>59</v>
-      </c>
-      <c r="D28" s="1">
-        <f>513000+2625000+1390000+14435000+257000</f>
-        <v>19220000</v>
-      </c>
+        <v>-7438500</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>-18559975</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="B29" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" s="1">
-        <f>14435000+9242000</f>
-        <v>23677000</v>
-      </c>
+        <v>-7438500</v>
+      </c>
+    </row>
+    <row r="29" spans="5:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>5117025</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="B30" t="s">
-        <v>71</v>
-      </c>
-      <c r="D30" s="1">
-        <v>290000</v>
-      </c>
+        <v>-7438500</v>
+      </c>
+    </row>
+    <row r="30" spans="5:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>4827025</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="B31" t="s">
-        <v>72</v>
-      </c>
-      <c r="D31" s="1">
-        <v>14000</v>
-      </c>
+        <v>-7438500</v>
+      </c>
+    </row>
+    <row r="31" spans="5:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>4813025</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="B32" t="s">
-        <v>63</v>
-      </c>
-      <c r="C32" s="1">
-        <f>4188975+9222025-9242000</f>
-        <v>4169000</v>
-      </c>
+        <v>-7438500</v>
+      </c>
+    </row>
+    <row r="32" spans="5:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>8982025</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="B33" t="s">
-        <v>70</v>
-      </c>
-      <c r="D33" s="1">
-        <v>59000</v>
-      </c>
+        <v>-7438500</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>8923025</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="B34" t="s">
-        <v>65</v>
-      </c>
-      <c r="D34" s="1">
-        <v>8000000</v>
-      </c>
+        <v>-7438500</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>923025</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="2">
-        <v>44309</v>
-      </c>
-      <c r="B35" t="s">
-        <v>25</v>
-      </c>
-      <c r="D35" s="1">
-        <f>60000+240000</f>
-        <v>300000</v>
-      </c>
+        <v>-7438500</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>623025</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="B36" t="s">
-        <v>72</v>
-      </c>
-      <c r="D36" s="1">
-        <f>5000</f>
-        <v>5000</v>
-      </c>
+        <v>-7438500</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>618025</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="B37" t="s">
-        <v>59</v>
-      </c>
-      <c r="D37" s="1">
-        <f>3150000+15000000+1911000+22860000</f>
-        <v>42921000</v>
-      </c>
+        <v>-7438500</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>-42302975</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="B38" t="s">
-        <v>60</v>
-      </c>
-      <c r="C38" s="1">
-        <f>15000000+22860000+14186000</f>
-        <v>52046000</v>
-      </c>
+        <v>-7438500</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>9743025</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="B39" t="s">
-        <v>63</v>
-      </c>
-      <c r="C39" s="1">
-        <f>4202975+16876525-14186000</f>
-        <v>6893500</v>
-      </c>
+        <v>-7438500</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>16636525</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="B40" t="s">
-        <v>70</v>
-      </c>
-      <c r="D40" s="1">
-        <v>16000</v>
-      </c>
+        <v>-7438500</v>
+      </c>
+    </row>
+    <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>16620525</v>
+        <v>-7438500</v>
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="1:6">
-      <c r="B41" t="s">
-        <v>65</v>
-      </c>
-      <c r="D41" s="1">
-        <f>16000000</f>
-        <v>16000000</v>
-      </c>
+    <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>620525</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="2">
-        <v>44310</v>
-      </c>
+        <v>-7438500</v>
+      </c>
+    </row>
+    <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>620525</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>-7438500</v>
+      </c>
+    </row>
+    <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>620525</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>-7438500</v>
+      </c>
+    </row>
+    <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>620525</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>-7438500</v>
+      </c>
+    </row>
+    <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>620525</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>-7438500</v>
+      </c>
+    </row>
+    <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>620525</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>-7438500</v>
+      </c>
+    </row>
+    <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>620525</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>-7438500</v>
+      </c>
+    </row>
+    <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>620525</v>
+        <v>-7438500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 29-Apr-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="70">
   <si>
     <t>Tgl</t>
   </si>
@@ -216,6 +216,18 @@
   </si>
   <si>
     <t>SETOR KE BANK</t>
+  </si>
+  <si>
+    <t>JASON - school fee</t>
+  </si>
+  <si>
+    <t>BELI abon</t>
+  </si>
+  <si>
+    <t>PAKET LEBARAN</t>
+  </si>
+  <si>
+    <t>BONUS FEE CANVASER 2020</t>
   </si>
 </sst>
 </file>
@@ -583,8 +595,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <pane ySplit="2" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -736,11 +748,12 @@
         <v>25</v>
       </c>
       <c r="D11" s="1">
-        <v>45000</v>
+        <f>45000+210000</f>
+        <v>255000</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>513525</v>
+        <v>303525</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -748,12 +761,12 @@
         <v>61</v>
       </c>
       <c r="C12" s="1">
-        <f>14625000+360000+28500000+8800000</f>
-        <v>52285000</v>
+        <f>14625000+360000+28500000+8800000+10009000</f>
+        <v>62294000</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>52798525</v>
+        <v>62597525</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -766,610 +779,703 @@
       </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>27669525</v>
+        <v>37468525</v>
       </c>
     </row>
     <row r="14" spans="1:6">
+      <c r="B14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="1">
+        <f>41859025-27669525-10009000</f>
+        <v>4180500</v>
+      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>27669525</v>
+        <v>41649025</v>
       </c>
     </row>
     <row r="15" spans="1:6">
+      <c r="B15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="1">
+        <v>11000000</v>
+      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>27669525</v>
+        <v>30649025</v>
       </c>
     </row>
     <row r="16" spans="1:6">
+      <c r="B16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="1">
+        <v>12000</v>
+      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>27669525</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5">
+        <v>30661025</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="B17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="1">
+        <f>30000000</f>
+        <v>30000000</v>
+      </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>27669525</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5">
+        <v>661025</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="2">
+        <v>44314</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="1">
+        <f>45000+180000</f>
+        <v>225000</v>
+      </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>27669525</v>
-      </c>
-    </row>
-    <row r="19" spans="5:5">
+        <v>436025</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="B19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="1">
+        <v>75000</v>
+      </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>27669525</v>
-      </c>
-    </row>
-    <row r="20" spans="5:5">
+        <v>361025</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="B20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="1">
+        <f>3500000+51000</f>
+        <v>3551000</v>
+      </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>27669525</v>
-      </c>
-    </row>
-    <row r="21" spans="5:5">
+        <v>-3189975</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="1">
+        <f>100000+5455530+1260000+1700000+4200000+300000+583000</f>
+        <v>13598530</v>
+      </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>27669525</v>
-      </c>
-    </row>
-    <row r="22" spans="5:5">
+        <v>-16788505</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="B22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="1">
+        <f>47787970</f>
+        <v>47787970</v>
+      </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>27669525</v>
-      </c>
-    </row>
-    <row r="23" spans="5:5">
+        <v>-64576475</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="B23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="1">
+        <f>428500+22875000+2175000+2790000+9560000+12800000+750000+940000+925000+10903000</f>
+        <v>64146500</v>
+      </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>27669525</v>
-      </c>
-    </row>
-    <row r="24" spans="5:5">
+        <v>-429975</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="B24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="1">
+        <f>11152975+9028025-10903000</f>
+        <v>9278000</v>
+      </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>27669525</v>
-      </c>
-    </row>
-    <row r="25" spans="5:5">
+        <v>8848025</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="B25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="1">
+        <v>8000000</v>
+      </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>27669525</v>
-      </c>
-    </row>
-    <row r="26" spans="5:5">
+        <v>848025</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="2">
+        <v>44315</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="1">
+        <f>45000</f>
+        <v>45000</v>
+      </c>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>27669525</v>
-      </c>
-    </row>
-    <row r="27" spans="5:5">
+        <v>803025</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>27669525</v>
-      </c>
-    </row>
-    <row r="28" spans="5:5">
+        <v>803025</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>27669525</v>
-      </c>
-    </row>
-    <row r="29" spans="5:5">
+        <v>803025</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>27669525</v>
-      </c>
-    </row>
-    <row r="30" spans="5:5">
+        <v>803025</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>27669525</v>
-      </c>
-    </row>
-    <row r="31" spans="5:5">
+        <v>803025</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>27669525</v>
-      </c>
-    </row>
-    <row r="32" spans="5:5">
+        <v>803025</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>27669525</v>
+        <v>803025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 7-Mei-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="75">
   <si>
     <t>Tgl</t>
   </si>
@@ -195,6 +195,54 @@
   </si>
   <si>
     <t>GUSTAVI</t>
+  </si>
+  <si>
+    <t>BELI lakban</t>
+  </si>
+  <si>
+    <t>A/P</t>
+  </si>
+  <si>
+    <t>TRANSFER BCA</t>
+  </si>
+  <si>
+    <t>IURAN DAERAH</t>
+  </si>
+  <si>
+    <t>A/R</t>
+  </si>
+  <si>
+    <t>SALES - cash/retail</t>
+  </si>
+  <si>
+    <t>SELISIH - lebih</t>
+  </si>
+  <si>
+    <t>SETOR KE BANK</t>
+  </si>
+  <si>
+    <t>TAX - Iuran ARIESTA</t>
+  </si>
+  <si>
+    <t>TAX - P.Tata</t>
+  </si>
+  <si>
+    <t>Dokter - PAPA</t>
+  </si>
+  <si>
+    <t>BENSIN - RUSH</t>
+  </si>
+  <si>
+    <t>PARKIR - bulanan</t>
+  </si>
+  <si>
+    <t>DANA KEBERSIHAN</t>
+  </si>
+  <si>
+    <t>TRANSFER DANAMON</t>
+  </si>
+  <si>
+    <t>PAPA - dokter</t>
   </si>
 </sst>
 </file>
@@ -562,8 +610,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <pane ySplit="2" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -609,673 +657,929 @@
       <c r="B3" t="s">
         <v>25</v>
       </c>
+      <c r="D3" s="1">
+        <f>45000+180000</f>
+        <v>225000</v>
+      </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>85025</v>
+        <v>-139975</v>
       </c>
     </row>
     <row r="4" spans="1:6">
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="1">
+        <f>67500</f>
+        <v>67500</v>
+      </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>85025</v>
+        <v>-207475</v>
       </c>
     </row>
     <row r="5" spans="1:6">
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="1">
+        <f>1374000</f>
+        <v>1374000</v>
+      </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>85025</v>
+        <v>-1581475</v>
       </c>
     </row>
     <row r="6" spans="1:6">
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="1">
+        <f>1400000+1070500+49050000+11000000</f>
+        <v>62520500</v>
+      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>85025</v>
+        <v>-64101975</v>
       </c>
     </row>
     <row r="7" spans="1:6">
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="1">
+        <v>25000</v>
+      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>85025</v>
+        <v>-64126975</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="1">
+        <f>48720000+330000+27014500</f>
+        <v>76064500</v>
+      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>85025</v>
+        <v>11937525</v>
       </c>
     </row>
     <row r="9" spans="1:6">
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="1">
+        <f>14896975+17682525-27014500</f>
+        <v>5565000</v>
+      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>85025</v>
+        <v>17502525</v>
       </c>
     </row>
     <row r="10" spans="1:6">
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="1">
+        <v>22500</v>
+      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>85025</v>
+        <v>17525025</v>
       </c>
     </row>
     <row r="11" spans="1:6">
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="1">
+        <v>17000000</v>
+      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>85025</v>
+        <v>525025</v>
       </c>
     </row>
     <row r="12" spans="1:6">
+      <c r="A12" s="2">
+        <v>44320</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="1">
+        <f>45000+195000</f>
+        <v>240000</v>
+      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>85025</v>
+        <v>285025</v>
       </c>
     </row>
     <row r="13" spans="1:6">
+      <c r="B13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="1">
+        <f>115000+10230000+2700000+1100000+2171000+814000</f>
+        <v>17130000</v>
+      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>85025</v>
+        <v>-16844975</v>
       </c>
     </row>
     <row r="14" spans="1:6">
+      <c r="B14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="1">
+        <v>660000</v>
+      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>85025</v>
+        <v>-17504975</v>
       </c>
     </row>
     <row r="15" spans="1:6">
+      <c r="B15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="1">
+        <v>200000</v>
+      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>85025</v>
+        <v>-17704975</v>
       </c>
     </row>
     <row r="16" spans="1:6">
+      <c r="B16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="1">
+        <f>9025000</f>
+        <v>9025000</v>
+      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>85025</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5">
+        <v>-26729975</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="1">
+        <f>2970000+7260000+26563000</f>
+        <v>36793000</v>
+      </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>85025</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5">
+        <v>10063025</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="B18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="1">
+        <f>16304975+17552525-26563000</f>
+        <v>7294500</v>
+      </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>85025</v>
-      </c>
-    </row>
-    <row r="19" spans="5:5">
+        <v>17357525</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="B19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="1">
+        <v>70000</v>
+      </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>85025</v>
-      </c>
-    </row>
-    <row r="20" spans="5:5">
+        <v>17427525</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="B20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="1">
+        <v>17000000</v>
+      </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>85025</v>
-      </c>
-    </row>
-    <row r="21" spans="5:5">
+        <v>427525</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2">
+        <v>44321</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="1">
+        <f>30000+140000</f>
+        <v>170000</v>
+      </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>85025</v>
-      </c>
-    </row>
-    <row r="22" spans="5:5">
+        <v>257525</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="B22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="1">
+        <v>250000</v>
+      </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>85025</v>
-      </c>
-    </row>
-    <row r="23" spans="5:5">
+        <v>7525</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="1">
+        <v>250000</v>
+      </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>85025</v>
-      </c>
-    </row>
-    <row r="24" spans="5:5">
+        <v>-242475</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="B24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="1">
+        <f>7428000+26658500</f>
+        <v>34086500</v>
+      </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>85025</v>
-      </c>
-    </row>
-    <row r="25" spans="5:5">
+        <v>33844025</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="B25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="1">
+        <f>7428000+3900000+8250000+1800000+122000+2500000+831500+650000</f>
+        <v>25481500</v>
+      </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>85025</v>
-      </c>
-    </row>
-    <row r="26" spans="5:5">
+        <v>8362525</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="B26" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="1">
+        <v>10000</v>
+      </c>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>85025</v>
-      </c>
-    </row>
-    <row r="27" spans="5:5">
+        <v>8352525</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="1">
+        <f>660000</f>
+        <v>660000</v>
+      </c>
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>85025</v>
-      </c>
-    </row>
-    <row r="28" spans="5:5">
+        <v>7692525</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="B28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="1">
+        <f>18075975+22740525+585000-26658500</f>
+        <v>14743000</v>
+      </c>
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>85025</v>
-      </c>
-    </row>
-    <row r="29" spans="5:5">
+        <v>22435525</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="B29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="1">
+        <v>100000</v>
+      </c>
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>85025</v>
-      </c>
-    </row>
-    <row r="30" spans="5:5">
+        <v>22535525</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="B30" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="1">
+        <v>22000000</v>
+      </c>
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>85025</v>
-      </c>
-    </row>
-    <row r="31" spans="5:5">
+        <v>535525</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="2">
+        <v>44322</v>
+      </c>
+      <c r="B31" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="1">
+        <f>30000+130000</f>
+        <v>160000</v>
+      </c>
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>85025</v>
-      </c>
-    </row>
-    <row r="32" spans="5:5">
+        <v>375525</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="B32" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="1">
+        <f>2250000+1300000+90000+616000+2993000</f>
+        <v>7249000</v>
+      </c>
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>85025</v>
-      </c>
-    </row>
-    <row r="33" spans="5:6">
+        <v>-6873475</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="B33" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" s="1">
+        <f>120000</f>
+        <v>120000</v>
+      </c>
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>85025</v>
-      </c>
-    </row>
-    <row r="34" spans="5:6">
+        <v>-6993475</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="B34" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" s="1">
+        <f>24600000+36259000</f>
+        <v>60859000</v>
+      </c>
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>85025</v>
-      </c>
-    </row>
-    <row r="35" spans="5:6">
+        <v>53865525</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="B35" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" s="1">
+        <f>24600000</f>
+        <v>24600000</v>
+      </c>
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>85025</v>
-      </c>
-    </row>
-    <row r="36" spans="5:6">
+        <v>29265525</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="B36" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="1">
+        <f>6863475+34421525-36259000</f>
+        <v>5026000</v>
+      </c>
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>85025</v>
-      </c>
-    </row>
-    <row r="37" spans="5:6">
+        <v>34291525</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="B37" t="s">
+        <v>74</v>
+      </c>
+      <c r="D37" s="1">
+        <f>250000</f>
+        <v>250000</v>
+      </c>
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>85025</v>
-      </c>
-    </row>
-    <row r="38" spans="5:6">
+        <v>34041525</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="B38" t="s">
+        <v>66</v>
+      </c>
+      <c r="D38" s="1">
+        <f>14000000</f>
+        <v>14000000</v>
+      </c>
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>85025</v>
-      </c>
-    </row>
-    <row r="39" spans="5:6">
+        <v>20041525</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="2">
+        <v>44323</v>
+      </c>
+      <c r="B39" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" s="1">
+        <f>30000</f>
+        <v>30000</v>
+      </c>
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>85025</v>
-      </c>
-    </row>
-    <row r="40" spans="5:6">
+        <v>20011525</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="5:6">
+    <row r="41" spans="1:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>85025</v>
-      </c>
-    </row>
-    <row r="42" spans="5:6">
+        <v>20011525</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>85025</v>
-      </c>
-    </row>
-    <row r="43" spans="5:6">
+        <v>20011525</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>85025</v>
-      </c>
-    </row>
-    <row r="44" spans="5:6">
+        <v>20011525</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>85025</v>
-      </c>
-    </row>
-    <row r="45" spans="5:6">
+        <v>20011525</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>85025</v>
-      </c>
-    </row>
-    <row r="46" spans="5:6">
+        <v>20011525</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>85025</v>
-      </c>
-    </row>
-    <row r="47" spans="5:6">
+        <v>20011525</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>85025</v>
-      </c>
-    </row>
-    <row r="48" spans="5:6">
+        <v>20011525</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>85025</v>
+        <v>20011525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 10-Mei-2021, end of day update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>Tgl</t>
   </si>
@@ -195,54 +195,6 @@
   </si>
   <si>
     <t>GUSTAVI</t>
-  </si>
-  <si>
-    <t>BELI lakban</t>
-  </si>
-  <si>
-    <t>A/P</t>
-  </si>
-  <si>
-    <t>TRANSFER BCA</t>
-  </si>
-  <si>
-    <t>IURAN DAERAH</t>
-  </si>
-  <si>
-    <t>A/R</t>
-  </si>
-  <si>
-    <t>SALES - cash/retail</t>
-  </si>
-  <si>
-    <t>SELISIH - lebih</t>
-  </si>
-  <si>
-    <t>SETOR KE BANK</t>
-  </si>
-  <si>
-    <t>TAX - Iuran ARIESTA</t>
-  </si>
-  <si>
-    <t>TAX - P.Tata</t>
-  </si>
-  <si>
-    <t>Dokter - PAPA</t>
-  </si>
-  <si>
-    <t>BENSIN - RUSH</t>
-  </si>
-  <si>
-    <t>PARKIR - bulanan</t>
-  </si>
-  <si>
-    <t>DANA KEBERSIHAN</t>
-  </si>
-  <si>
-    <t>TRANSFER DANAMON</t>
-  </si>
-  <si>
-    <t>PAPA - dokter</t>
   </si>
 </sst>
 </file>
@@ -610,8 +562,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C59" sqref="C59"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -647,939 +599,683 @@
         <v>5</v>
       </c>
       <c r="E2" s="1">
-        <v>85025</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>44319</v>
+        <v>44333</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="1">
-        <f>45000+180000</f>
-        <v>225000</v>
-      </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>-139975</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="B4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="1">
-        <f>67500</f>
-        <v>67500</v>
-      </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>-207475</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="B5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="1">
-        <f>1374000</f>
-        <v>1374000</v>
-      </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>-1581475</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="1">
-        <f>1400000+1070500+49050000+11000000</f>
-        <v>62520500</v>
-      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>-64101975</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="B7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="1">
-        <v>25000</v>
-      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>-64126975</v>
+        <v>647025</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="B8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="1">
-        <f>48720000+330000+27014500</f>
-        <v>76064500</v>
-      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>11937525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="B9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="1">
-        <f>14896975+17682525-27014500</f>
-        <v>5565000</v>
-      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>17502525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="B10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="1">
-        <v>22500</v>
-      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>17525025</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="B11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="1">
-        <v>17000000</v>
-      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>525025</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="2">
-        <v>44320</v>
-      </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="1">
-        <f>45000+195000</f>
-        <v>240000</v>
-      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>285025</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="1">
-        <f>115000+10230000+2700000+1100000+2171000+814000</f>
-        <v>17130000</v>
-      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>-16844975</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="B14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" s="1">
-        <v>660000</v>
-      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>-17504975</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="B15" t="s">
-        <v>68</v>
-      </c>
-      <c r="D15" s="1">
-        <v>200000</v>
-      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>-17704975</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="B16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="1">
-        <f>9025000</f>
-        <v>9025000</v>
-      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>-26729975</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="B17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="1">
-        <f>2970000+7260000+26563000</f>
-        <v>36793000</v>
-      </c>
+        <v>647025</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5">
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>10063025</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="B18" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" s="1">
-        <f>16304975+17552525-26563000</f>
-        <v>7294500</v>
-      </c>
+        <v>647025</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5">
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>17357525</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="B19" t="s">
-        <v>65</v>
-      </c>
-      <c r="C19" s="1">
-        <v>70000</v>
-      </c>
+        <v>647025</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5">
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>17427525</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="B20" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" s="1">
-        <v>17000000</v>
-      </c>
+        <v>647025</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5">
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>427525</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="2">
-        <v>44321</v>
-      </c>
-      <c r="B21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="1">
-        <f>30000+140000</f>
-        <v>170000</v>
-      </c>
+        <v>647025</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5">
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>257525</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="B22" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" s="1">
-        <v>250000</v>
-      </c>
+        <v>647025</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>7525</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="B23" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" s="1">
-        <v>250000</v>
-      </c>
+        <v>647025</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>-242475</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="B24" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="1">
-        <f>7428000+26658500</f>
-        <v>34086500</v>
-      </c>
+        <v>647025</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>33844025</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="B25" t="s">
-        <v>61</v>
-      </c>
-      <c r="D25" s="1">
-        <f>7428000+3900000+8250000+1800000+122000+2500000+831500+650000</f>
-        <v>25481500</v>
-      </c>
+        <v>647025</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>8362525</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="B26" t="s">
-        <v>71</v>
-      </c>
-      <c r="D26" s="1">
-        <v>10000</v>
-      </c>
+        <v>647025</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>8352525</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="B27" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="1">
-        <f>660000</f>
-        <v>660000</v>
-      </c>
+        <v>647025</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>7692525</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="B28" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" s="1">
-        <f>18075975+22740525+585000-26658500</f>
-        <v>14743000</v>
-      </c>
+        <v>647025</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>22435525</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="B29" t="s">
-        <v>65</v>
-      </c>
-      <c r="C29" s="1">
-        <v>100000</v>
-      </c>
+        <v>647025</v>
+      </c>
+    </row>
+    <row r="29" spans="5:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>22535525</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="B30" t="s">
-        <v>66</v>
-      </c>
-      <c r="D30" s="1">
-        <v>22000000</v>
-      </c>
+        <v>647025</v>
+      </c>
+    </row>
+    <row r="30" spans="5:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>535525</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="2">
-        <v>44322</v>
-      </c>
-      <c r="B31" t="s">
-        <v>25</v>
-      </c>
-      <c r="D31" s="1">
-        <f>30000+130000</f>
-        <v>160000</v>
-      </c>
+        <v>647025</v>
+      </c>
+    </row>
+    <row r="31" spans="5:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>375525</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="B32" t="s">
-        <v>61</v>
-      </c>
-      <c r="D32" s="1">
-        <f>2250000+1300000+90000+616000+2993000</f>
-        <v>7249000</v>
-      </c>
+        <v>647025</v>
+      </c>
+    </row>
+    <row r="32" spans="5:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>-6873475</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="B33" t="s">
-        <v>72</v>
-      </c>
-      <c r="D33" s="1">
-        <f>120000</f>
-        <v>120000</v>
-      </c>
+        <v>647025</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>-6993475</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="B34" t="s">
-        <v>63</v>
-      </c>
-      <c r="C34" s="1">
-        <f>24600000+36259000</f>
-        <v>60859000</v>
-      </c>
+        <v>647025</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>53865525</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="B35" t="s">
-        <v>73</v>
-      </c>
-      <c r="D35" s="1">
-        <f>24600000</f>
-        <v>24600000</v>
-      </c>
+        <v>647025</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>29265525</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="B36" t="s">
-        <v>64</v>
-      </c>
-      <c r="C36" s="1">
-        <f>6863475+34421525-36259000</f>
-        <v>5026000</v>
-      </c>
+        <v>647025</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>34291525</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="B37" t="s">
-        <v>74</v>
-      </c>
-      <c r="D37" s="1">
-        <f>250000</f>
-        <v>250000</v>
-      </c>
+        <v>647025</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>34041525</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="B38" t="s">
-        <v>66</v>
-      </c>
-      <c r="D38" s="1">
-        <f>14000000</f>
-        <v>14000000</v>
-      </c>
+        <v>647025</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>20041525</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="2">
-        <v>44323</v>
-      </c>
-      <c r="B39" t="s">
-        <v>25</v>
-      </c>
-      <c r="D39" s="1">
-        <f>30000</f>
-        <v>30000</v>
-      </c>
+        <v>647025</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>20011525</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>647025</v>
+      </c>
+    </row>
+    <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>20011525</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+        <v>647025</v>
+      </c>
+    </row>
+    <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>20011525</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>647025</v>
+      </c>
+    </row>
+    <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>20011525</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>647025</v>
+      </c>
+    </row>
+    <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>20011525</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>647025</v>
+      </c>
+    </row>
+    <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>20011525</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>647025</v>
+      </c>
+    </row>
+    <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>20011525</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>647025</v>
+      </c>
+    </row>
+    <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>20011525</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>647025</v>
+      </c>
+    </row>
+    <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>20011525</v>
+        <v>647025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 19-Mei-2021, end of day update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="69">
   <si>
     <t>Tgl</t>
   </si>
@@ -195,6 +195,36 @@
   </si>
   <si>
     <t>GUSTAVI</t>
+  </si>
+  <si>
+    <t>TRANSFER BCA</t>
+  </si>
+  <si>
+    <t>PLN - Astar 165</t>
+  </si>
+  <si>
+    <t>TELPON 5224823</t>
+  </si>
+  <si>
+    <t>A/R</t>
+  </si>
+  <si>
+    <t>SALES - cash/retail</t>
+  </si>
+  <si>
+    <t>PRIVE - andreas</t>
+  </si>
+  <si>
+    <t>SELISIH - lebih</t>
+  </si>
+  <si>
+    <t>SETOR KE BANK</t>
+  </si>
+  <si>
+    <t>TRANSFER BCA AA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LPG </t>
   </si>
 </sst>
 </file>
@@ -562,8 +592,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <pane ySplit="2" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -609,673 +639,811 @@
       <c r="B3" t="s">
         <v>25</v>
       </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
         <v>647025</v>
       </c>
     </row>
     <row r="4" spans="1:6">
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="1">
+        <f>1004000+6470000+3800000+25600000+10080000</f>
+        <v>46954000</v>
+      </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>647025</v>
+        <v>-46306975</v>
       </c>
     </row>
     <row r="5" spans="1:6">
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="1">
+        <f>895000</f>
+        <v>895000</v>
+      </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>647025</v>
+        <v>-47201975</v>
       </c>
     </row>
     <row r="6" spans="1:6">
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="1">
+        <f>223500</f>
+        <v>223500</v>
+      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>647025</v>
+        <v>-47425475</v>
       </c>
     </row>
     <row r="7" spans="1:6">
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="1">
+        <f>6470000+25600000+10080000+10834000</f>
+        <v>52984000</v>
+      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>647025</v>
+        <v>5558525</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="1">
+        <f>5275475+21002525-10834000</f>
+        <v>15444000</v>
+      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>647025</v>
+        <v>21002525</v>
       </c>
     </row>
     <row r="9" spans="1:6">
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2000000</v>
+      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>647025</v>
+        <v>19002525</v>
       </c>
     </row>
     <row r="10" spans="1:6">
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="1">
+        <f>50000</f>
+        <v>50000</v>
+      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>647025</v>
+        <v>19052525</v>
       </c>
     </row>
     <row r="11" spans="1:6">
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="1">
+        <v>18000000</v>
+      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>647025</v>
+        <v>1052525</v>
       </c>
     </row>
     <row r="12" spans="1:6">
+      <c r="A12" s="2">
+        <v>44334</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="1">
+        <f>45000+195000</f>
+        <v>240000</v>
+      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>647025</v>
+        <v>812525</v>
       </c>
     </row>
     <row r="13" spans="1:6">
+      <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="1">
+        <f>27020000+42656000</f>
+        <v>69676000</v>
+      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>647025</v>
+        <v>70488525</v>
       </c>
     </row>
     <row r="14" spans="1:6">
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="1">
+        <f>7000000+13633000+7508000+510000+497000+300000+1138000</f>
+        <v>30586000</v>
+      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>647025</v>
+        <v>39902525</v>
       </c>
     </row>
     <row r="15" spans="1:6">
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="1">
+        <f>2558475+49852525-42656000</f>
+        <v>9755000</v>
+      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>647025</v>
+        <v>49657525</v>
       </c>
     </row>
     <row r="16" spans="1:6">
+      <c r="B16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="1">
+        <v>18000</v>
+      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>647025</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5">
+        <v>49675525</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="B17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="1">
+        <f>49000000</f>
+        <v>49000000</v>
+      </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>647025</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5">
+        <v>675525</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="2">
+        <v>44335</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="1">
+        <f>45000</f>
+        <v>45000</v>
+      </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>647025</v>
-      </c>
-    </row>
-    <row r="19" spans="5:5">
+        <v>630525</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="1">
+        <f>3640000+1250000+1170000+440000+515000</f>
+        <v>7015000</v>
+      </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>647025</v>
-      </c>
-    </row>
-    <row r="20" spans="5:5">
+        <v>-6384475</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="1">
+        <f>9300000</f>
+        <v>9300000</v>
+      </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>647025</v>
-      </c>
-    </row>
-    <row r="21" spans="5:5">
+        <v>2915525</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="1">
+        <f>9300000</f>
+        <v>9300000</v>
+      </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>647025</v>
-      </c>
-    </row>
-    <row r="22" spans="5:5">
+        <v>-6384475</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="B22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="1">
+        <v>290000</v>
+      </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>647025</v>
-      </c>
-    </row>
-    <row r="23" spans="5:5">
+        <v>-6674475</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>647025</v>
-      </c>
-    </row>
-    <row r="24" spans="5:5">
+        <v>-6674475</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>647025</v>
-      </c>
-    </row>
-    <row r="25" spans="5:5">
+        <v>-6674475</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>647025</v>
-      </c>
-    </row>
-    <row r="26" spans="5:5">
+        <v>-6674475</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>647025</v>
-      </c>
-    </row>
-    <row r="27" spans="5:5">
+        <v>-6674475</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>647025</v>
-      </c>
-    </row>
-    <row r="28" spans="5:5">
+        <v>-6674475</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>647025</v>
-      </c>
-    </row>
-    <row r="29" spans="5:5">
+        <v>-6674475</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>647025</v>
-      </c>
-    </row>
-    <row r="30" spans="5:5">
+        <v>-6674475</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>647025</v>
-      </c>
-    </row>
-    <row r="31" spans="5:5">
+        <v>-6674475</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>647025</v>
-      </c>
-    </row>
-    <row r="32" spans="5:5">
+        <v>-6674475</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>647025</v>
+        <v>-6674475</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 20-Mei-2021, end of day update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="73">
   <si>
     <t>Tgl</t>
   </si>
@@ -225,6 +225,18 @@
   </si>
   <si>
     <t xml:space="preserve">LPG </t>
+  </si>
+  <si>
+    <t>BENSIN - RUSH</t>
+  </si>
+  <si>
+    <t>JASON - paspor</t>
+  </si>
+  <si>
+    <t>A/P</t>
+  </si>
+  <si>
+    <t>FREIGHT OUT</t>
   </si>
 </sst>
 </file>
@@ -592,8 +604,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D38" sqref="D38"/>
+      <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -838,12 +850,12 @@
         <v>25</v>
       </c>
       <c r="D18" s="1">
-        <f>45000</f>
-        <v>45000</v>
+        <f>45000+195000</f>
+        <v>240000</v>
       </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>630525</v>
+        <v>435525</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -851,12 +863,12 @@
         <v>59</v>
       </c>
       <c r="D19" s="1">
-        <f>3640000+1250000+1170000+440000+515000</f>
-        <v>7015000</v>
+        <f>3640000+1250000+1170000+440000+515000+2140000</f>
+        <v>9155000</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>-6384475</v>
+        <v>-8719475</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -864,12 +876,12 @@
         <v>62</v>
       </c>
       <c r="C20" s="1">
-        <f>9300000</f>
-        <v>9300000</v>
+        <f>9300000+17306000</f>
+        <v>26606000</v>
       </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>2915525</v>
+        <v>17886525</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -882,7 +894,7 @@
       </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>-6384475</v>
+        <v>8586525</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -894,556 +906,627 @@
       </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>-6674475</v>
+        <v>8296525</v>
       </c>
     </row>
     <row r="23" spans="1:5">
+      <c r="B23" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="1">
+        <f>250000</f>
+        <v>250000</v>
+      </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>-6674475</v>
+        <v>8046525</v>
       </c>
     </row>
     <row r="24" spans="1:5">
+      <c r="B24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1350000</v>
+      </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>-6674475</v>
+        <v>6696525</v>
       </c>
     </row>
     <row r="25" spans="1:5">
+      <c r="B25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="1">
+        <f>10414475+15258525-17306000</f>
+        <v>8367000</v>
+      </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>-6674475</v>
+        <v>15063525</v>
       </c>
     </row>
     <row r="26" spans="1:5">
+      <c r="B26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="1">
+        <v>2000</v>
+      </c>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>-6674475</v>
+        <v>15065525</v>
       </c>
     </row>
     <row r="27" spans="1:5">
+      <c r="B27" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="1">
+        <f>15000000</f>
+        <v>15000000</v>
+      </c>
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>-6674475</v>
+        <v>65525</v>
       </c>
     </row>
     <row r="28" spans="1:5">
+      <c r="A28" s="2">
+        <v>44336</v>
+      </c>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="1">
+        <f>45000</f>
+        <v>45000</v>
+      </c>
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>-6674475</v>
+        <v>20525</v>
       </c>
     </row>
     <row r="29" spans="1:5">
+      <c r="B29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="1">
+        <f>3360000</f>
+        <v>3360000</v>
+      </c>
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>-6674475</v>
+        <v>3380525</v>
       </c>
     </row>
     <row r="30" spans="1:5">
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="1">
+        <f>3360000</f>
+        <v>3360000</v>
+      </c>
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>-6674475</v>
+        <v>20525</v>
       </c>
     </row>
     <row r="31" spans="1:5">
+      <c r="B31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" s="1">
+        <f>1877000</f>
+        <v>1877000</v>
+      </c>
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>-6674475</v>
+        <v>-1856475</v>
       </c>
     </row>
     <row r="32" spans="1:5">
+      <c r="B32" t="s">
+        <v>72</v>
+      </c>
+      <c r="D32" s="1">
+        <f>14500</f>
+        <v>14500</v>
+      </c>
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>-6674475</v>
+        <v>-1870975</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 24-Mei-2021, end of day update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>Tgl</t>
   </si>
@@ -195,48 +195,6 @@
   </si>
   <si>
     <t>GUSTAVI</t>
-  </si>
-  <si>
-    <t>TRANSFER BCA</t>
-  </si>
-  <si>
-    <t>PLN - Astar 165</t>
-  </si>
-  <si>
-    <t>TELPON 5224823</t>
-  </si>
-  <si>
-    <t>A/R</t>
-  </si>
-  <si>
-    <t>SALES - cash/retail</t>
-  </si>
-  <si>
-    <t>PRIVE - andreas</t>
-  </si>
-  <si>
-    <t>SELISIH - lebih</t>
-  </si>
-  <si>
-    <t>SETOR KE BANK</t>
-  </si>
-  <si>
-    <t>TRANSFER BCA AA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LPG </t>
-  </si>
-  <si>
-    <t>BENSIN - RUSH</t>
-  </si>
-  <si>
-    <t>JASON - paspor</t>
-  </si>
-  <si>
-    <t>A/P</t>
-  </si>
-  <si>
-    <t>FREIGHT OUT</t>
   </si>
 </sst>
 </file>
@@ -604,8 +562,8 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -641,12 +599,12 @@
         <v>5</v>
       </c>
       <c r="E2" s="1">
-        <v>647025</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>44333</v>
+        <v>44340</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
@@ -656,877 +614,671 @@
       </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>647025</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="B4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="1">
-        <f>1004000+6470000+3800000+25600000+10080000</f>
-        <v>46954000</v>
-      </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>-46306975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="B5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="1">
-        <f>895000</f>
-        <v>895000</v>
-      </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>-47201975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="1">
-        <f>223500</f>
-        <v>223500</v>
-      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>-47425475</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="B7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="1">
-        <f>6470000+25600000+10080000+10834000</f>
-        <v>52984000</v>
-      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>5558525</v>
+        <v>1124025</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="B8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="1">
-        <f>5275475+21002525-10834000</f>
-        <v>15444000</v>
-      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>21002525</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="B9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="1">
-        <v>2000000</v>
-      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>19002525</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="B10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="1">
-        <f>50000</f>
-        <v>50000</v>
-      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>19052525</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="B11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="1">
-        <v>18000000</v>
-      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>1052525</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="2">
-        <v>44334</v>
-      </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="1">
-        <f>45000+195000</f>
-        <v>240000</v>
-      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>812525</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" s="1">
-        <f>27020000+42656000</f>
-        <v>69676000</v>
-      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>70488525</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="B14" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="1">
-        <f>7000000+13633000+7508000+510000+497000+300000+1138000</f>
-        <v>30586000</v>
-      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>39902525</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="B15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" s="1">
-        <f>2558475+49852525-42656000</f>
-        <v>9755000</v>
-      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>49657525</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="B16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="1">
-        <v>18000</v>
-      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>49675525</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="B17" t="s">
-        <v>66</v>
-      </c>
-      <c r="D17" s="1">
-        <f>49000000</f>
-        <v>49000000</v>
-      </c>
+        <v>1124025</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5">
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>675525</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="2">
-        <v>44335</v>
-      </c>
-      <c r="B18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="1">
-        <f>45000+195000</f>
-        <v>240000</v>
-      </c>
+        <v>1124025</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5">
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>435525</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="B19" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" s="1">
-        <f>3640000+1250000+1170000+440000+515000+2140000</f>
-        <v>9155000</v>
-      </c>
+        <v>1124025</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5">
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>-8719475</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="B20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="1">
-        <f>9300000+17306000</f>
-        <v>26606000</v>
-      </c>
+        <v>1124025</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5">
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>17886525</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="B21" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" s="1">
-        <f>9300000</f>
-        <v>9300000</v>
-      </c>
+        <v>1124025</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5">
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>8586525</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="B22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" s="1">
-        <v>290000</v>
-      </c>
+        <v>1124025</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>8296525</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="B23" t="s">
-        <v>69</v>
-      </c>
-      <c r="D23" s="1">
-        <f>250000</f>
-        <v>250000</v>
-      </c>
+        <v>1124025</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>8046525</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="B24" t="s">
-        <v>70</v>
-      </c>
-      <c r="D24" s="1">
-        <v>1350000</v>
-      </c>
+        <v>1124025</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>6696525</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="B25" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" s="1">
-        <f>10414475+15258525-17306000</f>
-        <v>8367000</v>
-      </c>
+        <v>1124025</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>15063525</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="B26" t="s">
-        <v>65</v>
-      </c>
-      <c r="C26" s="1">
-        <v>2000</v>
-      </c>
+        <v>1124025</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>15065525</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="B27" t="s">
-        <v>66</v>
-      </c>
-      <c r="D27" s="1">
-        <f>15000000</f>
-        <v>15000000</v>
-      </c>
+        <v>1124025</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>65525</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="2">
-        <v>44336</v>
-      </c>
-      <c r="B28" t="s">
-        <v>25</v>
-      </c>
-      <c r="D28" s="1">
-        <f>45000</f>
-        <v>45000</v>
-      </c>
+        <v>1124025</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>20525</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="B29" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="1">
-        <f>3360000</f>
-        <v>3360000</v>
-      </c>
+        <v>1124025</v>
+      </c>
+    </row>
+    <row r="29" spans="5:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>3380525</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="B30" t="s">
-        <v>59</v>
-      </c>
-      <c r="D30" s="1">
-        <f>3360000</f>
-        <v>3360000</v>
-      </c>
+        <v>1124025</v>
+      </c>
+    </row>
+    <row r="30" spans="5:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>20525</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="B31" t="s">
-        <v>71</v>
-      </c>
-      <c r="D31" s="1">
-        <f>1877000</f>
-        <v>1877000</v>
-      </c>
+        <v>1124025</v>
+      </c>
+    </row>
+    <row r="31" spans="5:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>-1856475</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="B32" t="s">
-        <v>72</v>
-      </c>
-      <c r="D32" s="1">
-        <f>14500</f>
-        <v>14500</v>
-      </c>
+        <v>1124025</v>
+      </c>
+    </row>
+    <row r="32" spans="5:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" si="3"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>-1870975</v>
+        <v>1124025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 26-Mei-2021, end of day update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="69">
   <si>
     <t>Tgl</t>
   </si>
@@ -195,6 +195,36 @@
   </si>
   <si>
     <t>GUSTAVI</t>
+  </si>
+  <si>
+    <t>BELI kresek</t>
+  </si>
+  <si>
+    <t>TRANSFER BCA</t>
+  </si>
+  <si>
+    <t>A/R</t>
+  </si>
+  <si>
+    <t>FREIGHT OUT</t>
+  </si>
+  <si>
+    <t>SALES - cash/retail</t>
+  </si>
+  <si>
+    <t>SELISIH - lebih</t>
+  </si>
+  <si>
+    <t>SETOR KE BANK</t>
+  </si>
+  <si>
+    <t>BELI nota</t>
+  </si>
+  <si>
+    <t>JASON - visa Kanada</t>
+  </si>
+  <si>
+    <t>SELISIH - kurang</t>
   </si>
 </sst>
 </file>
@@ -559,11 +589,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L113"/>
+  <dimension ref="A1:L114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -610,675 +640,809 @@
         <v>25</v>
       </c>
       <c r="D3" s="1">
-        <v>0</v>
+        <f>45000+210000</f>
+        <v>255000</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E34" si="0">E2+C3-D3</f>
-        <v>1124025</v>
+        <f t="shared" ref="E3:E35" si="0">E2+C3-D3</f>
+        <v>869025</v>
       </c>
     </row>
     <row r="4" spans="1:6">
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="1">
+        <f>92500</f>
+        <v>92500</v>
+      </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>1124025</v>
+        <v>776525</v>
       </c>
     </row>
     <row r="5" spans="1:6">
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="1">
+        <f>2550000+430000+3650000+60000+419000+120000+3005000+1879000+11000000</f>
+        <v>23113000</v>
+      </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>1124025</v>
+        <v>-22336475</v>
       </c>
     </row>
     <row r="6" spans="1:6">
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="1">
+        <f>3650000+9071000+11000000+45357000</f>
+        <v>69078000</v>
+      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>1124025</v>
+        <v>46741525</v>
       </c>
     </row>
     <row r="7" spans="1:6">
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="1">
+        <f>218500</f>
+        <v>218500</v>
+      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>1124025</v>
+        <v>46523025</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="1">
+        <f>64843525-12376025-45357000</f>
+        <v>7110500</v>
+      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>1124025</v>
+        <v>53633525</v>
       </c>
     </row>
     <row r="9" spans="1:6">
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="1">
+        <v>110000</v>
+      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>1124025</v>
+        <v>53743525</v>
       </c>
     </row>
     <row r="10" spans="1:6">
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="1">
+        <f>53000000</f>
+        <v>53000000</v>
+      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>1124025</v>
+        <v>743525</v>
       </c>
     </row>
     <row r="11" spans="1:6">
+      <c r="A11" s="2">
+        <v>44341</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="1">
+        <f>60000+240000</f>
+        <v>300000</v>
+      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>1124025</v>
+        <v>443525</v>
       </c>
     </row>
     <row r="12" spans="1:6">
+      <c r="B12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="1">
+        <f>100000</f>
+        <v>100000</v>
+      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>1124025</v>
+        <v>343525</v>
       </c>
     </row>
     <row r="13" spans="1:6">
+      <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="1">
+        <f>380000+1356500</f>
+        <v>1736500</v>
+      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>1124025</v>
+        <v>-1392975</v>
       </c>
     </row>
     <row r="14" spans="1:6">
+      <c r="B14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2950000</v>
+      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>1124025</v>
+        <v>-4342975</v>
       </c>
     </row>
     <row r="15" spans="1:6">
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="1">
+        <f>2755500</f>
+        <v>2755500</v>
+      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>1124025</v>
+        <v>-1587475</v>
       </c>
     </row>
     <row r="16" spans="1:6">
+      <c r="B16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="1">
+        <f>4102975+7102525-2755500</f>
+        <v>8450000</v>
+      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>1124025</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5">
+        <v>6862525</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="B17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="1">
+        <v>100000</v>
+      </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>1124025</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5">
+        <v>6762525</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="B18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="1">
+        <v>6000000</v>
+      </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>1124025</v>
-      </c>
-    </row>
-    <row r="19" spans="5:5">
+        <v>762525</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="2">
+        <v>44342</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="1">
+        <v>60000</v>
+      </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>1124025</v>
-      </c>
-    </row>
-    <row r="20" spans="5:5">
+        <v>702525</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="B20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="1">
+        <f>40965000+8890000+21622500</f>
+        <v>71477500</v>
+      </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>1124025</v>
-      </c>
-    </row>
-    <row r="21" spans="5:5">
+        <v>72180025</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="1">
+        <f>40965000+21082500+9432000</f>
+        <v>71479500</v>
+      </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>1124025</v>
-      </c>
-    </row>
-    <row r="22" spans="5:5">
+        <v>700525</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>1124025</v>
-      </c>
-    </row>
-    <row r="23" spans="5:5">
+        <v>700525</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>1124025</v>
-      </c>
-    </row>
-    <row r="24" spans="5:5">
+        <v>700525</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>1124025</v>
-      </c>
-    </row>
-    <row r="25" spans="5:5">
+        <v>700525</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>1124025</v>
-      </c>
-    </row>
-    <row r="26" spans="5:5">
+        <v>700525</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>1124025</v>
-      </c>
-    </row>
-    <row r="27" spans="5:5">
+        <v>700525</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>1124025</v>
-      </c>
-    </row>
-    <row r="28" spans="5:5">
+        <v>700525</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>1124025</v>
-      </c>
-    </row>
-    <row r="29" spans="5:5">
+        <v>700525</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>1124025</v>
-      </c>
-    </row>
-    <row r="30" spans="5:5">
+        <v>700525</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>1124025</v>
-      </c>
-    </row>
-    <row r="31" spans="5:5">
+        <v>700525</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>1124025</v>
-      </c>
-    </row>
-    <row r="32" spans="5:5">
+        <v>700525</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="35" spans="5:6">
       <c r="E35" s="1">
-        <f t="shared" ref="E35:E66" si="1">E34+C35-D35</f>
-        <v>1124025</v>
+        <f t="shared" si="0"/>
+        <v>700525</v>
       </c>
     </row>
     <row r="36" spans="5:6">
       <c r="E36" s="1">
-        <f t="shared" si="1"/>
-        <v>1124025</v>
+        <f t="shared" ref="E36:E67" si="1">E35+C36-D36</f>
+        <v>700525</v>
       </c>
     </row>
     <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>1124025</v>
-      </c>
-      <c r="F40" s="1"/>
+        <v>700525</v>
+      </c>
     </row>
     <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>1124025</v>
-      </c>
+        <v>700525</v>
+      </c>
+      <c r="F41" s="1"/>
     </row>
     <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>1124025</v>
-      </c>
-      <c r="F51" s="1"/>
+        <v>700525</v>
+      </c>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>1124025</v>
-      </c>
+        <v>700525</v>
+      </c>
+      <c r="F52" s="1"/>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
-        <f t="shared" ref="E67:E98" si="2">E66+C67-D67</f>
-        <v>1124025</v>
+        <f t="shared" si="1"/>
+        <v>700525</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
-        <f t="shared" si="2"/>
-        <v>1124025</v>
+        <f t="shared" ref="E68:E99" si="2">E67+C68-D68</f>
+        <v>700525</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>1124025</v>
-      </c>
-      <c r="G79" s="1"/>
+        <v>700525</v>
+      </c>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>1124025</v>
-      </c>
+        <v>700525</v>
+      </c>
+      <c r="G80" s="1"/>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
-        <f t="shared" ref="E99:E113" si="3">E98+C99-D99</f>
-        <v>1124025</v>
+        <f t="shared" si="2"/>
+        <v>700525</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
-        <f t="shared" si="3"/>
-        <v>1124025</v>
+        <f t="shared" ref="E100:E114" si="3">E99+C100-D100</f>
+        <v>700525</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>1124025</v>
+        <v>700525</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>1124025</v>
+        <v>700525</v>
+      </c>
+    </row>
+    <row r="114" spans="5:5">
+      <c r="E114" s="1">
+        <f t="shared" si="3"/>
+        <v>700525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 29-Mei-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="72">
   <si>
     <t>Tgl</t>
   </si>
@@ -225,6 +225,15 @@
   </si>
   <si>
     <t>SELISIH - kurang</t>
+  </si>
+  <si>
+    <t>PRIVE - andreas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOLAR - KIJANG </t>
+  </si>
+  <si>
+    <t>CHEQUE RECEIVED</t>
   </si>
 </sst>
 </file>
@@ -592,8 +601,8 @@
   <dimension ref="A1:L114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+      <pane ySplit="2" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -851,11 +860,12 @@
         <v>25</v>
       </c>
       <c r="D19" s="1">
-        <v>60000</v>
+        <f>60000+240000</f>
+        <v>300000</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>702525</v>
+        <v>462525</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -863,12 +873,12 @@
         <v>61</v>
       </c>
       <c r="C20" s="1">
-        <f>40965000+8890000+21622500</f>
-        <v>71477500</v>
+        <f>40965000+8892000+21622500+18858000</f>
+        <v>90337500</v>
       </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>72180025</v>
+        <v>90800025</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -876,573 +886,725 @@
         <v>60</v>
       </c>
       <c r="D21" s="1">
-        <f>40965000+21082500+9432000</f>
-        <v>71479500</v>
+        <f>40965000+21082500+9432500+640000+1100000+175000</f>
+        <v>73395000</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>700525</v>
+        <v>17405025</v>
       </c>
     </row>
     <row r="22" spans="1:5">
+      <c r="B22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="1">
+        <f>1212975+21250525-18858000</f>
+        <v>3605500</v>
+      </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>700525</v>
+        <v>21010525</v>
       </c>
     </row>
     <row r="23" spans="1:5">
+      <c r="B23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="1">
+        <f>20000000</f>
+        <v>20000000</v>
+      </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>700525</v>
+        <v>1010525</v>
       </c>
     </row>
     <row r="24" spans="1:5">
+      <c r="A24" s="2">
+        <v>44343</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="1">
+        <f>60000+280000</f>
+        <v>340000</v>
+      </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>700525</v>
+        <v>670525</v>
       </c>
     </row>
     <row r="25" spans="1:5">
+      <c r="B25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="1">
+        <f>5000000+1750000+15900000+3000000+10932500</f>
+        <v>36582500</v>
+      </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>700525</v>
+        <v>37253025</v>
       </c>
     </row>
     <row r="26" spans="1:5">
+      <c r="B26" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="1">
+        <f>144000+1750000+4281500+401000+18900000</f>
+        <v>25476500</v>
+      </c>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>700525</v>
+        <v>11776525</v>
       </c>
     </row>
     <row r="27" spans="1:5">
+      <c r="B27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" s="1">
+        <v>10000000</v>
+      </c>
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>700525</v>
+        <v>1776525</v>
       </c>
     </row>
     <row r="28" spans="1:5">
+      <c r="B28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="1">
+        <f>12144525+8875975-10932500</f>
+        <v>10088000</v>
+      </c>
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>700525</v>
+        <v>11864525</v>
       </c>
     </row>
     <row r="29" spans="1:5">
+      <c r="B29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" s="1">
+        <v>290000</v>
+      </c>
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>700525</v>
+        <v>11574525</v>
       </c>
     </row>
     <row r="30" spans="1:5">
+      <c r="B30" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30" s="1">
+        <v>11000000</v>
+      </c>
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>700525</v>
+        <v>574525</v>
       </c>
     </row>
     <row r="31" spans="1:5">
+      <c r="A31" s="2">
+        <v>44344</v>
+      </c>
+      <c r="B31" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="1">
+        <f>60000+240000</f>
+        <v>300000</v>
+      </c>
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>700525</v>
+        <v>274525</v>
       </c>
     </row>
     <row r="32" spans="1:5">
+      <c r="B32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="1">
+        <f>10000000+10364500+143000+14124000</f>
+        <v>34631500</v>
+      </c>
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>700525</v>
-      </c>
-    </row>
-    <row r="33" spans="5:6">
+        <v>34906025</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="B33" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" s="1">
+        <f>20507500+581000+135000</f>
+        <v>21223500</v>
+      </c>
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>700525</v>
-      </c>
-    </row>
-    <row r="34" spans="5:6">
+        <v>13682525</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="B34" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" s="1">
+        <f>14400</f>
+        <v>14400</v>
+      </c>
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>700525</v>
-      </c>
-    </row>
-    <row r="35" spans="5:6">
+        <v>13668125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="B35" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="1">
+        <f>23276125-500125-14124000</f>
+        <v>8652000</v>
+      </c>
       <c r="E35" s="1">
         <f t="shared" si="0"/>
-        <v>700525</v>
-      </c>
-    </row>
-    <row r="36" spans="5:6">
+        <v>22320125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="B36" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="1">
+        <v>10000</v>
+      </c>
       <c r="E36" s="1">
         <f t="shared" ref="E36:E67" si="1">E35+C36-D36</f>
-        <v>700525</v>
-      </c>
-    </row>
-    <row r="37" spans="5:6">
+        <v>22330125</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="B37" t="s">
+        <v>65</v>
+      </c>
+      <c r="D37" s="1">
+        <f>22000000</f>
+        <v>22000000</v>
+      </c>
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>700525</v>
-      </c>
-    </row>
-    <row r="38" spans="5:6">
+        <v>330125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="2">
+        <v>44345</v>
+      </c>
+      <c r="B38" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" s="1">
+        <f>60000</f>
+        <v>60000</v>
+      </c>
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>700525</v>
-      </c>
-    </row>
-    <row r="39" spans="5:6">
+        <v>270125</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="B39" t="s">
+        <v>70</v>
+      </c>
+      <c r="D39" s="1">
+        <f>300000</f>
+        <v>300000</v>
+      </c>
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>700525</v>
-      </c>
-    </row>
-    <row r="40" spans="5:6">
+        <v>-29875</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="B40" t="s">
+        <v>60</v>
+      </c>
+      <c r="D40" s="1">
+        <f>50000000+8330000+561500+875000</f>
+        <v>59766500</v>
+      </c>
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>700525</v>
-      </c>
-    </row>
-    <row r="41" spans="5:6">
+        <v>-59796375</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="B41" t="s">
+        <v>71</v>
+      </c>
+      <c r="D41" s="1">
+        <f>4043000</f>
+        <v>4043000</v>
+      </c>
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>700525</v>
+        <v>-63839375</v>
       </c>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="5:6">
+    <row r="42" spans="1:6">
+      <c r="B42" t="s">
+        <v>61</v>
+      </c>
+      <c r="C42" s="1">
+        <f>500000</f>
+        <v>500000</v>
+      </c>
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>700525</v>
-      </c>
-    </row>
-    <row r="43" spans="5:6">
+        <v>-63339375</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>700525</v>
-      </c>
-    </row>
-    <row r="44" spans="5:6">
+        <v>-63339375</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>700525</v>
-      </c>
-    </row>
-    <row r="45" spans="5:6">
+        <v>-63339375</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>700525</v>
-      </c>
-    </row>
-    <row r="46" spans="5:6">
+        <v>-63339375</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>700525</v>
-      </c>
-    </row>
-    <row r="47" spans="5:6">
+        <v>-63339375</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>700525</v>
-      </c>
-    </row>
-    <row r="48" spans="5:6">
+        <v>-63339375</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
       <c r="F52" s="1"/>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" si="1"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" ref="E68:E99" si="2">E67+C68-D68</f>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
       <c r="G80" s="1"/>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" si="2"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" ref="E100:E114" si="3">E99+C100-D100</f>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
     <row r="114" spans="5:5">
       <c r="E114" s="1">
         <f t="shared" si="3"/>
-        <v>700525</v>
+        <v>-63339375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 30-Mei-2021, end of day update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>Tgl</t>
   </si>
@@ -195,45 +195,6 @@
   </si>
   <si>
     <t>GUSTAVI</t>
-  </si>
-  <si>
-    <t>BELI kresek</t>
-  </si>
-  <si>
-    <t>TRANSFER BCA</t>
-  </si>
-  <si>
-    <t>A/R</t>
-  </si>
-  <si>
-    <t>FREIGHT OUT</t>
-  </si>
-  <si>
-    <t>SALES - cash/retail</t>
-  </si>
-  <si>
-    <t>SELISIH - lebih</t>
-  </si>
-  <si>
-    <t>SETOR KE BANK</t>
-  </si>
-  <si>
-    <t>BELI nota</t>
-  </si>
-  <si>
-    <t>JASON - visa Kanada</t>
-  </si>
-  <si>
-    <t>SELISIH - kurang</t>
-  </si>
-  <si>
-    <t>PRIVE - andreas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOLAR - KIJANG </t>
-  </si>
-  <si>
-    <t>CHEQUE RECEIVED</t>
   </si>
 </sst>
 </file>
@@ -601,8 +562,8 @@
   <dimension ref="A1:L114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D58" sqref="D58"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -638,973 +599,689 @@
         <v>5</v>
       </c>
       <c r="E2" s="1">
-        <v>1124025</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>44340</v>
+        <v>44347</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="1">
-        <f>45000+210000</f>
-        <v>255000</v>
-      </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E35" si="0">E2+C3-D3</f>
-        <v>869025</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="B4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="1">
-        <f>92500</f>
-        <v>92500</v>
-      </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>776525</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="B5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="1">
-        <f>2550000+430000+3650000+60000+419000+120000+3005000+1879000+11000000</f>
-        <v>23113000</v>
-      </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>-22336475</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="1">
-        <f>3650000+9071000+11000000+45357000</f>
-        <v>69078000</v>
-      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>46741525</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="B7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="1">
-        <f>218500</f>
-        <v>218500</v>
-      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>46523025</v>
+        <v>473125</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="B8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="1">
-        <f>64843525-12376025-45357000</f>
-        <v>7110500</v>
-      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>53633525</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="B9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="1">
-        <v>110000</v>
-      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>53743525</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="B10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="1">
-        <f>53000000</f>
-        <v>53000000</v>
-      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>743525</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="2">
-        <v>44341</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="1">
-        <f>60000+240000</f>
-        <v>300000</v>
-      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>443525</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="B12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" s="1">
-        <f>100000</f>
-        <v>100000</v>
-      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>343525</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="1">
-        <f>380000+1356500</f>
-        <v>1736500</v>
-      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>-1392975</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="B14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" s="1">
-        <v>2950000</v>
-      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>-4342975</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="B15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="1">
-        <f>2755500</f>
-        <v>2755500</v>
-      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>-1587475</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="B16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="1">
-        <f>4102975+7102525-2755500</f>
-        <v>8450000</v>
-      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>6862525</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="B17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" s="1">
-        <v>100000</v>
-      </c>
+        <v>473125</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5">
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>6762525</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="B18" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" s="1">
-        <v>6000000</v>
-      </c>
+        <v>473125</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5">
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>762525</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="2">
-        <v>44342</v>
-      </c>
-      <c r="B19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="1">
-        <f>60000+240000</f>
-        <v>300000</v>
-      </c>
+        <v>473125</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5">
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>462525</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="B20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="1">
-        <f>40965000+8892000+21622500+18858000</f>
-        <v>90337500</v>
-      </c>
+        <v>473125</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5">
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>90800025</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="B21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D21" s="1">
-        <f>40965000+21082500+9432500+640000+1100000+175000</f>
-        <v>73395000</v>
-      </c>
+        <v>473125</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5">
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>17405025</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="B22" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="1">
-        <f>1212975+21250525-18858000</f>
-        <v>3605500</v>
-      </c>
+        <v>473125</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>21010525</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="B23" t="s">
-        <v>65</v>
-      </c>
-      <c r="D23" s="1">
-        <f>20000000</f>
-        <v>20000000</v>
-      </c>
+        <v>473125</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>1010525</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="2">
-        <v>44343</v>
-      </c>
-      <c r="B24" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="1">
-        <f>60000+280000</f>
-        <v>340000</v>
-      </c>
+        <v>473125</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>670525</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="B25" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" s="1">
-        <f>5000000+1750000+15900000+3000000+10932500</f>
-        <v>36582500</v>
-      </c>
+        <v>473125</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>37253025</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="B26" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26" s="1">
-        <f>144000+1750000+4281500+401000+18900000</f>
-        <v>25476500</v>
-      </c>
+        <v>473125</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>11776525</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="B27" t="s">
-        <v>69</v>
-      </c>
-      <c r="D27" s="1">
-        <v>10000000</v>
-      </c>
+        <v>473125</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>1776525</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="B28" t="s">
-        <v>63</v>
-      </c>
-      <c r="C28" s="1">
-        <f>12144525+8875975-10932500</f>
-        <v>10088000</v>
-      </c>
+        <v>473125</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>11864525</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="B29" t="s">
-        <v>68</v>
-      </c>
-      <c r="D29" s="1">
-        <v>290000</v>
-      </c>
+        <v>473125</v>
+      </c>
+    </row>
+    <row r="29" spans="5:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>11574525</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="B30" t="s">
-        <v>65</v>
-      </c>
-      <c r="D30" s="1">
-        <v>11000000</v>
-      </c>
+        <v>473125</v>
+      </c>
+    </row>
+    <row r="30" spans="5:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>574525</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="2">
-        <v>44344</v>
-      </c>
-      <c r="B31" t="s">
-        <v>25</v>
-      </c>
-      <c r="D31" s="1">
-        <f>60000+240000</f>
-        <v>300000</v>
-      </c>
+        <v>473125</v>
+      </c>
+    </row>
+    <row r="31" spans="5:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>274525</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="B32" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="1">
-        <f>10000000+10364500+143000+14124000</f>
-        <v>34631500</v>
-      </c>
+        <v>473125</v>
+      </c>
+    </row>
+    <row r="32" spans="5:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>34906025</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="B33" t="s">
-        <v>60</v>
-      </c>
-      <c r="D33" s="1">
-        <f>20507500+581000+135000</f>
-        <v>21223500</v>
-      </c>
+        <v>473125</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>13682525</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="B34" t="s">
-        <v>62</v>
-      </c>
-      <c r="D34" s="1">
-        <f>14400</f>
-        <v>14400</v>
-      </c>
+        <v>473125</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>13668125</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="B35" t="s">
-        <v>63</v>
-      </c>
-      <c r="C35" s="1">
-        <f>23276125-500125-14124000</f>
-        <v>8652000</v>
-      </c>
+        <v>473125</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" si="0"/>
-        <v>22320125</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="B36" t="s">
-        <v>64</v>
-      </c>
-      <c r="C36" s="1">
-        <v>10000</v>
-      </c>
+        <v>473125</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" ref="E36:E67" si="1">E35+C36-D36</f>
-        <v>22330125</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="B37" t="s">
-        <v>65</v>
-      </c>
-      <c r="D37" s="1">
-        <f>22000000</f>
-        <v>22000000</v>
-      </c>
+        <v>473125</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>330125</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="2">
-        <v>44345</v>
-      </c>
-      <c r="B38" t="s">
-        <v>25</v>
-      </c>
-      <c r="D38" s="1">
-        <f>60000</f>
-        <v>60000</v>
-      </c>
+        <v>473125</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>270125</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="B39" t="s">
-        <v>70</v>
-      </c>
-      <c r="D39" s="1">
-        <f>300000</f>
-        <v>300000</v>
-      </c>
+        <v>473125</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>-29875</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="B40" t="s">
-        <v>60</v>
-      </c>
-      <c r="D40" s="1">
-        <f>50000000+8330000+561500+875000</f>
-        <v>59766500</v>
-      </c>
+        <v>473125</v>
+      </c>
+    </row>
+    <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>-59796375</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="B41" t="s">
-        <v>71</v>
-      </c>
-      <c r="D41" s="1">
-        <f>4043000</f>
-        <v>4043000</v>
-      </c>
+        <v>473125</v>
+      </c>
+    </row>
+    <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>-63839375</v>
+        <v>473125</v>
       </c>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="1:6">
-      <c r="B42" t="s">
-        <v>61</v>
-      </c>
-      <c r="C42" s="1">
-        <f>500000</f>
-        <v>500000</v>
-      </c>
+    <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>-63339375</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>473125</v>
+      </c>
+    </row>
+    <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>-63339375</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>473125</v>
+      </c>
+    </row>
+    <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>-63339375</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>473125</v>
+      </c>
+    </row>
+    <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>-63339375</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>473125</v>
+      </c>
+    </row>
+    <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>-63339375</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>473125</v>
+      </c>
+    </row>
+    <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>-63339375</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>473125</v>
+      </c>
+    </row>
+    <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
       <c r="F52" s="1"/>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" si="1"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" ref="E68:E99" si="2">E67+C68-D68</f>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
       <c r="G80" s="1"/>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" si="2"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" ref="E100:E114" si="3">E99+C100-D100</f>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
     <row r="114" spans="5:5">
       <c r="E114" s="1">
         <f t="shared" si="3"/>
-        <v>-63339375</v>
+        <v>473125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 3-Jun-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="71">
   <si>
     <t>Tgl</t>
   </si>
@@ -225,6 +225,12 @@
   </si>
   <si>
     <t>SELISIH - kurang</t>
+  </si>
+  <si>
+    <t>GARRETH - buku piano</t>
+  </si>
+  <si>
+    <t>BENSIN - RUSH</t>
   </si>
 </sst>
 </file>
@@ -592,8 +598,8 @@
   <dimension ref="A1:L114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
+      <pane ySplit="2" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -847,582 +853,631 @@
       <c r="A19" s="2">
         <v>44349</v>
       </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="1">
+        <f>60000+300000</f>
+        <v>360000</v>
+      </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>678125</v>
+        <v>318125</v>
       </c>
     </row>
     <row r="20" spans="1:5">
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="1">
+        <f>611500+385000+4557500+119000+5410000+16180000+521000+40000+4025000</f>
+        <v>31849000</v>
+      </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>678125</v>
+        <v>-31530875</v>
       </c>
     </row>
     <row r="21" spans="1:5">
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="1">
+        <f>4557500+119000+2700000+31598500</f>
+        <v>38975000</v>
+      </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>678125</v>
+        <v>7444125</v>
       </c>
     </row>
     <row r="22" spans="1:5">
+      <c r="B22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="1">
+        <v>515000</v>
+      </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>678125</v>
+        <v>6929125</v>
       </c>
     </row>
     <row r="23" spans="1:5">
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="1">
+        <v>250000</v>
+      </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>678125</v>
+        <v>6679125</v>
       </c>
     </row>
     <row r="24" spans="1:5">
+      <c r="B24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="1">
+        <f>24619375+18942625-31598500</f>
+        <v>11963500</v>
+      </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>678125</v>
+        <v>18642625</v>
       </c>
     </row>
     <row r="25" spans="1:5">
+      <c r="B25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="1">
+        <v>18000000</v>
+      </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="26" spans="1:5">
+      <c r="A26" s="2">
+        <v>44350</v>
+      </c>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" si="0"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" ref="E36:E67" si="1">E35+C36-D36</f>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
       <c r="F41" s="1"/>
     </row>
     <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
       <c r="F52" s="1"/>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" si="1"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" ref="E68:E99" si="2">E67+C68-D68</f>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
       <c r="G80" s="1"/>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" si="2"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" ref="E100:E114" si="3">E99+C100-D100</f>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
     <row r="114" spans="5:5">
       <c r="E114" s="1">
         <f t="shared" si="3"/>
-        <v>678125</v>
+        <v>642625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 7-Jun-2021, end of day update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>Tgl</t>
   </si>
@@ -195,51 +195,6 @@
   </si>
   <si>
     <t>GUSTAVI</t>
-  </si>
-  <si>
-    <t>TRANSFER BCA</t>
-  </si>
-  <si>
-    <t>A/R</t>
-  </si>
-  <si>
-    <t>TRANSFER BCA AA</t>
-  </si>
-  <si>
-    <t>PRIVE - andreas</t>
-  </si>
-  <si>
-    <t>SALES - cash/retail</t>
-  </si>
-  <si>
-    <t>PRIVE - bulanan</t>
-  </si>
-  <si>
-    <t>SETOR KE BANK</t>
-  </si>
-  <si>
-    <t>SELISIH - lebih</t>
-  </si>
-  <si>
-    <t>FREIGHT OUT</t>
-  </si>
-  <si>
-    <t>SELISIH - kurang</t>
-  </si>
-  <si>
-    <t>GARRETH - buku piano</t>
-  </si>
-  <si>
-    <t>BENSIN - RUSH</t>
-  </si>
-  <si>
-    <t>TAX - IURAN ARIESTA</t>
-  </si>
-  <si>
-    <t>TAX - P.Tata</t>
-  </si>
-  <si>
-    <t>A/P</t>
   </si>
 </sst>
 </file>
@@ -607,8 +562,8 @@
   <dimension ref="A1:L114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -644,913 +599,689 @@
         <v>5</v>
       </c>
       <c r="E2" s="1">
-        <v>473125</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>44347</v>
+        <v>44354</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="1">
-        <f>60000+6970000</f>
-        <v>7030000</v>
-      </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E35" si="0">E2+C3-D3</f>
-        <v>-6556875</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="B4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="1">
-        <f>2456000+3275000+100000000+13000000+13500000+3200000-960000+2206000</f>
-        <v>136677000</v>
-      </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>-143233875</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="B5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="1">
-        <f>100000000+12514400+485600+21050000+8950000+13500000+50921000</f>
-        <v>207421000</v>
-      </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>64187125</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="1">
-        <f>9240000</f>
-        <v>9240000</v>
-      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>54947125</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="B7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="1">
-        <f>2000000</f>
-        <v>2000000</v>
-      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>52947125</v>
+        <v>942625</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="B8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="1">
-        <f>83487125-8996125-50921000</f>
-        <v>23570000</v>
-      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>76517125</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="B9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="1">
-        <v>16000000</v>
-      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>60517125</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="B10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="1">
-        <v>60000000</v>
-      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>517125</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="B11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="1">
-        <v>60000</v>
-      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>577125</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="2">
-        <v>44348</v>
-      </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="1">
-        <f>60000+260000</f>
-        <v>320000</v>
-      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>257125</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="1">
-        <f>875000+4664500+2500000+4232000+457500</f>
-        <v>12729000</v>
-      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>-12471875</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="B14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" s="1">
-        <f>14500+22000+7000+57500</f>
-        <v>101000</v>
-      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>-12572875</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="B15" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="1">
-        <f>4664500+2500000+4232000+457500+4065000</f>
-        <v>15919000</v>
-      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>3346125</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="B16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="1">
-        <f>458875+8943125-4065000</f>
-        <v>5337000</v>
-      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>8683125</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="B17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" s="1">
-        <f>5000</f>
-        <v>5000</v>
-      </c>
+        <v>942625</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5">
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>8678125</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="B18" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" s="1">
-        <v>8000000</v>
-      </c>
+        <v>942625</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5">
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>678125</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="2">
-        <v>44349</v>
-      </c>
-      <c r="B19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="1">
-        <f>60000+300000</f>
-        <v>360000</v>
-      </c>
+        <v>942625</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5">
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>318125</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="B20" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" s="1">
-        <f>611500+385000+4557500+119000+5410000+16180000+521000+40000+4025000</f>
-        <v>31849000</v>
-      </c>
+        <v>942625</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5">
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>-31530875</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="B21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" s="1">
-        <f>4557500+119000+2700000+31598500</f>
-        <v>38975000</v>
-      </c>
+        <v>942625</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5">
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>7444125</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="B22" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" s="1">
-        <v>515000</v>
-      </c>
+        <v>942625</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>6929125</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="B23" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" s="1">
-        <v>250000</v>
-      </c>
+        <v>942625</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>6679125</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="B24" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="1">
-        <f>24619375+18942625-31598500</f>
-        <v>11963500</v>
-      </c>
+        <v>942625</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>18642625</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="B25" t="s">
-        <v>65</v>
-      </c>
-      <c r="D25" s="1">
-        <v>18000000</v>
-      </c>
+        <v>942625</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>642625</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="2">
-        <v>44350</v>
-      </c>
-      <c r="B26" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" s="1">
-        <f>60000+240000</f>
-        <v>300000</v>
-      </c>
+        <v>942625</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>342625</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="B27" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="1">
-        <f>17610000+23880000+2295000+6410000+221000</f>
-        <v>50416000</v>
-      </c>
+        <v>942625</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>-50073375</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="B28" t="s">
-        <v>71</v>
-      </c>
-      <c r="D28" s="1">
-        <v>660000</v>
-      </c>
+        <v>942625</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>-50733375</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="B29" t="s">
-        <v>72</v>
-      </c>
-      <c r="D29" s="1">
-        <f>200000</f>
-        <v>200000</v>
-      </c>
+        <v>942625</v>
+      </c>
+    </row>
+    <row r="29" spans="5:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>-50933375</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="B30" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="1">
-        <f>6410000</f>
-        <v>6410000</v>
-      </c>
+        <v>942625</v>
+      </c>
+    </row>
+    <row r="30" spans="5:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>-44523375</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="B31" t="s">
-        <v>63</v>
-      </c>
-      <c r="C31" s="1">
-        <f>44283375+26614925</f>
-        <v>70898300</v>
-      </c>
+        <v>942625</v>
+      </c>
+    </row>
+    <row r="31" spans="5:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>26374925</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="B32" t="s">
-        <v>73</v>
-      </c>
-      <c r="D32" s="1">
-        <f>2300000</f>
-        <v>2300000</v>
-      </c>
+        <v>942625</v>
+      </c>
+    </row>
+    <row r="32" spans="5:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>24074925</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="B33" t="s">
-        <v>66</v>
-      </c>
-      <c r="C33" s="1">
-        <v>89700</v>
-      </c>
+        <v>942625</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>24164625</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="B34" t="s">
-        <v>65</v>
-      </c>
-      <c r="D34" s="1">
-        <f>24000000</f>
-        <v>24000000</v>
-      </c>
+        <v>942625</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>164625</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="2">
-        <v>44351</v>
-      </c>
+        <v>942625</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" si="0"/>
-        <v>164625</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>942625</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" ref="E36:E67" si="1">E35+C36-D36</f>
-        <v>164625</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+        <v>942625</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>164625</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+        <v>942625</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>164625</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+        <v>942625</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>164625</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>942625</v>
+      </c>
+    </row>
+    <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>164625</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+        <v>942625</v>
+      </c>
+    </row>
+    <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>164625</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>942625</v>
+      </c>
+    </row>
+    <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>164625</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>942625</v>
+      </c>
+    </row>
+    <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>164625</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>942625</v>
+      </c>
+    </row>
+    <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>164625</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>942625</v>
+      </c>
+    </row>
+    <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>164625</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>942625</v>
+      </c>
+    </row>
+    <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>164625</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>942625</v>
+      </c>
+    </row>
+    <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
       <c r="F52" s="1"/>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" si="1"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" ref="E68:E99" si="2">E67+C68-D68</f>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
       <c r="G80" s="1"/>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" si="2"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" ref="E100:E114" si="3">E99+C100-D100</f>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
     <row r="114" spans="5:5">
       <c r="E114" s="1">
         <f t="shared" si="3"/>
-        <v>164625</v>
+        <v>942625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 14-Jun-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>Tgl</t>
   </si>
@@ -195,48 +195,6 @@
   </si>
   <si>
     <t>GUSTAVI</t>
-  </si>
-  <si>
-    <t>TRANSFER BCA</t>
-  </si>
-  <si>
-    <t>A/R</t>
-  </si>
-  <si>
-    <t>SALES - cash/retail</t>
-  </si>
-  <si>
-    <t>SELISIH - lebih</t>
-  </si>
-  <si>
-    <t>SETOR KE BANK</t>
-  </si>
-  <si>
-    <t>Other Income</t>
-  </si>
-  <si>
-    <t>JASON - les</t>
-  </si>
-  <si>
-    <t>DEBIT BCA</t>
-  </si>
-  <si>
-    <t>PLN - Astar 214</t>
-  </si>
-  <si>
-    <t>FREIGHT OUT</t>
-  </si>
-  <si>
-    <t>BELI amplop</t>
-  </si>
-  <si>
-    <t>CICILAN - Kukuh Ade</t>
-  </si>
-  <si>
-    <t>SELISIH - kurang</t>
-  </si>
-  <si>
-    <t>PRIVE - andreas</t>
   </si>
 </sst>
 </file>
@@ -604,8 +562,8 @@
   <dimension ref="A1:L114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D43" sqref="D43"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -641,967 +599,689 @@
         <v>5</v>
       </c>
       <c r="E2" s="1">
-        <v>942625</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>44354</v>
+        <v>44361</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="1">
-        <f>60000+460000</f>
-        <v>520000</v>
-      </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E35" si="0">E2+C3-D3</f>
-        <v>422625</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="B4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="1">
-        <f>21855000+4425000+2070000+1154000</f>
-        <v>29504000</v>
-      </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>-29081375</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="B5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="1">
-        <f>21855000+2683000+7562000+25070000</f>
-        <v>57170000</v>
-      </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>28088625</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="1">
-        <f>38175625-3478625-25070000</f>
-        <v>9627000</v>
-      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>37715625</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="B7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="1">
-        <v>135000</v>
-      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>37850625</v>
+        <v>276925</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="B8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" s="1">
-        <f>37000000</f>
-        <v>37000000</v>
-      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>850625</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="2">
-        <v>44355</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="1">
-        <f>60000+260000</f>
-        <v>320000</v>
-      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>530625</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="B10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="1">
-        <f>3630000+3259500+10000000+14235000+2029000+180000+4158000+231000</f>
-        <v>37722500</v>
-      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>-37191875</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="B11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="1">
-        <f>10000000+14235000+44296500</f>
-        <v>68531500</v>
-      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>31339625</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="B12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="1">
-        <f>12696875+38747125-44296500</f>
-        <v>7147500</v>
-      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>38487125</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" s="1">
-        <v>5000</v>
-      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>38492125</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="B14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="1">
-        <f>38000000</f>
-        <v>38000000</v>
-      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>492125</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="2">
-        <v>44356</v>
-      </c>
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="1">
-        <f>60000+260000</f>
-        <v>320000</v>
-      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>172125</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="B16" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" s="1">
-        <f>618000+15500000+1800000</f>
-        <v>17918000</v>
-      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>-17745875</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="B17" t="s">
-        <v>64</v>
-      </c>
-      <c r="C17" s="1">
-        <v>339000</v>
-      </c>
+        <v>276925</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5">
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>-17406875</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="B18" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="1">
-        <f>1800000+17280000+22840000</f>
-        <v>41920000</v>
-      </c>
+        <v>276925</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5">
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>24513125</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="B19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="1">
-        <f>36243125-1933125-22840000</f>
-        <v>11470000</v>
-      </c>
+        <v>276925</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5">
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>35983125</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="B20" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" s="1">
-        <v>610000</v>
-      </c>
+        <v>276925</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5">
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>35373125</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="B21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" s="1">
-        <v>150000</v>
-      </c>
+        <v>276925</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5">
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>35523125</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="B22" t="s">
-        <v>63</v>
-      </c>
-      <c r="D22" s="1">
-        <v>35000000</v>
-      </c>
+        <v>276925</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>523125</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="2">
-        <v>44357</v>
-      </c>
-      <c r="B23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23" s="1">
-        <f>60000+260000</f>
-        <v>320000</v>
-      </c>
+        <v>276925</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>203125</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="B24" t="s">
-        <v>59</v>
-      </c>
-      <c r="D24" s="1">
-        <f>6712000+2404000+30000+100000+23000+28236000</f>
-        <v>37505000</v>
-      </c>
+        <v>276925</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>-37301875</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="B25" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25" s="1">
-        <f>500000</f>
-        <v>500000</v>
-      </c>
+        <v>276925</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>-37801875</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="B26" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" s="1">
-        <f>6146500+3000000+28236000+67960000</f>
-        <v>105342500</v>
-      </c>
+        <v>276925</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>67540625</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="B27" t="s">
-        <v>67</v>
-      </c>
-      <c r="D27" s="1">
-        <v>103000</v>
-      </c>
+        <v>276925</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>67437625</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="B28" t="s">
-        <v>72</v>
-      </c>
-      <c r="D28" s="1">
-        <v>10000000</v>
-      </c>
+        <v>276925</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>57437625</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="B29" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" s="1">
-        <f>64432625+10262375-67960000</f>
-        <v>6735000</v>
-      </c>
+        <v>276925</v>
+      </c>
+    </row>
+    <row r="29" spans="5:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>64172625</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="B30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" s="1">
-        <v>235000</v>
-      </c>
+        <v>276925</v>
+      </c>
+    </row>
+    <row r="30" spans="5:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>64407625</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="B31" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" s="1">
-        <v>64000000</v>
-      </c>
+        <v>276925</v>
+      </c>
+    </row>
+    <row r="31" spans="5:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>407625</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="2">
-        <v>44358</v>
-      </c>
-      <c r="B32" t="s">
-        <v>25</v>
-      </c>
-      <c r="D32" s="1">
-        <f>60000+240000</f>
-        <v>300000</v>
-      </c>
+        <v>276925</v>
+      </c>
+    </row>
+    <row r="32" spans="5:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>107625</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="B33" t="s">
-        <v>60</v>
-      </c>
-      <c r="C33" s="1">
-        <f>176385000+3770000+19845000+52480000+14295000+26142500</f>
-        <v>292917500</v>
-      </c>
+        <v>276925</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>293025125</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="B34" t="s">
-        <v>59</v>
-      </c>
-      <c r="D34" s="1">
-        <f>200000000+1800000+4050000+1395000+52480000+3680000+14295000+1350000</f>
-        <v>279050000</v>
-      </c>
+        <v>276925</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>13975125</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="B35" t="s">
-        <v>68</v>
-      </c>
-      <c r="D35" s="1">
-        <f>7500</f>
-        <v>7500</v>
-      </c>
+        <v>276925</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" si="0"/>
-        <v>13967625</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="B36" t="s">
-        <v>69</v>
-      </c>
-      <c r="D36" s="1">
-        <v>26000</v>
-      </c>
+        <v>276925</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" ref="E36:E67" si="1">E35+C36-D36</f>
-        <v>13941625</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="B37" t="s">
-        <v>70</v>
-      </c>
-      <c r="C37" s="1">
-        <v>3000000</v>
-      </c>
+        <v>276925</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>16941625</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="B38" t="s">
-        <v>61</v>
-      </c>
-      <c r="C38" s="1">
-        <f>24856625+7610875-26142500</f>
-        <v>6325000</v>
-      </c>
+        <v>276925</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>23266625</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="B39" t="s">
-        <v>71</v>
-      </c>
-      <c r="D39" s="1">
-        <v>700</v>
-      </c>
+        <v>276925</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>23265925</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="B40" t="s">
-        <v>63</v>
-      </c>
-      <c r="D40" s="1">
-        <v>23000000</v>
-      </c>
+        <v>276925</v>
+      </c>
+    </row>
+    <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>265925</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="2">
-        <v>44359</v>
-      </c>
-      <c r="B41" t="s">
-        <v>25</v>
-      </c>
-      <c r="D41" s="1">
-        <f>60000</f>
-        <v>60000</v>
-      </c>
+        <v>276925</v>
+      </c>
+    </row>
+    <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>205925</v>
+        <v>276925</v>
       </c>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="1:6">
-      <c r="B42" t="s">
-        <v>59</v>
-      </c>
-      <c r="D42" s="1">
-        <f>11400000</f>
-        <v>11400000</v>
-      </c>
+    <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>-11194075</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>276925</v>
+      </c>
+    </row>
+    <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>-11194075</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>276925</v>
+      </c>
+    </row>
+    <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>-11194075</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>276925</v>
+      </c>
+    </row>
+    <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>-11194075</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>276925</v>
+      </c>
+    </row>
+    <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>-11194075</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>276925</v>
+      </c>
+    </row>
+    <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>-11194075</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>276925</v>
+      </c>
+    </row>
+    <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
       <c r="F52" s="1"/>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" si="1"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" ref="E68:E99" si="2">E67+C68-D68</f>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
       <c r="G80" s="1"/>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" si="2"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" ref="E100:E114" si="3">E99+C100-D100</f>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
     <row r="114" spans="5:5">
       <c r="E114" s="1">
         <f t="shared" si="3"/>
-        <v>-11194075</v>
+        <v>276925</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 21-Jun-2021, midday update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="71">
   <si>
     <t>Tgl</t>
   </si>
@@ -228,6 +228,9 @@
   </si>
   <si>
     <t>BELI lampu</t>
+  </si>
+  <si>
+    <t>BELI plastik</t>
   </si>
 </sst>
 </file>
@@ -595,8 +598,8 @@
   <dimension ref="A1:L114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
+      <pane ySplit="2" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1026,28 +1029,28 @@
         <v>25</v>
       </c>
       <c r="D32" s="1">
-        <f>60000</f>
-        <v>60000</v>
+        <f>60000+260000</f>
+        <v>320000</v>
       </c>
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>945725</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6">
+        <v>685725</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="B33" t="s">
         <v>59</v>
       </c>
       <c r="D33" s="1">
-        <f>775000+577200+1555000</f>
-        <v>2907200</v>
+        <f>775000+577200+1555000+25000000+1379000</f>
+        <v>29286200</v>
       </c>
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>-1961475</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6">
+        <v>-28600475</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="B34" t="s">
         <v>69</v>
       </c>
@@ -1056,23 +1059,23 @@
       </c>
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>-1993975</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6">
+        <v>-28632975</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="B35" t="s">
         <v>61</v>
       </c>
       <c r="C35" s="1">
-        <f>577200</f>
-        <v>577200</v>
+        <f>577200+1000000+30000000+9035000+9375000</f>
+        <v>49987200</v>
       </c>
       <c r="E35" s="1">
         <f t="shared" si="0"/>
-        <v>-1416775</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6">
+        <v>21354225</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="B36" t="s">
         <v>60</v>
       </c>
@@ -1082,478 +1085,508 @@
       </c>
       <c r="E36" s="1">
         <f t="shared" ref="E36:E67" si="1">E35+C36-D36</f>
-        <v>-1579275</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6">
+        <v>21191725</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="B37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" s="1">
+        <f>21768725-3041725-9375000</f>
+        <v>9352000</v>
+      </c>
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>-1579275</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6">
+        <v>30543725</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="B38" t="s">
+        <v>67</v>
+      </c>
+      <c r="D38" s="1">
+        <v>30000000</v>
+      </c>
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>-1579275</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6">
+        <v>543725</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="2">
+        <v>44366</v>
+      </c>
+      <c r="B39" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" s="1">
+        <f>60000</f>
+        <v>60000</v>
+      </c>
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>-1579275</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6">
+        <v>483725</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="B40" t="s">
+        <v>70</v>
+      </c>
+      <c r="D40" s="1">
+        <f>75000</f>
+        <v>75000</v>
+      </c>
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>-1579275</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6">
+        <v>408725</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="2:6">
+    <row r="42" spans="1:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>-1579275</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6">
+        <v>408725</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>-1579275</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6">
+        <v>408725</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>-1579275</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6">
+        <v>408725</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>-1579275</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6">
+        <v>408725</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>-1579275</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6">
+        <v>408725</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>-1579275</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6">
+        <v>408725</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
       <c r="F52" s="1"/>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" si="1"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" ref="E68:E99" si="2">E67+C68-D68</f>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
       <c r="G80" s="1"/>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" si="2"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" ref="E100:E114" si="3">E99+C100-D100</f>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
     <row r="114" spans="5:5">
       <c r="E114" s="1">
         <f t="shared" si="3"/>
-        <v>-1579275</v>
+        <v>408725</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 27-Jun-2021, end of day update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>Tgl</t>
   </si>
@@ -195,36 +195,6 @@
   </si>
   <si>
     <t>GUSTAVI</t>
-  </si>
-  <si>
-    <t>TRANSFER BCA</t>
-  </si>
-  <si>
-    <t>A/R</t>
-  </si>
-  <si>
-    <t>A/P</t>
-  </si>
-  <si>
-    <t>SALES - cash/retail</t>
-  </si>
-  <si>
-    <t>SELISIH - lebih</t>
-  </si>
-  <si>
-    <t>SETOR KE BANK</t>
-  </si>
-  <si>
-    <t>PRIVE - andreas</t>
-  </si>
-  <si>
-    <t>GANTI ONGKIR retur</t>
-  </si>
-  <si>
-    <t>SELISIH - kurang</t>
-  </si>
-  <si>
-    <t>BELi lampu</t>
   </si>
 </sst>
 </file>
@@ -592,8 +562,8 @@
   <dimension ref="A1:L114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B51" sqref="B51"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -629,905 +599,689 @@
         <v>5</v>
       </c>
       <c r="E2" s="1">
-        <v>895225</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>44368</v>
+        <v>44375</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="1">
-        <f>60000+240000</f>
-        <v>300000</v>
-      </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E35" si="0">E2+C3-D3</f>
-        <v>595225</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="B4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="1">
-        <f>2750000+6215000+5400000+1950000+450000+253000</f>
-        <v>17018000</v>
-      </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>-16422775</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="B5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="1">
-        <f>6215000+146005000+1950000+22791000</f>
-        <v>176961000</v>
-      </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>160538225</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="1">
-        <f>146005000+700000</f>
-        <v>146705000</v>
-      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>13833225</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="B7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="1">
-        <v>5000000</v>
-      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>8833225</v>
+        <v>479225</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="B8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="1">
-        <f>13717775+20849225-22791000</f>
-        <v>11776000</v>
-      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>20609225</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="B9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="1">
-        <v>48000</v>
-      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>20657225</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="B10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D10" s="1">
-        <v>20000000</v>
-      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>657225</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="2">
-        <v>44369</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="1">
-        <f>60000+260000</f>
-        <v>320000</v>
-      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>337225</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="B12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" s="1">
-        <f>11960000+9115200+1515000+10000000+745000+1210000+22800000+768000+3501000</f>
-        <v>61614200</v>
-      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>-61276975</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="1">
-        <f>6400000</f>
-        <v>6400000</v>
-      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>-67676975</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="B14" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" s="1">
-        <f>9115200+1515000+4571500+20000000+745000+530000+53959000</f>
-        <v>90435700</v>
-      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>22758725</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="B15" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" s="1">
-        <v>218000</v>
-      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>22976725</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="B16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" s="1">
-        <f>3653275+55310725-53959000</f>
-        <v>5005000</v>
-      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>27981725</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="B17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="1">
-        <v>2000</v>
-      </c>
+        <v>479225</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5">
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>27983725</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="B18" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="1">
-        <v>27000000</v>
-      </c>
+        <v>479225</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5">
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>983725</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="2">
-        <v>44370</v>
-      </c>
-      <c r="B19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="1">
-        <f>45000+195000</f>
-        <v>240000</v>
-      </c>
+        <v>479225</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5">
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>743725</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="B20" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" s="1">
-        <f>2750000+60000+24900000+9000000+643000+30000</f>
-        <v>37383000</v>
-      </c>
+        <v>479225</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5">
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>-36639275</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="B21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" s="1">
-        <f>4620000+18800000+11560000+37293000</f>
-        <v>72273000</v>
-      </c>
+        <v>479225</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5">
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>35633725</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="B22" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" s="1">
-        <f>1464275+41299725-37293000</f>
-        <v>5471000</v>
-      </c>
+        <v>479225</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>41104725</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="B23" t="s">
-        <v>67</v>
-      </c>
-      <c r="D23" s="1">
-        <v>980000</v>
-      </c>
+        <v>479225</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>40124725</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="B24" t="s">
-        <v>64</v>
-      </c>
-      <c r="D24" s="1">
-        <f>40000000</f>
-        <v>40000000</v>
-      </c>
+        <v>479225</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>124725</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="2">
-        <v>44371</v>
-      </c>
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="1">
-        <f>60000+260000</f>
-        <v>320000</v>
-      </c>
+        <v>479225</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>-195275</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="B26" t="s">
-        <v>59</v>
-      </c>
-      <c r="D26" s="1">
-        <f>5500000+500000+1000000+1350000+165000+1412500</f>
-        <v>9927500</v>
-      </c>
+        <v>479225</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>-10122775</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="B27" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="1">
-        <f>8000000+16258500</f>
-        <v>24258500</v>
-      </c>
+        <v>479225</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>14135725</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="B28" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" s="1">
-        <f>22885725+1862775-16258500</f>
-        <v>8490000</v>
-      </c>
+        <v>479225</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>22625725</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="B29" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" s="1">
-        <v>1015000</v>
-      </c>
+        <v>479225</v>
+      </c>
+    </row>
+    <row r="29" spans="5:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>23640725</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="B30" t="s">
-        <v>64</v>
-      </c>
-      <c r="D30" s="1">
-        <v>23000000</v>
-      </c>
+        <v>479225</v>
+      </c>
+    </row>
+    <row r="30" spans="5:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>640725</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="2">
-        <v>44372</v>
-      </c>
-      <c r="B31" t="s">
-        <v>25</v>
-      </c>
-      <c r="D31" s="1">
-        <f>60000</f>
-        <v>60000</v>
-      </c>
+        <v>479225</v>
+      </c>
+    </row>
+    <row r="31" spans="5:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>580725</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="B32" t="s">
-        <v>59</v>
-      </c>
-      <c r="D32" s="1">
-        <f>1740000</f>
-        <v>1740000</v>
-      </c>
+        <v>479225</v>
+      </c>
+    </row>
+    <row r="32" spans="5:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>-1159275</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6">
-      <c r="B33" t="s">
-        <v>68</v>
-      </c>
-      <c r="D33" s="1">
-        <v>15000</v>
-      </c>
+        <v>479225</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>-1174275</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6">
+        <v>479225</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>-1174275</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6">
+        <v>479225</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" si="0"/>
-        <v>-1174275</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6">
+        <v>479225</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" ref="E36:E67" si="1">E35+C36-D36</f>
-        <v>-1174275</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6">
+        <v>479225</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>-1174275</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6">
+        <v>479225</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>-1174275</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6">
+        <v>479225</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>-1174275</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6">
+        <v>479225</v>
+      </c>
+    </row>
+    <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>-1174275</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6">
+        <v>479225</v>
+      </c>
+    </row>
+    <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="2:6">
+    <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>-1174275</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6">
+        <v>479225</v>
+      </c>
+    </row>
+    <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>-1174275</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6">
+        <v>479225</v>
+      </c>
+    </row>
+    <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>-1174275</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6">
+        <v>479225</v>
+      </c>
+    </row>
+    <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>-1174275</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6">
+        <v>479225</v>
+      </c>
+    </row>
+    <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>-1174275</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6">
+        <v>479225</v>
+      </c>
+    </row>
+    <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>-1174275</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6">
+        <v>479225</v>
+      </c>
+    </row>
+    <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
       <c r="F52" s="1"/>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" si="1"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" ref="E68:E99" si="2">E67+C68-D68</f>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
       <c r="G80" s="1"/>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" si="2"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" ref="E100:E114" si="3">E99+C100-D100</f>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
     <row r="114" spans="5:5">
       <c r="E114" s="1">
         <f t="shared" si="3"/>
-        <v>-1174275</v>
+        <v>479225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 6-Jul-2021, end of day update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="68">
   <si>
     <t>Tgl</t>
   </si>
@@ -204,6 +204,24 @@
   </si>
   <si>
     <t>FREIGHT - OUT</t>
+  </si>
+  <si>
+    <t>PLN - Astar 214</t>
+  </si>
+  <si>
+    <t>SALES - cash/retail</t>
+  </si>
+  <si>
+    <t>SELISIH - lebih</t>
+  </si>
+  <si>
+    <t>SETOR KE BANK</t>
+  </si>
+  <si>
+    <t>TAX - P.Tata</t>
+  </si>
+  <si>
+    <t>TAX - Iuran ARIESTA</t>
   </si>
 </sst>
 </file>
@@ -571,8 +589,8 @@
   <dimension ref="A1:L114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <pane ySplit="2" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -619,12 +637,12 @@
         <v>25</v>
       </c>
       <c r="D3" s="1">
-        <f>60000</f>
-        <v>60000</v>
+        <f>60000+260000</f>
+        <v>320000</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E35" si="0">E2+C3-D3</f>
-        <v>227225</v>
+        <v>-32775</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -632,12 +650,12 @@
         <v>60</v>
       </c>
       <c r="C4" s="1">
-        <f>1000000+2681000+1545000</f>
-        <v>5226000</v>
+        <f>1000000+2681000+1545000+76848000</f>
+        <v>82074000</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>5453225</v>
+        <v>82041225</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -650,7 +668,7 @@
       </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>-5781775</v>
+        <v>70806225</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -663,659 +681,719 @@
       </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>-5841775</v>
+        <v>70746225</v>
       </c>
     </row>
     <row r="7" spans="1:6">
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="1">
+        <v>102500</v>
+      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>-5841775</v>
+        <v>70643725</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="1">
+        <f>5944275+82502725-76848000</f>
+        <v>11599000</v>
+      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>-5841775</v>
+        <v>82242725</v>
       </c>
     </row>
     <row r="9" spans="1:6">
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="1">
+        <v>20000</v>
+      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>-5841775</v>
+        <v>82262725</v>
       </c>
     </row>
     <row r="10" spans="1:6">
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="1">
+        <v>82000000</v>
+      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>-5841775</v>
+        <v>262725</v>
       </c>
     </row>
     <row r="11" spans="1:6">
+      <c r="A11" s="2">
+        <v>44383</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="1">
+        <f>60000</f>
+        <v>60000</v>
+      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>-5841775</v>
+        <v>202725</v>
       </c>
     </row>
     <row r="12" spans="1:6">
+      <c r="B12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="1">
+        <v>200000</v>
+      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>-5841775</v>
+        <v>2725</v>
       </c>
     </row>
     <row r="13" spans="1:6">
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="1">
+        <v>660000</v>
+      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>-5841775</v>
+        <v>-657275</v>
       </c>
     </row>
     <row r="14" spans="1:6">
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="1">
+        <f>4500000+432000+632000</f>
+        <v>5564000</v>
+      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>-5841775</v>
+        <v>-6221275</v>
       </c>
     </row>
     <row r="15" spans="1:6">
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="1">
+        <v>8000</v>
+      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="17" spans="5:5">
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="18" spans="5:5">
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="19" spans="5:5">
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="20" spans="5:5">
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="21" spans="5:5">
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="22" spans="5:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="23" spans="5:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="24" spans="5:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="25" spans="5:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="26" spans="5:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="27" spans="5:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="28" spans="5:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="29" spans="5:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="30" spans="5:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="31" spans="5:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="32" spans="5:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" si="0"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" ref="E36:E67" si="1">E35+C36-D36</f>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
       <c r="F41" s="1"/>
     </row>
     <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
       <c r="F52" s="1"/>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" si="1"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" ref="E68:E99" si="2">E67+C68-D68</f>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
       <c r="G80" s="1"/>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" si="2"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" ref="E100:E114" si="3">E99+C100-D100</f>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
     <row r="114" spans="5:5">
       <c r="E114" s="1">
         <f t="shared" si="3"/>
-        <v>-5841775</v>
+        <v>-6229275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 7-Jul-2021, end of day update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="69">
   <si>
     <t>Tgl</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>TAX - Iuran ARIESTA</t>
+  </si>
+  <si>
+    <t>STNK - suzuki</t>
   </si>
 </sst>
 </file>
@@ -589,8 +592,8 @@
   <dimension ref="A1:L114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
+      <pane ySplit="2" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -742,12 +745,12 @@
         <v>25</v>
       </c>
       <c r="D11" s="1">
-        <f>60000</f>
-        <v>60000</v>
+        <f>60000+260000</f>
+        <v>320000</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>202725</v>
+        <v>-57275</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -759,7 +762,7 @@
       </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>2725</v>
+        <v>-257275</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -771,7 +774,7 @@
       </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>-657275</v>
+        <v>-917275</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -779,12 +782,12 @@
         <v>59</v>
       </c>
       <c r="D14" s="1">
-        <f>4500000+432000+632000</f>
-        <v>5564000</v>
+        <f>4500000+432000+642000+4429000</f>
+        <v>10003000</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>-6221275</v>
+        <v>-10920275</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -796,604 +799,668 @@
       </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>-6229275</v>
+        <v>-10928275</v>
       </c>
     </row>
     <row r="16" spans="1:6">
+      <c r="B16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="1">
+        <f>12960000</f>
+        <v>12960000</v>
+      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>-6229275</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5">
+        <v>2031725</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="1">
+        <f>6498725+10928275-12960000</f>
+        <v>4467000</v>
+      </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>-6229275</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5">
+        <v>6498725</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="B18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="1">
+        <v>460000</v>
+      </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>-6229275</v>
-      </c>
-    </row>
-    <row r="19" spans="5:5">
+        <v>6958725</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="B19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="1">
+        <v>6000000</v>
+      </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>-6229275</v>
-      </c>
-    </row>
-    <row r="20" spans="5:5">
+        <v>958725</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="2">
+        <v>44384</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="1">
+        <f>60000</f>
+        <v>60000</v>
+      </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>-6229275</v>
-      </c>
-    </row>
-    <row r="21" spans="5:5">
+        <v>898725</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="1">
+        <f>1405000+1864000+6027200+9027000+3000000+9027000+2606000+1897000</f>
+        <v>34853200</v>
+      </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>-6229275</v>
-      </c>
-    </row>
-    <row r="22" spans="5:5">
+        <v>-33954475</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="B22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="1">
+        <f>529000</f>
+        <v>529000</v>
+      </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>-6229275</v>
-      </c>
-    </row>
-    <row r="23" spans="5:5">
+        <v>-34483475</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="B23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="1">
+        <f>6027200+9027000+3000000+9027000+29760000+2281500+1897000</f>
+        <v>61019700</v>
+      </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>-6229275</v>
-      </c>
-    </row>
-    <row r="24" spans="5:5">
+        <v>26536225</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="B24" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="1">
+        <f>60000</f>
+        <v>60000</v>
+      </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>-6229275</v>
-      </c>
-    </row>
-    <row r="25" spans="5:5">
+        <v>26476225</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>-6229275</v>
-      </c>
-    </row>
-    <row r="26" spans="5:5">
+        <v>26476225</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>-6229275</v>
-      </c>
-    </row>
-    <row r="27" spans="5:5">
+        <v>26476225</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>-6229275</v>
-      </c>
-    </row>
-    <row r="28" spans="5:5">
+        <v>26476225</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>-6229275</v>
-      </c>
-    </row>
-    <row r="29" spans="5:5">
+        <v>26476225</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>-6229275</v>
-      </c>
-    </row>
-    <row r="30" spans="5:5">
+        <v>26476225</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>-6229275</v>
-      </c>
-    </row>
-    <row r="31" spans="5:5">
+        <v>26476225</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>-6229275</v>
-      </c>
-    </row>
-    <row r="32" spans="5:5">
+        <v>26476225</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" si="0"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" ref="E36:E67" si="1">E35+C36-D36</f>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
       <c r="F41" s="1"/>
     </row>
     <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
       <c r="F52" s="1"/>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" si="1"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" ref="E68:E99" si="2">E67+C68-D68</f>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
       <c r="G80" s="1"/>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" si="2"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" ref="E100:E114" si="3">E99+C100-D100</f>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
     <row r="114" spans="5:5">
       <c r="E114" s="1">
         <f t="shared" si="3"/>
-        <v>-6229275</v>
+        <v>26476225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 12-Jul-2021, end of day update.
</commit_message>
<xml_diff>
--- a/petty-cashBook-2021.xlsx
+++ b/petty-cashBook-2021.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="64">
   <si>
     <t>Tgl</t>
   </si>
@@ -203,31 +203,13 @@
     <t>A/R</t>
   </si>
   <si>
-    <t>FREIGHT - OUT</t>
-  </si>
-  <si>
-    <t>PLN - Astar 214</t>
-  </si>
-  <si>
-    <t>SALES - cash/retail</t>
-  </si>
-  <si>
-    <t>SELISIH - lebih</t>
-  </si>
-  <si>
-    <t>SETOR KE BANK</t>
-  </si>
-  <si>
-    <t>TAX - P.Tata</t>
-  </si>
-  <si>
-    <t>TAX - Iuran ARIESTA</t>
-  </si>
-  <si>
-    <t>STNK - suzuki</t>
-  </si>
-  <si>
-    <t>SOLAR - kijang D-1682-QU</t>
+    <t>BELI - beras</t>
+  </si>
+  <si>
+    <t>FREIGHT OUT</t>
+  </si>
+  <si>
+    <t>A/P</t>
   </si>
 </sst>
 </file>
@@ -595,8 +577,8 @@
   <dimension ref="A1:L114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -632,74 +614,74 @@
         <v>5</v>
       </c>
       <c r="E2" s="1">
-        <v>287225</v>
+        <v>271225</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>44382</v>
+        <v>44389</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="1">
-        <f>60000+260000</f>
-        <v>320000</v>
+        <f>60000</f>
+        <v>60000</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E35" si="0">E2+C3-D3</f>
-        <v>-32775</v>
+        <v>211225</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="B4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="1">
-        <f>1000000+2681000+1545000+76848000</f>
-        <v>82074000</v>
+        <v>61</v>
+      </c>
+      <c r="D4" s="1">
+        <v>290000</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>82041225</v>
+        <v>-78775</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="B5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D5" s="1">
-        <f>2500000+1416000+510000+640000+2681000+1943000+1545000</f>
-        <v>11235000</v>
+        <f>144000</f>
+        <v>144000</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>70806225</v>
+        <v>-222775</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="B6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D6" s="1">
-        <f>60000</f>
-        <v>60000</v>
+        <f>406000+280000+4600000+5000000+3000000+41430000+3490000+580000+6560000</f>
+        <v>65346000</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>70746225</v>
+        <v>-65568775</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="B7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="1">
-        <v>102500</v>
+        <v>60</v>
+      </c>
+      <c r="C7" s="1">
+        <f>5000000+875000+41430000+6560000</f>
+        <v>53865000</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>70643725</v>
+        <v>-11703775</v>
       </c>
       <c r="F7" s="1"/>
     </row>
@@ -707,838 +689,652 @@
       <c r="B8" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="1">
-        <f>5944275+82502725-76848000</f>
-        <v>11599000</v>
+      <c r="D8" s="1">
+        <f>1051200</f>
+        <v>1051200</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>82242725</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="B9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="1">
-        <v>20000</v>
-      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>82262725</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="B10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="1">
-        <v>82000000</v>
-      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>262725</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="2">
-        <v>44383</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="1">
-        <f>60000+260000</f>
-        <v>320000</v>
-      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>-57275</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="B12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" s="1">
-        <v>200000</v>
-      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>-257275</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13" s="1">
-        <v>660000</v>
-      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>-917275</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="B14" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="1">
-        <f>4500000+432000+642000+4429000</f>
-        <v>10003000</v>
-      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>-10920275</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="B15" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" s="1">
-        <v>8000</v>
-      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>-10928275</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="B16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="1">
-        <f>12960000</f>
-        <v>12960000</v>
-      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>2031725</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="B17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="1">
-        <f>6498725+10928275-12960000</f>
-        <v>4467000</v>
-      </c>
+        <v>-12754975</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5">
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>6498725</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="B18" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" s="1">
-        <v>460000</v>
-      </c>
+        <v>-12754975</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5">
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>6958725</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="B19" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" s="1">
-        <v>6000000</v>
-      </c>
+        <v>-12754975</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5">
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>958725</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="2">
-        <v>44384</v>
-      </c>
-      <c r="B20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="1">
-        <f>60000+260000</f>
-        <v>320000</v>
-      </c>
+        <v>-12754975</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5">
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>638725</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="B21" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="1">
-        <f>1405000+1864000+6027200+9027000+3000000+9027000+2606000+1897000+1740000</f>
-        <v>36593200</v>
-      </c>
+        <v>-12754975</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5">
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>-35954475</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="B22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" s="1">
-        <f>529000</f>
-        <v>529000</v>
-      </c>
+        <v>-12754975</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5">
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>-36483475</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="B23" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="1">
-        <f>6027200+9027000+3000000+9027000+29760000+2281500+1897000+14393000</f>
-        <v>75412700</v>
-      </c>
+        <v>-12754975</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5">
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>38929225</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="B24" t="s">
-        <v>61</v>
-      </c>
-      <c r="D24" s="1">
-        <f>60000</f>
-        <v>60000</v>
-      </c>
+        <v>-12754975</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5">
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>38869225</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="B25" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" s="1">
-        <f>41437225-24476225-14393000</f>
-        <v>2568000</v>
-      </c>
+        <v>-12754975</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5">
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>41437225</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="B26" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26" s="1">
-        <v>10000</v>
-      </c>
+        <v>-12754975</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5">
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>41447225</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="B27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D27" s="1">
-        <f>41000000</f>
-        <v>41000000</v>
-      </c>
+        <v>-12754975</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5">
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>447225</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="2">
-        <v>44385</v>
-      </c>
-      <c r="B28" t="s">
-        <v>25</v>
-      </c>
-      <c r="D28" s="1">
-        <f>60000+260000</f>
-        <v>320000</v>
-      </c>
+        <v>-12754975</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5">
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>127225</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="B29" t="s">
-        <v>59</v>
-      </c>
-      <c r="D29" s="1">
-        <f>4402000+6027000+800000+1510000</f>
-        <v>12739000</v>
-      </c>
+        <v>-12754975</v>
+      </c>
+    </row>
+    <row r="29" spans="5:5">
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>-12611775</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="B30" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="1">
-        <f>6027000+6926500</f>
-        <v>12953500</v>
-      </c>
+        <v>-12754975</v>
+      </c>
+    </row>
+    <row r="30" spans="5:5">
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>341725</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="B31" t="s">
-        <v>63</v>
-      </c>
-      <c r="C31" s="1">
-        <f>4146725+6324775-6926500</f>
-        <v>3545000</v>
-      </c>
+        <v>-12754975</v>
+      </c>
+    </row>
+    <row r="31" spans="5:5">
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>3886725</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="B32" t="s">
-        <v>69</v>
-      </c>
-      <c r="D32" s="1">
-        <v>300000</v>
-      </c>
+        <v>-12754975</v>
+      </c>
+    </row>
+    <row r="32" spans="5:5">
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>3586725</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="B33" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" s="1">
-        <v>29500</v>
-      </c>
+        <v>-12754975</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6">
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>3616225</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="B34" t="s">
-        <v>65</v>
-      </c>
-      <c r="D34" s="1">
-        <v>3000000</v>
-      </c>
+        <v>-12754975</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6">
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>616225</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="2">
-        <v>44386</v>
-      </c>
-      <c r="B35" t="s">
-        <v>25</v>
-      </c>
+        <v>-12754975</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6">
       <c r="E35" s="1">
         <f t="shared" si="0"/>
-        <v>616225</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>-12754975</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6">
       <c r="E36" s="1">
         <f t="shared" ref="E36:E67" si="1">E35+C36-D36</f>
-        <v>616225</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+        <v>-12754975</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6">
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>616225</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+        <v>-12754975</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6">
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>616225</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+        <v>-12754975</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6">
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>616225</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>-12754975</v>
+      </c>
+    </row>
+    <row r="40" spans="5:6">
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>616225</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+        <v>-12754975</v>
+      </c>
+    </row>
+    <row r="41" spans="5:6">
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="5:6">
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>616225</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>-12754975</v>
+      </c>
+    </row>
+    <row r="43" spans="5:6">
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>616225</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>-12754975</v>
+      </c>
+    </row>
+    <row r="44" spans="5:6">
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>616225</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>-12754975</v>
+      </c>
+    </row>
+    <row r="45" spans="5:6">
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>616225</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>-12754975</v>
+      </c>
+    </row>
+    <row r="46" spans="5:6">
       <c r="E46" s="1">
         <f t="shared" si="1"/>
-        <v>616225</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>-12754975</v>
+      </c>
+    </row>
+    <row r="47" spans="5:6">
       <c r="E47" s="1">
         <f t="shared" si="1"/>
-        <v>616225</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>-12754975</v>
+      </c>
+    </row>
+    <row r="48" spans="5:6">
       <c r="E48" s="1">
         <f t="shared" si="1"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="49" spans="5:6">
       <c r="E49" s="1">
         <f t="shared" si="1"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="50" spans="5:6">
       <c r="E50" s="1">
         <f t="shared" si="1"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="52" spans="5:6">
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
       <c r="F52" s="1"/>
     </row>
     <row r="53" spans="5:6">
       <c r="E53" s="1">
         <f t="shared" si="1"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="54" spans="5:6">
       <c r="E54" s="1">
         <f t="shared" si="1"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="55" spans="5:6">
       <c r="E55" s="1">
         <f t="shared" si="1"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="56" spans="5:6">
       <c r="E56" s="1">
         <f t="shared" si="1"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="57" spans="5:6">
       <c r="E57" s="1">
         <f t="shared" si="1"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="58" spans="5:6">
       <c r="E58" s="1">
         <f t="shared" si="1"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="59" spans="5:6">
       <c r="E59" s="1">
         <f t="shared" si="1"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="60" spans="5:6">
       <c r="E60" s="1">
         <f t="shared" si="1"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="61" spans="5:6">
       <c r="E61" s="1">
         <f t="shared" si="1"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="62" spans="5:6">
       <c r="E62" s="1">
         <f t="shared" si="1"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="63" spans="5:6">
       <c r="E63" s="1">
         <f t="shared" si="1"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="64" spans="5:6">
       <c r="E64" s="1">
         <f t="shared" si="1"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="65" spans="5:7">
       <c r="E65" s="1">
         <f t="shared" si="1"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="66" spans="5:7">
       <c r="E66" s="1">
         <f t="shared" si="1"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="67" spans="5:7">
       <c r="E67" s="1">
         <f t="shared" si="1"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="68" spans="5:7">
       <c r="E68" s="1">
         <f t="shared" ref="E68:E99" si="2">E67+C68-D68</f>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="69" spans="5:7">
       <c r="E69" s="1">
         <f t="shared" si="2"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="70" spans="5:7">
       <c r="E70" s="1">
         <f t="shared" si="2"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="71" spans="5:7">
       <c r="E71" s="1">
         <f t="shared" si="2"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="72" spans="5:7">
       <c r="E72" s="1">
         <f t="shared" si="2"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="73" spans="5:7">
       <c r="E73" s="1">
         <f t="shared" si="2"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="74" spans="5:7">
       <c r="E74" s="1">
         <f t="shared" si="2"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="75" spans="5:7">
       <c r="E75" s="1">
         <f t="shared" si="2"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="76" spans="5:7">
       <c r="E76" s="1">
         <f t="shared" si="2"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="77" spans="5:7">
       <c r="E77" s="1">
         <f t="shared" si="2"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="78" spans="5:7">
       <c r="E78" s="1">
         <f t="shared" si="2"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="79" spans="5:7">
       <c r="E79" s="1">
         <f t="shared" si="2"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="80" spans="5:7">
       <c r="E80" s="1">
         <f t="shared" si="2"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
       <c r="G80" s="1"/>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="1">
         <f t="shared" si="2"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" s="1">
         <f t="shared" si="2"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" s="1">
         <f t="shared" si="2"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" s="1">
         <f t="shared" si="2"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" s="1">
         <f t="shared" si="2"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" s="1">
         <f t="shared" si="2"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" s="1">
         <f t="shared" si="2"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" s="1">
         <f t="shared" si="2"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" s="1">
         <f t="shared" si="2"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" s="1">
         <f t="shared" si="2"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" s="1">
         <f t="shared" si="2"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" s="1">
         <f t="shared" si="2"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="93" spans="5:5">
       <c r="E93" s="1">
         <f t="shared" si="2"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="94" spans="5:5">
       <c r="E94" s="1">
         <f t="shared" si="2"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" s="1">
         <f t="shared" si="2"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="96" spans="5:5">
       <c r="E96" s="1">
         <f t="shared" si="2"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="97" spans="5:5">
       <c r="E97" s="1">
         <f t="shared" si="2"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" s="1">
         <f t="shared" si="2"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" s="1">
         <f t="shared" si="2"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="100" spans="5:5">
       <c r="E100" s="1">
         <f t="shared" ref="E100:E114" si="3">E99+C100-D100</f>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="101" spans="5:5">
       <c r="E101" s="1">
         <f t="shared" si="3"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" s="1">
         <f t="shared" si="3"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" s="1">
         <f t="shared" si="3"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" s="1">
         <f t="shared" si="3"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="105" spans="5:5">
       <c r="E105" s="1">
         <f t="shared" si="3"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="106" spans="5:5">
       <c r="E106" s="1">
         <f t="shared" si="3"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="107" spans="5:5">
       <c r="E107" s="1">
         <f t="shared" si="3"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="108" spans="5:5">
       <c r="E108" s="1">
         <f t="shared" si="3"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="109" spans="5:5">
       <c r="E109" s="1">
         <f t="shared" si="3"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="110" spans="5:5">
       <c r="E110" s="1">
         <f t="shared" si="3"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="111" spans="5:5">
       <c r="E111" s="1">
         <f t="shared" si="3"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" s="1">
         <f t="shared" si="3"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="113" spans="5:5">
       <c r="E113" s="1">
         <f t="shared" si="3"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
     <row r="114" spans="5:5">
       <c r="E114" s="1">
         <f t="shared" si="3"/>
-        <v>616225</v>
+        <v>-12754975</v>
       </c>
     </row>
   </sheetData>

</xml_diff>